<commit_message>
Column width as a single function.
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -446,10 +446,10 @@
     <col width="60" customWidth="1" min="5" max="5"/>
     <col width="5" customWidth="1" min="6" max="6"/>
     <col width="5" customWidth="1" min="7" max="7"/>
-    <col width="9" customWidth="1" min="8" max="8"/>
+    <col width="12.78" customWidth="1" min="8" max="8"/>
     <col width="9" customWidth="1" min="9" max="9"/>
     <col width="9" customWidth="1" min="10" max="10"/>
-    <col width="9" customWidth="1" min="11" max="11"/>
+    <col width="11.22" customWidth="1" min="11" max="11"/>
     <col width="25" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
LC match logic modularized
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -446,14 +446,14 @@
     <col width="9" customWidth="1" min="1" max="1"/>
     <col width="30" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10.33" customWidth="1" min="4" max="4"/>
     <col width="60" customWidth="1" min="5" max="5"/>
     <col width="5" customWidth="1" min="6" max="6"/>
     <col width="5" customWidth="1" min="7" max="7"/>
     <col width="12.78" customWidth="1" min="8" max="8"/>
     <col width="9" customWidth="1" min="9" max="9"/>
-    <col width="9" customWidth="1" min="10" max="10"/>
-    <col width="11.22" customWidth="1" min="11" max="11"/>
+    <col width="12.78" customWidth="1" min="10" max="10"/>
+    <col width="14.22" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Sequential MID for all matches
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -1316,8 +1316,16 @@
       <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
-      <c r="B44" t="inlineStr"/>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>M073</t>
+        </is>
+      </c>
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "FOB/PO/2023/8/5023", "lender_amount": "95200.00", "borrower_amount": "95200.00", "po_number": "FOB/PO/2023/8/5023"}</t>
+        </is>
+      </c>
       <c r="C44" t="inlineStr">
         <is>
           <t>01/Jan/2025</t>
@@ -1463,8 +1471,16 @@
       <c r="K49" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr"/>
-      <c r="B50" t="inlineStr"/>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>M074</t>
+        </is>
+      </c>
+      <c r="B50" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "FOB/PO/2023/12/5124", "lender_amount": "164204.00", "borrower_amount": "164204.00", "po_number": "FOB/PO/2023/12/5124"}</t>
+        </is>
+      </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>01/Jan/2025</t>
@@ -1544,7 +1560,7 @@
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "5040781.68", "borrower_amount": "5040781.68"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "5040781.68", "borrower_amount": "5040781.68", "lc_number": "L/C-308524022796/24"}</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1625,7 +1641,7 @@
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "15737222.22", "borrower_amount": "15737222.22"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "15737222.22", "borrower_amount": "15737222.22", "lc_number": "L/C-308524022796/24"}</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1909,7 +1925,7 @@
       </c>
       <c r="B68" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "8884.77", "borrower_amount": "8884.77"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "8884.77", "borrower_amount": "8884.77", "lc_number": "L/C-308524022796/24"}</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1990,7 +2006,7 @@
       </c>
       <c r="B71" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "1575.00", "borrower_amount": "1575.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "1575.00", "borrower_amount": "1575.00", "lc_number": "L/C-308524027065/24"}</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2363,7 +2379,7 @@
       </c>
       <c r="B86" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-187724010124/24", "lender_amount": "1150.00", "borrower_amount": "1150.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-187724010124/24", "lender_amount": "1150.00", "borrower_amount": "1150.00", "lc_number": "L/C-187724010124/24"}</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2444,7 +2460,7 @@
       </c>
       <c r="B89" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "1575.00", "borrower_amount": "1575.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "1575.00", "borrower_amount": "1575.00", "lc_number": "L/C-308524027065/24"}</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2890,7 +2906,7 @@
       </c>
       <c r="B107" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "26246.93", "borrower_amount": "26246.93"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "26246.93", "borrower_amount": "26246.93", "lc_number": "L/C-308524022796/24"}</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4096,8 +4112,16 @@
       <c r="K161" t="inlineStr"/>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr"/>
-      <c r="B162" t="inlineStr"/>
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>M075</t>
+        </is>
+      </c>
+      <c r="B162" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "FOB/PO/2023/8/5000", "lender_amount": "289000.00", "borrower_amount": "289000.00", "po_number": "FOB/PO/2023/8/5000"}</t>
+        </is>
+      </c>
       <c r="C162" t="inlineStr">
         <is>
           <t>01/Feb/2025</t>
@@ -5712,7 +5736,7 @@
       </c>
       <c r="B229" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-187724010124/24", "lender_amount": "1150.00", "borrower_amount": "1150.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-187724010124/24", "lender_amount": "1150.00", "borrower_amount": "1150.00", "lc_number": "L/C-187724010124/24"}</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -5866,7 +5890,7 @@
       </c>
       <c r="B235" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-187724010124/24", "lender_amount": "8761.79", "borrower_amount": "8761.79"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-187724010124/24", "lender_amount": "8761.79", "borrower_amount": "8761.79", "lc_number": "L/C-187724010124/24"}</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -6350,7 +6374,7 @@
       </c>
       <c r="B255" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "1862.50", "borrower_amount": "1862.50"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "1862.50", "borrower_amount": "1862.50", "lc_number": "L/C-308524027065/24"}</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -6853,7 +6877,7 @@
       </c>
       <c r="B276" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020003/25", "lender_amount": "27383.77", "borrower_amount": "27383.77"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020003/25", "lender_amount": "27383.77", "borrower_amount": "27383.77", "lc_number": "L/C-147125020003/25"}</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -7606,8 +7630,16 @@
       <c r="K307" t="inlineStr"/>
     </row>
     <row r="308">
-      <c r="A308" t="inlineStr"/>
-      <c r="B308" t="inlineStr"/>
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>M076</t>
+        </is>
+      </c>
+      <c r="B308" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2024/6/27130", "lender_amount": "1100.00", "borrower_amount": "1100.00", "po_number": "OPE/PO/2024/6/27130"}</t>
+        </is>
+      </c>
       <c r="C308" t="inlineStr">
         <is>
           <t>16/Feb/2025</t>
@@ -8308,7 +8340,7 @@
       </c>
       <c r="B337" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524990243/24", "lender_amount": "71971.54", "borrower_amount": "71971.54"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524990243/24", "lender_amount": "71971.54", "borrower_amount": "71971.54", "lc_number": "L/C-308524990243/24"}</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
@@ -8389,7 +8421,7 @@
       </c>
       <c r="B340" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524990243/24", "lender_amount": "20527984.90", "borrower_amount": "20527984.90"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524990243/24", "lender_amount": "20527984.90", "borrower_amount": "20527984.90", "lc_number": "L/C-308524990243/24"}</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
@@ -8470,7 +8502,7 @@
       </c>
       <c r="B343" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147124020653/25", "lender_amount": "665048.82", "borrower_amount": "665048.82"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147124020653/25", "lender_amount": "665048.82", "borrower_amount": "665048.82", "lc_number": "L/C-147124020653/25"}</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
@@ -8551,7 +8583,7 @@
       </c>
       <c r="B346" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147124020708/24", "lender_amount": "25042.61", "borrower_amount": "25042.61"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147124020708/24", "lender_amount": "25042.61", "borrower_amount": "25042.61", "lc_number": "L/C-147124020708/24"}</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
@@ -8925,7 +8957,7 @@
       </c>
       <c r="B361" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020063/25", "lender_amount": "5995080.00", "borrower_amount": "5995080.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020063/25", "lender_amount": "5995080.00", "borrower_amount": "5995080.00", "lc_number": "L/C-141325020063/25"}</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
@@ -9006,7 +9038,7 @@
       </c>
       <c r="B364" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020068/25", "lender_amount": "33573.89", "borrower_amount": "33573.89"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020068/25", "lender_amount": "33573.89", "borrower_amount": "33573.89", "lc_number": "L/C-141325020068/25"}</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
@@ -9087,7 +9119,7 @@
       </c>
       <c r="B367" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020068/25", "lender_amount": "1650660.00", "borrower_amount": "1650660.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020068/25", "lender_amount": "1650660.00", "borrower_amount": "1650660.00", "lc_number": "L/C-141325020068/25"}</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
@@ -9308,8 +9340,16 @@
       <c r="K375" t="inlineStr"/>
     </row>
     <row r="376">
-      <c r="A376" t="inlineStr"/>
-      <c r="B376" t="inlineStr"/>
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>M077</t>
+        </is>
+      </c>
+      <c r="B376" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "GEO/PO/2023/3/12915", "lender_amount": "400000.00", "borrower_amount": "400000.00", "po_number": "GEO/PO/2023/3/12915"}</t>
+        </is>
+      </c>
       <c r="C376" t="inlineStr">
         <is>
           <t>27/Feb/2025</t>
@@ -9388,7 +9428,7 @@
       </c>
       <c r="B379" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-155824020001/24", "lender_amount": "7641878.37", "borrower_amount": "7641878.37"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-155824020001/24", "lender_amount": "7641878.37", "borrower_amount": "7641878.37", "lc_number": "LC-155824020001/24"}</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
@@ -10531,7 +10571,7 @@
       </c>
       <c r="B432" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020063/25", "lender_amount": "246401.97", "borrower_amount": "246401.97"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020063/25", "lender_amount": "246401.97", "borrower_amount": "246401.97", "lc_number": "L/C-141325020063/25"}</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
@@ -10758,7 +10798,7 @@
       </c>
       <c r="B441" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "26369.63", "borrower_amount": "26369.63"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "26369.63", "borrower_amount": "26369.63", "lc_number": "L/C-308524022796/24"}</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
@@ -11162,8 +11202,16 @@
       <c r="K457" t="inlineStr"/>
     </row>
     <row r="458">
-      <c r="A458" t="inlineStr"/>
-      <c r="B458" t="inlineStr"/>
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>M078</t>
+        </is>
+      </c>
+      <c r="B458" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2024/9/29742", "lender_amount": "124670.00", "borrower_amount": "124670.00", "po_number": "OPE/PO/2024/9/29742"}</t>
+        </is>
+      </c>
       <c r="C458" t="inlineStr">
         <is>
           <t>05/Mar/2025</t>
@@ -11242,7 +11290,7 @@
       </c>
       <c r="B461" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-222825150235/25", "lender_amount": "2357.50", "borrower_amount": "2357.50"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-222825150235/25", "lender_amount": "2357.50", "borrower_amount": "2357.50", "lc_number": "L/C-222825150235/25"}</t>
         </is>
       </c>
       <c r="C461" t="inlineStr">
@@ -11396,7 +11444,7 @@
       </c>
       <c r="B467" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-222825150235/25", "lender_amount": "213500.00", "borrower_amount": "213500.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-222825150235/25", "lender_amount": "213500.00", "borrower_amount": "213500.00", "lc_number": "L/C-222825150235/25"}</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
@@ -11477,7 +11525,7 @@
       </c>
       <c r="B470" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "1725.00", "borrower_amount": "1725.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "1725.00", "borrower_amount": "1725.00", "lc_number": "L/C-308524027065/24"}</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
@@ -11558,7 +11606,7 @@
       </c>
       <c r="B473" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-187724010122/24", "lender_amount": "276518.90", "borrower_amount": "276518.90"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-187724010122/24", "lender_amount": "276518.90", "borrower_amount": "276518.90", "lc_number": "L/C-187724010122/24"}</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
@@ -12407,7 +12455,7 @@
       </c>
       <c r="B508" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020027/25", "lender_amount": "54431.58", "borrower_amount": "54431.58"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020027/25", "lender_amount": "54431.58", "borrower_amount": "54431.58", "lc_number": "L/C-147125020027/25"}</t>
         </is>
       </c>
       <c r="C508" t="inlineStr">
@@ -12707,7 +12755,7 @@
       </c>
       <c r="B520" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "8231.99", "borrower_amount": "8231.99"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "8231.99", "borrower_amount": "8231.99", "lc_number": "L/C-308524027065/24"}</t>
         </is>
       </c>
       <c r="C520" t="inlineStr">
@@ -13825,7 +13873,7 @@
       </c>
       <c r="B570" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147124020708/24", "lender_amount": "19399.10", "borrower_amount": "19399.10"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147124020708/24", "lender_amount": "19399.10", "borrower_amount": "19399.10", "lc_number": "L/C-147124020708/24"}</t>
         </is>
       </c>
       <c r="C570" t="inlineStr">
@@ -13906,7 +13954,7 @@
       </c>
       <c r="B573" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524990243/24", "lender_amount": "15160.97", "borrower_amount": "15160.97"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524990243/24", "lender_amount": "15160.97", "borrower_amount": "15160.97", "lc_number": "L/C-308524990243/24"}</t>
         </is>
       </c>
       <c r="C573" t="inlineStr">
@@ -14136,7 +14184,7 @@
       </c>
       <c r="B583" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020104/25", "lender_amount": "6125933.94", "borrower_amount": "6125933.94"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020104/25", "lender_amount": "6125933.94", "borrower_amount": "6125933.94", "lc_number": "L/C-141325020104/25"}</t>
         </is>
       </c>
       <c r="C583" t="inlineStr">
@@ -14255,7 +14303,7 @@
       </c>
       <c r="B588" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022495/24", "lender_amount": "12425.77", "borrower_amount": "12425.77"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022495/24", "lender_amount": "12425.77", "borrower_amount": "12425.77", "lc_number": "L/C-308524022495/24"}</t>
         </is>
       </c>
       <c r="C588" t="inlineStr">
@@ -14336,7 +14384,7 @@
       </c>
       <c r="B591" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022495/24", "lender_amount": "23580.68", "borrower_amount": "23580.68"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022495/24", "lender_amount": "23580.68", "borrower_amount": "23580.68", "lc_number": "L/C-308524022495/24"}</t>
         </is>
       </c>
       <c r="C591" t="inlineStr">
@@ -14410,8 +14458,16 @@
       <c r="K593" t="inlineStr"/>
     </row>
     <row r="594">
-      <c r="A594" t="inlineStr"/>
-      <c r="B594" t="inlineStr"/>
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>M079</t>
+        </is>
+      </c>
+      <c r="B594" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "MBD/PO/2024/9/10", "lender_amount": "25000.00", "borrower_amount": "25000.00", "po_number": "MBD/PO/2024/9/10"}</t>
+        </is>
+      </c>
       <c r="C594" t="inlineStr">
         <is>
           <t>31/Mar/2025</t>
@@ -15177,8 +15233,16 @@
       <c r="K630" t="inlineStr"/>
     </row>
     <row r="631">
-      <c r="A631" t="inlineStr"/>
-      <c r="B631" t="inlineStr"/>
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>M080</t>
+        </is>
+      </c>
+      <c r="B631" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "CHA/PO/2023/12/20766", "lender_amount": "2000000.00", "borrower_amount": "2000000.00", "po_number": "CHA/PO/2023/12/20766"}</t>
+        </is>
+      </c>
       <c r="C631" t="inlineStr">
         <is>
           <t>01/Apr/2025</t>
@@ -15403,7 +15467,7 @@
       </c>
       <c r="B640" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308525021741/25", "lender_amount": "22671.95", "borrower_amount": "22671.95"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308525021741/25", "lender_amount": "22671.95", "borrower_amount": "22671.95", "lc_number": "L/C-308525021741/25"}</t>
         </is>
       </c>
       <c r="C640" t="inlineStr">
@@ -15484,7 +15548,7 @@
       </c>
       <c r="B643" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308525021745/25", "lender_amount": "28854.86", "borrower_amount": "28854.86"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308525021745/25", "lender_amount": "28854.86", "borrower_amount": "28854.86", "lc_number": "L/C-308525021745/25"}</t>
         </is>
       </c>
       <c r="C643" t="inlineStr">
@@ -15565,7 +15629,7 @@
       </c>
       <c r="B646" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524026037/24", "lender_amount": "1725.00", "borrower_amount": "1725.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524026037/24", "lender_amount": "1725.00", "borrower_amount": "1725.00", "lc_number": "L/C-308524026037/24"}</t>
         </is>
       </c>
       <c r="C646" t="inlineStr">
@@ -16157,7 +16221,7 @@
       </c>
       <c r="B670" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020063/25", "lender_amount": "80051.03", "borrower_amount": "80051.03"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020063/25", "lender_amount": "80051.03", "borrower_amount": "80051.03", "lc_number": "LC-141325020063/25"}</t>
         </is>
       </c>
       <c r="C670" t="inlineStr">
@@ -16238,7 +16302,7 @@
       </c>
       <c r="B673" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020063/25", "lender_amount": "6777058.20", "borrower_amount": "6777058.20"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020063/25", "lender_amount": "6777058.20", "borrower_amount": "6777058.20", "lc_number": "L/C-141325020063/25"}</t>
         </is>
       </c>
       <c r="C673" t="inlineStr">
@@ -16430,7 +16494,7 @@
       </c>
       <c r="B681" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-155823010186/23", "lender_amount": "76000.00", "borrower_amount": "76000.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-155823010186/23", "lender_amount": "76000.00", "borrower_amount": "76000.00", "lc_number": "L/C-155823010186/23"}</t>
         </is>
       </c>
       <c r="C681" t="inlineStr">
@@ -16768,7 +16832,7 @@
       </c>
       <c r="B695" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524026037/222824023549", "lender_amount": "1226351.09", "borrower_amount": "1226351.09"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524026037/222824023549", "lender_amount": "1226351.09", "borrower_amount": "1226351.09", "lc_number": "LC-308524026037/222824023549"}</t>
         </is>
       </c>
       <c r="C695" t="inlineStr">
@@ -16922,7 +16986,7 @@
       </c>
       <c r="B701" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524022495/24", "lender_amount": "1675000.00", "borrower_amount": "1675000.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524022495/24", "lender_amount": "1675000.00", "borrower_amount": "1675000.00", "lc_number": "LC-308524022495/24"}</t>
         </is>
       </c>
       <c r="C701" t="inlineStr">
@@ -17149,7 +17213,7 @@
       </c>
       <c r="B710" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020027/25", "lender_amount": "10691988.92", "borrower_amount": "10691988.92"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020027/25", "lender_amount": "10691988.92", "borrower_amount": "10691988.92", "lc_number": "L/C-147125020027/25"}</t>
         </is>
       </c>
       <c r="C710" t="inlineStr">
@@ -17230,7 +17294,7 @@
       </c>
       <c r="B713" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-222825150151/25", "lender_amount": "333706.76", "borrower_amount": "333706.76"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-222825150151/25", "lender_amount": "333706.76", "borrower_amount": "333706.76", "lc_number": "L/C-222825150151/25"}</t>
         </is>
       </c>
       <c r="C713" t="inlineStr">
@@ -17311,7 +17375,7 @@
       </c>
       <c r="B716" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020063/25", "lender_amount": "299000.00", "borrower_amount": "299000.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020063/25", "lender_amount": "299000.00", "borrower_amount": "299000.00", "lc_number": "L/C-141325020063/25"}</t>
         </is>
       </c>
       <c r="C716" t="inlineStr">
@@ -17465,7 +17529,7 @@
       </c>
       <c r="B722" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524026037/24", "lender_amount": "13743.52", "borrower_amount": "13743.52"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524026037/24", "lender_amount": "13743.52", "borrower_amount": "13743.52", "lc_number": "L/C-308524026037/24"}</t>
         </is>
       </c>
       <c r="C722" t="inlineStr">
@@ -17787,7 +17851,7 @@
       </c>
       <c r="B736" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-155825020020/25", "lender_amount": "60302.55", "borrower_amount": "60302.55"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-155825020020/25", "lender_amount": "60302.55", "borrower_amount": "60302.55", "lc_number": "LC-155825020020/25"}</t>
         </is>
       </c>
       <c r="C736" t="inlineStr">
@@ -17868,7 +17932,7 @@
       </c>
       <c r="B739" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020104/25", "lender_amount": "124008.78", "borrower_amount": "124008.78"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020104/25", "lender_amount": "124008.78", "borrower_amount": "124008.78", "lc_number": "L/C-141325020104/25"}</t>
         </is>
       </c>
       <c r="C739" t="inlineStr">
@@ -17949,7 +18013,7 @@
       </c>
       <c r="B742" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020063/25", "lender_amount": "31609.80", "borrower_amount": "31609.80"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020063/25", "lender_amount": "31609.80", "borrower_amount": "31609.80", "lc_number": "LC-141325020063/25"}</t>
         </is>
       </c>
       <c r="C742" t="inlineStr">
@@ -18433,7 +18497,7 @@
       </c>
       <c r="B762" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020104/25", "lender_amount": "10424886.36", "borrower_amount": "10424886.36"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020104/25", "lender_amount": "10424886.36", "borrower_amount": "10424886.36", "lc_number": "L/C-141325020104/25"}</t>
         </is>
       </c>
       <c r="C762" t="inlineStr">
@@ -18514,7 +18578,7 @@
       </c>
       <c r="B765" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020063/25", "lender_amount": "2168751.40", "borrower_amount": "2168751.40"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020063/25", "lender_amount": "2168751.40", "borrower_amount": "2168751.40", "lc_number": "L/C-147125020063/25"}</t>
         </is>
       </c>
       <c r="C765" t="inlineStr">
@@ -18668,7 +18732,7 @@
       </c>
       <c r="B771" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020068/25", "lender_amount": "63787.54", "borrower_amount": "63787.54"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020068/25", "lender_amount": "63787.54", "borrower_amount": "63787.54", "lc_number": "L/C-141325020068/25"}</t>
         </is>
       </c>
       <c r="C771" t="inlineStr">
@@ -19583,8 +19647,16 @@
       <c r="K813" t="inlineStr"/>
     </row>
     <row r="814">
-      <c r="A814" t="inlineStr"/>
-      <c r="B814" t="inlineStr"/>
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>M081</t>
+        </is>
+      </c>
+      <c r="B814" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "BPD/PO/2025/3/32659", "lender_amount": "768000.00", "borrower_amount": "768000.00", "po_number": "BPD/PO/2025/3/32659"}</t>
+        </is>
+      </c>
       <c r="C814" t="inlineStr">
         <is>
           <t>01/May/2025</t>
@@ -19875,8 +19947,16 @@
       <c r="K825" t="inlineStr"/>
     </row>
     <row r="826">
-      <c r="A826" t="inlineStr"/>
-      <c r="B826" t="inlineStr"/>
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>M082</t>
+        </is>
+      </c>
+      <c r="B826" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2023/10/18781", "lender_amount": "13920.00", "borrower_amount": "13920.00", "po_number": "OPE/PO/2023/10/18781"}</t>
+        </is>
+      </c>
       <c r="C826" t="inlineStr">
         <is>
           <t>01/May/2025</t>
@@ -22132,7 +22212,7 @@
       </c>
       <c r="B920" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020104/25", "lender_amount": "111771.42", "borrower_amount": "111771.42"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020104/25", "lender_amount": "111771.42", "borrower_amount": "111771.42", "lc_number": "LC-141325020104/25"}</t>
         </is>
       </c>
       <c r="C920" t="inlineStr">
@@ -22213,7 +22293,7 @@
       </c>
       <c r="B923" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020112/25", "lender_amount": "80701.76", "borrower_amount": "80701.76"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020112/25", "lender_amount": "80701.76", "borrower_amount": "80701.76", "lc_number": "LC-141325020112/25"}</t>
         </is>
       </c>
       <c r="C923" t="inlineStr">
@@ -22294,7 +22374,7 @@
       </c>
       <c r="B926" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020112/25", "lender_amount": "657.81", "borrower_amount": "657.81"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020112/25", "lender_amount": "657.81", "borrower_amount": "657.81", "lc_number": "LC-141325020112/25"}</t>
         </is>
       </c>
       <c r="C926" t="inlineStr">
@@ -22667,7 +22747,7 @@
       </c>
       <c r="B941" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020063/25", "lender_amount": "81730.06", "borrower_amount": "81730.06"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020063/25", "lender_amount": "81730.06", "borrower_amount": "81730.06", "lc_number": "LC-141325020063/25"}</t>
         </is>
       </c>
       <c r="C941" t="inlineStr">
@@ -23113,7 +23193,7 @@
       </c>
       <c r="B959" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020163/25", "lender_amount": "341847.68", "borrower_amount": "341847.68"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020163/25", "lender_amount": "341847.68", "borrower_amount": "341847.68", "lc_number": "LC-141325020163/25"}</t>
         </is>
       </c>
       <c r="C959" t="inlineStr">
@@ -23416,7 +23496,7 @@
       </c>
       <c r="B972" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-222825150235/25", "lender_amount": "36757.00", "borrower_amount": "36757.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-222825150235/25", "lender_amount": "36757.00", "borrower_amount": "36757.00", "lc_number": "LC-222825150235/25"}</t>
         </is>
       </c>
       <c r="C972" t="inlineStr">
@@ -23570,7 +23650,7 @@
       </c>
       <c r="B978" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020068/25", "lender_amount": "3587219.00", "borrower_amount": "3587219.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020068/25", "lender_amount": "3587219.00", "borrower_amount": "3587219.00", "lc_number": "LC-141325020068/25"}</t>
         </is>
       </c>
       <c r="C978" t="inlineStr">
@@ -23708,7 +23788,7 @@
       </c>
       <c r="B984" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524990243/24", "lender_amount": "68747.06", "borrower_amount": "68747.06"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524990243/24", "lender_amount": "68747.06", "borrower_amount": "68747.06", "lc_number": "LC-308524990243/24"}</t>
         </is>
       </c>
       <c r="C984" t="inlineStr">
@@ -24323,7 +24403,7 @@
       </c>
       <c r="B1010" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308525021741/25", "lender_amount": "31411.11", "borrower_amount": "31411.11"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308525021741/25", "lender_amount": "31411.11", "borrower_amount": "31411.11", "lc_number": "LC-308525021741/25"}</t>
         </is>
       </c>
       <c r="C1010" t="inlineStr">
@@ -24397,8 +24477,16 @@
       <c r="K1012" t="inlineStr"/>
     </row>
     <row r="1013">
-      <c r="A1013" t="inlineStr"/>
-      <c r="B1013" t="inlineStr"/>
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>M083</t>
+        </is>
+      </c>
+      <c r="B1013" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "MOD/PO/2024/10/30061", "lender_amount": "89910.00", "borrower_amount": "89910.00", "po_number": "MOD/PO/2024/10/30061"}</t>
+        </is>
+      </c>
       <c r="C1013" t="inlineStr">
         <is>
           <t>01/Jun/2025</t>
@@ -24543,8 +24631,16 @@
       <c r="K1018" t="inlineStr"/>
     </row>
     <row r="1019">
-      <c r="A1019" t="inlineStr"/>
-      <c r="B1019" t="inlineStr"/>
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>M084</t>
+        </is>
+      </c>
+      <c r="B1019" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2024/10/29964", "lender_amount": "24800.00", "borrower_amount": "24800.00", "po_number": "OPE/PO/2024/10/29964"}</t>
+        </is>
+      </c>
       <c r="C1019" t="inlineStr">
         <is>
           <t>02/Jun/2025</t>
@@ -24843,7 +24939,7 @@
       </c>
       <c r="B1031" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-155825010037/25", "lender_amount": "853297.01", "borrower_amount": "853297.01"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-155825010037/25", "lender_amount": "853297.01", "borrower_amount": "853297.01", "lc_number": "LC-155825010037/25"}</t>
         </is>
       </c>
       <c r="C1031" t="inlineStr">
@@ -26069,8 +26165,16 @@
       <c r="K1081" t="inlineStr"/>
     </row>
     <row r="1082">
-      <c r="A1082" t="inlineStr"/>
-      <c r="B1082" t="inlineStr"/>
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>M085</t>
+        </is>
+      </c>
+      <c r="B1082" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2025/4/33343", "lender_amount": "199850.00", "borrower_amount": "199850.00", "po_number": "OPE/PO/2025/4/33343"}</t>
+        </is>
+      </c>
       <c r="C1082" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
@@ -26142,8 +26246,16 @@
       <c r="K1084" t="inlineStr"/>
     </row>
     <row r="1085">
-      <c r="A1085" t="inlineStr"/>
-      <c r="B1085" t="inlineStr"/>
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>M086</t>
+        </is>
+      </c>
+      <c r="B1085" s="4" t="inlineStr">
+        <is>
+          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2024/11/30293", "lender_amount": "45094.20", "borrower_amount": "45094.20", "po_number": "OPE/PO/2024/11/30293"}</t>
+        </is>
+      </c>
       <c r="C1085" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
@@ -26514,7 +26626,7 @@
       </c>
       <c r="B1100" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020163/25", "lender_amount": "1725.00", "borrower_amount": "1725.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020163/25", "lender_amount": "1725.00", "borrower_amount": "1725.00", "lc_number": "LC-141325020163/25"}</t>
         </is>
       </c>
       <c r="C1100" t="inlineStr">
@@ -26595,7 +26707,7 @@
       </c>
       <c r="B1103" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308525021746/25", "lender_amount": "35373.50", "borrower_amount": "35373.50"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308525021746/25", "lender_amount": "35373.50", "borrower_amount": "35373.50", "lc_number": "LC-308525021746/25"}</t>
         </is>
       </c>
       <c r="C1103" t="inlineStr">
@@ -27152,7 +27264,7 @@
       </c>
       <c r="B1126" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020063/141325020112", "lender_amount": "576120.39", "borrower_amount": "576120.39"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020063/141325020112", "lender_amount": "576120.39", "borrower_amount": "576120.39", "lc_number": "LC-141325020063/141325020112"}</t>
         </is>
       </c>
       <c r="C1126" t="inlineStr">
@@ -27309,7 +27421,7 @@
       </c>
       <c r="B1133" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524022166 ", "lender_amount": "758000.00", "borrower_amount": "758000.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524022166 ", "lender_amount": "758000.00", "borrower_amount": "758000.00", "lc_number": "LC-308524022166 "}</t>
         </is>
       </c>
       <c r="C1133" t="inlineStr">
@@ -27974,7 +28086,7 @@
       </c>
       <c r="B1160" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524022166 ", "lender_amount": "4009000.00", "borrower_amount": "4009000.00"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524022166 ", "lender_amount": "4009000.00", "borrower_amount": "4009000.00", "lc_number": "LC-308524022166 "}</t>
         </is>
       </c>
       <c r="C1160" t="inlineStr">
@@ -28201,7 +28313,7 @@
       </c>
       <c r="B1169" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524026037/24", "lender_amount": "14417.98", "borrower_amount": "14417.98"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524026037/24", "lender_amount": "14417.98", "borrower_amount": "14417.98", "lc_number": "L/C-308524026037/24"}</t>
         </is>
       </c>
       <c r="C1169" t="inlineStr">
@@ -28866,7 +28978,7 @@
       </c>
       <c r="B1196" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020202/25", "lender_amount": "3499168.01", "borrower_amount": "3499168.01"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020202/25", "lender_amount": "3499168.01", "borrower_amount": "3499168.01", "lc_number": "L/C-147125020202/25"}</t>
         </is>
       </c>
       <c r="C1196" t="inlineStr">
@@ -29375,7 +29487,7 @@
       </c>
       <c r="B1219" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147124020074/24", "lender_amount": "6242871.55", "borrower_amount": "6242871.55"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147124020074/24", "lender_amount": "6242871.55", "borrower_amount": "6242871.55", "lc_number": "L/C-147124020074/24"}</t>
         </is>
       </c>
       <c r="C1219" t="inlineStr">

</xml_diff>

<commit_message>
Revert "Sequential MID for all matches"
This reverts commit 4c84f50a9c7735eb61f1b9c8fc2d83f46b912bca.
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -1316,16 +1316,8 @@
       <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>M073</t>
-        </is>
-      </c>
-      <c r="B44" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "FOB/PO/2023/8/5023", "lender_amount": "95200.00", "borrower_amount": "95200.00", "po_number": "FOB/PO/2023/8/5023"}</t>
-        </is>
-      </c>
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
           <t>01/Jan/2025</t>
@@ -1471,16 +1463,8 @@
       <c r="K49" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>M074</t>
-        </is>
-      </c>
-      <c r="B50" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "FOB/PO/2023/12/5124", "lender_amount": "164204.00", "borrower_amount": "164204.00", "po_number": "FOB/PO/2023/12/5124"}</t>
-        </is>
-      </c>
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
         <is>
           <t>01/Jan/2025</t>
@@ -1560,7 +1544,7 @@
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "5040781.68", "borrower_amount": "5040781.68", "lc_number": "L/C-308524022796/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "5040781.68", "borrower_amount": "5040781.68"}</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1641,7 +1625,7 @@
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "15737222.22", "borrower_amount": "15737222.22", "lc_number": "L/C-308524022796/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "15737222.22", "borrower_amount": "15737222.22"}</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1925,7 +1909,7 @@
       </c>
       <c r="B68" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "8884.77", "borrower_amount": "8884.77", "lc_number": "L/C-308524022796/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "8884.77", "borrower_amount": "8884.77"}</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2006,7 +1990,7 @@
       </c>
       <c r="B71" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "1575.00", "borrower_amount": "1575.00", "lc_number": "L/C-308524027065/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "1575.00", "borrower_amount": "1575.00"}</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2379,7 +2363,7 @@
       </c>
       <c r="B86" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-187724010124/24", "lender_amount": "1150.00", "borrower_amount": "1150.00", "lc_number": "L/C-187724010124/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-187724010124/24", "lender_amount": "1150.00", "borrower_amount": "1150.00"}</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2460,7 +2444,7 @@
       </c>
       <c r="B89" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "1575.00", "borrower_amount": "1575.00", "lc_number": "L/C-308524027065/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "1575.00", "borrower_amount": "1575.00"}</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2906,7 +2890,7 @@
       </c>
       <c r="B107" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "26246.93", "borrower_amount": "26246.93", "lc_number": "L/C-308524022796/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "26246.93", "borrower_amount": "26246.93"}</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4112,16 +4096,8 @@
       <c r="K161" t="inlineStr"/>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>M075</t>
-        </is>
-      </c>
-      <c r="B162" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "FOB/PO/2023/8/5000", "lender_amount": "289000.00", "borrower_amount": "289000.00", "po_number": "FOB/PO/2023/8/5000"}</t>
-        </is>
-      </c>
+      <c r="A162" t="inlineStr"/>
+      <c r="B162" t="inlineStr"/>
       <c r="C162" t="inlineStr">
         <is>
           <t>01/Feb/2025</t>
@@ -5736,7 +5712,7 @@
       </c>
       <c r="B229" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-187724010124/24", "lender_amount": "1150.00", "borrower_amount": "1150.00", "lc_number": "L/C-187724010124/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-187724010124/24", "lender_amount": "1150.00", "borrower_amount": "1150.00"}</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -5890,7 +5866,7 @@
       </c>
       <c r="B235" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-187724010124/24", "lender_amount": "8761.79", "borrower_amount": "8761.79", "lc_number": "L/C-187724010124/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-187724010124/24", "lender_amount": "8761.79", "borrower_amount": "8761.79"}</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -6374,7 +6350,7 @@
       </c>
       <c r="B255" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "1862.50", "borrower_amount": "1862.50", "lc_number": "L/C-308524027065/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "1862.50", "borrower_amount": "1862.50"}</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -6877,7 +6853,7 @@
       </c>
       <c r="B276" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020003/25", "lender_amount": "27383.77", "borrower_amount": "27383.77", "lc_number": "L/C-147125020003/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020003/25", "lender_amount": "27383.77", "borrower_amount": "27383.77"}</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -7630,16 +7606,8 @@
       <c r="K307" t="inlineStr"/>
     </row>
     <row r="308">
-      <c r="A308" t="inlineStr">
-        <is>
-          <t>M076</t>
-        </is>
-      </c>
-      <c r="B308" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2024/6/27130", "lender_amount": "1100.00", "borrower_amount": "1100.00", "po_number": "OPE/PO/2024/6/27130"}</t>
-        </is>
-      </c>
+      <c r="A308" t="inlineStr"/>
+      <c r="B308" t="inlineStr"/>
       <c r="C308" t="inlineStr">
         <is>
           <t>16/Feb/2025</t>
@@ -8340,7 +8308,7 @@
       </c>
       <c r="B337" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524990243/24", "lender_amount": "71971.54", "borrower_amount": "71971.54", "lc_number": "L/C-308524990243/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524990243/24", "lender_amount": "71971.54", "borrower_amount": "71971.54"}</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
@@ -8421,7 +8389,7 @@
       </c>
       <c r="B340" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524990243/24", "lender_amount": "20527984.90", "borrower_amount": "20527984.90", "lc_number": "L/C-308524990243/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524990243/24", "lender_amount": "20527984.90", "borrower_amount": "20527984.90"}</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
@@ -8502,7 +8470,7 @@
       </c>
       <c r="B343" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147124020653/25", "lender_amount": "665048.82", "borrower_amount": "665048.82", "lc_number": "L/C-147124020653/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147124020653/25", "lender_amount": "665048.82", "borrower_amount": "665048.82"}</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
@@ -8583,7 +8551,7 @@
       </c>
       <c r="B346" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147124020708/24", "lender_amount": "25042.61", "borrower_amount": "25042.61", "lc_number": "L/C-147124020708/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147124020708/24", "lender_amount": "25042.61", "borrower_amount": "25042.61"}</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
@@ -8957,7 +8925,7 @@
       </c>
       <c r="B361" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020063/25", "lender_amount": "5995080.00", "borrower_amount": "5995080.00", "lc_number": "L/C-141325020063/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020063/25", "lender_amount": "5995080.00", "borrower_amount": "5995080.00"}</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
@@ -9038,7 +9006,7 @@
       </c>
       <c r="B364" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020068/25", "lender_amount": "33573.89", "borrower_amount": "33573.89", "lc_number": "L/C-141325020068/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020068/25", "lender_amount": "33573.89", "borrower_amount": "33573.89"}</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
@@ -9119,7 +9087,7 @@
       </c>
       <c r="B367" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020068/25", "lender_amount": "1650660.00", "borrower_amount": "1650660.00", "lc_number": "L/C-141325020068/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020068/25", "lender_amount": "1650660.00", "borrower_amount": "1650660.00"}</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
@@ -9340,16 +9308,8 @@
       <c r="K375" t="inlineStr"/>
     </row>
     <row r="376">
-      <c r="A376" t="inlineStr">
-        <is>
-          <t>M077</t>
-        </is>
-      </c>
-      <c r="B376" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "GEO/PO/2023/3/12915", "lender_amount": "400000.00", "borrower_amount": "400000.00", "po_number": "GEO/PO/2023/3/12915"}</t>
-        </is>
-      </c>
+      <c r="A376" t="inlineStr"/>
+      <c r="B376" t="inlineStr"/>
       <c r="C376" t="inlineStr">
         <is>
           <t>27/Feb/2025</t>
@@ -9428,7 +9388,7 @@
       </c>
       <c r="B379" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-155824020001/24", "lender_amount": "7641878.37", "borrower_amount": "7641878.37", "lc_number": "LC-155824020001/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-155824020001/24", "lender_amount": "7641878.37", "borrower_amount": "7641878.37"}</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
@@ -10571,7 +10531,7 @@
       </c>
       <c r="B432" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020063/25", "lender_amount": "246401.97", "borrower_amount": "246401.97", "lc_number": "L/C-141325020063/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020063/25", "lender_amount": "246401.97", "borrower_amount": "246401.97"}</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
@@ -10798,7 +10758,7 @@
       </c>
       <c r="B441" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022796/24", "lender_amount": "26369.63", "borrower_amount": "26369.63", "lc_number": "L/C-308524022796/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022796/24", "lender_amount": "26369.63", "borrower_amount": "26369.63"}</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
@@ -11202,16 +11162,8 @@
       <c r="K457" t="inlineStr"/>
     </row>
     <row r="458">
-      <c r="A458" t="inlineStr">
-        <is>
-          <t>M078</t>
-        </is>
-      </c>
-      <c r="B458" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2024/9/29742", "lender_amount": "124670.00", "borrower_amount": "124670.00", "po_number": "OPE/PO/2024/9/29742"}</t>
-        </is>
-      </c>
+      <c r="A458" t="inlineStr"/>
+      <c r="B458" t="inlineStr"/>
       <c r="C458" t="inlineStr">
         <is>
           <t>05/Mar/2025</t>
@@ -11290,7 +11242,7 @@
       </c>
       <c r="B461" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-222825150235/25", "lender_amount": "2357.50", "borrower_amount": "2357.50", "lc_number": "L/C-222825150235/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-222825150235/25", "lender_amount": "2357.50", "borrower_amount": "2357.50"}</t>
         </is>
       </c>
       <c r="C461" t="inlineStr">
@@ -11444,7 +11396,7 @@
       </c>
       <c r="B467" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-222825150235/25", "lender_amount": "213500.00", "borrower_amount": "213500.00", "lc_number": "L/C-222825150235/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-222825150235/25", "lender_amount": "213500.00", "borrower_amount": "213500.00"}</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
@@ -11525,7 +11477,7 @@
       </c>
       <c r="B470" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "1725.00", "borrower_amount": "1725.00", "lc_number": "L/C-308524027065/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "1725.00", "borrower_amount": "1725.00"}</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
@@ -11606,7 +11558,7 @@
       </c>
       <c r="B473" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-187724010122/24", "lender_amount": "276518.90", "borrower_amount": "276518.90", "lc_number": "L/C-187724010122/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-187724010122/24", "lender_amount": "276518.90", "borrower_amount": "276518.90"}</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
@@ -12455,7 +12407,7 @@
       </c>
       <c r="B508" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020027/25", "lender_amount": "54431.58", "borrower_amount": "54431.58", "lc_number": "L/C-147125020027/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020027/25", "lender_amount": "54431.58", "borrower_amount": "54431.58"}</t>
         </is>
       </c>
       <c r="C508" t="inlineStr">
@@ -12755,7 +12707,7 @@
       </c>
       <c r="B520" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524027065/24", "lender_amount": "8231.99", "borrower_amount": "8231.99", "lc_number": "L/C-308524027065/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524027065/24", "lender_amount": "8231.99", "borrower_amount": "8231.99"}</t>
         </is>
       </c>
       <c r="C520" t="inlineStr">
@@ -13873,7 +13825,7 @@
       </c>
       <c r="B570" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147124020708/24", "lender_amount": "19399.10", "borrower_amount": "19399.10", "lc_number": "L/C-147124020708/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147124020708/24", "lender_amount": "19399.10", "borrower_amount": "19399.10"}</t>
         </is>
       </c>
       <c r="C570" t="inlineStr">
@@ -13954,7 +13906,7 @@
       </c>
       <c r="B573" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524990243/24", "lender_amount": "15160.97", "borrower_amount": "15160.97", "lc_number": "L/C-308524990243/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524990243/24", "lender_amount": "15160.97", "borrower_amount": "15160.97"}</t>
         </is>
       </c>
       <c r="C573" t="inlineStr">
@@ -14184,7 +14136,7 @@
       </c>
       <c r="B583" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020104/25", "lender_amount": "6125933.94", "borrower_amount": "6125933.94", "lc_number": "L/C-141325020104/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020104/25", "lender_amount": "6125933.94", "borrower_amount": "6125933.94"}</t>
         </is>
       </c>
       <c r="C583" t="inlineStr">
@@ -14303,7 +14255,7 @@
       </c>
       <c r="B588" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022495/24", "lender_amount": "12425.77", "borrower_amount": "12425.77", "lc_number": "L/C-308524022495/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022495/24", "lender_amount": "12425.77", "borrower_amount": "12425.77"}</t>
         </is>
       </c>
       <c r="C588" t="inlineStr">
@@ -14384,7 +14336,7 @@
       </c>
       <c r="B591" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524022495/24", "lender_amount": "23580.68", "borrower_amount": "23580.68", "lc_number": "L/C-308524022495/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524022495/24", "lender_amount": "23580.68", "borrower_amount": "23580.68"}</t>
         </is>
       </c>
       <c r="C591" t="inlineStr">
@@ -14458,16 +14410,8 @@
       <c r="K593" t="inlineStr"/>
     </row>
     <row r="594">
-      <c r="A594" t="inlineStr">
-        <is>
-          <t>M079</t>
-        </is>
-      </c>
-      <c r="B594" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "MBD/PO/2024/9/10", "lender_amount": "25000.00", "borrower_amount": "25000.00", "po_number": "MBD/PO/2024/9/10"}</t>
-        </is>
-      </c>
+      <c r="A594" t="inlineStr"/>
+      <c r="B594" t="inlineStr"/>
       <c r="C594" t="inlineStr">
         <is>
           <t>31/Mar/2025</t>
@@ -15233,16 +15177,8 @@
       <c r="K630" t="inlineStr"/>
     </row>
     <row r="631">
-      <c r="A631" t="inlineStr">
-        <is>
-          <t>M080</t>
-        </is>
-      </c>
-      <c r="B631" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "CHA/PO/2023/12/20766", "lender_amount": "2000000.00", "borrower_amount": "2000000.00", "po_number": "CHA/PO/2023/12/20766"}</t>
-        </is>
-      </c>
+      <c r="A631" t="inlineStr"/>
+      <c r="B631" t="inlineStr"/>
       <c r="C631" t="inlineStr">
         <is>
           <t>01/Apr/2025</t>
@@ -15467,7 +15403,7 @@
       </c>
       <c r="B640" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308525021741/25", "lender_amount": "22671.95", "borrower_amount": "22671.95", "lc_number": "L/C-308525021741/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308525021741/25", "lender_amount": "22671.95", "borrower_amount": "22671.95"}</t>
         </is>
       </c>
       <c r="C640" t="inlineStr">
@@ -15548,7 +15484,7 @@
       </c>
       <c r="B643" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308525021745/25", "lender_amount": "28854.86", "borrower_amount": "28854.86", "lc_number": "L/C-308525021745/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308525021745/25", "lender_amount": "28854.86", "borrower_amount": "28854.86"}</t>
         </is>
       </c>
       <c r="C643" t="inlineStr">
@@ -15629,7 +15565,7 @@
       </c>
       <c r="B646" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524026037/24", "lender_amount": "1725.00", "borrower_amount": "1725.00", "lc_number": "L/C-308524026037/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524026037/24", "lender_amount": "1725.00", "borrower_amount": "1725.00"}</t>
         </is>
       </c>
       <c r="C646" t="inlineStr">
@@ -16221,7 +16157,7 @@
       </c>
       <c r="B670" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020063/25", "lender_amount": "80051.03", "borrower_amount": "80051.03", "lc_number": "LC-141325020063/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020063/25", "lender_amount": "80051.03", "borrower_amount": "80051.03"}</t>
         </is>
       </c>
       <c r="C670" t="inlineStr">
@@ -16302,7 +16238,7 @@
       </c>
       <c r="B673" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020063/25", "lender_amount": "6777058.20", "borrower_amount": "6777058.20", "lc_number": "L/C-141325020063/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020063/25", "lender_amount": "6777058.20", "borrower_amount": "6777058.20"}</t>
         </is>
       </c>
       <c r="C673" t="inlineStr">
@@ -16494,7 +16430,7 @@
       </c>
       <c r="B681" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-155823010186/23", "lender_amount": "76000.00", "borrower_amount": "76000.00", "lc_number": "L/C-155823010186/23"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-155823010186/23", "lender_amount": "76000.00", "borrower_amount": "76000.00"}</t>
         </is>
       </c>
       <c r="C681" t="inlineStr">
@@ -16832,7 +16768,7 @@
       </c>
       <c r="B695" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524026037/222824023549", "lender_amount": "1226351.09", "borrower_amount": "1226351.09", "lc_number": "LC-308524026037/222824023549"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524026037/222824023549", "lender_amount": "1226351.09", "borrower_amount": "1226351.09"}</t>
         </is>
       </c>
       <c r="C695" t="inlineStr">
@@ -16986,7 +16922,7 @@
       </c>
       <c r="B701" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524022495/24", "lender_amount": "1675000.00", "borrower_amount": "1675000.00", "lc_number": "LC-308524022495/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524022495/24", "lender_amount": "1675000.00", "borrower_amount": "1675000.00"}</t>
         </is>
       </c>
       <c r="C701" t="inlineStr">
@@ -17213,7 +17149,7 @@
       </c>
       <c r="B710" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020027/25", "lender_amount": "10691988.92", "borrower_amount": "10691988.92", "lc_number": "L/C-147125020027/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020027/25", "lender_amount": "10691988.92", "borrower_amount": "10691988.92"}</t>
         </is>
       </c>
       <c r="C710" t="inlineStr">
@@ -17294,7 +17230,7 @@
       </c>
       <c r="B713" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-222825150151/25", "lender_amount": "333706.76", "borrower_amount": "333706.76", "lc_number": "L/C-222825150151/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-222825150151/25", "lender_amount": "333706.76", "borrower_amount": "333706.76"}</t>
         </is>
       </c>
       <c r="C713" t="inlineStr">
@@ -17375,7 +17311,7 @@
       </c>
       <c r="B716" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020063/25", "lender_amount": "299000.00", "borrower_amount": "299000.00", "lc_number": "L/C-141325020063/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020063/25", "lender_amount": "299000.00", "borrower_amount": "299000.00"}</t>
         </is>
       </c>
       <c r="C716" t="inlineStr">
@@ -17529,7 +17465,7 @@
       </c>
       <c r="B722" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524026037/24", "lender_amount": "13743.52", "borrower_amount": "13743.52", "lc_number": "L/C-308524026037/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524026037/24", "lender_amount": "13743.52", "borrower_amount": "13743.52"}</t>
         </is>
       </c>
       <c r="C722" t="inlineStr">
@@ -17851,7 +17787,7 @@
       </c>
       <c r="B736" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-155825020020/25", "lender_amount": "60302.55", "borrower_amount": "60302.55", "lc_number": "LC-155825020020/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-155825020020/25", "lender_amount": "60302.55", "borrower_amount": "60302.55"}</t>
         </is>
       </c>
       <c r="C736" t="inlineStr">
@@ -17932,7 +17868,7 @@
       </c>
       <c r="B739" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020104/25", "lender_amount": "124008.78", "borrower_amount": "124008.78", "lc_number": "L/C-141325020104/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020104/25", "lender_amount": "124008.78", "borrower_amount": "124008.78"}</t>
         </is>
       </c>
       <c r="C739" t="inlineStr">
@@ -18013,7 +17949,7 @@
       </c>
       <c r="B742" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020063/25", "lender_amount": "31609.80", "borrower_amount": "31609.80", "lc_number": "LC-141325020063/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020063/25", "lender_amount": "31609.80", "borrower_amount": "31609.80"}</t>
         </is>
       </c>
       <c r="C742" t="inlineStr">
@@ -18497,7 +18433,7 @@
       </c>
       <c r="B762" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020104/25", "lender_amount": "10424886.36", "borrower_amount": "10424886.36", "lc_number": "L/C-141325020104/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020104/25", "lender_amount": "10424886.36", "borrower_amount": "10424886.36"}</t>
         </is>
       </c>
       <c r="C762" t="inlineStr">
@@ -18578,7 +18514,7 @@
       </c>
       <c r="B765" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020063/25", "lender_amount": "2168751.40", "borrower_amount": "2168751.40", "lc_number": "L/C-147125020063/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020063/25", "lender_amount": "2168751.40", "borrower_amount": "2168751.40"}</t>
         </is>
       </c>
       <c r="C765" t="inlineStr">
@@ -18732,7 +18668,7 @@
       </c>
       <c r="B771" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-141325020068/25", "lender_amount": "63787.54", "borrower_amount": "63787.54", "lc_number": "L/C-141325020068/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-141325020068/25", "lender_amount": "63787.54", "borrower_amount": "63787.54"}</t>
         </is>
       </c>
       <c r="C771" t="inlineStr">
@@ -19647,16 +19583,8 @@
       <c r="K813" t="inlineStr"/>
     </row>
     <row r="814">
-      <c r="A814" t="inlineStr">
-        <is>
-          <t>M081</t>
-        </is>
-      </c>
-      <c r="B814" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "BPD/PO/2025/3/32659", "lender_amount": "768000.00", "borrower_amount": "768000.00", "po_number": "BPD/PO/2025/3/32659"}</t>
-        </is>
-      </c>
+      <c r="A814" t="inlineStr"/>
+      <c r="B814" t="inlineStr"/>
       <c r="C814" t="inlineStr">
         <is>
           <t>01/May/2025</t>
@@ -19947,16 +19875,8 @@
       <c r="K825" t="inlineStr"/>
     </row>
     <row r="826">
-      <c r="A826" t="inlineStr">
-        <is>
-          <t>M082</t>
-        </is>
-      </c>
-      <c r="B826" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2023/10/18781", "lender_amount": "13920.00", "borrower_amount": "13920.00", "po_number": "OPE/PO/2023/10/18781"}</t>
-        </is>
-      </c>
+      <c r="A826" t="inlineStr"/>
+      <c r="B826" t="inlineStr"/>
       <c r="C826" t="inlineStr">
         <is>
           <t>01/May/2025</t>
@@ -22212,7 +22132,7 @@
       </c>
       <c r="B920" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020104/25", "lender_amount": "111771.42", "borrower_amount": "111771.42", "lc_number": "LC-141325020104/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020104/25", "lender_amount": "111771.42", "borrower_amount": "111771.42"}</t>
         </is>
       </c>
       <c r="C920" t="inlineStr">
@@ -22293,7 +22213,7 @@
       </c>
       <c r="B923" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020112/25", "lender_amount": "80701.76", "borrower_amount": "80701.76", "lc_number": "LC-141325020112/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020112/25", "lender_amount": "80701.76", "borrower_amount": "80701.76"}</t>
         </is>
       </c>
       <c r="C923" t="inlineStr">
@@ -22374,7 +22294,7 @@
       </c>
       <c r="B926" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020112/25", "lender_amount": "657.81", "borrower_amount": "657.81", "lc_number": "LC-141325020112/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020112/25", "lender_amount": "657.81", "borrower_amount": "657.81"}</t>
         </is>
       </c>
       <c r="C926" t="inlineStr">
@@ -22747,7 +22667,7 @@
       </c>
       <c r="B941" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020063/25", "lender_amount": "81730.06", "borrower_amount": "81730.06", "lc_number": "LC-141325020063/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020063/25", "lender_amount": "81730.06", "borrower_amount": "81730.06"}</t>
         </is>
       </c>
       <c r="C941" t="inlineStr">
@@ -23193,7 +23113,7 @@
       </c>
       <c r="B959" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020163/25", "lender_amount": "341847.68", "borrower_amount": "341847.68", "lc_number": "LC-141325020163/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020163/25", "lender_amount": "341847.68", "borrower_amount": "341847.68"}</t>
         </is>
       </c>
       <c r="C959" t="inlineStr">
@@ -23496,7 +23416,7 @@
       </c>
       <c r="B972" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-222825150235/25", "lender_amount": "36757.00", "borrower_amount": "36757.00", "lc_number": "LC-222825150235/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-222825150235/25", "lender_amount": "36757.00", "borrower_amount": "36757.00"}</t>
         </is>
       </c>
       <c r="C972" t="inlineStr">
@@ -23650,7 +23570,7 @@
       </c>
       <c r="B978" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020068/25", "lender_amount": "3587219.00", "borrower_amount": "3587219.00", "lc_number": "LC-141325020068/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020068/25", "lender_amount": "3587219.00", "borrower_amount": "3587219.00"}</t>
         </is>
       </c>
       <c r="C978" t="inlineStr">
@@ -23788,7 +23708,7 @@
       </c>
       <c r="B984" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524990243/24", "lender_amount": "68747.06", "borrower_amount": "68747.06", "lc_number": "LC-308524990243/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524990243/24", "lender_amount": "68747.06", "borrower_amount": "68747.06"}</t>
         </is>
       </c>
       <c r="C984" t="inlineStr">
@@ -24403,7 +24323,7 @@
       </c>
       <c r="B1010" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308525021741/25", "lender_amount": "31411.11", "borrower_amount": "31411.11", "lc_number": "LC-308525021741/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308525021741/25", "lender_amount": "31411.11", "borrower_amount": "31411.11"}</t>
         </is>
       </c>
       <c r="C1010" t="inlineStr">
@@ -24477,16 +24397,8 @@
       <c r="K1012" t="inlineStr"/>
     </row>
     <row r="1013">
-      <c r="A1013" t="inlineStr">
-        <is>
-          <t>M083</t>
-        </is>
-      </c>
-      <c r="B1013" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "MOD/PO/2024/10/30061", "lender_amount": "89910.00", "borrower_amount": "89910.00", "po_number": "MOD/PO/2024/10/30061"}</t>
-        </is>
-      </c>
+      <c r="A1013" t="inlineStr"/>
+      <c r="B1013" t="inlineStr"/>
       <c r="C1013" t="inlineStr">
         <is>
           <t>01/Jun/2025</t>
@@ -24631,16 +24543,8 @@
       <c r="K1018" t="inlineStr"/>
     </row>
     <row r="1019">
-      <c r="A1019" t="inlineStr">
-        <is>
-          <t>M084</t>
-        </is>
-      </c>
-      <c r="B1019" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2024/10/29964", "lender_amount": "24800.00", "borrower_amount": "24800.00", "po_number": "OPE/PO/2024/10/29964"}</t>
-        </is>
-      </c>
+      <c r="A1019" t="inlineStr"/>
+      <c r="B1019" t="inlineStr"/>
       <c r="C1019" t="inlineStr">
         <is>
           <t>02/Jun/2025</t>
@@ -24939,7 +24843,7 @@
       </c>
       <c r="B1031" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-155825010037/25", "lender_amount": "853297.01", "borrower_amount": "853297.01", "lc_number": "LC-155825010037/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-155825010037/25", "lender_amount": "853297.01", "borrower_amount": "853297.01"}</t>
         </is>
       </c>
       <c r="C1031" t="inlineStr">
@@ -26165,16 +26069,8 @@
       <c r="K1081" t="inlineStr"/>
     </row>
     <row r="1082">
-      <c r="A1082" t="inlineStr">
-        <is>
-          <t>M085</t>
-        </is>
-      </c>
-      <c r="B1082" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2025/4/33343", "lender_amount": "199850.00", "borrower_amount": "199850.00", "po_number": "OPE/PO/2025/4/33343"}</t>
-        </is>
-      </c>
+      <c r="A1082" t="inlineStr"/>
+      <c r="B1082" t="inlineStr"/>
       <c r="C1082" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
@@ -26246,16 +26142,8 @@
       <c r="K1084" t="inlineStr"/>
     </row>
     <row r="1085">
-      <c r="A1085" t="inlineStr">
-        <is>
-          <t>M086</t>
-        </is>
-      </c>
-      <c r="B1085" s="4" t="inlineStr">
-        <is>
-          <t>{"match_type": "PO", "match_method": "reference_match", "reference_number": "OPE/PO/2024/11/30293", "lender_amount": "45094.20", "borrower_amount": "45094.20", "po_number": "OPE/PO/2024/11/30293"}</t>
-        </is>
-      </c>
+      <c r="A1085" t="inlineStr"/>
+      <c r="B1085" t="inlineStr"/>
       <c r="C1085" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
@@ -26626,7 +26514,7 @@
       </c>
       <c r="B1100" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020163/25", "lender_amount": "1725.00", "borrower_amount": "1725.00", "lc_number": "LC-141325020163/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020163/25", "lender_amount": "1725.00", "borrower_amount": "1725.00"}</t>
         </is>
       </c>
       <c r="C1100" t="inlineStr">
@@ -26707,7 +26595,7 @@
       </c>
       <c r="B1103" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308525021746/25", "lender_amount": "35373.50", "borrower_amount": "35373.50", "lc_number": "LC-308525021746/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308525021746/25", "lender_amount": "35373.50", "borrower_amount": "35373.50"}</t>
         </is>
       </c>
       <c r="C1103" t="inlineStr">
@@ -27264,7 +27152,7 @@
       </c>
       <c r="B1126" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-141325020063/141325020112", "lender_amount": "576120.39", "borrower_amount": "576120.39", "lc_number": "LC-141325020063/141325020112"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-141325020063/141325020112", "lender_amount": "576120.39", "borrower_amount": "576120.39"}</t>
         </is>
       </c>
       <c r="C1126" t="inlineStr">
@@ -27421,7 +27309,7 @@
       </c>
       <c r="B1133" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524022166 ", "lender_amount": "758000.00", "borrower_amount": "758000.00", "lc_number": "LC-308524022166 "}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524022166 ", "lender_amount": "758000.00", "borrower_amount": "758000.00"}</t>
         </is>
       </c>
       <c r="C1133" t="inlineStr">
@@ -28086,7 +27974,7 @@
       </c>
       <c r="B1160" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "LC-308524022166 ", "lender_amount": "4009000.00", "borrower_amount": "4009000.00", "lc_number": "LC-308524022166 "}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "LC-308524022166 ", "lender_amount": "4009000.00", "borrower_amount": "4009000.00"}</t>
         </is>
       </c>
       <c r="C1160" t="inlineStr">
@@ -28313,7 +28201,7 @@
       </c>
       <c r="B1169" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-308524026037/24", "lender_amount": "14417.98", "borrower_amount": "14417.98", "lc_number": "L/C-308524026037/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-308524026037/24", "lender_amount": "14417.98", "borrower_amount": "14417.98"}</t>
         </is>
       </c>
       <c r="C1169" t="inlineStr">
@@ -28978,7 +28866,7 @@
       </c>
       <c r="B1196" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147125020202/25", "lender_amount": "3499168.01", "borrower_amount": "3499168.01", "lc_number": "L/C-147125020202/25"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147125020202/25", "lender_amount": "3499168.01", "borrower_amount": "3499168.01"}</t>
         </is>
       </c>
       <c r="C1196" t="inlineStr">
@@ -29487,7 +29375,7 @@
       </c>
       <c r="B1219" s="4" t="inlineStr">
         <is>
-          <t>{"match_type": "LC", "match_method": "reference_match", "reference_number": "L/C-147124020074/24", "lender_amount": "6242871.55", "borrower_amount": "6242871.55", "lc_number": "L/C-147124020074/24"}</t>
+          <t>{"match_type": "LC", "match_method": "reference_match", "lc_number": "L/C-147124020074/24", "lender_amount": "6242871.55", "borrower_amount": "6242871.55"}</t>
         </is>
       </c>
       <c r="C1219" t="inlineStr">

</xml_diff>

<commit_message>
Audit info only in parent row
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -1588,14 +1588,7 @@
           <t>M001</t>
         </is>
       </c>
-      <c r="B54" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 5040781.68
-Borrower Amount: 5040781.68</t>
-        </is>
-      </c>
+      <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" s="4" t="inlineStr">
@@ -1616,14 +1609,7 @@
           <t>M001</t>
         </is>
       </c>
-      <c r="B55" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 5040781.68
-Borrower Amount: 5040781.68</t>
-        </is>
-      </c>
+      <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
@@ -1694,14 +1680,7 @@
           <t>M002</t>
         </is>
       </c>
-      <c r="B57" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
       <c r="E57" s="4" t="inlineStr">
@@ -1724,14 +1703,7 @@
           <t>M002</t>
         </is>
       </c>
-      <c r="B58" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" s="4" t="inlineStr">
@@ -1754,14 +1726,7 @@
           <t>M002</t>
         </is>
       </c>
-      <c r="B59" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" s="4" t="inlineStr">
@@ -1784,14 +1749,7 @@
           <t>M002</t>
         </is>
       </c>
-      <c r="B60" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" s="4" t="inlineStr">
@@ -1812,14 +1770,7 @@
           <t>M002</t>
         </is>
       </c>
-      <c r="B61" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
@@ -1844,14 +1795,7 @@
           <t>M002</t>
         </is>
       </c>
-      <c r="B62" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
           <t>01/Jan/2025</t>
@@ -2047,14 +1991,7 @@
           <t>M003</t>
         </is>
       </c>
-      <c r="B69" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 8884.77
-Borrower Amount: 8884.77</t>
-        </is>
-      </c>
+      <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" s="4" t="inlineStr">
@@ -2075,14 +2012,7 @@
           <t>M003</t>
         </is>
       </c>
-      <c r="B70" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 8884.77
-Borrower Amount: 8884.77</t>
-        </is>
-      </c>
+      <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
@@ -2153,14 +2083,7 @@
           <t>M005</t>
         </is>
       </c>
-      <c r="B72" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
       <c r="E72" s="4" t="inlineStr">
@@ -2181,14 +2104,7 @@
           <t>M005</t>
         </is>
       </c>
-      <c r="B73" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
@@ -2213,14 +2129,7 @@
           <t>M005</t>
         </is>
       </c>
-      <c r="B74" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr">
         <is>
           <t>07/Jan/2025</t>
@@ -2562,14 +2471,7 @@
           <t>M007</t>
         </is>
       </c>
-      <c r="B87" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
       <c r="E87" s="4" t="inlineStr">
@@ -2590,14 +2492,7 @@
           <t>M007</t>
         </is>
       </c>
-      <c r="B88" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
@@ -2668,14 +2563,7 @@
           <t>M009</t>
         </is>
       </c>
-      <c r="B90" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
       <c r="E90" s="4" t="inlineStr">
@@ -2696,14 +2584,7 @@
           <t>M009</t>
         </is>
       </c>
-      <c r="B91" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
         <is>
@@ -2728,14 +2609,7 @@
           <t>M009</t>
         </is>
       </c>
-      <c r="B92" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr">
         <is>
           <t>19/Jan/2025</t>
@@ -3150,14 +3024,7 @@
           <t>M010</t>
         </is>
       </c>
-      <c r="B108" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 26246.93
-Borrower Amount: 26246.93</t>
-        </is>
-      </c>
+      <c r="B108" t="inlineStr"/>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
       <c r="E108" s="4" t="inlineStr">
@@ -3178,14 +3045,7 @@
           <t>M010</t>
         </is>
       </c>
-      <c r="B109" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 26246.93
-Borrower Amount: 26246.93</t>
-        </is>
-      </c>
+      <c r="B109" t="inlineStr"/>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr">
         <is>
@@ -3210,14 +3070,7 @@
           <t>M010</t>
         </is>
       </c>
-      <c r="B110" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 26246.93
-Borrower Amount: 26246.93</t>
-        </is>
-      </c>
+      <c r="B110" t="inlineStr"/>
       <c r="C110" t="inlineStr">
         <is>
           <t>29/Jan/2025</t>
@@ -6008,14 +5861,7 @@
           <t>M012</t>
         </is>
       </c>
-      <c r="B230" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="B230" t="inlineStr"/>
       <c r="C230" t="inlineStr"/>
       <c r="D230" t="inlineStr"/>
       <c r="E230" s="4" t="inlineStr">
@@ -6036,14 +5882,7 @@
           <t>M012</t>
         </is>
       </c>
-      <c r="B231" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="B231" t="inlineStr"/>
       <c r="C231" t="inlineStr"/>
       <c r="D231" t="inlineStr">
         <is>
@@ -6068,14 +5907,7 @@
           <t>M012</t>
         </is>
       </c>
-      <c r="B232" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="B232" t="inlineStr"/>
       <c r="C232" t="inlineStr">
         <is>
           <t>04/Feb/2025</t>
@@ -6198,14 +6030,7 @@
           <t>M013</t>
         </is>
       </c>
-      <c r="B236" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
-Lender Amount: 8761.79
-Borrower Amount: 8761.79</t>
-        </is>
-      </c>
+      <c r="B236" t="inlineStr"/>
       <c r="C236" t="inlineStr"/>
       <c r="D236" t="inlineStr"/>
       <c r="E236" s="4" t="inlineStr">
@@ -6226,14 +6051,7 @@
           <t>M013</t>
         </is>
       </c>
-      <c r="B237" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
-Lender Amount: 8761.79
-Borrower Amount: 8761.79</t>
-        </is>
-      </c>
+      <c r="B237" t="inlineStr"/>
       <c r="C237" t="inlineStr"/>
       <c r="D237" t="inlineStr">
         <is>
@@ -6258,14 +6076,7 @@
           <t>M013</t>
         </is>
       </c>
-      <c r="B238" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
-Lender Amount: 8761.79
-Borrower Amount: 8761.79</t>
-        </is>
-      </c>
+      <c r="B238" t="inlineStr"/>
       <c r="C238" t="inlineStr">
         <is>
           <t>05/Feb/2025</t>
@@ -6718,14 +6529,7 @@
           <t>M014</t>
         </is>
       </c>
-      <c r="B256" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1862.50
-Borrower Amount: 1862.50</t>
-        </is>
-      </c>
+      <c r="B256" t="inlineStr"/>
       <c r="C256" t="inlineStr"/>
       <c r="D256" t="inlineStr"/>
       <c r="E256" s="4" t="inlineStr">
@@ -6746,14 +6550,7 @@
           <t>M014</t>
         </is>
       </c>
-      <c r="B257" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1862.50
-Borrower Amount: 1862.50</t>
-        </is>
-      </c>
+      <c r="B257" t="inlineStr"/>
       <c r="C257" t="inlineStr"/>
       <c r="D257" t="inlineStr">
         <is>
@@ -6778,14 +6575,7 @@
           <t>M014</t>
         </is>
       </c>
-      <c r="B258" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1862.50
-Borrower Amount: 1862.50</t>
-        </is>
-      </c>
+      <c r="B258" t="inlineStr"/>
       <c r="C258" t="inlineStr">
         <is>
           <t>10/Feb/2025</t>
@@ -7257,14 +7047,7 @@
           <t>M015</t>
         </is>
       </c>
-      <c r="B277" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020003/25
-Lender Amount: 27383.77
-Borrower Amount: 27383.77</t>
-        </is>
-      </c>
+      <c r="B277" t="inlineStr"/>
       <c r="C277" t="inlineStr"/>
       <c r="D277" t="inlineStr"/>
       <c r="E277" s="4" t="inlineStr">
@@ -7285,14 +7068,7 @@
           <t>M015</t>
         </is>
       </c>
-      <c r="B278" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020003/25
-Lender Amount: 27383.77
-Borrower Amount: 27383.77</t>
-        </is>
-      </c>
+      <c r="B278" t="inlineStr"/>
       <c r="C278" t="inlineStr"/>
       <c r="D278" t="inlineStr">
         <is>
@@ -7317,14 +7093,7 @@
           <t>M015</t>
         </is>
       </c>
-      <c r="B279" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020003/25
-Lender Amount: 27383.77
-Borrower Amount: 27383.77</t>
-        </is>
-      </c>
+      <c r="B279" t="inlineStr"/>
       <c r="C279" t="inlineStr">
         <is>
           <t>12/Feb/2025</t>
@@ -8748,14 +8517,7 @@
           <t>M016</t>
         </is>
       </c>
-      <c r="B338" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
-Lender Amount: 71971.54
-Borrower Amount: 71971.54</t>
-        </is>
-      </c>
+      <c r="B338" t="inlineStr"/>
       <c r="C338" t="inlineStr"/>
       <c r="D338" t="inlineStr"/>
       <c r="E338" s="4" t="inlineStr">
@@ -8776,14 +8538,7 @@
           <t>M016</t>
         </is>
       </c>
-      <c r="B339" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
-Lender Amount: 71971.54
-Borrower Amount: 71971.54</t>
-        </is>
-      </c>
+      <c r="B339" t="inlineStr"/>
       <c r="C339" t="inlineStr"/>
       <c r="D339" t="inlineStr">
         <is>
@@ -8854,14 +8609,7 @@
           <t>M017</t>
         </is>
       </c>
-      <c r="B341" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
-Lender Amount: 20527984.90
-Borrower Amount: 20527984.90</t>
-        </is>
-      </c>
+      <c r="B341" t="inlineStr"/>
       <c r="C341" t="inlineStr"/>
       <c r="D341" t="inlineStr"/>
       <c r="E341" s="4" t="inlineStr">
@@ -8882,14 +8630,7 @@
           <t>M017</t>
         </is>
       </c>
-      <c r="B342" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
-Lender Amount: 20527984.90
-Borrower Amount: 20527984.90</t>
-        </is>
-      </c>
+      <c r="B342" t="inlineStr"/>
       <c r="C342" t="inlineStr"/>
       <c r="D342" t="inlineStr">
         <is>
@@ -8960,14 +8701,7 @@
           <t>M018</t>
         </is>
       </c>
-      <c r="B344" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020653/25
-Lender Amount: 665048.82
-Borrower Amount: 665048.82</t>
-        </is>
-      </c>
+      <c r="B344" t="inlineStr"/>
       <c r="C344" t="inlineStr"/>
       <c r="D344" t="inlineStr"/>
       <c r="E344" s="4" t="inlineStr">
@@ -8988,14 +8722,7 @@
           <t>M018</t>
         </is>
       </c>
-      <c r="B345" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020653/25
-Lender Amount: 665048.82
-Borrower Amount: 665048.82</t>
-        </is>
-      </c>
+      <c r="B345" t="inlineStr"/>
       <c r="C345" t="inlineStr"/>
       <c r="D345" t="inlineStr">
         <is>
@@ -9066,14 +8793,7 @@
           <t>M019</t>
         </is>
       </c>
-      <c r="B347" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020708/24
-Lender Amount: 25042.61
-Borrower Amount: 25042.61</t>
-        </is>
-      </c>
+      <c r="B347" t="inlineStr"/>
       <c r="C347" t="inlineStr"/>
       <c r="D347" t="inlineStr"/>
       <c r="E347" s="4" t="inlineStr">
@@ -9094,14 +8814,7 @@
           <t>M019</t>
         </is>
       </c>
-      <c r="B348" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020708/24
-Lender Amount: 25042.61
-Borrower Amount: 25042.61</t>
-        </is>
-      </c>
+      <c r="B348" t="inlineStr"/>
       <c r="C348" t="inlineStr"/>
       <c r="D348" t="inlineStr">
         <is>
@@ -9126,14 +8839,7 @@
           <t>M019</t>
         </is>
       </c>
-      <c r="B349" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020708/24
-Lender Amount: 25042.61
-Borrower Amount: 25042.61</t>
-        </is>
-      </c>
+      <c r="B349" t="inlineStr"/>
       <c r="C349" t="inlineStr">
         <is>
           <t>24/Feb/2025</t>
@@ -9476,14 +9182,7 @@
           <t>M020</t>
         </is>
       </c>
-      <c r="B362" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 5995080.00
-Borrower Amount: 5995080.00</t>
-        </is>
-      </c>
+      <c r="B362" t="inlineStr"/>
       <c r="C362" t="inlineStr"/>
       <c r="D362" t="inlineStr"/>
       <c r="E362" s="4" t="inlineStr">
@@ -9504,14 +9203,7 @@
           <t>M020</t>
         </is>
       </c>
-      <c r="B363" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 5995080.00
-Borrower Amount: 5995080.00</t>
-        </is>
-      </c>
+      <c r="B363" t="inlineStr"/>
       <c r="C363" t="inlineStr"/>
       <c r="D363" t="inlineStr">
         <is>
@@ -9582,14 +9274,7 @@
           <t>M021</t>
         </is>
       </c>
-      <c r="B365" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
-Lender Amount: 33573.89
-Borrower Amount: 33573.89</t>
-        </is>
-      </c>
+      <c r="B365" t="inlineStr"/>
       <c r="C365" t="inlineStr"/>
       <c r="D365" t="inlineStr"/>
       <c r="E365" s="4" t="inlineStr">
@@ -9610,14 +9295,7 @@
           <t>M021</t>
         </is>
       </c>
-      <c r="B366" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
-Lender Amount: 33573.89
-Borrower Amount: 33573.89</t>
-        </is>
-      </c>
+      <c r="B366" t="inlineStr"/>
       <c r="C366" t="inlineStr"/>
       <c r="D366" t="inlineStr">
         <is>
@@ -9688,14 +9366,7 @@
           <t>M022</t>
         </is>
       </c>
-      <c r="B368" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
-Lender Amount: 1650660.00
-Borrower Amount: 1650660.00</t>
-        </is>
-      </c>
+      <c r="B368" t="inlineStr"/>
       <c r="C368" t="inlineStr"/>
       <c r="D368" t="inlineStr"/>
       <c r="E368" s="4" t="inlineStr">
@@ -9716,14 +9387,7 @@
           <t>M022</t>
         </is>
       </c>
-      <c r="B369" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
-Lender Amount: 1650660.00
-Borrower Amount: 1650660.00</t>
-        </is>
-      </c>
+      <c r="B369" t="inlineStr"/>
       <c r="C369" t="inlineStr"/>
       <c r="D369" t="inlineStr">
         <is>
@@ -9748,14 +9412,7 @@
           <t>M022</t>
         </is>
       </c>
-      <c r="B370" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
-Lender Amount: 1650660.00
-Borrower Amount: 1650660.00</t>
-        </is>
-      </c>
+      <c r="B370" t="inlineStr"/>
       <c r="C370" t="inlineStr">
         <is>
           <t>26/Feb/2025</t>
@@ -10025,14 +9682,7 @@
           <t>M023</t>
         </is>
       </c>
-      <c r="B380" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="B380" t="inlineStr"/>
       <c r="C380" t="inlineStr"/>
       <c r="D380" t="inlineStr"/>
       <c r="E380" s="4" t="inlineStr">
@@ -10055,14 +9705,7 @@
           <t>M023</t>
         </is>
       </c>
-      <c r="B381" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="B381" t="inlineStr"/>
       <c r="C381" t="inlineStr"/>
       <c r="D381" t="inlineStr"/>
       <c r="E381" s="4" t="inlineStr">
@@ -10085,14 +9728,7 @@
           <t>M023</t>
         </is>
       </c>
-      <c r="B382" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="B382" t="inlineStr"/>
       <c r="C382" t="inlineStr"/>
       <c r="D382" t="inlineStr"/>
       <c r="E382" s="4" t="inlineStr">
@@ -10113,14 +9749,7 @@
           <t>M023</t>
         </is>
       </c>
-      <c r="B383" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="B383" t="inlineStr"/>
       <c r="C383" t="inlineStr"/>
       <c r="D383" t="inlineStr">
         <is>
@@ -10145,14 +9774,7 @@
           <t>M023</t>
         </is>
       </c>
-      <c r="B384" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="B384" t="inlineStr"/>
       <c r="C384" t="inlineStr">
         <is>
           <t>27/Feb/2025</t>
@@ -11226,14 +10848,7 @@
           <t>M024</t>
         </is>
       </c>
-      <c r="B433" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 246401.97
-Borrower Amount: 246401.97</t>
-        </is>
-      </c>
+      <c r="B433" t="inlineStr"/>
       <c r="C433" t="inlineStr"/>
       <c r="D433" t="inlineStr"/>
       <c r="E433" s="4" t="inlineStr">
@@ -11254,14 +10869,7 @@
           <t>M024</t>
         </is>
       </c>
-      <c r="B434" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 246401.97
-Borrower Amount: 246401.97</t>
-        </is>
-      </c>
+      <c r="B434" t="inlineStr"/>
       <c r="C434" t="inlineStr"/>
       <c r="D434" t="inlineStr">
         <is>
@@ -11286,14 +10894,7 @@
           <t>M024</t>
         </is>
       </c>
-      <c r="B435" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 246401.97
-Borrower Amount: 246401.97</t>
-        </is>
-      </c>
+      <c r="B435" t="inlineStr"/>
       <c r="C435" t="inlineStr">
         <is>
           <t>01/Mar/2025</t>
@@ -11489,14 +11090,7 @@
           <t>M025</t>
         </is>
       </c>
-      <c r="B442" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 26369.63
-Borrower Amount: 26369.63</t>
-        </is>
-      </c>
+      <c r="B442" t="inlineStr"/>
       <c r="C442" t="inlineStr"/>
       <c r="D442" t="inlineStr"/>
       <c r="E442" s="4" t="inlineStr">
@@ -11517,14 +11111,7 @@
           <t>M025</t>
         </is>
       </c>
-      <c r="B443" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 26369.63
-Borrower Amount: 26369.63</t>
-        </is>
-      </c>
+      <c r="B443" t="inlineStr"/>
       <c r="C443" t="inlineStr"/>
       <c r="D443" t="inlineStr">
         <is>
@@ -11549,14 +11136,7 @@
           <t>M025</t>
         </is>
       </c>
-      <c r="B444" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
-Lender Amount: 26369.63
-Borrower Amount: 26369.63</t>
-        </is>
-      </c>
+      <c r="B444" t="inlineStr"/>
       <c r="C444" t="inlineStr">
         <is>
           <t>02/Mar/2025</t>
@@ -12009,14 +11589,7 @@
           <t>M026</t>
         </is>
       </c>
-      <c r="B462" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-222825150235/25
-Lender Amount: 2357.50
-Borrower Amount: 2357.50</t>
-        </is>
-      </c>
+      <c r="B462" t="inlineStr"/>
       <c r="C462" t="inlineStr"/>
       <c r="D462" t="inlineStr"/>
       <c r="E462" s="4" t="inlineStr">
@@ -12037,14 +11610,7 @@
           <t>M026</t>
         </is>
       </c>
-      <c r="B463" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-222825150235/25
-Lender Amount: 2357.50
-Borrower Amount: 2357.50</t>
-        </is>
-      </c>
+      <c r="B463" t="inlineStr"/>
       <c r="C463" t="inlineStr"/>
       <c r="D463" t="inlineStr">
         <is>
@@ -12069,14 +11635,7 @@
           <t>M026</t>
         </is>
       </c>
-      <c r="B464" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-222825150235/25
-Lender Amount: 2357.50
-Borrower Amount: 2357.50</t>
-        </is>
-      </c>
+      <c r="B464" t="inlineStr"/>
       <c r="C464" t="inlineStr">
         <is>
           <t>09/Mar/2025</t>
@@ -12199,14 +11758,7 @@
           <t>M027</t>
         </is>
       </c>
-      <c r="B468" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-222825150235/25
-Lender Amount: 213500.00
-Borrower Amount: 213500.00</t>
-        </is>
-      </c>
+      <c r="B468" t="inlineStr"/>
       <c r="C468" t="inlineStr"/>
       <c r="D468" t="inlineStr"/>
       <c r="E468" s="4" t="inlineStr">
@@ -12227,14 +11779,7 @@
           <t>M027</t>
         </is>
       </c>
-      <c r="B469" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-222825150235/25
-Lender Amount: 213500.00
-Borrower Amount: 213500.00</t>
-        </is>
-      </c>
+      <c r="B469" t="inlineStr"/>
       <c r="C469" t="inlineStr"/>
       <c r="D469" t="inlineStr">
         <is>
@@ -12305,14 +11850,7 @@
           <t>M028</t>
         </is>
       </c>
-      <c r="B471" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="B471" t="inlineStr"/>
       <c r="C471" t="inlineStr"/>
       <c r="D471" t="inlineStr"/>
       <c r="E471" s="4" t="inlineStr">
@@ -12333,14 +11871,7 @@
           <t>M028</t>
         </is>
       </c>
-      <c r="B472" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="B472" t="inlineStr"/>
       <c r="C472" t="inlineStr"/>
       <c r="D472" t="inlineStr">
         <is>
@@ -12411,14 +11942,7 @@
           <t>M029</t>
         </is>
       </c>
-      <c r="B474" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="B474" t="inlineStr"/>
       <c r="C474" t="inlineStr"/>
       <c r="D474" t="inlineStr"/>
       <c r="E474" s="4" t="inlineStr">
@@ -12441,14 +11965,7 @@
           <t>M029</t>
         </is>
       </c>
-      <c r="B475" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="B475" t="inlineStr"/>
       <c r="C475" t="inlineStr"/>
       <c r="D475" t="inlineStr"/>
       <c r="E475" s="4" t="inlineStr">
@@ -12471,14 +11988,7 @@
           <t>M029</t>
         </is>
       </c>
-      <c r="B476" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="B476" t="inlineStr"/>
       <c r="C476" t="inlineStr"/>
       <c r="D476" t="inlineStr"/>
       <c r="E476" s="4" t="inlineStr">
@@ -12499,14 +12009,7 @@
           <t>M029</t>
         </is>
       </c>
-      <c r="B477" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="B477" t="inlineStr"/>
       <c r="C477" t="inlineStr"/>
       <c r="D477" t="inlineStr">
         <is>
@@ -12531,14 +12034,7 @@
           <t>M029</t>
         </is>
       </c>
-      <c r="B478" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="B478" t="inlineStr"/>
       <c r="C478" t="inlineStr">
         <is>
           <t>10/Mar/2025</t>
@@ -13318,14 +12814,7 @@
           <t>M030</t>
         </is>
       </c>
-      <c r="B509" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020027/25
-Lender Amount: 54431.58
-Borrower Amount: 54431.58</t>
-        </is>
-      </c>
+      <c r="B509" t="inlineStr"/>
       <c r="C509" t="inlineStr"/>
       <c r="D509" t="inlineStr"/>
       <c r="E509" s="4" t="inlineStr">
@@ -13346,14 +12835,7 @@
           <t>M030</t>
         </is>
       </c>
-      <c r="B510" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020027/25
-Lender Amount: 54431.58
-Borrower Amount: 54431.58</t>
-        </is>
-      </c>
+      <c r="B510" t="inlineStr"/>
       <c r="C510" t="inlineStr"/>
       <c r="D510" t="inlineStr">
         <is>
@@ -13378,14 +12860,7 @@
           <t>M030</t>
         </is>
       </c>
-      <c r="B511" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020027/25
-Lender Amount: 54431.58
-Borrower Amount: 54431.58</t>
-        </is>
-      </c>
+      <c r="B511" t="inlineStr"/>
       <c r="C511" t="inlineStr">
         <is>
           <t>18/Mar/2025</t>
@@ -13654,14 +13129,7 @@
           <t>M031</t>
         </is>
       </c>
-      <c r="B521" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 8231.99
-Borrower Amount: 8231.99</t>
-        </is>
-      </c>
+      <c r="B521" t="inlineStr"/>
       <c r="C521" t="inlineStr"/>
       <c r="D521" t="inlineStr"/>
       <c r="E521" s="4" t="inlineStr">
@@ -13682,14 +13150,7 @@
           <t>M031</t>
         </is>
       </c>
-      <c r="B522" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 8231.99
-Borrower Amount: 8231.99</t>
-        </is>
-      </c>
+      <c r="B522" t="inlineStr"/>
       <c r="C522" t="inlineStr"/>
       <c r="D522" t="inlineStr">
         <is>
@@ -13714,14 +13175,7 @@
           <t>M031</t>
         </is>
       </c>
-      <c r="B523" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
-Lender Amount: 8231.99
-Borrower Amount: 8231.99</t>
-        </is>
-      </c>
+      <c r="B523" t="inlineStr"/>
       <c r="C523" t="inlineStr">
         <is>
           <t>20/Mar/2025</t>
@@ -14808,14 +14262,7 @@
           <t>M032</t>
         </is>
       </c>
-      <c r="B571" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020708/24
-Lender Amount: 19399.10
-Borrower Amount: 19399.10</t>
-        </is>
-      </c>
+      <c r="B571" t="inlineStr"/>
       <c r="C571" t="inlineStr"/>
       <c r="D571" t="inlineStr"/>
       <c r="E571" s="4" t="inlineStr">
@@ -14836,14 +14283,7 @@
           <t>M032</t>
         </is>
       </c>
-      <c r="B572" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020708/24
-Lender Amount: 19399.10
-Borrower Amount: 19399.10</t>
-        </is>
-      </c>
+      <c r="B572" t="inlineStr"/>
       <c r="C572" t="inlineStr"/>
       <c r="D572" t="inlineStr">
         <is>
@@ -14914,14 +14354,7 @@
           <t>M033</t>
         </is>
       </c>
-      <c r="B574" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
-Lender Amount: 15160.97
-Borrower Amount: 15160.97</t>
-        </is>
-      </c>
+      <c r="B574" t="inlineStr"/>
       <c r="C574" t="inlineStr"/>
       <c r="D574" t="inlineStr"/>
       <c r="E574" s="4" t="inlineStr">
@@ -14942,14 +14375,7 @@
           <t>M033</t>
         </is>
       </c>
-      <c r="B575" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
-Lender Amount: 15160.97
-Borrower Amount: 15160.97</t>
-        </is>
-      </c>
+      <c r="B575" t="inlineStr"/>
       <c r="C575" t="inlineStr"/>
       <c r="D575" t="inlineStr">
         <is>
@@ -14974,14 +14400,7 @@
           <t>M033</t>
         </is>
       </c>
-      <c r="B576" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
-Lender Amount: 15160.97
-Borrower Amount: 15160.97</t>
-        </is>
-      </c>
+      <c r="B576" t="inlineStr"/>
       <c r="C576" t="inlineStr">
         <is>
           <t>27/Mar/2025</t>
@@ -15180,14 +14599,7 @@
           <t>M034</t>
         </is>
       </c>
-      <c r="B584" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
-Lender Amount: 6125933.94
-Borrower Amount: 6125933.94</t>
-        </is>
-      </c>
+      <c r="B584" t="inlineStr"/>
       <c r="C584" t="inlineStr"/>
       <c r="D584" t="inlineStr"/>
       <c r="E584" s="4" t="inlineStr">
@@ -15210,14 +14622,7 @@
           <t>M034</t>
         </is>
       </c>
-      <c r="B585" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
-Lender Amount: 6125933.94
-Borrower Amount: 6125933.94</t>
-        </is>
-      </c>
+      <c r="B585" t="inlineStr"/>
       <c r="C585" t="inlineStr"/>
       <c r="D585" t="inlineStr"/>
       <c r="E585" s="4" t="inlineStr">
@@ -15240,14 +14645,7 @@
           <t>M034</t>
         </is>
       </c>
-      <c r="B586" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
-Lender Amount: 6125933.94
-Borrower Amount: 6125933.94</t>
-        </is>
-      </c>
+      <c r="B586" t="inlineStr"/>
       <c r="C586" t="inlineStr"/>
       <c r="D586" t="inlineStr"/>
       <c r="E586" s="4" t="inlineStr">
@@ -15268,14 +14666,7 @@
           <t>M034</t>
         </is>
       </c>
-      <c r="B587" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
-Lender Amount: 6125933.94
-Borrower Amount: 6125933.94</t>
-        </is>
-      </c>
+      <c r="B587" t="inlineStr"/>
       <c r="C587" t="inlineStr"/>
       <c r="D587" t="inlineStr">
         <is>
@@ -15346,14 +14737,7 @@
           <t>M035</t>
         </is>
       </c>
-      <c r="B589" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022495/24
-Lender Amount: 12425.77
-Borrower Amount: 12425.77</t>
-        </is>
-      </c>
+      <c r="B589" t="inlineStr"/>
       <c r="C589" t="inlineStr"/>
       <c r="D589" t="inlineStr"/>
       <c r="E589" s="4" t="inlineStr">
@@ -15374,14 +14758,7 @@
           <t>M035</t>
         </is>
       </c>
-      <c r="B590" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022495/24
-Lender Amount: 12425.77
-Borrower Amount: 12425.77</t>
-        </is>
-      </c>
+      <c r="B590" t="inlineStr"/>
       <c r="C590" t="inlineStr"/>
       <c r="D590" t="inlineStr">
         <is>
@@ -15452,14 +14829,7 @@
           <t>M036</t>
         </is>
       </c>
-      <c r="B592" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022495/24
-Lender Amount: 23580.68
-Borrower Amount: 23580.68</t>
-        </is>
-      </c>
+      <c r="B592" t="inlineStr"/>
       <c r="C592" t="inlineStr"/>
       <c r="D592" t="inlineStr"/>
       <c r="E592" s="4" t="inlineStr">
@@ -15480,14 +14850,7 @@
           <t>M036</t>
         </is>
       </c>
-      <c r="B593" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022495/24
-Lender Amount: 23580.68
-Borrower Amount: 23580.68</t>
-        </is>
-      </c>
+      <c r="B593" t="inlineStr"/>
       <c r="C593" t="inlineStr"/>
       <c r="D593" t="inlineStr">
         <is>
@@ -15512,14 +14875,7 @@
           <t>M036</t>
         </is>
       </c>
-      <c r="B594" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524022495/24
-Lender Amount: 23580.68
-Borrower Amount: 23580.68</t>
-        </is>
-      </c>
+      <c r="B594" t="inlineStr"/>
       <c r="C594" t="inlineStr">
         <is>
           <t>31/Mar/2025</t>
@@ -16555,14 +15911,7 @@
           <t>M037</t>
         </is>
       </c>
-      <c r="B641" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308525021741/25
-Lender Amount: 22671.95
-Borrower Amount: 22671.95</t>
-        </is>
-      </c>
+      <c r="B641" t="inlineStr"/>
       <c r="C641" t="inlineStr"/>
       <c r="D641" t="inlineStr"/>
       <c r="E641" s="4" t="inlineStr">
@@ -16583,14 +15932,7 @@
           <t>M037</t>
         </is>
       </c>
-      <c r="B642" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308525021741/25
-Lender Amount: 22671.95
-Borrower Amount: 22671.95</t>
-        </is>
-      </c>
+      <c r="B642" t="inlineStr"/>
       <c r="C642" t="inlineStr"/>
       <c r="D642" t="inlineStr">
         <is>
@@ -16661,14 +16003,7 @@
           <t>M038</t>
         </is>
       </c>
-      <c r="B644" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308525021745/25
-Lender Amount: 28854.86
-Borrower Amount: 28854.86</t>
-        </is>
-      </c>
+      <c r="B644" t="inlineStr"/>
       <c r="C644" t="inlineStr"/>
       <c r="D644" t="inlineStr"/>
       <c r="E644" s="4" t="inlineStr">
@@ -16689,14 +16024,7 @@
           <t>M038</t>
         </is>
       </c>
-      <c r="B645" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308525021745/25
-Lender Amount: 28854.86
-Borrower Amount: 28854.86</t>
-        </is>
-      </c>
+      <c r="B645" t="inlineStr"/>
       <c r="C645" t="inlineStr"/>
       <c r="D645" t="inlineStr">
         <is>
@@ -16767,14 +16095,7 @@
           <t>M039</t>
         </is>
       </c>
-      <c r="B647" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="B647" t="inlineStr"/>
       <c r="C647" t="inlineStr"/>
       <c r="D647" t="inlineStr"/>
       <c r="E647" s="4" t="inlineStr">
@@ -16795,14 +16116,7 @@
           <t>M039</t>
         </is>
       </c>
-      <c r="B648" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="B648" t="inlineStr"/>
       <c r="C648" t="inlineStr"/>
       <c r="D648" t="inlineStr">
         <is>
@@ -16827,14 +16141,7 @@
           <t>M039</t>
         </is>
       </c>
-      <c r="B649" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="B649" t="inlineStr"/>
       <c r="C649" t="inlineStr">
         <is>
           <t>07/Apr/2025</t>
@@ -17395,14 +16702,7 @@
           <t>M040</t>
         </is>
       </c>
-      <c r="B671" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
-Lender Amount: 80051.03
-Borrower Amount: 80051.03</t>
-        </is>
-      </c>
+      <c r="B671" t="inlineStr"/>
       <c r="C671" t="inlineStr"/>
       <c r="D671" t="inlineStr"/>
       <c r="E671" s="4" t="inlineStr">
@@ -17423,14 +16723,7 @@
           <t>M040</t>
         </is>
       </c>
-      <c r="B672" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
-Lender Amount: 80051.03
-Borrower Amount: 80051.03</t>
-        </is>
-      </c>
+      <c r="B672" t="inlineStr"/>
       <c r="C672" t="inlineStr"/>
       <c r="D672" t="inlineStr">
         <is>
@@ -17501,14 +16794,7 @@
           <t>M041</t>
         </is>
       </c>
-      <c r="B674" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="B674" t="inlineStr"/>
       <c r="C674" t="inlineStr"/>
       <c r="D674" t="inlineStr"/>
       <c r="E674" s="4" t="inlineStr">
@@ -17531,14 +16817,7 @@
           <t>M041</t>
         </is>
       </c>
-      <c r="B675" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="B675" t="inlineStr"/>
       <c r="C675" t="inlineStr"/>
       <c r="D675" t="inlineStr"/>
       <c r="E675" s="4" t="inlineStr">
@@ -17561,14 +16840,7 @@
           <t>M041</t>
         </is>
       </c>
-      <c r="B676" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="B676" t="inlineStr"/>
       <c r="C676" t="inlineStr"/>
       <c r="D676" t="inlineStr"/>
       <c r="E676" s="4" t="inlineStr">
@@ -17589,14 +16861,7 @@
           <t>M041</t>
         </is>
       </c>
-      <c r="B677" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="B677" t="inlineStr"/>
       <c r="C677" t="inlineStr"/>
       <c r="D677" t="inlineStr">
         <is>
@@ -17621,14 +16886,7 @@
           <t>M041</t>
         </is>
       </c>
-      <c r="B678" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="B678" t="inlineStr"/>
       <c r="C678" t="inlineStr">
         <is>
           <t>16/Apr/2025</t>
@@ -17751,14 +17009,7 @@
           <t>M042</t>
         </is>
       </c>
-      <c r="B682" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="B682" t="inlineStr"/>
       <c r="C682" t="inlineStr"/>
       <c r="D682" t="inlineStr"/>
       <c r="E682" s="4" t="inlineStr">
@@ -17781,14 +17032,7 @@
           <t>M042</t>
         </is>
       </c>
-      <c r="B683" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="B683" t="inlineStr"/>
       <c r="C683" t="inlineStr"/>
       <c r="D683" t="inlineStr"/>
       <c r="E683" s="4" t="inlineStr">
@@ -17811,14 +17055,7 @@
           <t>M042</t>
         </is>
       </c>
-      <c r="B684" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="B684" t="inlineStr"/>
       <c r="C684" t="inlineStr"/>
       <c r="D684" t="inlineStr"/>
       <c r="E684" s="4" t="inlineStr">
@@ -17839,14 +17076,7 @@
           <t>M042</t>
         </is>
       </c>
-      <c r="B685" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="B685" t="inlineStr"/>
       <c r="C685" t="inlineStr"/>
       <c r="D685" t="inlineStr">
         <is>
@@ -17871,14 +17101,7 @@
           <t>M042</t>
         </is>
       </c>
-      <c r="B686" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="B686" t="inlineStr"/>
       <c r="C686" t="inlineStr">
         <is>
           <t>17/Apr/2025</t>
@@ -18147,14 +17370,7 @@
           <t>M043</t>
         </is>
       </c>
-      <c r="B696" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524026037/222824023549
-Lender Amount: 1226351.09
-Borrower Amount: 1226351.09</t>
-        </is>
-      </c>
+      <c r="B696" t="inlineStr"/>
       <c r="C696" t="inlineStr"/>
       <c r="D696" t="inlineStr"/>
       <c r="E696" s="4" t="inlineStr">
@@ -18175,14 +17391,7 @@
           <t>M043</t>
         </is>
       </c>
-      <c r="B697" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524026037/222824023549
-Lender Amount: 1226351.09
-Borrower Amount: 1226351.09</t>
-        </is>
-      </c>
+      <c r="B697" t="inlineStr"/>
       <c r="C697" t="inlineStr"/>
       <c r="D697" t="inlineStr">
         <is>
@@ -18207,14 +17416,7 @@
           <t>M043</t>
         </is>
       </c>
-      <c r="B698" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524026037/222824023549
-Lender Amount: 1226351.09
-Borrower Amount: 1226351.09</t>
-        </is>
-      </c>
+      <c r="B698" t="inlineStr"/>
       <c r="C698" t="inlineStr">
         <is>
           <t>21/Apr/2025</t>
@@ -18337,14 +17539,7 @@
           <t>M044</t>
         </is>
       </c>
-      <c r="B702" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524022495/24
-Lender Amount: 1675000.00
-Borrower Amount: 1675000.00</t>
-        </is>
-      </c>
+      <c r="B702" t="inlineStr"/>
       <c r="C702" t="inlineStr"/>
       <c r="D702" t="inlineStr"/>
       <c r="E702" s="4" t="inlineStr">
@@ -18365,14 +17560,7 @@
           <t>M044</t>
         </is>
       </c>
-      <c r="B703" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524022495/24
-Lender Amount: 1675000.00
-Borrower Amount: 1675000.00</t>
-        </is>
-      </c>
+      <c r="B703" t="inlineStr"/>
       <c r="C703" t="inlineStr"/>
       <c r="D703" t="inlineStr">
         <is>
@@ -18397,14 +17585,7 @@
           <t>M044</t>
         </is>
       </c>
-      <c r="B704" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524022495/24
-Lender Amount: 1675000.00
-Borrower Amount: 1675000.00</t>
-        </is>
-      </c>
+      <c r="B704" t="inlineStr"/>
       <c r="C704" t="inlineStr">
         <is>
           <t>21/Apr/2025</t>
@@ -18600,14 +17781,7 @@
           <t>M045</t>
         </is>
       </c>
-      <c r="B711" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020027/25
-Lender Amount: 10691988.92
-Borrower Amount: 10691988.92</t>
-        </is>
-      </c>
+      <c r="B711" t="inlineStr"/>
       <c r="C711" t="inlineStr"/>
       <c r="D711" t="inlineStr"/>
       <c r="E711" s="4" t="inlineStr">
@@ -18628,14 +17802,7 @@
           <t>M045</t>
         </is>
       </c>
-      <c r="B712" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020027/25
-Lender Amount: 10691988.92
-Borrower Amount: 10691988.92</t>
-        </is>
-      </c>
+      <c r="B712" t="inlineStr"/>
       <c r="C712" t="inlineStr"/>
       <c r="D712" t="inlineStr">
         <is>
@@ -18706,14 +17873,7 @@
           <t>M046</t>
         </is>
       </c>
-      <c r="B714" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-222825150151/25
-Lender Amount: 333706.76
-Borrower Amount: 333706.76</t>
-        </is>
-      </c>
+      <c r="B714" t="inlineStr"/>
       <c r="C714" t="inlineStr"/>
       <c r="D714" t="inlineStr"/>
       <c r="E714" s="4" t="inlineStr">
@@ -18734,14 +17894,7 @@
           <t>M046</t>
         </is>
       </c>
-      <c r="B715" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-222825150151/25
-Lender Amount: 333706.76
-Borrower Amount: 333706.76</t>
-        </is>
-      </c>
+      <c r="B715" t="inlineStr"/>
       <c r="C715" t="inlineStr"/>
       <c r="D715" t="inlineStr">
         <is>
@@ -18812,14 +17965,7 @@
           <t>M047</t>
         </is>
       </c>
-      <c r="B717" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 299000.00
-Borrower Amount: 299000.00</t>
-        </is>
-      </c>
+      <c r="B717" t="inlineStr"/>
       <c r="C717" t="inlineStr"/>
       <c r="D717" t="inlineStr"/>
       <c r="E717" s="4" t="inlineStr">
@@ -18840,14 +17986,7 @@
           <t>M047</t>
         </is>
       </c>
-      <c r="B718" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 299000.00
-Borrower Amount: 299000.00</t>
-        </is>
-      </c>
+      <c r="B718" t="inlineStr"/>
       <c r="C718" t="inlineStr"/>
       <c r="D718" t="inlineStr">
         <is>
@@ -18872,14 +18011,7 @@
           <t>M047</t>
         </is>
       </c>
-      <c r="B719" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
-Lender Amount: 299000.00
-Borrower Amount: 299000.00</t>
-        </is>
-      </c>
+      <c r="B719" t="inlineStr"/>
       <c r="C719" t="inlineStr">
         <is>
           <t>23/Apr/2025</t>
@@ -19002,14 +18134,7 @@
           <t>M048</t>
         </is>
       </c>
-      <c r="B723" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
-Lender Amount: 13743.52
-Borrower Amount: 13743.52</t>
-        </is>
-      </c>
+      <c r="B723" t="inlineStr"/>
       <c r="C723" t="inlineStr"/>
       <c r="D723" t="inlineStr"/>
       <c r="E723" s="4" t="inlineStr">
@@ -19030,14 +18155,7 @@
           <t>M048</t>
         </is>
       </c>
-      <c r="B724" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
-Lender Amount: 13743.52
-Borrower Amount: 13743.52</t>
-        </is>
-      </c>
+      <c r="B724" t="inlineStr"/>
       <c r="C724" t="inlineStr"/>
       <c r="D724" t="inlineStr">
         <is>
@@ -19062,14 +18180,7 @@
           <t>M048</t>
         </is>
       </c>
-      <c r="B725" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
-Lender Amount: 13743.52
-Borrower Amount: 13743.52</t>
-        </is>
-      </c>
+      <c r="B725" t="inlineStr"/>
       <c r="C725" t="inlineStr">
         <is>
           <t>24/Apr/2025</t>
@@ -19360,14 +18471,7 @@
           <t>M049</t>
         </is>
       </c>
-      <c r="B737" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155825020020/25
-Lender Amount: 60302.55
-Borrower Amount: 60302.55</t>
-        </is>
-      </c>
+      <c r="B737" t="inlineStr"/>
       <c r="C737" t="inlineStr"/>
       <c r="D737" t="inlineStr"/>
       <c r="E737" s="4" t="inlineStr">
@@ -19388,14 +18492,7 @@
           <t>M049</t>
         </is>
       </c>
-      <c r="B738" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155825020020/25
-Lender Amount: 60302.55
-Borrower Amount: 60302.55</t>
-        </is>
-      </c>
+      <c r="B738" t="inlineStr"/>
       <c r="C738" t="inlineStr"/>
       <c r="D738" t="inlineStr">
         <is>
@@ -19466,14 +18563,7 @@
           <t>M050</t>
         </is>
       </c>
-      <c r="B740" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
-Lender Amount: 124008.78
-Borrower Amount: 124008.78</t>
-        </is>
-      </c>
+      <c r="B740" t="inlineStr"/>
       <c r="C740" t="inlineStr"/>
       <c r="D740" t="inlineStr"/>
       <c r="E740" s="4" t="inlineStr">
@@ -19494,14 +18584,7 @@
           <t>M050</t>
         </is>
       </c>
-      <c r="B741" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
-Lender Amount: 124008.78
-Borrower Amount: 124008.78</t>
-        </is>
-      </c>
+      <c r="B741" t="inlineStr"/>
       <c r="C741" t="inlineStr"/>
       <c r="D741" t="inlineStr">
         <is>
@@ -19572,14 +18655,7 @@
           <t>M051</t>
         </is>
       </c>
-      <c r="B743" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
-Lender Amount: 31609.80
-Borrower Amount: 31609.80</t>
-        </is>
-      </c>
+      <c r="B743" t="inlineStr"/>
       <c r="C743" t="inlineStr"/>
       <c r="D743" t="inlineStr"/>
       <c r="E743" s="4" t="inlineStr">
@@ -19600,14 +18676,7 @@
           <t>M051</t>
         </is>
       </c>
-      <c r="B744" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
-Lender Amount: 31609.80
-Borrower Amount: 31609.80</t>
-        </is>
-      </c>
+      <c r="B744" t="inlineStr"/>
       <c r="C744" t="inlineStr"/>
       <c r="D744" t="inlineStr">
         <is>
@@ -19632,14 +18701,7 @@
           <t>M051</t>
         </is>
       </c>
-      <c r="B745" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
-Lender Amount: 31609.80
-Borrower Amount: 31609.80</t>
-        </is>
-      </c>
+      <c r="B745" t="inlineStr"/>
       <c r="C745" t="inlineStr">
         <is>
           <t>28/Apr/2025</t>
@@ -20092,14 +19154,7 @@
           <t>M052</t>
         </is>
       </c>
-      <c r="B763" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
-Lender Amount: 10424886.36
-Borrower Amount: 10424886.36</t>
-        </is>
-      </c>
+      <c r="B763" t="inlineStr"/>
       <c r="C763" t="inlineStr"/>
       <c r="D763" t="inlineStr"/>
       <c r="E763" s="4" t="inlineStr">
@@ -20120,14 +19175,7 @@
           <t>M052</t>
         </is>
       </c>
-      <c r="B764" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
-Lender Amount: 10424886.36
-Borrower Amount: 10424886.36</t>
-        </is>
-      </c>
+      <c r="B764" t="inlineStr"/>
       <c r="C764" t="inlineStr"/>
       <c r="D764" t="inlineStr">
         <is>
@@ -20198,14 +19246,7 @@
           <t>M053</t>
         </is>
       </c>
-      <c r="B766" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020063/25
-Lender Amount: 2168751.40
-Borrower Amount: 2168751.40</t>
-        </is>
-      </c>
+      <c r="B766" t="inlineStr"/>
       <c r="C766" t="inlineStr"/>
       <c r="D766" t="inlineStr"/>
       <c r="E766" s="4" t="inlineStr">
@@ -20226,14 +19267,7 @@
           <t>M053</t>
         </is>
       </c>
-      <c r="B767" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020063/25
-Lender Amount: 2168751.40
-Borrower Amount: 2168751.40</t>
-        </is>
-      </c>
+      <c r="B767" t="inlineStr"/>
       <c r="C767" t="inlineStr"/>
       <c r="D767" t="inlineStr">
         <is>
@@ -20258,14 +19292,7 @@
           <t>M053</t>
         </is>
       </c>
-      <c r="B768" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020063/25
-Lender Amount: 2168751.40
-Borrower Amount: 2168751.40</t>
-        </is>
-      </c>
+      <c r="B768" t="inlineStr"/>
       <c r="C768" t="inlineStr">
         <is>
           <t>30/Apr/2025</t>
@@ -20388,14 +19415,7 @@
           <t>M054</t>
         </is>
       </c>
-      <c r="B772" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
-Lender Amount: 63787.54
-Borrower Amount: 63787.54</t>
-        </is>
-      </c>
+      <c r="B772" t="inlineStr"/>
       <c r="C772" t="inlineStr"/>
       <c r="D772" t="inlineStr"/>
       <c r="E772" s="4" t="inlineStr">
@@ -20416,14 +19436,7 @@
           <t>M054</t>
         </is>
       </c>
-      <c r="B773" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
-Lender Amount: 63787.54
-Borrower Amount: 63787.54</t>
-        </is>
-      </c>
+      <c r="B773" t="inlineStr"/>
       <c r="C773" t="inlineStr"/>
       <c r="D773" t="inlineStr">
         <is>
@@ -20448,14 +19461,7 @@
           <t>M054</t>
         </is>
       </c>
-      <c r="B774" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
-Lender Amount: 63787.54
-Borrower Amount: 63787.54</t>
-        </is>
-      </c>
+      <c r="B774" t="inlineStr"/>
       <c r="C774" t="inlineStr">
         <is>
           <t>30/Apr/2025</t>
@@ -23888,14 +22894,7 @@
           <t>M055</t>
         </is>
       </c>
-      <c r="B921" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020104/25
-Lender Amount: 111771.42
-Borrower Amount: 111771.42</t>
-        </is>
-      </c>
+      <c r="B921" t="inlineStr"/>
       <c r="C921" t="inlineStr"/>
       <c r="D921" t="inlineStr"/>
       <c r="E921" s="4" t="inlineStr">
@@ -23916,14 +22915,7 @@
           <t>M055</t>
         </is>
       </c>
-      <c r="B922" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020104/25
-Lender Amount: 111771.42
-Borrower Amount: 111771.42</t>
-        </is>
-      </c>
+      <c r="B922" t="inlineStr"/>
       <c r="C922" t="inlineStr"/>
       <c r="D922" t="inlineStr">
         <is>
@@ -23994,14 +22986,7 @@
           <t>M056</t>
         </is>
       </c>
-      <c r="B924" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020112/25
-Lender Amount: 80701.76
-Borrower Amount: 80701.76</t>
-        </is>
-      </c>
+      <c r="B924" t="inlineStr"/>
       <c r="C924" t="inlineStr"/>
       <c r="D924" t="inlineStr"/>
       <c r="E924" s="4" t="inlineStr">
@@ -24022,14 +23007,7 @@
           <t>M056</t>
         </is>
       </c>
-      <c r="B925" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020112/25
-Lender Amount: 80701.76
-Borrower Amount: 80701.76</t>
-        </is>
-      </c>
+      <c r="B925" t="inlineStr"/>
       <c r="C925" t="inlineStr"/>
       <c r="D925" t="inlineStr">
         <is>
@@ -24100,14 +23078,7 @@
           <t>M057</t>
         </is>
       </c>
-      <c r="B927" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020112/25
-Lender Amount: 657.81
-Borrower Amount: 657.81</t>
-        </is>
-      </c>
+      <c r="B927" t="inlineStr"/>
       <c r="C927" t="inlineStr"/>
       <c r="D927" t="inlineStr"/>
       <c r="E927" s="4" t="inlineStr">
@@ -24128,14 +23099,7 @@
           <t>M057</t>
         </is>
       </c>
-      <c r="B928" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020112/25
-Lender Amount: 657.81
-Borrower Amount: 657.81</t>
-        </is>
-      </c>
+      <c r="B928" t="inlineStr"/>
       <c r="C928" t="inlineStr"/>
       <c r="D928" t="inlineStr">
         <is>
@@ -24160,14 +23124,7 @@
           <t>M057</t>
         </is>
       </c>
-      <c r="B929" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020112/25
-Lender Amount: 657.81
-Borrower Amount: 657.81</t>
-        </is>
-      </c>
+      <c r="B929" t="inlineStr"/>
       <c r="C929" t="inlineStr">
         <is>
           <t>17/May/2025</t>
@@ -24509,14 +23466,7 @@
           <t>M058</t>
         </is>
       </c>
-      <c r="B942" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
-Lender Amount: 81730.06
-Borrower Amount: 81730.06</t>
-        </is>
-      </c>
+      <c r="B942" t="inlineStr"/>
       <c r="C942" t="inlineStr"/>
       <c r="D942" t="inlineStr"/>
       <c r="E942" s="4" t="inlineStr">
@@ -24537,14 +23487,7 @@
           <t>M058</t>
         </is>
       </c>
-      <c r="B943" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
-Lender Amount: 81730.06
-Borrower Amount: 81730.06</t>
-        </is>
-      </c>
+      <c r="B943" t="inlineStr"/>
       <c r="C943" t="inlineStr"/>
       <c r="D943" t="inlineStr">
         <is>
@@ -24569,14 +23512,7 @@
           <t>M058</t>
         </is>
       </c>
-      <c r="B944" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
-Lender Amount: 81730.06
-Borrower Amount: 81730.06</t>
-        </is>
-      </c>
+      <c r="B944" t="inlineStr"/>
       <c r="C944" t="inlineStr">
         <is>
           <t>18/May/2025</t>
@@ -24991,14 +23927,7 @@
           <t>M059</t>
         </is>
       </c>
-      <c r="B960" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020163/25
-Lender Amount: 341847.68
-Borrower Amount: 341847.68</t>
-        </is>
-      </c>
+      <c r="B960" t="inlineStr"/>
       <c r="C960" t="inlineStr"/>
       <c r="D960" t="inlineStr"/>
       <c r="E960" s="4" t="inlineStr">
@@ -25021,14 +23950,7 @@
           <t>M059</t>
         </is>
       </c>
-      <c r="B961" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020163/25
-Lender Amount: 341847.68
-Borrower Amount: 341847.68</t>
-        </is>
-      </c>
+      <c r="B961" t="inlineStr"/>
       <c r="C961" t="inlineStr"/>
       <c r="D961" t="inlineStr"/>
       <c r="E961" s="4" t="inlineStr">
@@ -25051,14 +23973,7 @@
           <t>M059</t>
         </is>
       </c>
-      <c r="B962" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020163/25
-Lender Amount: 341847.68
-Borrower Amount: 341847.68</t>
-        </is>
-      </c>
+      <c r="B962" t="inlineStr"/>
       <c r="C962" t="inlineStr"/>
       <c r="D962" t="inlineStr"/>
       <c r="E962" s="4" t="inlineStr">
@@ -25079,14 +23994,7 @@
           <t>M059</t>
         </is>
       </c>
-      <c r="B963" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020163/25
-Lender Amount: 341847.68
-Borrower Amount: 341847.68</t>
-        </is>
-      </c>
+      <c r="B963" t="inlineStr"/>
       <c r="C963" t="inlineStr"/>
       <c r="D963" t="inlineStr">
         <is>
@@ -25111,14 +24019,7 @@
           <t>M059</t>
         </is>
       </c>
-      <c r="B964" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020163/25
-Lender Amount: 341847.68
-Borrower Amount: 341847.68</t>
-        </is>
-      </c>
+      <c r="B964" t="inlineStr"/>
       <c r="C964" t="inlineStr">
         <is>
           <t>28/May/2025</t>
@@ -25352,14 +24253,7 @@
           <t>M060</t>
         </is>
       </c>
-      <c r="B973" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-222825150235/25
-Lender Amount: 36757.00
-Borrower Amount: 36757.00</t>
-        </is>
-      </c>
+      <c r="B973" t="inlineStr"/>
       <c r="C973" t="inlineStr"/>
       <c r="D973" t="inlineStr"/>
       <c r="E973" s="4" t="inlineStr">
@@ -25380,14 +24274,7 @@
           <t>M060</t>
         </is>
       </c>
-      <c r="B974" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-222825150235/25
-Lender Amount: 36757.00
-Borrower Amount: 36757.00</t>
-        </is>
-      </c>
+      <c r="B974" t="inlineStr"/>
       <c r="C974" t="inlineStr"/>
       <c r="D974" t="inlineStr">
         <is>
@@ -25412,14 +24299,7 @@
           <t>M060</t>
         </is>
       </c>
-      <c r="B975" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-222825150235/25
-Lender Amount: 36757.00
-Borrower Amount: 36757.00</t>
-        </is>
-      </c>
+      <c r="B975" t="inlineStr"/>
       <c r="C975" t="inlineStr">
         <is>
           <t>29/May/2025</t>
@@ -25542,14 +24422,7 @@
           <t>M061</t>
         </is>
       </c>
-      <c r="B979" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="B979" t="inlineStr"/>
       <c r="C979" t="inlineStr"/>
       <c r="D979" t="inlineStr"/>
       <c r="E979" s="4" t="inlineStr">
@@ -25572,14 +24445,7 @@
           <t>M061</t>
         </is>
       </c>
-      <c r="B980" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="B980" t="inlineStr"/>
       <c r="C980" t="inlineStr"/>
       <c r="D980" t="inlineStr"/>
       <c r="E980" s="4" t="inlineStr">
@@ -25602,14 +24468,7 @@
           <t>M061</t>
         </is>
       </c>
-      <c r="B981" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="B981" t="inlineStr"/>
       <c r="C981" t="inlineStr"/>
       <c r="D981" t="inlineStr"/>
       <c r="E981" s="4" t="inlineStr">
@@ -25632,14 +24491,7 @@
           <t>M061</t>
         </is>
       </c>
-      <c r="B982" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="B982" t="inlineStr"/>
       <c r="C982" t="inlineStr"/>
       <c r="D982" t="inlineStr"/>
       <c r="E982" s="4" t="inlineStr">
@@ -25660,14 +24512,7 @@
           <t>M061</t>
         </is>
       </c>
-      <c r="B983" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="B983" t="inlineStr"/>
       <c r="C983" t="inlineStr"/>
       <c r="D983" t="inlineStr">
         <is>
@@ -25738,14 +24583,7 @@
           <t>M062</t>
         </is>
       </c>
-      <c r="B985" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524990243/24
-Lender Amount: 68747.06
-Borrower Amount: 68747.06</t>
-        </is>
-      </c>
+      <c r="B985" t="inlineStr"/>
       <c r="C985" t="inlineStr"/>
       <c r="D985" t="inlineStr"/>
       <c r="E985" s="4" t="inlineStr">
@@ -25766,14 +24604,7 @@
           <t>M062</t>
         </is>
       </c>
-      <c r="B986" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524990243/24
-Lender Amount: 68747.06
-Borrower Amount: 68747.06</t>
-        </is>
-      </c>
+      <c r="B986" t="inlineStr"/>
       <c r="C986" t="inlineStr"/>
       <c r="D986" t="inlineStr">
         <is>
@@ -25798,14 +24629,7 @@
           <t>M062</t>
         </is>
       </c>
-      <c r="B987" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524990243/24
-Lender Amount: 68747.06
-Borrower Amount: 68747.06</t>
-        </is>
-      </c>
+      <c r="B987" t="inlineStr"/>
       <c r="C987" t="inlineStr">
         <is>
           <t>29/May/2025</t>
@@ -26389,14 +25213,7 @@
           <t>M063</t>
         </is>
       </c>
-      <c r="B1011" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308525021741/25
-Lender Amount: 31411.11
-Borrower Amount: 31411.11</t>
-        </is>
-      </c>
+      <c r="B1011" t="inlineStr"/>
       <c r="C1011" t="inlineStr"/>
       <c r="D1011" t="inlineStr"/>
       <c r="E1011" s="4" t="inlineStr">
@@ -26417,14 +25234,7 @@
           <t>M063</t>
         </is>
       </c>
-      <c r="B1012" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308525021741/25
-Lender Amount: 31411.11
-Borrower Amount: 31411.11</t>
-        </is>
-      </c>
+      <c r="B1012" t="inlineStr"/>
       <c r="C1012" t="inlineStr"/>
       <c r="D1012" t="inlineStr">
         <is>
@@ -26449,14 +25259,7 @@
           <t>M063</t>
         </is>
       </c>
-      <c r="B1013" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308525021741/25
-Lender Amount: 31411.11
-Borrower Amount: 31411.11</t>
-        </is>
-      </c>
+      <c r="B1013" t="inlineStr"/>
       <c r="C1013" t="inlineStr">
         <is>
           <t>01/Jun/2025</t>
@@ -26945,14 +25748,7 @@
           <t>M064</t>
         </is>
       </c>
-      <c r="B1032" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155825010037/25
-Lender Amount: 853297.01
-Borrower Amount: 853297.01</t>
-        </is>
-      </c>
+      <c r="B1032" t="inlineStr"/>
       <c r="C1032" t="inlineStr"/>
       <c r="D1032" t="inlineStr"/>
       <c r="E1032" s="4" t="inlineStr">
@@ -26973,14 +25769,7 @@
           <t>M064</t>
         </is>
       </c>
-      <c r="B1033" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155825010037/25
-Lender Amount: 853297.01
-Borrower Amount: 853297.01</t>
-        </is>
-      </c>
+      <c r="B1033" t="inlineStr"/>
       <c r="C1033" t="inlineStr"/>
       <c r="D1033" t="inlineStr">
         <is>
@@ -27005,14 +25794,7 @@
           <t>M064</t>
         </is>
       </c>
-      <c r="B1034" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-155825010037/25
-Lender Amount: 853297.01
-Borrower Amount: 853297.01</t>
-        </is>
-      </c>
+      <c r="B1034" t="inlineStr"/>
       <c r="C1034" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
@@ -28652,14 +27434,7 @@
           <t>M065</t>
         </is>
       </c>
-      <c r="B1101" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020163/25
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="B1101" t="inlineStr"/>
       <c r="C1101" t="inlineStr"/>
       <c r="D1101" t="inlineStr"/>
       <c r="E1101" s="4" t="inlineStr">
@@ -28680,14 +27455,7 @@
           <t>M065</t>
         </is>
       </c>
-      <c r="B1102" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020163/25
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="B1102" t="inlineStr"/>
       <c r="C1102" t="inlineStr"/>
       <c r="D1102" t="inlineStr">
         <is>
@@ -28758,14 +27526,7 @@
           <t>M066</t>
         </is>
       </c>
-      <c r="B1104" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308525021746/25
-Lender Amount: 35373.50
-Borrower Amount: 35373.50</t>
-        </is>
-      </c>
+      <c r="B1104" t="inlineStr"/>
       <c r="C1104" t="inlineStr"/>
       <c r="D1104" t="inlineStr"/>
       <c r="E1104" s="4" t="inlineStr">
@@ -28786,14 +27547,7 @@
           <t>M066</t>
         </is>
       </c>
-      <c r="B1105" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308525021746/25
-Lender Amount: 35373.50
-Borrower Amount: 35373.50</t>
-        </is>
-      </c>
+      <c r="B1105" t="inlineStr"/>
       <c r="C1105" t="inlineStr"/>
       <c r="D1105" t="inlineStr">
         <is>
@@ -28818,14 +27572,7 @@
           <t>M066</t>
         </is>
       </c>
-      <c r="B1106" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308525021746/25
-Lender Amount: 35373.50
-Borrower Amount: 35373.50</t>
-        </is>
-      </c>
+      <c r="B1106" t="inlineStr"/>
       <c r="C1106" t="inlineStr">
         <is>
           <t>17/Jun/2025</t>
@@ -29351,14 +28098,7 @@
           <t>M067</t>
         </is>
       </c>
-      <c r="B1127" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="B1127" t="inlineStr"/>
       <c r="C1127" t="inlineStr"/>
       <c r="D1127" t="inlineStr"/>
       <c r="E1127" s="4" t="inlineStr">
@@ -29381,14 +28121,7 @@
           <t>M067</t>
         </is>
       </c>
-      <c r="B1128" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="B1128" t="inlineStr"/>
       <c r="C1128" t="inlineStr"/>
       <c r="D1128" t="inlineStr"/>
       <c r="E1128" s="4" t="inlineStr">
@@ -29411,14 +28144,7 @@
           <t>M067</t>
         </is>
       </c>
-      <c r="B1129" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="B1129" t="inlineStr"/>
       <c r="C1129" t="inlineStr"/>
       <c r="D1129" t="inlineStr"/>
       <c r="E1129" s="4" t="inlineStr">
@@ -29441,14 +28167,7 @@
           <t>M067</t>
         </is>
       </c>
-      <c r="B1130" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="B1130" t="inlineStr"/>
       <c r="C1130" t="inlineStr"/>
       <c r="D1130" t="inlineStr"/>
       <c r="E1130" s="4" t="inlineStr">
@@ -29471,14 +28190,7 @@
           <t>M067</t>
         </is>
       </c>
-      <c r="B1131" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="B1131" t="inlineStr"/>
       <c r="C1131" t="inlineStr"/>
       <c r="D1131" t="inlineStr"/>
       <c r="E1131" s="4" t="inlineStr">
@@ -29499,14 +28211,7 @@
           <t>M067</t>
         </is>
       </c>
-      <c r="B1132" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="B1132" t="inlineStr"/>
       <c r="C1132" t="inlineStr"/>
       <c r="D1132" t="inlineStr">
         <is>
@@ -29577,14 +28282,7 @@
           <t>M068</t>
         </is>
       </c>
-      <c r="B1134" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524022166 
-Lender Amount: 758000.00
-Borrower Amount: 758000.00</t>
-        </is>
-      </c>
+      <c r="B1134" t="inlineStr"/>
       <c r="C1134" t="inlineStr"/>
       <c r="D1134" t="inlineStr"/>
       <c r="E1134" s="4" t="inlineStr">
@@ -29605,14 +28303,7 @@
           <t>M068</t>
         </is>
       </c>
-      <c r="B1135" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524022166 
-Lender Amount: 758000.00
-Borrower Amount: 758000.00</t>
-        </is>
-      </c>
+      <c r="B1135" t="inlineStr"/>
       <c r="C1135" t="inlineStr"/>
       <c r="D1135" t="inlineStr">
         <is>
@@ -29637,14 +28328,7 @@
           <t>M068</t>
         </is>
       </c>
-      <c r="B1136" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524022166 
-Lender Amount: 758000.00
-Borrower Amount: 758000.00</t>
-        </is>
-      </c>
+      <c r="B1136" t="inlineStr"/>
       <c r="C1136" t="inlineStr">
         <is>
           <t>23/Jun/2025</t>
@@ -30278,14 +28962,7 @@
           <t>M069</t>
         </is>
       </c>
-      <c r="B1161" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524022166 
-Lender Amount: 4009000.00
-Borrower Amount: 4009000.00</t>
-        </is>
-      </c>
+      <c r="B1161" t="inlineStr"/>
       <c r="C1161" t="inlineStr"/>
       <c r="D1161" t="inlineStr"/>
       <c r="E1161" s="4" t="inlineStr">
@@ -30306,14 +28983,7 @@
           <t>M069</t>
         </is>
       </c>
-      <c r="B1162" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524022166 
-Lender Amount: 4009000.00
-Borrower Amount: 4009000.00</t>
-        </is>
-      </c>
+      <c r="B1162" t="inlineStr"/>
       <c r="C1162" t="inlineStr"/>
       <c r="D1162" t="inlineStr">
         <is>
@@ -30338,14 +29008,7 @@
           <t>M069</t>
         </is>
       </c>
-      <c r="B1163" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-LC-308524022166 
-Lender Amount: 4009000.00
-Borrower Amount: 4009000.00</t>
-        </is>
-      </c>
+      <c r="B1163" t="inlineStr"/>
       <c r="C1163" t="inlineStr">
         <is>
           <t>24/Jun/2025</t>
@@ -30541,14 +29204,7 @@
           <t>M070</t>
         </is>
       </c>
-      <c r="B1170" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
-Lender Amount: 14417.98
-Borrower Amount: 14417.98</t>
-        </is>
-      </c>
+      <c r="B1170" t="inlineStr"/>
       <c r="C1170" t="inlineStr"/>
       <c r="D1170" t="inlineStr"/>
       <c r="E1170" s="4" t="inlineStr">
@@ -30569,14 +29225,7 @@
           <t>M070</t>
         </is>
       </c>
-      <c r="B1171" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
-Lender Amount: 14417.98
-Borrower Amount: 14417.98</t>
-        </is>
-      </c>
+      <c r="B1171" t="inlineStr"/>
       <c r="C1171" t="inlineStr"/>
       <c r="D1171" t="inlineStr">
         <is>
@@ -30601,14 +29250,7 @@
           <t>M070</t>
         </is>
       </c>
-      <c r="B1172" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
-Lender Amount: 14417.98
-Borrower Amount: 14417.98</t>
-        </is>
-      </c>
+      <c r="B1172" t="inlineStr"/>
       <c r="C1172" t="inlineStr">
         <is>
           <t>24/Jun/2025</t>
@@ -31242,14 +29884,7 @@
           <t>M071</t>
         </is>
       </c>
-      <c r="B1197" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020202/25
-Lender Amount: 3499168.01
-Borrower Amount: 3499168.01</t>
-        </is>
-      </c>
+      <c r="B1197" t="inlineStr"/>
       <c r="C1197" t="inlineStr"/>
       <c r="D1197" t="inlineStr"/>
       <c r="E1197" s="4" t="inlineStr">
@@ -31270,14 +29905,7 @@
           <t>M071</t>
         </is>
       </c>
-      <c r="B1198" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020202/25
-Lender Amount: 3499168.01
-Borrower Amount: 3499168.01</t>
-        </is>
-      </c>
+      <c r="B1198" t="inlineStr"/>
       <c r="C1198" t="inlineStr"/>
       <c r="D1198" t="inlineStr">
         <is>
@@ -31302,14 +29930,7 @@
           <t>M071</t>
         </is>
       </c>
-      <c r="B1199" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147125020202/25
-Lender Amount: 3499168.01
-Borrower Amount: 3499168.01</t>
-        </is>
-      </c>
+      <c r="B1199" t="inlineStr"/>
       <c r="C1199" t="inlineStr">
         <is>
           <t>26/Jun/2025</t>
@@ -31787,14 +30408,7 @@
           <t>M072</t>
         </is>
       </c>
-      <c r="B1220" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020074/24
-Lender Amount: 6242871.55
-Borrower Amount: 6242871.55</t>
-        </is>
-      </c>
+      <c r="B1220" t="inlineStr"/>
       <c r="C1220" t="inlineStr"/>
       <c r="D1220" t="inlineStr"/>
       <c r="E1220" s="4" t="inlineStr">
@@ -31815,14 +30429,7 @@
           <t>M072</t>
         </is>
       </c>
-      <c r="B1221" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020074/24
-Lender Amount: 6242871.55
-Borrower Amount: 6242871.55</t>
-        </is>
-      </c>
+      <c r="B1221" t="inlineStr"/>
       <c r="C1221" t="inlineStr"/>
       <c r="D1221" t="inlineStr">
         <is>
@@ -31847,14 +30454,7 @@
           <t>M072</t>
         </is>
       </c>
-      <c r="B1222" s="4" t="inlineStr">
-        <is>
-          <t>Match Type: LC Match
-L/C-147124020074/24
-Lender Amount: 6242871.55
-Borrower Amount: 6242871.55</t>
-        </is>
-      </c>
+      <c r="B1222" t="inlineStr"/>
       <c r="C1222" t="inlineStr">
         <is>
           <t>30/Jun/2025</t>

</xml_diff>

<commit_message>
Transaction block logic fixed
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -1583,11 +1583,7 @@
       <c r="K53" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>M001</t>
-        </is>
-      </c>
+      <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
@@ -1604,11 +1600,7 @@
       <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>M001</t>
-        </is>
-      </c>
+      <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
@@ -1675,11 +1667,7 @@
       <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
+      <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
@@ -1698,11 +1686,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
+      <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
@@ -1721,11 +1705,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
+      <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
@@ -1744,11 +1724,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
+      <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
@@ -1765,11 +1741,7 @@
       <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
+      <c r="A61" t="inlineStr"/>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
@@ -1790,11 +1762,7 @@
       <c r="K61" t="inlineStr"/>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
+      <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
@@ -1986,11 +1954,7 @@
       <c r="K68" t="inlineStr"/>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
+      <c r="A69" t="inlineStr"/>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
@@ -2007,11 +1971,7 @@
       <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
+      <c r="A70" t="inlineStr"/>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
@@ -2078,11 +2038,7 @@
       <c r="K71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>M005</t>
-        </is>
-      </c>
+      <c r="A72" t="inlineStr"/>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
@@ -2099,11 +2055,7 @@
       <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>M005</t>
-        </is>
-      </c>
+      <c r="A73" t="inlineStr"/>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
@@ -2124,11 +2076,7 @@
       <c r="K73" t="inlineStr"/>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>M005</t>
-        </is>
-      </c>
+      <c r="A74" t="inlineStr"/>
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr">
         <is>
@@ -2466,11 +2414,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>M007</t>
-        </is>
-      </c>
+      <c r="A87" t="inlineStr"/>
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
@@ -2487,11 +2431,7 @@
       <c r="K87" t="inlineStr"/>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>M007</t>
-        </is>
-      </c>
+      <c r="A88" t="inlineStr"/>
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
@@ -2558,11 +2498,7 @@
       <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>M009</t>
-        </is>
-      </c>
+      <c r="A90" t="inlineStr"/>
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
@@ -2579,11 +2515,7 @@
       <c r="K90" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>M009</t>
-        </is>
-      </c>
+      <c r="A91" t="inlineStr"/>
       <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
@@ -2604,11 +2536,7 @@
       <c r="K91" t="inlineStr"/>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>M009</t>
-        </is>
-      </c>
+      <c r="A92" t="inlineStr"/>
       <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr">
         <is>
@@ -3019,11 +2947,7 @@
       <c r="K107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>M010</t>
-        </is>
-      </c>
+      <c r="A108" t="inlineStr"/>
       <c r="B108" t="inlineStr"/>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
@@ -3040,11 +2964,7 @@
       <c r="K108" t="inlineStr"/>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>M010</t>
-        </is>
-      </c>
+      <c r="A109" t="inlineStr"/>
       <c r="B109" t="inlineStr"/>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr">
@@ -3065,11 +2985,7 @@
       <c r="K109" t="inlineStr"/>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>M010</t>
-        </is>
-      </c>
+      <c r="A110" t="inlineStr"/>
       <c r="B110" t="inlineStr"/>
       <c r="C110" t="inlineStr">
         <is>
@@ -5856,11 +5772,7 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" t="inlineStr">
-        <is>
-          <t>M012</t>
-        </is>
-      </c>
+      <c r="A230" t="inlineStr"/>
       <c r="B230" t="inlineStr"/>
       <c r="C230" t="inlineStr"/>
       <c r="D230" t="inlineStr"/>
@@ -5877,11 +5789,7 @@
       <c r="K230" t="inlineStr"/>
     </row>
     <row r="231">
-      <c r="A231" t="inlineStr">
-        <is>
-          <t>M012</t>
-        </is>
-      </c>
+      <c r="A231" t="inlineStr"/>
       <c r="B231" t="inlineStr"/>
       <c r="C231" t="inlineStr"/>
       <c r="D231" t="inlineStr">
@@ -5902,11 +5810,7 @@
       <c r="K231" t="inlineStr"/>
     </row>
     <row r="232">
-      <c r="A232" t="inlineStr">
-        <is>
-          <t>M012</t>
-        </is>
-      </c>
+      <c r="A232" t="inlineStr"/>
       <c r="B232" t="inlineStr"/>
       <c r="C232" t="inlineStr">
         <is>
@@ -6025,11 +5929,7 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" t="inlineStr">
-        <is>
-          <t>M013</t>
-        </is>
-      </c>
+      <c r="A236" t="inlineStr"/>
       <c r="B236" t="inlineStr"/>
       <c r="C236" t="inlineStr"/>
       <c r="D236" t="inlineStr"/>
@@ -6046,11 +5946,7 @@
       <c r="K236" t="inlineStr"/>
     </row>
     <row r="237">
-      <c r="A237" t="inlineStr">
-        <is>
-          <t>M013</t>
-        </is>
-      </c>
+      <c r="A237" t="inlineStr"/>
       <c r="B237" t="inlineStr"/>
       <c r="C237" t="inlineStr"/>
       <c r="D237" t="inlineStr">
@@ -6071,11 +5967,7 @@
       <c r="K237" t="inlineStr"/>
     </row>
     <row r="238">
-      <c r="A238" t="inlineStr">
-        <is>
-          <t>M013</t>
-        </is>
-      </c>
+      <c r="A238" t="inlineStr"/>
       <c r="B238" t="inlineStr"/>
       <c r="C238" t="inlineStr">
         <is>
@@ -6524,11 +6416,7 @@
       <c r="K255" t="inlineStr"/>
     </row>
     <row r="256">
-      <c r="A256" t="inlineStr">
-        <is>
-          <t>M014</t>
-        </is>
-      </c>
+      <c r="A256" t="inlineStr"/>
       <c r="B256" t="inlineStr"/>
       <c r="C256" t="inlineStr"/>
       <c r="D256" t="inlineStr"/>
@@ -6545,11 +6433,7 @@
       <c r="K256" t="inlineStr"/>
     </row>
     <row r="257">
-      <c r="A257" t="inlineStr">
-        <is>
-          <t>M014</t>
-        </is>
-      </c>
+      <c r="A257" t="inlineStr"/>
       <c r="B257" t="inlineStr"/>
       <c r="C257" t="inlineStr"/>
       <c r="D257" t="inlineStr">
@@ -6570,11 +6454,7 @@
       <c r="K257" t="inlineStr"/>
     </row>
     <row r="258">
-      <c r="A258" t="inlineStr">
-        <is>
-          <t>M014</t>
-        </is>
-      </c>
+      <c r="A258" t="inlineStr"/>
       <c r="B258" t="inlineStr"/>
       <c r="C258" t="inlineStr">
         <is>
@@ -7042,11 +6922,7 @@
       <c r="K276" t="inlineStr"/>
     </row>
     <row r="277">
-      <c r="A277" t="inlineStr">
-        <is>
-          <t>M015</t>
-        </is>
-      </c>
+      <c r="A277" t="inlineStr"/>
       <c r="B277" t="inlineStr"/>
       <c r="C277" t="inlineStr"/>
       <c r="D277" t="inlineStr"/>
@@ -7063,11 +6939,7 @@
       <c r="K277" t="inlineStr"/>
     </row>
     <row r="278">
-      <c r="A278" t="inlineStr">
-        <is>
-          <t>M015</t>
-        </is>
-      </c>
+      <c r="A278" t="inlineStr"/>
       <c r="B278" t="inlineStr"/>
       <c r="C278" t="inlineStr"/>
       <c r="D278" t="inlineStr">
@@ -7088,11 +6960,7 @@
       <c r="K278" t="inlineStr"/>
     </row>
     <row r="279">
-      <c r="A279" t="inlineStr">
-        <is>
-          <t>M015</t>
-        </is>
-      </c>
+      <c r="A279" t="inlineStr"/>
       <c r="B279" t="inlineStr"/>
       <c r="C279" t="inlineStr">
         <is>
@@ -8512,11 +8380,7 @@
       <c r="K337" t="inlineStr"/>
     </row>
     <row r="338">
-      <c r="A338" t="inlineStr">
-        <is>
-          <t>M016</t>
-        </is>
-      </c>
+      <c r="A338" t="inlineStr"/>
       <c r="B338" t="inlineStr"/>
       <c r="C338" t="inlineStr"/>
       <c r="D338" t="inlineStr"/>
@@ -8533,11 +8397,7 @@
       <c r="K338" t="inlineStr"/>
     </row>
     <row r="339">
-      <c r="A339" t="inlineStr">
-        <is>
-          <t>M016</t>
-        </is>
-      </c>
+      <c r="A339" t="inlineStr"/>
       <c r="B339" t="inlineStr"/>
       <c r="C339" t="inlineStr"/>
       <c r="D339" t="inlineStr">
@@ -8604,11 +8464,7 @@
       <c r="K340" t="inlineStr"/>
     </row>
     <row r="341">
-      <c r="A341" t="inlineStr">
-        <is>
-          <t>M017</t>
-        </is>
-      </c>
+      <c r="A341" t="inlineStr"/>
       <c r="B341" t="inlineStr"/>
       <c r="C341" t="inlineStr"/>
       <c r="D341" t="inlineStr"/>
@@ -8625,11 +8481,7 @@
       <c r="K341" t="inlineStr"/>
     </row>
     <row r="342">
-      <c r="A342" t="inlineStr">
-        <is>
-          <t>M017</t>
-        </is>
-      </c>
+      <c r="A342" t="inlineStr"/>
       <c r="B342" t="inlineStr"/>
       <c r="C342" t="inlineStr"/>
       <c r="D342" t="inlineStr">
@@ -8696,11 +8548,7 @@
       <c r="K343" t="inlineStr"/>
     </row>
     <row r="344">
-      <c r="A344" t="inlineStr">
-        <is>
-          <t>M018</t>
-        </is>
-      </c>
+      <c r="A344" t="inlineStr"/>
       <c r="B344" t="inlineStr"/>
       <c r="C344" t="inlineStr"/>
       <c r="D344" t="inlineStr"/>
@@ -8717,11 +8565,7 @@
       <c r="K344" t="inlineStr"/>
     </row>
     <row r="345">
-      <c r="A345" t="inlineStr">
-        <is>
-          <t>M018</t>
-        </is>
-      </c>
+      <c r="A345" t="inlineStr"/>
       <c r="B345" t="inlineStr"/>
       <c r="C345" t="inlineStr"/>
       <c r="D345" t="inlineStr">
@@ -8788,11 +8632,7 @@
       <c r="K346" t="inlineStr"/>
     </row>
     <row r="347">
-      <c r="A347" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
+      <c r="A347" t="inlineStr"/>
       <c r="B347" t="inlineStr"/>
       <c r="C347" t="inlineStr"/>
       <c r="D347" t="inlineStr"/>
@@ -8809,11 +8649,7 @@
       <c r="K347" t="inlineStr"/>
     </row>
     <row r="348">
-      <c r="A348" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
+      <c r="A348" t="inlineStr"/>
       <c r="B348" t="inlineStr"/>
       <c r="C348" t="inlineStr"/>
       <c r="D348" t="inlineStr">
@@ -8834,11 +8670,7 @@
       <c r="K348" t="inlineStr"/>
     </row>
     <row r="349">
-      <c r="A349" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
+      <c r="A349" t="inlineStr"/>
       <c r="B349" t="inlineStr"/>
       <c r="C349" t="inlineStr">
         <is>
@@ -9177,11 +9009,7 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" t="inlineStr">
-        <is>
-          <t>M020</t>
-        </is>
-      </c>
+      <c r="A362" t="inlineStr"/>
       <c r="B362" t="inlineStr"/>
       <c r="C362" t="inlineStr"/>
       <c r="D362" t="inlineStr"/>
@@ -9198,11 +9026,7 @@
       <c r="K362" t="inlineStr"/>
     </row>
     <row r="363">
-      <c r="A363" t="inlineStr">
-        <is>
-          <t>M020</t>
-        </is>
-      </c>
+      <c r="A363" t="inlineStr"/>
       <c r="B363" t="inlineStr"/>
       <c r="C363" t="inlineStr"/>
       <c r="D363" t="inlineStr">
@@ -9269,11 +9093,7 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" t="inlineStr">
-        <is>
-          <t>M021</t>
-        </is>
-      </c>
+      <c r="A365" t="inlineStr"/>
       <c r="B365" t="inlineStr"/>
       <c r="C365" t="inlineStr"/>
       <c r="D365" t="inlineStr"/>
@@ -9290,11 +9110,7 @@
       <c r="K365" t="inlineStr"/>
     </row>
     <row r="366">
-      <c r="A366" t="inlineStr">
-        <is>
-          <t>M021</t>
-        </is>
-      </c>
+      <c r="A366" t="inlineStr"/>
       <c r="B366" t="inlineStr"/>
       <c r="C366" t="inlineStr"/>
       <c r="D366" t="inlineStr">
@@ -9361,11 +9177,7 @@
       </c>
     </row>
     <row r="368">
-      <c r="A368" t="inlineStr">
-        <is>
-          <t>M022</t>
-        </is>
-      </c>
+      <c r="A368" t="inlineStr"/>
       <c r="B368" t="inlineStr"/>
       <c r="C368" t="inlineStr"/>
       <c r="D368" t="inlineStr"/>
@@ -9382,11 +9194,7 @@
       <c r="K368" t="inlineStr"/>
     </row>
     <row r="369">
-      <c r="A369" t="inlineStr">
-        <is>
-          <t>M022</t>
-        </is>
-      </c>
+      <c r="A369" t="inlineStr"/>
       <c r="B369" t="inlineStr"/>
       <c r="C369" t="inlineStr"/>
       <c r="D369" t="inlineStr">
@@ -9407,11 +9215,7 @@
       <c r="K369" t="inlineStr"/>
     </row>
     <row r="370">
-      <c r="A370" t="inlineStr">
-        <is>
-          <t>M022</t>
-        </is>
-      </c>
+      <c r="A370" t="inlineStr"/>
       <c r="B370" t="inlineStr"/>
       <c r="C370" t="inlineStr">
         <is>
@@ -9677,11 +9481,7 @@
       <c r="K379" t="inlineStr"/>
     </row>
     <row r="380">
-      <c r="A380" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
+      <c r="A380" t="inlineStr"/>
       <c r="B380" t="inlineStr"/>
       <c r="C380" t="inlineStr"/>
       <c r="D380" t="inlineStr"/>
@@ -9700,11 +9500,7 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
+      <c r="A381" t="inlineStr"/>
       <c r="B381" t="inlineStr"/>
       <c r="C381" t="inlineStr"/>
       <c r="D381" t="inlineStr"/>
@@ -9723,11 +9519,7 @@
       </c>
     </row>
     <row r="382">
-      <c r="A382" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
+      <c r="A382" t="inlineStr"/>
       <c r="B382" t="inlineStr"/>
       <c r="C382" t="inlineStr"/>
       <c r="D382" t="inlineStr"/>
@@ -9744,11 +9536,7 @@
       <c r="K382" t="inlineStr"/>
     </row>
     <row r="383">
-      <c r="A383" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
+      <c r="A383" t="inlineStr"/>
       <c r="B383" t="inlineStr"/>
       <c r="C383" t="inlineStr"/>
       <c r="D383" t="inlineStr">
@@ -9769,11 +9557,7 @@
       <c r="K383" t="inlineStr"/>
     </row>
     <row r="384">
-      <c r="A384" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
+      <c r="A384" t="inlineStr"/>
       <c r="B384" t="inlineStr"/>
       <c r="C384" t="inlineStr">
         <is>
@@ -10843,11 +10627,7 @@
       </c>
     </row>
     <row r="433">
-      <c r="A433" t="inlineStr">
-        <is>
-          <t>M024</t>
-        </is>
-      </c>
+      <c r="A433" t="inlineStr"/>
       <c r="B433" t="inlineStr"/>
       <c r="C433" t="inlineStr"/>
       <c r="D433" t="inlineStr"/>
@@ -10864,11 +10644,7 @@
       <c r="K433" t="inlineStr"/>
     </row>
     <row r="434">
-      <c r="A434" t="inlineStr">
-        <is>
-          <t>M024</t>
-        </is>
-      </c>
+      <c r="A434" t="inlineStr"/>
       <c r="B434" t="inlineStr"/>
       <c r="C434" t="inlineStr"/>
       <c r="D434" t="inlineStr">
@@ -10889,11 +10665,7 @@
       <c r="K434" t="inlineStr"/>
     </row>
     <row r="435">
-      <c r="A435" t="inlineStr">
-        <is>
-          <t>M024</t>
-        </is>
-      </c>
+      <c r="A435" t="inlineStr"/>
       <c r="B435" t="inlineStr"/>
       <c r="C435" t="inlineStr">
         <is>
@@ -11085,11 +10857,7 @@
       <c r="K441" t="inlineStr"/>
     </row>
     <row r="442">
-      <c r="A442" t="inlineStr">
-        <is>
-          <t>M025</t>
-        </is>
-      </c>
+      <c r="A442" t="inlineStr"/>
       <c r="B442" t="inlineStr"/>
       <c r="C442" t="inlineStr"/>
       <c r="D442" t="inlineStr"/>
@@ -11106,11 +10874,7 @@
       <c r="K442" t="inlineStr"/>
     </row>
     <row r="443">
-      <c r="A443" t="inlineStr">
-        <is>
-          <t>M025</t>
-        </is>
-      </c>
+      <c r="A443" t="inlineStr"/>
       <c r="B443" t="inlineStr"/>
       <c r="C443" t="inlineStr"/>
       <c r="D443" t="inlineStr">
@@ -11131,11 +10895,7 @@
       <c r="K443" t="inlineStr"/>
     </row>
     <row r="444">
-      <c r="A444" t="inlineStr">
-        <is>
-          <t>M025</t>
-        </is>
-      </c>
+      <c r="A444" t="inlineStr"/>
       <c r="B444" t="inlineStr"/>
       <c r="C444" t="inlineStr">
         <is>
@@ -11584,11 +11344,7 @@
       </c>
     </row>
     <row r="462">
-      <c r="A462" t="inlineStr">
-        <is>
-          <t>M026</t>
-        </is>
-      </c>
+      <c r="A462" t="inlineStr"/>
       <c r="B462" t="inlineStr"/>
       <c r="C462" t="inlineStr"/>
       <c r="D462" t="inlineStr"/>
@@ -11605,11 +11361,7 @@
       <c r="K462" t="inlineStr"/>
     </row>
     <row r="463">
-      <c r="A463" t="inlineStr">
-        <is>
-          <t>M026</t>
-        </is>
-      </c>
+      <c r="A463" t="inlineStr"/>
       <c r="B463" t="inlineStr"/>
       <c r="C463" t="inlineStr"/>
       <c r="D463" t="inlineStr">
@@ -11630,11 +11382,7 @@
       <c r="K463" t="inlineStr"/>
     </row>
     <row r="464">
-      <c r="A464" t="inlineStr">
-        <is>
-          <t>M026</t>
-        </is>
-      </c>
+      <c r="A464" t="inlineStr"/>
       <c r="B464" t="inlineStr"/>
       <c r="C464" t="inlineStr">
         <is>
@@ -11753,11 +11501,7 @@
       </c>
     </row>
     <row r="468">
-      <c r="A468" t="inlineStr">
-        <is>
-          <t>M027</t>
-        </is>
-      </c>
+      <c r="A468" t="inlineStr"/>
       <c r="B468" t="inlineStr"/>
       <c r="C468" t="inlineStr"/>
       <c r="D468" t="inlineStr"/>
@@ -11774,11 +11518,7 @@
       <c r="K468" t="inlineStr"/>
     </row>
     <row r="469">
-      <c r="A469" t="inlineStr">
-        <is>
-          <t>M027</t>
-        </is>
-      </c>
+      <c r="A469" t="inlineStr"/>
       <c r="B469" t="inlineStr"/>
       <c r="C469" t="inlineStr"/>
       <c r="D469" t="inlineStr">
@@ -11845,11 +11585,7 @@
       <c r="K470" t="inlineStr"/>
     </row>
     <row r="471">
-      <c r="A471" t="inlineStr">
-        <is>
-          <t>M028</t>
-        </is>
-      </c>
+      <c r="A471" t="inlineStr"/>
       <c r="B471" t="inlineStr"/>
       <c r="C471" t="inlineStr"/>
       <c r="D471" t="inlineStr"/>
@@ -11866,11 +11602,7 @@
       <c r="K471" t="inlineStr"/>
     </row>
     <row r="472">
-      <c r="A472" t="inlineStr">
-        <is>
-          <t>M028</t>
-        </is>
-      </c>
+      <c r="A472" t="inlineStr"/>
       <c r="B472" t="inlineStr"/>
       <c r="C472" t="inlineStr"/>
       <c r="D472" t="inlineStr">
@@ -11937,11 +11669,7 @@
       <c r="K473" t="inlineStr"/>
     </row>
     <row r="474">
-      <c r="A474" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
+      <c r="A474" t="inlineStr"/>
       <c r="B474" t="inlineStr"/>
       <c r="C474" t="inlineStr"/>
       <c r="D474" t="inlineStr"/>
@@ -11960,11 +11688,7 @@
       </c>
     </row>
     <row r="475">
-      <c r="A475" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
+      <c r="A475" t="inlineStr"/>
       <c r="B475" t="inlineStr"/>
       <c r="C475" t="inlineStr"/>
       <c r="D475" t="inlineStr"/>
@@ -11983,11 +11707,7 @@
       </c>
     </row>
     <row r="476">
-      <c r="A476" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
+      <c r="A476" t="inlineStr"/>
       <c r="B476" t="inlineStr"/>
       <c r="C476" t="inlineStr"/>
       <c r="D476" t="inlineStr"/>
@@ -12004,11 +11724,7 @@
       <c r="K476" t="inlineStr"/>
     </row>
     <row r="477">
-      <c r="A477" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
+      <c r="A477" t="inlineStr"/>
       <c r="B477" t="inlineStr"/>
       <c r="C477" t="inlineStr"/>
       <c r="D477" t="inlineStr">
@@ -12029,11 +11745,7 @@
       <c r="K477" t="inlineStr"/>
     </row>
     <row r="478">
-      <c r="A478" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
+      <c r="A478" t="inlineStr"/>
       <c r="B478" t="inlineStr"/>
       <c r="C478" t="inlineStr">
         <is>
@@ -12809,11 +12521,7 @@
       <c r="K508" t="inlineStr"/>
     </row>
     <row r="509">
-      <c r="A509" t="inlineStr">
-        <is>
-          <t>M030</t>
-        </is>
-      </c>
+      <c r="A509" t="inlineStr"/>
       <c r="B509" t="inlineStr"/>
       <c r="C509" t="inlineStr"/>
       <c r="D509" t="inlineStr"/>
@@ -12830,11 +12538,7 @@
       <c r="K509" t="inlineStr"/>
     </row>
     <row r="510">
-      <c r="A510" t="inlineStr">
-        <is>
-          <t>M030</t>
-        </is>
-      </c>
+      <c r="A510" t="inlineStr"/>
       <c r="B510" t="inlineStr"/>
       <c r="C510" t="inlineStr"/>
       <c r="D510" t="inlineStr">
@@ -12855,11 +12559,7 @@
       <c r="K510" t="inlineStr"/>
     </row>
     <row r="511">
-      <c r="A511" t="inlineStr">
-        <is>
-          <t>M030</t>
-        </is>
-      </c>
+      <c r="A511" t="inlineStr"/>
       <c r="B511" t="inlineStr"/>
       <c r="C511" t="inlineStr">
         <is>
@@ -13124,11 +12824,7 @@
       <c r="K520" t="inlineStr"/>
     </row>
     <row r="521">
-      <c r="A521" t="inlineStr">
-        <is>
-          <t>M031</t>
-        </is>
-      </c>
+      <c r="A521" t="inlineStr"/>
       <c r="B521" t="inlineStr"/>
       <c r="C521" t="inlineStr"/>
       <c r="D521" t="inlineStr"/>
@@ -13145,11 +12841,7 @@
       <c r="K521" t="inlineStr"/>
     </row>
     <row r="522">
-      <c r="A522" t="inlineStr">
-        <is>
-          <t>M031</t>
-        </is>
-      </c>
+      <c r="A522" t="inlineStr"/>
       <c r="B522" t="inlineStr"/>
       <c r="C522" t="inlineStr"/>
       <c r="D522" t="inlineStr">
@@ -13170,11 +12862,7 @@
       <c r="K522" t="inlineStr"/>
     </row>
     <row r="523">
-      <c r="A523" t="inlineStr">
-        <is>
-          <t>M031</t>
-        </is>
-      </c>
+      <c r="A523" t="inlineStr"/>
       <c r="B523" t="inlineStr"/>
       <c r="C523" t="inlineStr">
         <is>
@@ -14257,11 +13945,7 @@
       <c r="K570" t="inlineStr"/>
     </row>
     <row r="571">
-      <c r="A571" t="inlineStr">
-        <is>
-          <t>M032</t>
-        </is>
-      </c>
+      <c r="A571" t="inlineStr"/>
       <c r="B571" t="inlineStr"/>
       <c r="C571" t="inlineStr"/>
       <c r="D571" t="inlineStr"/>
@@ -14278,11 +13962,7 @@
       <c r="K571" t="inlineStr"/>
     </row>
     <row r="572">
-      <c r="A572" t="inlineStr">
-        <is>
-          <t>M032</t>
-        </is>
-      </c>
+      <c r="A572" t="inlineStr"/>
       <c r="B572" t="inlineStr"/>
       <c r="C572" t="inlineStr"/>
       <c r="D572" t="inlineStr">
@@ -14349,11 +14029,7 @@
       <c r="K573" t="inlineStr"/>
     </row>
     <row r="574">
-      <c r="A574" t="inlineStr">
-        <is>
-          <t>M033</t>
-        </is>
-      </c>
+      <c r="A574" t="inlineStr"/>
       <c r="B574" t="inlineStr"/>
       <c r="C574" t="inlineStr"/>
       <c r="D574" t="inlineStr"/>
@@ -14370,11 +14046,7 @@
       <c r="K574" t="inlineStr"/>
     </row>
     <row r="575">
-      <c r="A575" t="inlineStr">
-        <is>
-          <t>M033</t>
-        </is>
-      </c>
+      <c r="A575" t="inlineStr"/>
       <c r="B575" t="inlineStr"/>
       <c r="C575" t="inlineStr"/>
       <c r="D575" t="inlineStr">
@@ -14395,11 +14067,7 @@
       <c r="K575" t="inlineStr"/>
     </row>
     <row r="576">
-      <c r="A576" t="inlineStr">
-        <is>
-          <t>M033</t>
-        </is>
-      </c>
+      <c r="A576" t="inlineStr"/>
       <c r="B576" t="inlineStr"/>
       <c r="C576" t="inlineStr">
         <is>
@@ -14594,11 +14262,7 @@
       </c>
     </row>
     <row r="584">
-      <c r="A584" t="inlineStr">
-        <is>
-          <t>M034</t>
-        </is>
-      </c>
+      <c r="A584" t="inlineStr"/>
       <c r="B584" t="inlineStr"/>
       <c r="C584" t="inlineStr"/>
       <c r="D584" t="inlineStr"/>
@@ -14617,11 +14281,7 @@
       <c r="K584" t="inlineStr"/>
     </row>
     <row r="585">
-      <c r="A585" t="inlineStr">
-        <is>
-          <t>M034</t>
-        </is>
-      </c>
+      <c r="A585" t="inlineStr"/>
       <c r="B585" t="inlineStr"/>
       <c r="C585" t="inlineStr"/>
       <c r="D585" t="inlineStr"/>
@@ -14640,11 +14300,7 @@
       <c r="K585" t="inlineStr"/>
     </row>
     <row r="586">
-      <c r="A586" t="inlineStr">
-        <is>
-          <t>M034</t>
-        </is>
-      </c>
+      <c r="A586" t="inlineStr"/>
       <c r="B586" t="inlineStr"/>
       <c r="C586" t="inlineStr"/>
       <c r="D586" t="inlineStr"/>
@@ -14661,11 +14317,7 @@
       <c r="K586" t="inlineStr"/>
     </row>
     <row r="587">
-      <c r="A587" t="inlineStr">
-        <is>
-          <t>M034</t>
-        </is>
-      </c>
+      <c r="A587" t="inlineStr"/>
       <c r="B587" t="inlineStr"/>
       <c r="C587" t="inlineStr"/>
       <c r="D587" t="inlineStr">
@@ -14732,11 +14384,7 @@
       <c r="K588" t="inlineStr"/>
     </row>
     <row r="589">
-      <c r="A589" t="inlineStr">
-        <is>
-          <t>M035</t>
-        </is>
-      </c>
+      <c r="A589" t="inlineStr"/>
       <c r="B589" t="inlineStr"/>
       <c r="C589" t="inlineStr"/>
       <c r="D589" t="inlineStr"/>
@@ -14753,11 +14401,7 @@
       <c r="K589" t="inlineStr"/>
     </row>
     <row r="590">
-      <c r="A590" t="inlineStr">
-        <is>
-          <t>M035</t>
-        </is>
-      </c>
+      <c r="A590" t="inlineStr"/>
       <c r="B590" t="inlineStr"/>
       <c r="C590" t="inlineStr"/>
       <c r="D590" t="inlineStr">
@@ -14824,11 +14468,7 @@
       <c r="K591" t="inlineStr"/>
     </row>
     <row r="592">
-      <c r="A592" t="inlineStr">
-        <is>
-          <t>M036</t>
-        </is>
-      </c>
+      <c r="A592" t="inlineStr"/>
       <c r="B592" t="inlineStr"/>
       <c r="C592" t="inlineStr"/>
       <c r="D592" t="inlineStr"/>
@@ -14845,11 +14485,7 @@
       <c r="K592" t="inlineStr"/>
     </row>
     <row r="593">
-      <c r="A593" t="inlineStr">
-        <is>
-          <t>M036</t>
-        </is>
-      </c>
+      <c r="A593" t="inlineStr"/>
       <c r="B593" t="inlineStr"/>
       <c r="C593" t="inlineStr"/>
       <c r="D593" t="inlineStr">
@@ -14870,11 +14506,7 @@
       <c r="K593" t="inlineStr"/>
     </row>
     <row r="594">
-      <c r="A594" t="inlineStr">
-        <is>
-          <t>M036</t>
-        </is>
-      </c>
+      <c r="A594" t="inlineStr"/>
       <c r="B594" t="inlineStr"/>
       <c r="C594" t="inlineStr">
         <is>
@@ -15906,11 +15538,7 @@
       <c r="K640" t="inlineStr"/>
     </row>
     <row r="641">
-      <c r="A641" t="inlineStr">
-        <is>
-          <t>M037</t>
-        </is>
-      </c>
+      <c r="A641" t="inlineStr"/>
       <c r="B641" t="inlineStr"/>
       <c r="C641" t="inlineStr"/>
       <c r="D641" t="inlineStr"/>
@@ -15927,11 +15555,7 @@
       <c r="K641" t="inlineStr"/>
     </row>
     <row r="642">
-      <c r="A642" t="inlineStr">
-        <is>
-          <t>M037</t>
-        </is>
-      </c>
+      <c r="A642" t="inlineStr"/>
       <c r="B642" t="inlineStr"/>
       <c r="C642" t="inlineStr"/>
       <c r="D642" t="inlineStr">
@@ -15998,11 +15622,7 @@
       <c r="K643" t="inlineStr"/>
     </row>
     <row r="644">
-      <c r="A644" t="inlineStr">
-        <is>
-          <t>M038</t>
-        </is>
-      </c>
+      <c r="A644" t="inlineStr"/>
       <c r="B644" t="inlineStr"/>
       <c r="C644" t="inlineStr"/>
       <c r="D644" t="inlineStr"/>
@@ -16019,11 +15639,7 @@
       <c r="K644" t="inlineStr"/>
     </row>
     <row r="645">
-      <c r="A645" t="inlineStr">
-        <is>
-          <t>M038</t>
-        </is>
-      </c>
+      <c r="A645" t="inlineStr"/>
       <c r="B645" t="inlineStr"/>
       <c r="C645" t="inlineStr"/>
       <c r="D645" t="inlineStr">
@@ -16090,11 +15706,7 @@
       <c r="K646" t="inlineStr"/>
     </row>
     <row r="647">
-      <c r="A647" t="inlineStr">
-        <is>
-          <t>M039</t>
-        </is>
-      </c>
+      <c r="A647" t="inlineStr"/>
       <c r="B647" t="inlineStr"/>
       <c r="C647" t="inlineStr"/>
       <c r="D647" t="inlineStr"/>
@@ -16111,11 +15723,7 @@
       <c r="K647" t="inlineStr"/>
     </row>
     <row r="648">
-      <c r="A648" t="inlineStr">
-        <is>
-          <t>M039</t>
-        </is>
-      </c>
+      <c r="A648" t="inlineStr"/>
       <c r="B648" t="inlineStr"/>
       <c r="C648" t="inlineStr"/>
       <c r="D648" t="inlineStr">
@@ -16136,11 +15744,7 @@
       <c r="K648" t="inlineStr"/>
     </row>
     <row r="649">
-      <c r="A649" t="inlineStr">
-        <is>
-          <t>M039</t>
-        </is>
-      </c>
+      <c r="A649" t="inlineStr"/>
       <c r="B649" t="inlineStr"/>
       <c r="C649" t="inlineStr">
         <is>
@@ -16697,11 +16301,7 @@
       </c>
     </row>
     <row r="671">
-      <c r="A671" t="inlineStr">
-        <is>
-          <t>M040</t>
-        </is>
-      </c>
+      <c r="A671" t="inlineStr"/>
       <c r="B671" t="inlineStr"/>
       <c r="C671" t="inlineStr"/>
       <c r="D671" t="inlineStr"/>
@@ -16718,11 +16318,7 @@
       <c r="K671" t="inlineStr"/>
     </row>
     <row r="672">
-      <c r="A672" t="inlineStr">
-        <is>
-          <t>M040</t>
-        </is>
-      </c>
+      <c r="A672" t="inlineStr"/>
       <c r="B672" t="inlineStr"/>
       <c r="C672" t="inlineStr"/>
       <c r="D672" t="inlineStr">
@@ -16789,11 +16385,7 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
+      <c r="A674" t="inlineStr"/>
       <c r="B674" t="inlineStr"/>
       <c r="C674" t="inlineStr"/>
       <c r="D674" t="inlineStr"/>
@@ -16812,11 +16404,7 @@
       <c r="K674" t="inlineStr"/>
     </row>
     <row r="675">
-      <c r="A675" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
+      <c r="A675" t="inlineStr"/>
       <c r="B675" t="inlineStr"/>
       <c r="C675" t="inlineStr"/>
       <c r="D675" t="inlineStr"/>
@@ -16835,11 +16423,7 @@
       <c r="K675" t="inlineStr"/>
     </row>
     <row r="676">
-      <c r="A676" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
+      <c r="A676" t="inlineStr"/>
       <c r="B676" t="inlineStr"/>
       <c r="C676" t="inlineStr"/>
       <c r="D676" t="inlineStr"/>
@@ -16856,11 +16440,7 @@
       <c r="K676" t="inlineStr"/>
     </row>
     <row r="677">
-      <c r="A677" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
+      <c r="A677" t="inlineStr"/>
       <c r="B677" t="inlineStr"/>
       <c r="C677" t="inlineStr"/>
       <c r="D677" t="inlineStr">
@@ -16881,11 +16461,7 @@
       <c r="K677" t="inlineStr"/>
     </row>
     <row r="678">
-      <c r="A678" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
+      <c r="A678" t="inlineStr"/>
       <c r="B678" t="inlineStr"/>
       <c r="C678" t="inlineStr">
         <is>
@@ -17004,11 +16580,7 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
+      <c r="A682" t="inlineStr"/>
       <c r="B682" t="inlineStr"/>
       <c r="C682" t="inlineStr"/>
       <c r="D682" t="inlineStr"/>
@@ -17027,11 +16599,7 @@
       <c r="K682" t="inlineStr"/>
     </row>
     <row r="683">
-      <c r="A683" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
+      <c r="A683" t="inlineStr"/>
       <c r="B683" t="inlineStr"/>
       <c r="C683" t="inlineStr"/>
       <c r="D683" t="inlineStr"/>
@@ -17050,11 +16618,7 @@
       <c r="K683" t="inlineStr"/>
     </row>
     <row r="684">
-      <c r="A684" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
+      <c r="A684" t="inlineStr"/>
       <c r="B684" t="inlineStr"/>
       <c r="C684" t="inlineStr"/>
       <c r="D684" t="inlineStr"/>
@@ -17071,11 +16635,7 @@
       <c r="K684" t="inlineStr"/>
     </row>
     <row r="685">
-      <c r="A685" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
+      <c r="A685" t="inlineStr"/>
       <c r="B685" t="inlineStr"/>
       <c r="C685" t="inlineStr"/>
       <c r="D685" t="inlineStr">
@@ -17096,11 +16656,7 @@
       <c r="K685" t="inlineStr"/>
     </row>
     <row r="686">
-      <c r="A686" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
+      <c r="A686" t="inlineStr"/>
       <c r="B686" t="inlineStr"/>
       <c r="C686" t="inlineStr">
         <is>
@@ -17365,11 +16921,7 @@
       <c r="K695" t="inlineStr"/>
     </row>
     <row r="696">
-      <c r="A696" t="inlineStr">
-        <is>
-          <t>M043</t>
-        </is>
-      </c>
+      <c r="A696" t="inlineStr"/>
       <c r="B696" t="inlineStr"/>
       <c r="C696" t="inlineStr"/>
       <c r="D696" t="inlineStr"/>
@@ -17386,11 +16938,7 @@
       <c r="K696" t="inlineStr"/>
     </row>
     <row r="697">
-      <c r="A697" t="inlineStr">
-        <is>
-          <t>M043</t>
-        </is>
-      </c>
+      <c r="A697" t="inlineStr"/>
       <c r="B697" t="inlineStr"/>
       <c r="C697" t="inlineStr"/>
       <c r="D697" t="inlineStr">
@@ -17411,11 +16959,7 @@
       <c r="K697" t="inlineStr"/>
     </row>
     <row r="698">
-      <c r="A698" t="inlineStr">
-        <is>
-          <t>M043</t>
-        </is>
-      </c>
+      <c r="A698" t="inlineStr"/>
       <c r="B698" t="inlineStr"/>
       <c r="C698" t="inlineStr">
         <is>
@@ -17534,11 +17078,7 @@
       </c>
     </row>
     <row r="702">
-      <c r="A702" t="inlineStr">
-        <is>
-          <t>M044</t>
-        </is>
-      </c>
+      <c r="A702" t="inlineStr"/>
       <c r="B702" t="inlineStr"/>
       <c r="C702" t="inlineStr"/>
       <c r="D702" t="inlineStr"/>
@@ -17555,11 +17095,7 @@
       <c r="K702" t="inlineStr"/>
     </row>
     <row r="703">
-      <c r="A703" t="inlineStr">
-        <is>
-          <t>M044</t>
-        </is>
-      </c>
+      <c r="A703" t="inlineStr"/>
       <c r="B703" t="inlineStr"/>
       <c r="C703" t="inlineStr"/>
       <c r="D703" t="inlineStr">
@@ -17580,11 +17116,7 @@
       <c r="K703" t="inlineStr"/>
     </row>
     <row r="704">
-      <c r="A704" t="inlineStr">
-        <is>
-          <t>M044</t>
-        </is>
-      </c>
+      <c r="A704" t="inlineStr"/>
       <c r="B704" t="inlineStr"/>
       <c r="C704" t="inlineStr">
         <is>
@@ -17776,11 +17308,7 @@
       <c r="K710" t="inlineStr"/>
     </row>
     <row r="711">
-      <c r="A711" t="inlineStr">
-        <is>
-          <t>M045</t>
-        </is>
-      </c>
+      <c r="A711" t="inlineStr"/>
       <c r="B711" t="inlineStr"/>
       <c r="C711" t="inlineStr"/>
       <c r="D711" t="inlineStr"/>
@@ -17797,11 +17325,7 @@
       <c r="K711" t="inlineStr"/>
     </row>
     <row r="712">
-      <c r="A712" t="inlineStr">
-        <is>
-          <t>M045</t>
-        </is>
-      </c>
+      <c r="A712" t="inlineStr"/>
       <c r="B712" t="inlineStr"/>
       <c r="C712" t="inlineStr"/>
       <c r="D712" t="inlineStr">
@@ -17868,11 +17392,7 @@
       <c r="K713" t="inlineStr"/>
     </row>
     <row r="714">
-      <c r="A714" t="inlineStr">
-        <is>
-          <t>M046</t>
-        </is>
-      </c>
+      <c r="A714" t="inlineStr"/>
       <c r="B714" t="inlineStr"/>
       <c r="C714" t="inlineStr"/>
       <c r="D714" t="inlineStr"/>
@@ -17889,11 +17409,7 @@
       <c r="K714" t="inlineStr"/>
     </row>
     <row r="715">
-      <c r="A715" t="inlineStr">
-        <is>
-          <t>M046</t>
-        </is>
-      </c>
+      <c r="A715" t="inlineStr"/>
       <c r="B715" t="inlineStr"/>
       <c r="C715" t="inlineStr"/>
       <c r="D715" t="inlineStr">
@@ -17960,11 +17476,7 @@
       </c>
     </row>
     <row r="717">
-      <c r="A717" t="inlineStr">
-        <is>
-          <t>M047</t>
-        </is>
-      </c>
+      <c r="A717" t="inlineStr"/>
       <c r="B717" t="inlineStr"/>
       <c r="C717" t="inlineStr"/>
       <c r="D717" t="inlineStr"/>
@@ -17981,11 +17493,7 @@
       <c r="K717" t="inlineStr"/>
     </row>
     <row r="718">
-      <c r="A718" t="inlineStr">
-        <is>
-          <t>M047</t>
-        </is>
-      </c>
+      <c r="A718" t="inlineStr"/>
       <c r="B718" t="inlineStr"/>
       <c r="C718" t="inlineStr"/>
       <c r="D718" t="inlineStr">
@@ -18006,11 +17514,7 @@
       <c r="K718" t="inlineStr"/>
     </row>
     <row r="719">
-      <c r="A719" t="inlineStr">
-        <is>
-          <t>M047</t>
-        </is>
-      </c>
+      <c r="A719" t="inlineStr"/>
       <c r="B719" t="inlineStr"/>
       <c r="C719" t="inlineStr">
         <is>
@@ -18129,11 +17633,7 @@
       <c r="K722" t="inlineStr"/>
     </row>
     <row r="723">
-      <c r="A723" t="inlineStr">
-        <is>
-          <t>M048</t>
-        </is>
-      </c>
+      <c r="A723" t="inlineStr"/>
       <c r="B723" t="inlineStr"/>
       <c r="C723" t="inlineStr"/>
       <c r="D723" t="inlineStr"/>
@@ -18150,11 +17650,7 @@
       <c r="K723" t="inlineStr"/>
     </row>
     <row r="724">
-      <c r="A724" t="inlineStr">
-        <is>
-          <t>M048</t>
-        </is>
-      </c>
+      <c r="A724" t="inlineStr"/>
       <c r="B724" t="inlineStr"/>
       <c r="C724" t="inlineStr"/>
       <c r="D724" t="inlineStr">
@@ -18175,11 +17671,7 @@
       <c r="K724" t="inlineStr"/>
     </row>
     <row r="725">
-      <c r="A725" t="inlineStr">
-        <is>
-          <t>M048</t>
-        </is>
-      </c>
+      <c r="A725" t="inlineStr"/>
       <c r="B725" t="inlineStr"/>
       <c r="C725" t="inlineStr">
         <is>
@@ -18466,11 +17958,7 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" t="inlineStr">
-        <is>
-          <t>M049</t>
-        </is>
-      </c>
+      <c r="A737" t="inlineStr"/>
       <c r="B737" t="inlineStr"/>
       <c r="C737" t="inlineStr"/>
       <c r="D737" t="inlineStr"/>
@@ -18487,11 +17975,7 @@
       <c r="K737" t="inlineStr"/>
     </row>
     <row r="738">
-      <c r="A738" t="inlineStr">
-        <is>
-          <t>M049</t>
-        </is>
-      </c>
+      <c r="A738" t="inlineStr"/>
       <c r="B738" t="inlineStr"/>
       <c r="C738" t="inlineStr"/>
       <c r="D738" t="inlineStr">
@@ -18558,11 +18042,7 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" t="inlineStr">
-        <is>
-          <t>M050</t>
-        </is>
-      </c>
+      <c r="A740" t="inlineStr"/>
       <c r="B740" t="inlineStr"/>
       <c r="C740" t="inlineStr"/>
       <c r="D740" t="inlineStr"/>
@@ -18579,11 +18059,7 @@
       <c r="K740" t="inlineStr"/>
     </row>
     <row r="741">
-      <c r="A741" t="inlineStr">
-        <is>
-          <t>M050</t>
-        </is>
-      </c>
+      <c r="A741" t="inlineStr"/>
       <c r="B741" t="inlineStr"/>
       <c r="C741" t="inlineStr"/>
       <c r="D741" t="inlineStr">
@@ -18650,11 +18126,7 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" t="inlineStr">
-        <is>
-          <t>M051</t>
-        </is>
-      </c>
+      <c r="A743" t="inlineStr"/>
       <c r="B743" t="inlineStr"/>
       <c r="C743" t="inlineStr"/>
       <c r="D743" t="inlineStr"/>
@@ -18671,11 +18143,7 @@
       <c r="K743" t="inlineStr"/>
     </row>
     <row r="744">
-      <c r="A744" t="inlineStr">
-        <is>
-          <t>M051</t>
-        </is>
-      </c>
+      <c r="A744" t="inlineStr"/>
       <c r="B744" t="inlineStr"/>
       <c r="C744" t="inlineStr"/>
       <c r="D744" t="inlineStr">
@@ -18696,11 +18164,7 @@
       <c r="K744" t="inlineStr"/>
     </row>
     <row r="745">
-      <c r="A745" t="inlineStr">
-        <is>
-          <t>M051</t>
-        </is>
-      </c>
+      <c r="A745" t="inlineStr"/>
       <c r="B745" t="inlineStr"/>
       <c r="C745" t="inlineStr">
         <is>
@@ -19149,11 +18613,7 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" t="inlineStr">
-        <is>
-          <t>M052</t>
-        </is>
-      </c>
+      <c r="A763" t="inlineStr"/>
       <c r="B763" t="inlineStr"/>
       <c r="C763" t="inlineStr"/>
       <c r="D763" t="inlineStr"/>
@@ -19170,11 +18630,7 @@
       <c r="K763" t="inlineStr"/>
     </row>
     <row r="764">
-      <c r="A764" t="inlineStr">
-        <is>
-          <t>M052</t>
-        </is>
-      </c>
+      <c r="A764" t="inlineStr"/>
       <c r="B764" t="inlineStr"/>
       <c r="C764" t="inlineStr"/>
       <c r="D764" t="inlineStr">
@@ -19241,11 +18697,7 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" t="inlineStr">
-        <is>
-          <t>M053</t>
-        </is>
-      </c>
+      <c r="A766" t="inlineStr"/>
       <c r="B766" t="inlineStr"/>
       <c r="C766" t="inlineStr"/>
       <c r="D766" t="inlineStr"/>
@@ -19262,11 +18714,7 @@
       <c r="K766" t="inlineStr"/>
     </row>
     <row r="767">
-      <c r="A767" t="inlineStr">
-        <is>
-          <t>M053</t>
-        </is>
-      </c>
+      <c r="A767" t="inlineStr"/>
       <c r="B767" t="inlineStr"/>
       <c r="C767" t="inlineStr"/>
       <c r="D767" t="inlineStr">
@@ -19287,11 +18735,7 @@
       <c r="K767" t="inlineStr"/>
     </row>
     <row r="768">
-      <c r="A768" t="inlineStr">
-        <is>
-          <t>M053</t>
-        </is>
-      </c>
+      <c r="A768" t="inlineStr"/>
       <c r="B768" t="inlineStr"/>
       <c r="C768" t="inlineStr">
         <is>
@@ -19410,11 +18854,7 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" t="inlineStr">
-        <is>
-          <t>M054</t>
-        </is>
-      </c>
+      <c r="A772" t="inlineStr"/>
       <c r="B772" t="inlineStr"/>
       <c r="C772" t="inlineStr"/>
       <c r="D772" t="inlineStr"/>
@@ -19431,11 +18871,7 @@
       <c r="K772" t="inlineStr"/>
     </row>
     <row r="773">
-      <c r="A773" t="inlineStr">
-        <is>
-          <t>M054</t>
-        </is>
-      </c>
+      <c r="A773" t="inlineStr"/>
       <c r="B773" t="inlineStr"/>
       <c r="C773" t="inlineStr"/>
       <c r="D773" t="inlineStr">
@@ -19456,11 +18892,7 @@
       <c r="K773" t="inlineStr"/>
     </row>
     <row r="774">
-      <c r="A774" t="inlineStr">
-        <is>
-          <t>M054</t>
-        </is>
-      </c>
+      <c r="A774" t="inlineStr"/>
       <c r="B774" t="inlineStr"/>
       <c r="C774" t="inlineStr">
         <is>
@@ -22889,11 +22321,7 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" t="inlineStr">
-        <is>
-          <t>M055</t>
-        </is>
-      </c>
+      <c r="A921" t="inlineStr"/>
       <c r="B921" t="inlineStr"/>
       <c r="C921" t="inlineStr"/>
       <c r="D921" t="inlineStr"/>
@@ -22910,11 +22338,7 @@
       <c r="K921" t="inlineStr"/>
     </row>
     <row r="922">
-      <c r="A922" t="inlineStr">
-        <is>
-          <t>M055</t>
-        </is>
-      </c>
+      <c r="A922" t="inlineStr"/>
       <c r="B922" t="inlineStr"/>
       <c r="C922" t="inlineStr"/>
       <c r="D922" t="inlineStr">
@@ -22981,11 +22405,7 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" t="inlineStr">
-        <is>
-          <t>M056</t>
-        </is>
-      </c>
+      <c r="A924" t="inlineStr"/>
       <c r="B924" t="inlineStr"/>
       <c r="C924" t="inlineStr"/>
       <c r="D924" t="inlineStr"/>
@@ -23002,11 +22422,7 @@
       <c r="K924" t="inlineStr"/>
     </row>
     <row r="925">
-      <c r="A925" t="inlineStr">
-        <is>
-          <t>M056</t>
-        </is>
-      </c>
+      <c r="A925" t="inlineStr"/>
       <c r="B925" t="inlineStr"/>
       <c r="C925" t="inlineStr"/>
       <c r="D925" t="inlineStr">
@@ -23073,11 +22489,7 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" t="inlineStr">
-        <is>
-          <t>M057</t>
-        </is>
-      </c>
+      <c r="A927" t="inlineStr"/>
       <c r="B927" t="inlineStr"/>
       <c r="C927" t="inlineStr"/>
       <c r="D927" t="inlineStr"/>
@@ -23094,11 +22506,7 @@
       <c r="K927" t="inlineStr"/>
     </row>
     <row r="928">
-      <c r="A928" t="inlineStr">
-        <is>
-          <t>M057</t>
-        </is>
-      </c>
+      <c r="A928" t="inlineStr"/>
       <c r="B928" t="inlineStr"/>
       <c r="C928" t="inlineStr"/>
       <c r="D928" t="inlineStr">
@@ -23119,11 +22527,7 @@
       <c r="K928" t="inlineStr"/>
     </row>
     <row r="929">
-      <c r="A929" t="inlineStr">
-        <is>
-          <t>M057</t>
-        </is>
-      </c>
+      <c r="A929" t="inlineStr"/>
       <c r="B929" t="inlineStr"/>
       <c r="C929" t="inlineStr">
         <is>
@@ -23461,11 +22865,7 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" t="inlineStr">
-        <is>
-          <t>M058</t>
-        </is>
-      </c>
+      <c r="A942" t="inlineStr"/>
       <c r="B942" t="inlineStr"/>
       <c r="C942" t="inlineStr"/>
       <c r="D942" t="inlineStr"/>
@@ -23482,11 +22882,7 @@
       <c r="K942" t="inlineStr"/>
     </row>
     <row r="943">
-      <c r="A943" t="inlineStr">
-        <is>
-          <t>M058</t>
-        </is>
-      </c>
+      <c r="A943" t="inlineStr"/>
       <c r="B943" t="inlineStr"/>
       <c r="C943" t="inlineStr"/>
       <c r="D943" t="inlineStr">
@@ -23507,11 +22903,7 @@
       <c r="K943" t="inlineStr"/>
     </row>
     <row r="944">
-      <c r="A944" t="inlineStr">
-        <is>
-          <t>M058</t>
-        </is>
-      </c>
+      <c r="A944" t="inlineStr"/>
       <c r="B944" t="inlineStr"/>
       <c r="C944" t="inlineStr">
         <is>
@@ -23922,11 +23314,7 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" t="inlineStr">
-        <is>
-          <t>M059</t>
-        </is>
-      </c>
+      <c r="A960" t="inlineStr"/>
       <c r="B960" t="inlineStr"/>
       <c r="C960" t="inlineStr"/>
       <c r="D960" t="inlineStr"/>
@@ -23945,11 +23333,7 @@
       <c r="K960" t="inlineStr"/>
     </row>
     <row r="961">
-      <c r="A961" t="inlineStr">
-        <is>
-          <t>M059</t>
-        </is>
-      </c>
+      <c r="A961" t="inlineStr"/>
       <c r="B961" t="inlineStr"/>
       <c r="C961" t="inlineStr"/>
       <c r="D961" t="inlineStr"/>
@@ -23968,11 +23352,7 @@
       <c r="K961" t="inlineStr"/>
     </row>
     <row r="962">
-      <c r="A962" t="inlineStr">
-        <is>
-          <t>M059</t>
-        </is>
-      </c>
+      <c r="A962" t="inlineStr"/>
       <c r="B962" t="inlineStr"/>
       <c r="C962" t="inlineStr"/>
       <c r="D962" t="inlineStr"/>
@@ -23989,11 +23369,7 @@
       <c r="K962" t="inlineStr"/>
     </row>
     <row r="963">
-      <c r="A963" t="inlineStr">
-        <is>
-          <t>M059</t>
-        </is>
-      </c>
+      <c r="A963" t="inlineStr"/>
       <c r="B963" t="inlineStr"/>
       <c r="C963" t="inlineStr"/>
       <c r="D963" t="inlineStr">
@@ -24014,11 +23390,7 @@
       <c r="K963" t="inlineStr"/>
     </row>
     <row r="964">
-      <c r="A964" t="inlineStr">
-        <is>
-          <t>M059</t>
-        </is>
-      </c>
+      <c r="A964" t="inlineStr"/>
       <c r="B964" t="inlineStr"/>
       <c r="C964" t="inlineStr">
         <is>
@@ -24248,11 +23620,7 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" t="inlineStr">
-        <is>
-          <t>M060</t>
-        </is>
-      </c>
+      <c r="A973" t="inlineStr"/>
       <c r="B973" t="inlineStr"/>
       <c r="C973" t="inlineStr"/>
       <c r="D973" t="inlineStr"/>
@@ -24269,11 +23637,7 @@
       <c r="K973" t="inlineStr"/>
     </row>
     <row r="974">
-      <c r="A974" t="inlineStr">
-        <is>
-          <t>M060</t>
-        </is>
-      </c>
+      <c r="A974" t="inlineStr"/>
       <c r="B974" t="inlineStr"/>
       <c r="C974" t="inlineStr"/>
       <c r="D974" t="inlineStr">
@@ -24294,11 +23658,7 @@
       <c r="K974" t="inlineStr"/>
     </row>
     <row r="975">
-      <c r="A975" t="inlineStr">
-        <is>
-          <t>M060</t>
-        </is>
-      </c>
+      <c r="A975" t="inlineStr"/>
       <c r="B975" t="inlineStr"/>
       <c r="C975" t="inlineStr">
         <is>
@@ -24417,11 +23777,7 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
+      <c r="A979" t="inlineStr"/>
       <c r="B979" t="inlineStr"/>
       <c r="C979" t="inlineStr"/>
       <c r="D979" t="inlineStr"/>
@@ -24440,11 +23796,7 @@
       <c r="K979" t="inlineStr"/>
     </row>
     <row r="980">
-      <c r="A980" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
+      <c r="A980" t="inlineStr"/>
       <c r="B980" t="inlineStr"/>
       <c r="C980" t="inlineStr"/>
       <c r="D980" t="inlineStr"/>
@@ -24463,11 +23815,7 @@
       <c r="K980" t="inlineStr"/>
     </row>
     <row r="981">
-      <c r="A981" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
+      <c r="A981" t="inlineStr"/>
       <c r="B981" t="inlineStr"/>
       <c r="C981" t="inlineStr"/>
       <c r="D981" t="inlineStr"/>
@@ -24486,11 +23834,7 @@
       <c r="K981" t="inlineStr"/>
     </row>
     <row r="982">
-      <c r="A982" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
+      <c r="A982" t="inlineStr"/>
       <c r="B982" t="inlineStr"/>
       <c r="C982" t="inlineStr"/>
       <c r="D982" t="inlineStr"/>
@@ -24507,11 +23851,7 @@
       <c r="K982" t="inlineStr"/>
     </row>
     <row r="983">
-      <c r="A983" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
+      <c r="A983" t="inlineStr"/>
       <c r="B983" t="inlineStr"/>
       <c r="C983" t="inlineStr"/>
       <c r="D983" t="inlineStr">
@@ -24578,11 +23918,7 @@
       <c r="K984" t="inlineStr"/>
     </row>
     <row r="985">
-      <c r="A985" t="inlineStr">
-        <is>
-          <t>M062</t>
-        </is>
-      </c>
+      <c r="A985" t="inlineStr"/>
       <c r="B985" t="inlineStr"/>
       <c r="C985" t="inlineStr"/>
       <c r="D985" t="inlineStr"/>
@@ -24599,11 +23935,7 @@
       <c r="K985" t="inlineStr"/>
     </row>
     <row r="986">
-      <c r="A986" t="inlineStr">
-        <is>
-          <t>M062</t>
-        </is>
-      </c>
+      <c r="A986" t="inlineStr"/>
       <c r="B986" t="inlineStr"/>
       <c r="C986" t="inlineStr"/>
       <c r="D986" t="inlineStr">
@@ -24624,11 +23956,7 @@
       <c r="K986" t="inlineStr"/>
     </row>
     <row r="987">
-      <c r="A987" t="inlineStr">
-        <is>
-          <t>M062</t>
-        </is>
-      </c>
+      <c r="A987" t="inlineStr"/>
       <c r="B987" t="inlineStr"/>
       <c r="C987" t="inlineStr">
         <is>
@@ -25208,11 +24536,7 @@
       <c r="K1010" t="inlineStr"/>
     </row>
     <row r="1011">
-      <c r="A1011" t="inlineStr">
-        <is>
-          <t>M063</t>
-        </is>
-      </c>
+      <c r="A1011" t="inlineStr"/>
       <c r="B1011" t="inlineStr"/>
       <c r="C1011" t="inlineStr"/>
       <c r="D1011" t="inlineStr"/>
@@ -25229,11 +24553,7 @@
       <c r="K1011" t="inlineStr"/>
     </row>
     <row r="1012">
-      <c r="A1012" t="inlineStr">
-        <is>
-          <t>M063</t>
-        </is>
-      </c>
+      <c r="A1012" t="inlineStr"/>
       <c r="B1012" t="inlineStr"/>
       <c r="C1012" t="inlineStr"/>
       <c r="D1012" t="inlineStr">
@@ -25254,11 +24574,7 @@
       <c r="K1012" t="inlineStr"/>
     </row>
     <row r="1013">
-      <c r="A1013" t="inlineStr">
-        <is>
-          <t>M063</t>
-        </is>
-      </c>
+      <c r="A1013" t="inlineStr"/>
       <c r="B1013" t="inlineStr"/>
       <c r="C1013" t="inlineStr">
         <is>
@@ -25743,11 +25059,7 @@
       <c r="K1031" t="inlineStr"/>
     </row>
     <row r="1032">
-      <c r="A1032" t="inlineStr">
-        <is>
-          <t>M064</t>
-        </is>
-      </c>
+      <c r="A1032" t="inlineStr"/>
       <c r="B1032" t="inlineStr"/>
       <c r="C1032" t="inlineStr"/>
       <c r="D1032" t="inlineStr"/>
@@ -25764,11 +25076,7 @@
       <c r="K1032" t="inlineStr"/>
     </row>
     <row r="1033">
-      <c r="A1033" t="inlineStr">
-        <is>
-          <t>M064</t>
-        </is>
-      </c>
+      <c r="A1033" t="inlineStr"/>
       <c r="B1033" t="inlineStr"/>
       <c r="C1033" t="inlineStr"/>
       <c r="D1033" t="inlineStr">
@@ -25789,11 +25097,7 @@
       <c r="K1033" t="inlineStr"/>
     </row>
     <row r="1034">
-      <c r="A1034" t="inlineStr">
-        <is>
-          <t>M064</t>
-        </is>
-      </c>
+      <c r="A1034" t="inlineStr"/>
       <c r="B1034" t="inlineStr"/>
       <c r="C1034" t="inlineStr">
         <is>
@@ -27429,11 +26733,7 @@
       </c>
     </row>
     <row r="1101">
-      <c r="A1101" t="inlineStr">
-        <is>
-          <t>M065</t>
-        </is>
-      </c>
+      <c r="A1101" t="inlineStr"/>
       <c r="B1101" t="inlineStr"/>
       <c r="C1101" t="inlineStr"/>
       <c r="D1101" t="inlineStr"/>
@@ -27450,11 +26750,7 @@
       <c r="K1101" t="inlineStr"/>
     </row>
     <row r="1102">
-      <c r="A1102" t="inlineStr">
-        <is>
-          <t>M065</t>
-        </is>
-      </c>
+      <c r="A1102" t="inlineStr"/>
       <c r="B1102" t="inlineStr"/>
       <c r="C1102" t="inlineStr"/>
       <c r="D1102" t="inlineStr">
@@ -27521,11 +26817,7 @@
       <c r="K1103" t="inlineStr"/>
     </row>
     <row r="1104">
-      <c r="A1104" t="inlineStr">
-        <is>
-          <t>M066</t>
-        </is>
-      </c>
+      <c r="A1104" t="inlineStr"/>
       <c r="B1104" t="inlineStr"/>
       <c r="C1104" t="inlineStr"/>
       <c r="D1104" t="inlineStr"/>
@@ -27542,11 +26834,7 @@
       <c r="K1104" t="inlineStr"/>
     </row>
     <row r="1105">
-      <c r="A1105" t="inlineStr">
-        <is>
-          <t>M066</t>
-        </is>
-      </c>
+      <c r="A1105" t="inlineStr"/>
       <c r="B1105" t="inlineStr"/>
       <c r="C1105" t="inlineStr"/>
       <c r="D1105" t="inlineStr">
@@ -27567,11 +26855,7 @@
       <c r="K1105" t="inlineStr"/>
     </row>
     <row r="1106">
-      <c r="A1106" t="inlineStr">
-        <is>
-          <t>M066</t>
-        </is>
-      </c>
+      <c r="A1106" t="inlineStr"/>
       <c r="B1106" t="inlineStr"/>
       <c r="C1106" t="inlineStr">
         <is>
@@ -28093,11 +27377,7 @@
       <c r="K1126" t="inlineStr"/>
     </row>
     <row r="1127">
-      <c r="A1127" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
+      <c r="A1127" t="inlineStr"/>
       <c r="B1127" t="inlineStr"/>
       <c r="C1127" t="inlineStr"/>
       <c r="D1127" t="inlineStr"/>
@@ -28116,11 +27396,7 @@
       </c>
     </row>
     <row r="1128">
-      <c r="A1128" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
+      <c r="A1128" t="inlineStr"/>
       <c r="B1128" t="inlineStr"/>
       <c r="C1128" t="inlineStr"/>
       <c r="D1128" t="inlineStr"/>
@@ -28139,11 +27415,7 @@
       </c>
     </row>
     <row r="1129">
-      <c r="A1129" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
+      <c r="A1129" t="inlineStr"/>
       <c r="B1129" t="inlineStr"/>
       <c r="C1129" t="inlineStr"/>
       <c r="D1129" t="inlineStr"/>
@@ -28162,11 +27434,7 @@
       </c>
     </row>
     <row r="1130">
-      <c r="A1130" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
+      <c r="A1130" t="inlineStr"/>
       <c r="B1130" t="inlineStr"/>
       <c r="C1130" t="inlineStr"/>
       <c r="D1130" t="inlineStr"/>
@@ -28185,11 +27453,7 @@
       </c>
     </row>
     <row r="1131">
-      <c r="A1131" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
+      <c r="A1131" t="inlineStr"/>
       <c r="B1131" t="inlineStr"/>
       <c r="C1131" t="inlineStr"/>
       <c r="D1131" t="inlineStr"/>
@@ -28206,11 +27470,7 @@
       <c r="K1131" t="inlineStr"/>
     </row>
     <row r="1132">
-      <c r="A1132" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
+      <c r="A1132" t="inlineStr"/>
       <c r="B1132" t="inlineStr"/>
       <c r="C1132" t="inlineStr"/>
       <c r="D1132" t="inlineStr">
@@ -28277,11 +27537,7 @@
       </c>
     </row>
     <row r="1134">
-      <c r="A1134" t="inlineStr">
-        <is>
-          <t>M068</t>
-        </is>
-      </c>
+      <c r="A1134" t="inlineStr"/>
       <c r="B1134" t="inlineStr"/>
       <c r="C1134" t="inlineStr"/>
       <c r="D1134" t="inlineStr"/>
@@ -28298,11 +27554,7 @@
       <c r="K1134" t="inlineStr"/>
     </row>
     <row r="1135">
-      <c r="A1135" t="inlineStr">
-        <is>
-          <t>M068</t>
-        </is>
-      </c>
+      <c r="A1135" t="inlineStr"/>
       <c r="B1135" t="inlineStr"/>
       <c r="C1135" t="inlineStr"/>
       <c r="D1135" t="inlineStr">
@@ -28323,11 +27575,7 @@
       <c r="K1135" t="inlineStr"/>
     </row>
     <row r="1136">
-      <c r="A1136" t="inlineStr">
-        <is>
-          <t>M068</t>
-        </is>
-      </c>
+      <c r="A1136" t="inlineStr"/>
       <c r="B1136" t="inlineStr"/>
       <c r="C1136" t="inlineStr">
         <is>
@@ -28957,11 +28205,7 @@
       </c>
     </row>
     <row r="1161">
-      <c r="A1161" t="inlineStr">
-        <is>
-          <t>M069</t>
-        </is>
-      </c>
+      <c r="A1161" t="inlineStr"/>
       <c r="B1161" t="inlineStr"/>
       <c r="C1161" t="inlineStr"/>
       <c r="D1161" t="inlineStr"/>
@@ -28978,11 +28222,7 @@
       <c r="K1161" t="inlineStr"/>
     </row>
     <row r="1162">
-      <c r="A1162" t="inlineStr">
-        <is>
-          <t>M069</t>
-        </is>
-      </c>
+      <c r="A1162" t="inlineStr"/>
       <c r="B1162" t="inlineStr"/>
       <c r="C1162" t="inlineStr"/>
       <c r="D1162" t="inlineStr">
@@ -29003,11 +28243,7 @@
       <c r="K1162" t="inlineStr"/>
     </row>
     <row r="1163">
-      <c r="A1163" t="inlineStr">
-        <is>
-          <t>M069</t>
-        </is>
-      </c>
+      <c r="A1163" t="inlineStr"/>
       <c r="B1163" t="inlineStr"/>
       <c r="C1163" t="inlineStr">
         <is>
@@ -29199,11 +28435,7 @@
       <c r="K1169" t="inlineStr"/>
     </row>
     <row r="1170">
-      <c r="A1170" t="inlineStr">
-        <is>
-          <t>M070</t>
-        </is>
-      </c>
+      <c r="A1170" t="inlineStr"/>
       <c r="B1170" t="inlineStr"/>
       <c r="C1170" t="inlineStr"/>
       <c r="D1170" t="inlineStr"/>
@@ -29220,11 +28452,7 @@
       <c r="K1170" t="inlineStr"/>
     </row>
     <row r="1171">
-      <c r="A1171" t="inlineStr">
-        <is>
-          <t>M070</t>
-        </is>
-      </c>
+      <c r="A1171" t="inlineStr"/>
       <c r="B1171" t="inlineStr"/>
       <c r="C1171" t="inlineStr"/>
       <c r="D1171" t="inlineStr">
@@ -29245,11 +28473,7 @@
       <c r="K1171" t="inlineStr"/>
     </row>
     <row r="1172">
-      <c r="A1172" t="inlineStr">
-        <is>
-          <t>M070</t>
-        </is>
-      </c>
+      <c r="A1172" t="inlineStr"/>
       <c r="B1172" t="inlineStr"/>
       <c r="C1172" t="inlineStr">
         <is>
@@ -29879,11 +29103,7 @@
       <c r="K1196" t="inlineStr"/>
     </row>
     <row r="1197">
-      <c r="A1197" t="inlineStr">
-        <is>
-          <t>M071</t>
-        </is>
-      </c>
+      <c r="A1197" t="inlineStr"/>
       <c r="B1197" t="inlineStr"/>
       <c r="C1197" t="inlineStr"/>
       <c r="D1197" t="inlineStr"/>
@@ -29900,11 +29120,7 @@
       <c r="K1197" t="inlineStr"/>
     </row>
     <row r="1198">
-      <c r="A1198" t="inlineStr">
-        <is>
-          <t>M071</t>
-        </is>
-      </c>
+      <c r="A1198" t="inlineStr"/>
       <c r="B1198" t="inlineStr"/>
       <c r="C1198" t="inlineStr"/>
       <c r="D1198" t="inlineStr">
@@ -29925,11 +29141,7 @@
       <c r="K1198" t="inlineStr"/>
     </row>
     <row r="1199">
-      <c r="A1199" t="inlineStr">
-        <is>
-          <t>M071</t>
-        </is>
-      </c>
+      <c r="A1199" t="inlineStr"/>
       <c r="B1199" t="inlineStr"/>
       <c r="C1199" t="inlineStr">
         <is>
@@ -30403,11 +29615,7 @@
       <c r="K1219" t="inlineStr"/>
     </row>
     <row r="1220">
-      <c r="A1220" t="inlineStr">
-        <is>
-          <t>M072</t>
-        </is>
-      </c>
+      <c r="A1220" t="inlineStr"/>
       <c r="B1220" t="inlineStr"/>
       <c r="C1220" t="inlineStr"/>
       <c r="D1220" t="inlineStr"/>
@@ -30424,11 +29632,7 @@
       <c r="K1220" t="inlineStr"/>
     </row>
     <row r="1221">
-      <c r="A1221" t="inlineStr">
-        <is>
-          <t>M072</t>
-        </is>
-      </c>
+      <c r="A1221" t="inlineStr"/>
       <c r="B1221" t="inlineStr"/>
       <c r="C1221" t="inlineStr"/>
       <c r="D1221" t="inlineStr">
@@ -30449,11 +29653,7 @@
       <c r="K1221" t="inlineStr"/>
     </row>
     <row r="1222">
-      <c r="A1222" t="inlineStr">
-        <is>
-          <t>M072</t>
-        </is>
-      </c>
+      <c r="A1222" t="inlineStr"/>
       <c r="B1222" t="inlineStr"/>
       <c r="C1222" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
MID and Audit Info in all transaction rows
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -1544,8 +1544,7 @@
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
+          <t>LC Match: L/C-308524022796/24
 Lender Amount: 5040781.68
 Borrower Amount: 5040781.68</t>
         </is>
@@ -1583,8 +1582,18 @@
       <c r="K53" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr"/>
-      <c r="B54" t="inlineStr"/>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>M001</t>
+        </is>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 5040781.68
+Borrower Amount: 5040781.68</t>
+        </is>
+      </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" s="4" t="inlineStr">
@@ -1600,8 +1609,18 @@
       <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr"/>
-      <c r="B55" t="inlineStr"/>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>M001</t>
+        </is>
+      </c>
+      <c r="B55" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 5040781.68
+Borrower Amount: 5040781.68</t>
+        </is>
+      </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
@@ -1628,8 +1647,7 @@
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
+          <t>LC Match: L/C-308524022796/24
 Lender Amount: 15737222.22
 Borrower Amount: 15737222.22</t>
         </is>
@@ -1667,8 +1685,18 @@
       <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr"/>
-      <c r="B57" t="inlineStr"/>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="B57" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 15737222.22
+Borrower Amount: 15737222.22</t>
+        </is>
+      </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
       <c r="E57" s="4" t="inlineStr">
@@ -1686,8 +1714,18 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr"/>
-      <c r="B58" t="inlineStr"/>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="B58" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 15737222.22
+Borrower Amount: 15737222.22</t>
+        </is>
+      </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" s="4" t="inlineStr">
@@ -1705,8 +1743,18 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr"/>
-      <c r="B59" t="inlineStr"/>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="B59" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 15737222.22
+Borrower Amount: 15737222.22</t>
+        </is>
+      </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" s="4" t="inlineStr">
@@ -1724,8 +1772,18 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr"/>
-      <c r="B60" t="inlineStr"/>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 15737222.22
+Borrower Amount: 15737222.22</t>
+        </is>
+      </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" s="4" t="inlineStr">
@@ -1741,8 +1799,18 @@
       <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr"/>
-      <c r="B61" t="inlineStr"/>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="B61" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 15737222.22
+Borrower Amount: 15737222.22</t>
+        </is>
+      </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
@@ -1915,8 +1983,7 @@
       </c>
       <c r="B68" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
+          <t>LC Match: L/C-308524022796/24
 Lender Amount: 8884.77
 Borrower Amount: 8884.77</t>
         </is>
@@ -1954,8 +2021,18 @@
       <c r="K68" t="inlineStr"/>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr"/>
-      <c r="B69" t="inlineStr"/>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="B69" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 8884.77
+Borrower Amount: 8884.77</t>
+        </is>
+      </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" s="4" t="inlineStr">
@@ -1971,8 +2048,18 @@
       <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr"/>
-      <c r="B70" t="inlineStr"/>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="B70" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 8884.77
+Borrower Amount: 8884.77</t>
+        </is>
+      </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
@@ -1999,8 +2086,7 @@
       </c>
       <c r="B71" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
+          <t>LC Match: L/C-308524027065/24
 Lender Amount: 1575.00
 Borrower Amount: 1575.00</t>
         </is>
@@ -2038,8 +2124,18 @@
       <c r="K71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr"/>
-      <c r="B72" t="inlineStr"/>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>M005</t>
+        </is>
+      </c>
+      <c r="B72" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1575.00
+Borrower Amount: 1575.00</t>
+        </is>
+      </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
       <c r="E72" s="4" t="inlineStr">
@@ -2055,8 +2151,18 @@
       <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr"/>
-      <c r="B73" t="inlineStr"/>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>M005</t>
+        </is>
+      </c>
+      <c r="B73" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1575.00
+Borrower Amount: 1575.00</t>
+        </is>
+      </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
@@ -2375,8 +2481,7 @@
       </c>
       <c r="B86" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
+          <t>LC Match: L/C-187724010124/24
 Lender Amount: 1150.00
 Borrower Amount: 1150.00</t>
         </is>
@@ -2414,8 +2519,18 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr"/>
-      <c r="B87" t="inlineStr"/>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>M007</t>
+        </is>
+      </c>
+      <c r="B87" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010124/24
+Lender Amount: 1150.00
+Borrower Amount: 1150.00</t>
+        </is>
+      </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
       <c r="E87" s="4" t="inlineStr">
@@ -2431,8 +2546,18 @@
       <c r="K87" t="inlineStr"/>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr"/>
-      <c r="B88" t="inlineStr"/>
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>M007</t>
+        </is>
+      </c>
+      <c r="B88" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010124/24
+Lender Amount: 1150.00
+Borrower Amount: 1150.00</t>
+        </is>
+      </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
@@ -2459,8 +2584,7 @@
       </c>
       <c r="B89" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
+          <t>LC Match: L/C-308524027065/24
 Lender Amount: 1575.00
 Borrower Amount: 1575.00</t>
         </is>
@@ -2498,8 +2622,18 @@
       <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr"/>
-      <c r="B90" t="inlineStr"/>
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>M009</t>
+        </is>
+      </c>
+      <c r="B90" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1575.00
+Borrower Amount: 1575.00</t>
+        </is>
+      </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
       <c r="E90" s="4" t="inlineStr">
@@ -2515,8 +2649,18 @@
       <c r="K90" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr"/>
-      <c r="B91" t="inlineStr"/>
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>M009</t>
+        </is>
+      </c>
+      <c r="B91" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1575.00
+Borrower Amount: 1575.00</t>
+        </is>
+      </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
         <is>
@@ -2908,8 +3052,7 @@
       </c>
       <c r="B107" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
+          <t>LC Match: L/C-308524022796/24
 Lender Amount: 26246.93
 Borrower Amount: 26246.93</t>
         </is>
@@ -2947,8 +3090,18 @@
       <c r="K107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr"/>
-      <c r="B108" t="inlineStr"/>
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>M010</t>
+        </is>
+      </c>
+      <c r="B108" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 26246.93
+Borrower Amount: 26246.93</t>
+        </is>
+      </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
       <c r="E108" s="4" t="inlineStr">
@@ -2964,8 +3117,18 @@
       <c r="K108" t="inlineStr"/>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr"/>
-      <c r="B109" t="inlineStr"/>
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>M010</t>
+        </is>
+      </c>
+      <c r="B109" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 26246.93
+Borrower Amount: 26246.93</t>
+        </is>
+      </c>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr">
         <is>
@@ -5733,8 +5896,7 @@
       </c>
       <c r="B229" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
+          <t>LC Match: L/C-187724010124/24
 Lender Amount: 1150.00
 Borrower Amount: 1150.00</t>
         </is>
@@ -5772,8 +5934,18 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" t="inlineStr"/>
-      <c r="B230" t="inlineStr"/>
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>M012</t>
+        </is>
+      </c>
+      <c r="B230" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010124/24
+Lender Amount: 1150.00
+Borrower Amount: 1150.00</t>
+        </is>
+      </c>
       <c r="C230" t="inlineStr"/>
       <c r="D230" t="inlineStr"/>
       <c r="E230" s="4" t="inlineStr">
@@ -5789,8 +5961,18 @@
       <c r="K230" t="inlineStr"/>
     </row>
     <row r="231">
-      <c r="A231" t="inlineStr"/>
-      <c r="B231" t="inlineStr"/>
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>M012</t>
+        </is>
+      </c>
+      <c r="B231" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010124/24
+Lender Amount: 1150.00
+Borrower Amount: 1150.00</t>
+        </is>
+      </c>
       <c r="C231" t="inlineStr"/>
       <c r="D231" t="inlineStr">
         <is>
@@ -5890,8 +6072,7 @@
       </c>
       <c r="B235" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-187724010124/24
+          <t>LC Match: L/C-187724010124/24
 Lender Amount: 8761.79
 Borrower Amount: 8761.79</t>
         </is>
@@ -5929,8 +6110,18 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" t="inlineStr"/>
-      <c r="B236" t="inlineStr"/>
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>M013</t>
+        </is>
+      </c>
+      <c r="B236" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010124/24
+Lender Amount: 8761.79
+Borrower Amount: 8761.79</t>
+        </is>
+      </c>
       <c r="C236" t="inlineStr"/>
       <c r="D236" t="inlineStr"/>
       <c r="E236" s="4" t="inlineStr">
@@ -5946,8 +6137,18 @@
       <c r="K236" t="inlineStr"/>
     </row>
     <row r="237">
-      <c r="A237" t="inlineStr"/>
-      <c r="B237" t="inlineStr"/>
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>M013</t>
+        </is>
+      </c>
+      <c r="B237" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010124/24
+Lender Amount: 8761.79
+Borrower Amount: 8761.79</t>
+        </is>
+      </c>
       <c r="C237" t="inlineStr"/>
       <c r="D237" t="inlineStr">
         <is>
@@ -6377,8 +6578,7 @@
       </c>
       <c r="B255" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
+          <t>LC Match: L/C-308524027065/24
 Lender Amount: 1862.50
 Borrower Amount: 1862.50</t>
         </is>
@@ -6416,8 +6616,18 @@
       <c r="K255" t="inlineStr"/>
     </row>
     <row r="256">
-      <c r="A256" t="inlineStr"/>
-      <c r="B256" t="inlineStr"/>
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>M014</t>
+        </is>
+      </c>
+      <c r="B256" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1862.50
+Borrower Amount: 1862.50</t>
+        </is>
+      </c>
       <c r="C256" t="inlineStr"/>
       <c r="D256" t="inlineStr"/>
       <c r="E256" s="4" t="inlineStr">
@@ -6433,8 +6643,18 @@
       <c r="K256" t="inlineStr"/>
     </row>
     <row r="257">
-      <c r="A257" t="inlineStr"/>
-      <c r="B257" t="inlineStr"/>
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>M014</t>
+        </is>
+      </c>
+      <c r="B257" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1862.50
+Borrower Amount: 1862.50</t>
+        </is>
+      </c>
       <c r="C257" t="inlineStr"/>
       <c r="D257" t="inlineStr">
         <is>
@@ -6883,8 +7103,7 @@
       </c>
       <c r="B276" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-147125020003/25
+          <t>LC Match: L/C-147125020003/25
 Lender Amount: 27383.77
 Borrower Amount: 27383.77</t>
         </is>
@@ -6922,8 +7141,18 @@
       <c r="K276" t="inlineStr"/>
     </row>
     <row r="277">
-      <c r="A277" t="inlineStr"/>
-      <c r="B277" t="inlineStr"/>
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>M015</t>
+        </is>
+      </c>
+      <c r="B277" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020003/25
+Lender Amount: 27383.77
+Borrower Amount: 27383.77</t>
+        </is>
+      </c>
       <c r="C277" t="inlineStr"/>
       <c r="D277" t="inlineStr"/>
       <c r="E277" s="4" t="inlineStr">
@@ -6939,8 +7168,18 @@
       <c r="K277" t="inlineStr"/>
     </row>
     <row r="278">
-      <c r="A278" t="inlineStr"/>
-      <c r="B278" t="inlineStr"/>
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>M015</t>
+        </is>
+      </c>
+      <c r="B278" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020003/25
+Lender Amount: 27383.77
+Borrower Amount: 27383.77</t>
+        </is>
+      </c>
       <c r="C278" t="inlineStr"/>
       <c r="D278" t="inlineStr">
         <is>
@@ -8341,8 +8580,7 @@
       </c>
       <c r="B337" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
+          <t>LC Match: L/C-308524990243/24
 Lender Amount: 71971.54
 Borrower Amount: 71971.54</t>
         </is>
@@ -8380,8 +8618,18 @@
       <c r="K337" t="inlineStr"/>
     </row>
     <row r="338">
-      <c r="A338" t="inlineStr"/>
-      <c r="B338" t="inlineStr"/>
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>M016</t>
+        </is>
+      </c>
+      <c r="B338" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524990243/24
+Lender Amount: 71971.54
+Borrower Amount: 71971.54</t>
+        </is>
+      </c>
       <c r="C338" t="inlineStr"/>
       <c r="D338" t="inlineStr"/>
       <c r="E338" s="4" t="inlineStr">
@@ -8397,8 +8645,18 @@
       <c r="K338" t="inlineStr"/>
     </row>
     <row r="339">
-      <c r="A339" t="inlineStr"/>
-      <c r="B339" t="inlineStr"/>
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>M016</t>
+        </is>
+      </c>
+      <c r="B339" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524990243/24
+Lender Amount: 71971.54
+Borrower Amount: 71971.54</t>
+        </is>
+      </c>
       <c r="C339" t="inlineStr"/>
       <c r="D339" t="inlineStr">
         <is>
@@ -8425,8 +8683,7 @@
       </c>
       <c r="B340" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
+          <t>LC Match: L/C-308524990243/24
 Lender Amount: 20527984.90
 Borrower Amount: 20527984.90</t>
         </is>
@@ -8464,8 +8721,18 @@
       <c r="K340" t="inlineStr"/>
     </row>
     <row r="341">
-      <c r="A341" t="inlineStr"/>
-      <c r="B341" t="inlineStr"/>
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>M017</t>
+        </is>
+      </c>
+      <c r="B341" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524990243/24
+Lender Amount: 20527984.90
+Borrower Amount: 20527984.90</t>
+        </is>
+      </c>
       <c r="C341" t="inlineStr"/>
       <c r="D341" t="inlineStr"/>
       <c r="E341" s="4" t="inlineStr">
@@ -8481,8 +8748,18 @@
       <c r="K341" t="inlineStr"/>
     </row>
     <row r="342">
-      <c r="A342" t="inlineStr"/>
-      <c r="B342" t="inlineStr"/>
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>M017</t>
+        </is>
+      </c>
+      <c r="B342" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524990243/24
+Lender Amount: 20527984.90
+Borrower Amount: 20527984.90</t>
+        </is>
+      </c>
       <c r="C342" t="inlineStr"/>
       <c r="D342" t="inlineStr">
         <is>
@@ -8509,8 +8786,7 @@
       </c>
       <c r="B343" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-147124020653/25
+          <t>LC Match: L/C-147124020653/25
 Lender Amount: 665048.82
 Borrower Amount: 665048.82</t>
         </is>
@@ -8548,8 +8824,18 @@
       <c r="K343" t="inlineStr"/>
     </row>
     <row r="344">
-      <c r="A344" t="inlineStr"/>
-      <c r="B344" t="inlineStr"/>
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>M018</t>
+        </is>
+      </c>
+      <c r="B344" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020653/25
+Lender Amount: 665048.82
+Borrower Amount: 665048.82</t>
+        </is>
+      </c>
       <c r="C344" t="inlineStr"/>
       <c r="D344" t="inlineStr"/>
       <c r="E344" s="4" t="inlineStr">
@@ -8565,8 +8851,18 @@
       <c r="K344" t="inlineStr"/>
     </row>
     <row r="345">
-      <c r="A345" t="inlineStr"/>
-      <c r="B345" t="inlineStr"/>
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>M018</t>
+        </is>
+      </c>
+      <c r="B345" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020653/25
+Lender Amount: 665048.82
+Borrower Amount: 665048.82</t>
+        </is>
+      </c>
       <c r="C345" t="inlineStr"/>
       <c r="D345" t="inlineStr">
         <is>
@@ -8593,8 +8889,7 @@
       </c>
       <c r="B346" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-147124020708/24
+          <t>LC Match: L/C-147124020708/24
 Lender Amount: 25042.61
 Borrower Amount: 25042.61</t>
         </is>
@@ -8632,8 +8927,18 @@
       <c r="K346" t="inlineStr"/>
     </row>
     <row r="347">
-      <c r="A347" t="inlineStr"/>
-      <c r="B347" t="inlineStr"/>
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
+      <c r="B347" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020708/24
+Lender Amount: 25042.61
+Borrower Amount: 25042.61</t>
+        </is>
+      </c>
       <c r="C347" t="inlineStr"/>
       <c r="D347" t="inlineStr"/>
       <c r="E347" s="4" t="inlineStr">
@@ -8649,8 +8954,18 @@
       <c r="K347" t="inlineStr"/>
     </row>
     <row r="348">
-      <c r="A348" t="inlineStr"/>
-      <c r="B348" t="inlineStr"/>
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
+      <c r="B348" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020708/24
+Lender Amount: 25042.61
+Borrower Amount: 25042.61</t>
+        </is>
+      </c>
       <c r="C348" t="inlineStr"/>
       <c r="D348" t="inlineStr">
         <is>
@@ -8970,8 +9285,7 @@
       </c>
       <c r="B361" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
+          <t>LC Match: L/C-141325020063/25
 Lender Amount: 5995080.00
 Borrower Amount: 5995080.00</t>
         </is>
@@ -9009,8 +9323,18 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" t="inlineStr"/>
-      <c r="B362" t="inlineStr"/>
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>M020</t>
+        </is>
+      </c>
+      <c r="B362" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 5995080.00
+Borrower Amount: 5995080.00</t>
+        </is>
+      </c>
       <c r="C362" t="inlineStr"/>
       <c r="D362" t="inlineStr"/>
       <c r="E362" s="4" t="inlineStr">
@@ -9026,8 +9350,18 @@
       <c r="K362" t="inlineStr"/>
     </row>
     <row r="363">
-      <c r="A363" t="inlineStr"/>
-      <c r="B363" t="inlineStr"/>
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>M020</t>
+        </is>
+      </c>
+      <c r="B363" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 5995080.00
+Borrower Amount: 5995080.00</t>
+        </is>
+      </c>
       <c r="C363" t="inlineStr"/>
       <c r="D363" t="inlineStr">
         <is>
@@ -9054,8 +9388,7 @@
       </c>
       <c r="B364" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
+          <t>LC Match: L/C-141325020068/25
 Lender Amount: 33573.89
 Borrower Amount: 33573.89</t>
         </is>
@@ -9093,8 +9426,18 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" t="inlineStr"/>
-      <c r="B365" t="inlineStr"/>
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>M021</t>
+        </is>
+      </c>
+      <c r="B365" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020068/25
+Lender Amount: 33573.89
+Borrower Amount: 33573.89</t>
+        </is>
+      </c>
       <c r="C365" t="inlineStr"/>
       <c r="D365" t="inlineStr"/>
       <c r="E365" s="4" t="inlineStr">
@@ -9110,8 +9453,18 @@
       <c r="K365" t="inlineStr"/>
     </row>
     <row r="366">
-      <c r="A366" t="inlineStr"/>
-      <c r="B366" t="inlineStr"/>
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>M021</t>
+        </is>
+      </c>
+      <c r="B366" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020068/25
+Lender Amount: 33573.89
+Borrower Amount: 33573.89</t>
+        </is>
+      </c>
       <c r="C366" t="inlineStr"/>
       <c r="D366" t="inlineStr">
         <is>
@@ -9138,8 +9491,7 @@
       </c>
       <c r="B367" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
+          <t>LC Match: L/C-141325020068/25
 Lender Amount: 1650660.00
 Borrower Amount: 1650660.00</t>
         </is>
@@ -9177,8 +9529,18 @@
       </c>
     </row>
     <row r="368">
-      <c r="A368" t="inlineStr"/>
-      <c r="B368" t="inlineStr"/>
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>M022</t>
+        </is>
+      </c>
+      <c r="B368" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020068/25
+Lender Amount: 1650660.00
+Borrower Amount: 1650660.00</t>
+        </is>
+      </c>
       <c r="C368" t="inlineStr"/>
       <c r="D368" t="inlineStr"/>
       <c r="E368" s="4" t="inlineStr">
@@ -9194,8 +9556,18 @@
       <c r="K368" t="inlineStr"/>
     </row>
     <row r="369">
-      <c r="A369" t="inlineStr"/>
-      <c r="B369" t="inlineStr"/>
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>M022</t>
+        </is>
+      </c>
+      <c r="B369" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020068/25
+Lender Amount: 1650660.00
+Borrower Amount: 1650660.00</t>
+        </is>
+      </c>
       <c r="C369" t="inlineStr"/>
       <c r="D369" t="inlineStr">
         <is>
@@ -9442,8 +9814,7 @@
       </c>
       <c r="B379" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-155824020001/24
+          <t>LC Match: LC-155824020001/24
 Lender Amount: 7641878.37
 Borrower Amount: 7641878.37</t>
         </is>
@@ -9481,8 +9852,18 @@
       <c r="K379" t="inlineStr"/>
     </row>
     <row r="380">
-      <c r="A380" t="inlineStr"/>
-      <c r="B380" t="inlineStr"/>
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>M023</t>
+        </is>
+      </c>
+      <c r="B380" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155824020001/24
+Lender Amount: 7641878.37
+Borrower Amount: 7641878.37</t>
+        </is>
+      </c>
       <c r="C380" t="inlineStr"/>
       <c r="D380" t="inlineStr"/>
       <c r="E380" s="4" t="inlineStr">
@@ -9500,8 +9881,18 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" t="inlineStr"/>
-      <c r="B381" t="inlineStr"/>
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>M023</t>
+        </is>
+      </c>
+      <c r="B381" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155824020001/24
+Lender Amount: 7641878.37
+Borrower Amount: 7641878.37</t>
+        </is>
+      </c>
       <c r="C381" t="inlineStr"/>
       <c r="D381" t="inlineStr"/>
       <c r="E381" s="4" t="inlineStr">
@@ -9519,8 +9910,18 @@
       </c>
     </row>
     <row r="382">
-      <c r="A382" t="inlineStr"/>
-      <c r="B382" t="inlineStr"/>
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>M023</t>
+        </is>
+      </c>
+      <c r="B382" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155824020001/24
+Lender Amount: 7641878.37
+Borrower Amount: 7641878.37</t>
+        </is>
+      </c>
       <c r="C382" t="inlineStr"/>
       <c r="D382" t="inlineStr"/>
       <c r="E382" s="4" t="inlineStr">
@@ -9536,8 +9937,18 @@
       <c r="K382" t="inlineStr"/>
     </row>
     <row r="383">
-      <c r="A383" t="inlineStr"/>
-      <c r="B383" t="inlineStr"/>
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>M023</t>
+        </is>
+      </c>
+      <c r="B383" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155824020001/24
+Lender Amount: 7641878.37
+Borrower Amount: 7641878.37</t>
+        </is>
+      </c>
       <c r="C383" t="inlineStr"/>
       <c r="D383" t="inlineStr">
         <is>
@@ -10588,8 +10999,7 @@
       </c>
       <c r="B432" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
+          <t>LC Match: L/C-141325020063/25
 Lender Amount: 246401.97
 Borrower Amount: 246401.97</t>
         </is>
@@ -10627,8 +11037,18 @@
       </c>
     </row>
     <row r="433">
-      <c r="A433" t="inlineStr"/>
-      <c r="B433" t="inlineStr"/>
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>M024</t>
+        </is>
+      </c>
+      <c r="B433" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 246401.97
+Borrower Amount: 246401.97</t>
+        </is>
+      </c>
       <c r="C433" t="inlineStr"/>
       <c r="D433" t="inlineStr"/>
       <c r="E433" s="4" t="inlineStr">
@@ -10644,8 +11064,18 @@
       <c r="K433" t="inlineStr"/>
     </row>
     <row r="434">
-      <c r="A434" t="inlineStr"/>
-      <c r="B434" t="inlineStr"/>
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>M024</t>
+        </is>
+      </c>
+      <c r="B434" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 246401.97
+Borrower Amount: 246401.97</t>
+        </is>
+      </c>
       <c r="C434" t="inlineStr"/>
       <c r="D434" t="inlineStr">
         <is>
@@ -10818,8 +11248,7 @@
       </c>
       <c r="B441" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524022796/24
+          <t>LC Match: L/C-308524022796/24
 Lender Amount: 26369.63
 Borrower Amount: 26369.63</t>
         </is>
@@ -10857,8 +11286,18 @@
       <c r="K441" t="inlineStr"/>
     </row>
     <row r="442">
-      <c r="A442" t="inlineStr"/>
-      <c r="B442" t="inlineStr"/>
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>M025</t>
+        </is>
+      </c>
+      <c r="B442" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 26369.63
+Borrower Amount: 26369.63</t>
+        </is>
+      </c>
       <c r="C442" t="inlineStr"/>
       <c r="D442" t="inlineStr"/>
       <c r="E442" s="4" t="inlineStr">
@@ -10874,8 +11313,18 @@
       <c r="K442" t="inlineStr"/>
     </row>
     <row r="443">
-      <c r="A443" t="inlineStr"/>
-      <c r="B443" t="inlineStr"/>
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>M025</t>
+        </is>
+      </c>
+      <c r="B443" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 26369.63
+Borrower Amount: 26369.63</t>
+        </is>
+      </c>
       <c r="C443" t="inlineStr"/>
       <c r="D443" t="inlineStr">
         <is>
@@ -11305,8 +11754,7 @@
       </c>
       <c r="B461" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-222825150235/25
+          <t>LC Match: L/C-222825150235/25
 Lender Amount: 2357.50
 Borrower Amount: 2357.50</t>
         </is>
@@ -11344,8 +11792,18 @@
       </c>
     </row>
     <row r="462">
-      <c r="A462" t="inlineStr"/>
-      <c r="B462" t="inlineStr"/>
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>M026</t>
+        </is>
+      </c>
+      <c r="B462" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-222825150235/25
+Lender Amount: 2357.50
+Borrower Amount: 2357.50</t>
+        </is>
+      </c>
       <c r="C462" t="inlineStr"/>
       <c r="D462" t="inlineStr"/>
       <c r="E462" s="4" t="inlineStr">
@@ -11361,8 +11819,18 @@
       <c r="K462" t="inlineStr"/>
     </row>
     <row r="463">
-      <c r="A463" t="inlineStr"/>
-      <c r="B463" t="inlineStr"/>
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>M026</t>
+        </is>
+      </c>
+      <c r="B463" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-222825150235/25
+Lender Amount: 2357.50
+Borrower Amount: 2357.50</t>
+        </is>
+      </c>
       <c r="C463" t="inlineStr"/>
       <c r="D463" t="inlineStr">
         <is>
@@ -11462,8 +11930,7 @@
       </c>
       <c r="B467" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-222825150235/25
+          <t>LC Match: L/C-222825150235/25
 Lender Amount: 213500.00
 Borrower Amount: 213500.00</t>
         </is>
@@ -11501,8 +11968,18 @@
       </c>
     </row>
     <row r="468">
-      <c r="A468" t="inlineStr"/>
-      <c r="B468" t="inlineStr"/>
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>M027</t>
+        </is>
+      </c>
+      <c r="B468" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-222825150235/25
+Lender Amount: 213500.00
+Borrower Amount: 213500.00</t>
+        </is>
+      </c>
       <c r="C468" t="inlineStr"/>
       <c r="D468" t="inlineStr"/>
       <c r="E468" s="4" t="inlineStr">
@@ -11518,8 +11995,18 @@
       <c r="K468" t="inlineStr"/>
     </row>
     <row r="469">
-      <c r="A469" t="inlineStr"/>
-      <c r="B469" t="inlineStr"/>
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>M027</t>
+        </is>
+      </c>
+      <c r="B469" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-222825150235/25
+Lender Amount: 213500.00
+Borrower Amount: 213500.00</t>
+        </is>
+      </c>
       <c r="C469" t="inlineStr"/>
       <c r="D469" t="inlineStr">
         <is>
@@ -11546,8 +12033,7 @@
       </c>
       <c r="B470" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
+          <t>LC Match: L/C-308524027065/24
 Lender Amount: 1725.00
 Borrower Amount: 1725.00</t>
         </is>
@@ -11585,8 +12071,18 @@
       <c r="K470" t="inlineStr"/>
     </row>
     <row r="471">
-      <c r="A471" t="inlineStr"/>
-      <c r="B471" t="inlineStr"/>
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>M028</t>
+        </is>
+      </c>
+      <c r="B471" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1725.00
+Borrower Amount: 1725.00</t>
+        </is>
+      </c>
       <c r="C471" t="inlineStr"/>
       <c r="D471" t="inlineStr"/>
       <c r="E471" s="4" t="inlineStr">
@@ -11602,8 +12098,18 @@
       <c r="K471" t="inlineStr"/>
     </row>
     <row r="472">
-      <c r="A472" t="inlineStr"/>
-      <c r="B472" t="inlineStr"/>
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>M028</t>
+        </is>
+      </c>
+      <c r="B472" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1725.00
+Borrower Amount: 1725.00</t>
+        </is>
+      </c>
       <c r="C472" t="inlineStr"/>
       <c r="D472" t="inlineStr">
         <is>
@@ -11630,8 +12136,7 @@
       </c>
       <c r="B473" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-187724010122/24
+          <t>LC Match: L/C-187724010122/24
 Lender Amount: 276518.90
 Borrower Amount: 276518.90</t>
         </is>
@@ -11669,8 +12174,18 @@
       <c r="K473" t="inlineStr"/>
     </row>
     <row r="474">
-      <c r="A474" t="inlineStr"/>
-      <c r="B474" t="inlineStr"/>
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
+      <c r="B474" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010122/24
+Lender Amount: 276518.90
+Borrower Amount: 276518.90</t>
+        </is>
+      </c>
       <c r="C474" t="inlineStr"/>
       <c r="D474" t="inlineStr"/>
       <c r="E474" s="4" t="inlineStr">
@@ -11688,8 +12203,18 @@
       </c>
     </row>
     <row r="475">
-      <c r="A475" t="inlineStr"/>
-      <c r="B475" t="inlineStr"/>
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
+      <c r="B475" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010122/24
+Lender Amount: 276518.90
+Borrower Amount: 276518.90</t>
+        </is>
+      </c>
       <c r="C475" t="inlineStr"/>
       <c r="D475" t="inlineStr"/>
       <c r="E475" s="4" t="inlineStr">
@@ -11707,8 +12232,18 @@
       </c>
     </row>
     <row r="476">
-      <c r="A476" t="inlineStr"/>
-      <c r="B476" t="inlineStr"/>
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
+      <c r="B476" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010122/24
+Lender Amount: 276518.90
+Borrower Amount: 276518.90</t>
+        </is>
+      </c>
       <c r="C476" t="inlineStr"/>
       <c r="D476" t="inlineStr"/>
       <c r="E476" s="4" t="inlineStr">
@@ -11724,8 +12259,18 @@
       <c r="K476" t="inlineStr"/>
     </row>
     <row r="477">
-      <c r="A477" t="inlineStr"/>
-      <c r="B477" t="inlineStr"/>
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
+      <c r="B477" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010122/24
+Lender Amount: 276518.90
+Borrower Amount: 276518.90</t>
+        </is>
+      </c>
       <c r="C477" t="inlineStr"/>
       <c r="D477" t="inlineStr">
         <is>
@@ -12482,8 +13027,7 @@
       </c>
       <c r="B508" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-147125020027/25
+          <t>LC Match: L/C-147125020027/25
 Lender Amount: 54431.58
 Borrower Amount: 54431.58</t>
         </is>
@@ -12521,8 +13065,18 @@
       <c r="K508" t="inlineStr"/>
     </row>
     <row r="509">
-      <c r="A509" t="inlineStr"/>
-      <c r="B509" t="inlineStr"/>
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>M030</t>
+        </is>
+      </c>
+      <c r="B509" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020027/25
+Lender Amount: 54431.58
+Borrower Amount: 54431.58</t>
+        </is>
+      </c>
       <c r="C509" t="inlineStr"/>
       <c r="D509" t="inlineStr"/>
       <c r="E509" s="4" t="inlineStr">
@@ -12538,8 +13092,18 @@
       <c r="K509" t="inlineStr"/>
     </row>
     <row r="510">
-      <c r="A510" t="inlineStr"/>
-      <c r="B510" t="inlineStr"/>
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>M030</t>
+        </is>
+      </c>
+      <c r="B510" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020027/25
+Lender Amount: 54431.58
+Borrower Amount: 54431.58</t>
+        </is>
+      </c>
       <c r="C510" t="inlineStr"/>
       <c r="D510" t="inlineStr">
         <is>
@@ -12785,8 +13349,7 @@
       </c>
       <c r="B520" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524027065/24
+          <t>LC Match: L/C-308524027065/24
 Lender Amount: 8231.99
 Borrower Amount: 8231.99</t>
         </is>
@@ -12824,8 +13387,18 @@
       <c r="K520" t="inlineStr"/>
     </row>
     <row r="521">
-      <c r="A521" t="inlineStr"/>
-      <c r="B521" t="inlineStr"/>
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>M031</t>
+        </is>
+      </c>
+      <c r="B521" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 8231.99
+Borrower Amount: 8231.99</t>
+        </is>
+      </c>
       <c r="C521" t="inlineStr"/>
       <c r="D521" t="inlineStr"/>
       <c r="E521" s="4" t="inlineStr">
@@ -12841,8 +13414,18 @@
       <c r="K521" t="inlineStr"/>
     </row>
     <row r="522">
-      <c r="A522" t="inlineStr"/>
-      <c r="B522" t="inlineStr"/>
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>M031</t>
+        </is>
+      </c>
+      <c r="B522" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 8231.99
+Borrower Amount: 8231.99</t>
+        </is>
+      </c>
       <c r="C522" t="inlineStr"/>
       <c r="D522" t="inlineStr">
         <is>
@@ -13906,8 +14489,7 @@
       </c>
       <c r="B570" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-147124020708/24
+          <t>LC Match: L/C-147124020708/24
 Lender Amount: 19399.10
 Borrower Amount: 19399.10</t>
         </is>
@@ -13945,8 +14527,18 @@
       <c r="K570" t="inlineStr"/>
     </row>
     <row r="571">
-      <c r="A571" t="inlineStr"/>
-      <c r="B571" t="inlineStr"/>
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>M032</t>
+        </is>
+      </c>
+      <c r="B571" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020708/24
+Lender Amount: 19399.10
+Borrower Amount: 19399.10</t>
+        </is>
+      </c>
       <c r="C571" t="inlineStr"/>
       <c r="D571" t="inlineStr"/>
       <c r="E571" s="4" t="inlineStr">
@@ -13962,8 +14554,18 @@
       <c r="K571" t="inlineStr"/>
     </row>
     <row r="572">
-      <c r="A572" t="inlineStr"/>
-      <c r="B572" t="inlineStr"/>
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>M032</t>
+        </is>
+      </c>
+      <c r="B572" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020708/24
+Lender Amount: 19399.10
+Borrower Amount: 19399.10</t>
+        </is>
+      </c>
       <c r="C572" t="inlineStr"/>
       <c r="D572" t="inlineStr">
         <is>
@@ -13990,8 +14592,7 @@
       </c>
       <c r="B573" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524990243/24
+          <t>LC Match: L/C-308524990243/24
 Lender Amount: 15160.97
 Borrower Amount: 15160.97</t>
         </is>
@@ -14029,8 +14630,18 @@
       <c r="K573" t="inlineStr"/>
     </row>
     <row r="574">
-      <c r="A574" t="inlineStr"/>
-      <c r="B574" t="inlineStr"/>
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>M033</t>
+        </is>
+      </c>
+      <c r="B574" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524990243/24
+Lender Amount: 15160.97
+Borrower Amount: 15160.97</t>
+        </is>
+      </c>
       <c r="C574" t="inlineStr"/>
       <c r="D574" t="inlineStr"/>
       <c r="E574" s="4" t="inlineStr">
@@ -14046,8 +14657,18 @@
       <c r="K574" t="inlineStr"/>
     </row>
     <row r="575">
-      <c r="A575" t="inlineStr"/>
-      <c r="B575" t="inlineStr"/>
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>M033</t>
+        </is>
+      </c>
+      <c r="B575" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524990243/24
+Lender Amount: 15160.97
+Borrower Amount: 15160.97</t>
+        </is>
+      </c>
       <c r="C575" t="inlineStr"/>
       <c r="D575" t="inlineStr">
         <is>
@@ -14223,8 +14844,7 @@
       </c>
       <c r="B583" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
+          <t>LC Match: L/C-141325020104/25
 Lender Amount: 6125933.94
 Borrower Amount: 6125933.94</t>
         </is>
@@ -14262,8 +14882,18 @@
       </c>
     </row>
     <row r="584">
-      <c r="A584" t="inlineStr"/>
-      <c r="B584" t="inlineStr"/>
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>M034</t>
+        </is>
+      </c>
+      <c r="B584" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 6125933.94
+Borrower Amount: 6125933.94</t>
+        </is>
+      </c>
       <c r="C584" t="inlineStr"/>
       <c r="D584" t="inlineStr"/>
       <c r="E584" s="4" t="inlineStr">
@@ -14281,8 +14911,18 @@
       <c r="K584" t="inlineStr"/>
     </row>
     <row r="585">
-      <c r="A585" t="inlineStr"/>
-      <c r="B585" t="inlineStr"/>
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>M034</t>
+        </is>
+      </c>
+      <c r="B585" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 6125933.94
+Borrower Amount: 6125933.94</t>
+        </is>
+      </c>
       <c r="C585" t="inlineStr"/>
       <c r="D585" t="inlineStr"/>
       <c r="E585" s="4" t="inlineStr">
@@ -14300,8 +14940,18 @@
       <c r="K585" t="inlineStr"/>
     </row>
     <row r="586">
-      <c r="A586" t="inlineStr"/>
-      <c r="B586" t="inlineStr"/>
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>M034</t>
+        </is>
+      </c>
+      <c r="B586" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 6125933.94
+Borrower Amount: 6125933.94</t>
+        </is>
+      </c>
       <c r="C586" t="inlineStr"/>
       <c r="D586" t="inlineStr"/>
       <c r="E586" s="4" t="inlineStr">
@@ -14317,8 +14967,18 @@
       <c r="K586" t="inlineStr"/>
     </row>
     <row r="587">
-      <c r="A587" t="inlineStr"/>
-      <c r="B587" t="inlineStr"/>
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>M034</t>
+        </is>
+      </c>
+      <c r="B587" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 6125933.94
+Borrower Amount: 6125933.94</t>
+        </is>
+      </c>
       <c r="C587" t="inlineStr"/>
       <c r="D587" t="inlineStr">
         <is>
@@ -14345,8 +15005,7 @@
       </c>
       <c r="B588" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524022495/24
+          <t>LC Match: L/C-308524022495/24
 Lender Amount: 12425.77
 Borrower Amount: 12425.77</t>
         </is>
@@ -14384,8 +15043,18 @@
       <c r="K588" t="inlineStr"/>
     </row>
     <row r="589">
-      <c r="A589" t="inlineStr"/>
-      <c r="B589" t="inlineStr"/>
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>M035</t>
+        </is>
+      </c>
+      <c r="B589" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022495/24
+Lender Amount: 12425.77
+Borrower Amount: 12425.77</t>
+        </is>
+      </c>
       <c r="C589" t="inlineStr"/>
       <c r="D589" t="inlineStr"/>
       <c r="E589" s="4" t="inlineStr">
@@ -14401,8 +15070,18 @@
       <c r="K589" t="inlineStr"/>
     </row>
     <row r="590">
-      <c r="A590" t="inlineStr"/>
-      <c r="B590" t="inlineStr"/>
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>M035</t>
+        </is>
+      </c>
+      <c r="B590" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022495/24
+Lender Amount: 12425.77
+Borrower Amount: 12425.77</t>
+        </is>
+      </c>
       <c r="C590" t="inlineStr"/>
       <c r="D590" t="inlineStr">
         <is>
@@ -14429,8 +15108,7 @@
       </c>
       <c r="B591" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524022495/24
+          <t>LC Match: L/C-308524022495/24
 Lender Amount: 23580.68
 Borrower Amount: 23580.68</t>
         </is>
@@ -14468,8 +15146,18 @@
       <c r="K591" t="inlineStr"/>
     </row>
     <row r="592">
-      <c r="A592" t="inlineStr"/>
-      <c r="B592" t="inlineStr"/>
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>M036</t>
+        </is>
+      </c>
+      <c r="B592" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022495/24
+Lender Amount: 23580.68
+Borrower Amount: 23580.68</t>
+        </is>
+      </c>
       <c r="C592" t="inlineStr"/>
       <c r="D592" t="inlineStr"/>
       <c r="E592" s="4" t="inlineStr">
@@ -14485,8 +15173,18 @@
       <c r="K592" t="inlineStr"/>
     </row>
     <row r="593">
-      <c r="A593" t="inlineStr"/>
-      <c r="B593" t="inlineStr"/>
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>M036</t>
+        </is>
+      </c>
+      <c r="B593" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022495/24
+Lender Amount: 23580.68
+Borrower Amount: 23580.68</t>
+        </is>
+      </c>
       <c r="C593" t="inlineStr"/>
       <c r="D593" t="inlineStr">
         <is>
@@ -15499,8 +16197,7 @@
       </c>
       <c r="B640" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308525021741/25
+          <t>LC Match: L/C-308525021741/25
 Lender Amount: 22671.95
 Borrower Amount: 22671.95</t>
         </is>
@@ -15538,8 +16235,18 @@
       <c r="K640" t="inlineStr"/>
     </row>
     <row r="641">
-      <c r="A641" t="inlineStr"/>
-      <c r="B641" t="inlineStr"/>
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>M037</t>
+        </is>
+      </c>
+      <c r="B641" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308525021741/25
+Lender Amount: 22671.95
+Borrower Amount: 22671.95</t>
+        </is>
+      </c>
       <c r="C641" t="inlineStr"/>
       <c r="D641" t="inlineStr"/>
       <c r="E641" s="4" t="inlineStr">
@@ -15555,8 +16262,18 @@
       <c r="K641" t="inlineStr"/>
     </row>
     <row r="642">
-      <c r="A642" t="inlineStr"/>
-      <c r="B642" t="inlineStr"/>
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>M037</t>
+        </is>
+      </c>
+      <c r="B642" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308525021741/25
+Lender Amount: 22671.95
+Borrower Amount: 22671.95</t>
+        </is>
+      </c>
       <c r="C642" t="inlineStr"/>
       <c r="D642" t="inlineStr">
         <is>
@@ -15583,8 +16300,7 @@
       </c>
       <c r="B643" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308525021745/25
+          <t>LC Match: L/C-308525021745/25
 Lender Amount: 28854.86
 Borrower Amount: 28854.86</t>
         </is>
@@ -15622,8 +16338,18 @@
       <c r="K643" t="inlineStr"/>
     </row>
     <row r="644">
-      <c r="A644" t="inlineStr"/>
-      <c r="B644" t="inlineStr"/>
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>M038</t>
+        </is>
+      </c>
+      <c r="B644" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308525021745/25
+Lender Amount: 28854.86
+Borrower Amount: 28854.86</t>
+        </is>
+      </c>
       <c r="C644" t="inlineStr"/>
       <c r="D644" t="inlineStr"/>
       <c r="E644" s="4" t="inlineStr">
@@ -15639,8 +16365,18 @@
       <c r="K644" t="inlineStr"/>
     </row>
     <row r="645">
-      <c r="A645" t="inlineStr"/>
-      <c r="B645" t="inlineStr"/>
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>M038</t>
+        </is>
+      </c>
+      <c r="B645" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308525021745/25
+Lender Amount: 28854.86
+Borrower Amount: 28854.86</t>
+        </is>
+      </c>
       <c r="C645" t="inlineStr"/>
       <c r="D645" t="inlineStr">
         <is>
@@ -15667,8 +16403,7 @@
       </c>
       <c r="B646" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
+          <t>LC Match: L/C-308524026037/24
 Lender Amount: 1725.00
 Borrower Amount: 1725.00</t>
         </is>
@@ -15706,8 +16441,18 @@
       <c r="K646" t="inlineStr"/>
     </row>
     <row r="647">
-      <c r="A647" t="inlineStr"/>
-      <c r="B647" t="inlineStr"/>
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>M039</t>
+        </is>
+      </c>
+      <c r="B647" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524026037/24
+Lender Amount: 1725.00
+Borrower Amount: 1725.00</t>
+        </is>
+      </c>
       <c r="C647" t="inlineStr"/>
       <c r="D647" t="inlineStr"/>
       <c r="E647" s="4" t="inlineStr">
@@ -15723,8 +16468,18 @@
       <c r="K647" t="inlineStr"/>
     </row>
     <row r="648">
-      <c r="A648" t="inlineStr"/>
-      <c r="B648" t="inlineStr"/>
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>M039</t>
+        </is>
+      </c>
+      <c r="B648" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524026037/24
+Lender Amount: 1725.00
+Borrower Amount: 1725.00</t>
+        </is>
+      </c>
       <c r="C648" t="inlineStr"/>
       <c r="D648" t="inlineStr">
         <is>
@@ -16262,8 +17017,7 @@
       </c>
       <c r="B670" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
+          <t>LC Match: LC-141325020063/25
 Lender Amount: 80051.03
 Borrower Amount: 80051.03</t>
         </is>
@@ -16301,8 +17055,18 @@
       </c>
     </row>
     <row r="671">
-      <c r="A671" t="inlineStr"/>
-      <c r="B671" t="inlineStr"/>
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>M040</t>
+        </is>
+      </c>
+      <c r="B671" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/25
+Lender Amount: 80051.03
+Borrower Amount: 80051.03</t>
+        </is>
+      </c>
       <c r="C671" t="inlineStr"/>
       <c r="D671" t="inlineStr"/>
       <c r="E671" s="4" t="inlineStr">
@@ -16318,8 +17082,18 @@
       <c r="K671" t="inlineStr"/>
     </row>
     <row r="672">
-      <c r="A672" t="inlineStr"/>
-      <c r="B672" t="inlineStr"/>
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>M040</t>
+        </is>
+      </c>
+      <c r="B672" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/25
+Lender Amount: 80051.03
+Borrower Amount: 80051.03</t>
+        </is>
+      </c>
       <c r="C672" t="inlineStr"/>
       <c r="D672" t="inlineStr">
         <is>
@@ -16346,8 +17120,7 @@
       </c>
       <c r="B673" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
+          <t>LC Match: L/C-141325020063/25
 Lender Amount: 6777058.20
 Borrower Amount: 6777058.20</t>
         </is>
@@ -16385,8 +17158,18 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" t="inlineStr"/>
-      <c r="B674" t="inlineStr"/>
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>M041</t>
+        </is>
+      </c>
+      <c r="B674" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 6777058.20
+Borrower Amount: 6777058.20</t>
+        </is>
+      </c>
       <c r="C674" t="inlineStr"/>
       <c r="D674" t="inlineStr"/>
       <c r="E674" s="4" t="inlineStr">
@@ -16404,8 +17187,18 @@
       <c r="K674" t="inlineStr"/>
     </row>
     <row r="675">
-      <c r="A675" t="inlineStr"/>
-      <c r="B675" t="inlineStr"/>
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>M041</t>
+        </is>
+      </c>
+      <c r="B675" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 6777058.20
+Borrower Amount: 6777058.20</t>
+        </is>
+      </c>
       <c r="C675" t="inlineStr"/>
       <c r="D675" t="inlineStr"/>
       <c r="E675" s="4" t="inlineStr">
@@ -16423,8 +17216,18 @@
       <c r="K675" t="inlineStr"/>
     </row>
     <row r="676">
-      <c r="A676" t="inlineStr"/>
-      <c r="B676" t="inlineStr"/>
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>M041</t>
+        </is>
+      </c>
+      <c r="B676" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 6777058.20
+Borrower Amount: 6777058.20</t>
+        </is>
+      </c>
       <c r="C676" t="inlineStr"/>
       <c r="D676" t="inlineStr"/>
       <c r="E676" s="4" t="inlineStr">
@@ -16440,8 +17243,18 @@
       <c r="K676" t="inlineStr"/>
     </row>
     <row r="677">
-      <c r="A677" t="inlineStr"/>
-      <c r="B677" t="inlineStr"/>
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>M041</t>
+        </is>
+      </c>
+      <c r="B677" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 6777058.20
+Borrower Amount: 6777058.20</t>
+        </is>
+      </c>
       <c r="C677" t="inlineStr"/>
       <c r="D677" t="inlineStr">
         <is>
@@ -16541,8 +17354,7 @@
       </c>
       <c r="B681" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-155823010186/23
+          <t>LC Match: L/C-155823010186/23
 Lender Amount: 76000.00
 Borrower Amount: 76000.00</t>
         </is>
@@ -16580,8 +17392,18 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" t="inlineStr"/>
-      <c r="B682" t="inlineStr"/>
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>M042</t>
+        </is>
+      </c>
+      <c r="B682" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-155823010186/23
+Lender Amount: 76000.00
+Borrower Amount: 76000.00</t>
+        </is>
+      </c>
       <c r="C682" t="inlineStr"/>
       <c r="D682" t="inlineStr"/>
       <c r="E682" s="4" t="inlineStr">
@@ -16599,8 +17421,18 @@
       <c r="K682" t="inlineStr"/>
     </row>
     <row r="683">
-      <c r="A683" t="inlineStr"/>
-      <c r="B683" t="inlineStr"/>
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>M042</t>
+        </is>
+      </c>
+      <c r="B683" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-155823010186/23
+Lender Amount: 76000.00
+Borrower Amount: 76000.00</t>
+        </is>
+      </c>
       <c r="C683" t="inlineStr"/>
       <c r="D683" t="inlineStr"/>
       <c r="E683" s="4" t="inlineStr">
@@ -16618,8 +17450,18 @@
       <c r="K683" t="inlineStr"/>
     </row>
     <row r="684">
-      <c r="A684" t="inlineStr"/>
-      <c r="B684" t="inlineStr"/>
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>M042</t>
+        </is>
+      </c>
+      <c r="B684" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-155823010186/23
+Lender Amount: 76000.00
+Borrower Amount: 76000.00</t>
+        </is>
+      </c>
       <c r="C684" t="inlineStr"/>
       <c r="D684" t="inlineStr"/>
       <c r="E684" s="4" t="inlineStr">
@@ -16635,8 +17477,18 @@
       <c r="K684" t="inlineStr"/>
     </row>
     <row r="685">
-      <c r="A685" t="inlineStr"/>
-      <c r="B685" t="inlineStr"/>
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>M042</t>
+        </is>
+      </c>
+      <c r="B685" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-155823010186/23
+Lender Amount: 76000.00
+Borrower Amount: 76000.00</t>
+        </is>
+      </c>
       <c r="C685" t="inlineStr"/>
       <c r="D685" t="inlineStr">
         <is>
@@ -16882,8 +17734,7 @@
       </c>
       <c r="B695" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-308524026037/222824023549
+          <t>LC Match: LC-308524026037/222824023549
 Lender Amount: 1226351.09
 Borrower Amount: 1226351.09</t>
         </is>
@@ -16921,8 +17772,18 @@
       <c r="K695" t="inlineStr"/>
     </row>
     <row r="696">
-      <c r="A696" t="inlineStr"/>
-      <c r="B696" t="inlineStr"/>
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>M043</t>
+        </is>
+      </c>
+      <c r="B696" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524026037/222824023549
+Lender Amount: 1226351.09
+Borrower Amount: 1226351.09</t>
+        </is>
+      </c>
       <c r="C696" t="inlineStr"/>
       <c r="D696" t="inlineStr"/>
       <c r="E696" s="4" t="inlineStr">
@@ -16938,8 +17799,18 @@
       <c r="K696" t="inlineStr"/>
     </row>
     <row r="697">
-      <c r="A697" t="inlineStr"/>
-      <c r="B697" t="inlineStr"/>
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>M043</t>
+        </is>
+      </c>
+      <c r="B697" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524026037/222824023549
+Lender Amount: 1226351.09
+Borrower Amount: 1226351.09</t>
+        </is>
+      </c>
       <c r="C697" t="inlineStr"/>
       <c r="D697" t="inlineStr">
         <is>
@@ -17039,8 +17910,7 @@
       </c>
       <c r="B701" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-308524022495/24
+          <t>LC Match: LC-308524022495/24
 Lender Amount: 1675000.00
 Borrower Amount: 1675000.00</t>
         </is>
@@ -17078,8 +17948,18 @@
       </c>
     </row>
     <row r="702">
-      <c r="A702" t="inlineStr"/>
-      <c r="B702" t="inlineStr"/>
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>M044</t>
+        </is>
+      </c>
+      <c r="B702" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524022495/24
+Lender Amount: 1675000.00
+Borrower Amount: 1675000.00</t>
+        </is>
+      </c>
       <c r="C702" t="inlineStr"/>
       <c r="D702" t="inlineStr"/>
       <c r="E702" s="4" t="inlineStr">
@@ -17095,8 +17975,18 @@
       <c r="K702" t="inlineStr"/>
     </row>
     <row r="703">
-      <c r="A703" t="inlineStr"/>
-      <c r="B703" t="inlineStr"/>
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>M044</t>
+        </is>
+      </c>
+      <c r="B703" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524022495/24
+Lender Amount: 1675000.00
+Borrower Amount: 1675000.00</t>
+        </is>
+      </c>
       <c r="C703" t="inlineStr"/>
       <c r="D703" t="inlineStr">
         <is>
@@ -17269,8 +18159,7 @@
       </c>
       <c r="B710" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-147125020027/25
+          <t>LC Match: L/C-147125020027/25
 Lender Amount: 10691988.92
 Borrower Amount: 10691988.92</t>
         </is>
@@ -17308,8 +18197,18 @@
       <c r="K710" t="inlineStr"/>
     </row>
     <row r="711">
-      <c r="A711" t="inlineStr"/>
-      <c r="B711" t="inlineStr"/>
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>M045</t>
+        </is>
+      </c>
+      <c r="B711" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020027/25
+Lender Amount: 10691988.92
+Borrower Amount: 10691988.92</t>
+        </is>
+      </c>
       <c r="C711" t="inlineStr"/>
       <c r="D711" t="inlineStr"/>
       <c r="E711" s="4" t="inlineStr">
@@ -17325,8 +18224,18 @@
       <c r="K711" t="inlineStr"/>
     </row>
     <row r="712">
-      <c r="A712" t="inlineStr"/>
-      <c r="B712" t="inlineStr"/>
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>M045</t>
+        </is>
+      </c>
+      <c r="B712" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020027/25
+Lender Amount: 10691988.92
+Borrower Amount: 10691988.92</t>
+        </is>
+      </c>
       <c r="C712" t="inlineStr"/>
       <c r="D712" t="inlineStr">
         <is>
@@ -17353,8 +18262,7 @@
       </c>
       <c r="B713" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-222825150151/25
+          <t>LC Match: L/C-222825150151/25
 Lender Amount: 333706.76
 Borrower Amount: 333706.76</t>
         </is>
@@ -17392,8 +18300,18 @@
       <c r="K713" t="inlineStr"/>
     </row>
     <row r="714">
-      <c r="A714" t="inlineStr"/>
-      <c r="B714" t="inlineStr"/>
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>M046</t>
+        </is>
+      </c>
+      <c r="B714" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-222825150151/25
+Lender Amount: 333706.76
+Borrower Amount: 333706.76</t>
+        </is>
+      </c>
       <c r="C714" t="inlineStr"/>
       <c r="D714" t="inlineStr"/>
       <c r="E714" s="4" t="inlineStr">
@@ -17409,8 +18327,18 @@
       <c r="K714" t="inlineStr"/>
     </row>
     <row r="715">
-      <c r="A715" t="inlineStr"/>
-      <c r="B715" t="inlineStr"/>
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>M046</t>
+        </is>
+      </c>
+      <c r="B715" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-222825150151/25
+Lender Amount: 333706.76
+Borrower Amount: 333706.76</t>
+        </is>
+      </c>
       <c r="C715" t="inlineStr"/>
       <c r="D715" t="inlineStr">
         <is>
@@ -17437,8 +18365,7 @@
       </c>
       <c r="B716" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020063/25
+          <t>LC Match: L/C-141325020063/25
 Lender Amount: 299000.00
 Borrower Amount: 299000.00</t>
         </is>
@@ -17476,8 +18403,18 @@
       </c>
     </row>
     <row r="717">
-      <c r="A717" t="inlineStr"/>
-      <c r="B717" t="inlineStr"/>
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>M047</t>
+        </is>
+      </c>
+      <c r="B717" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 299000.00
+Borrower Amount: 299000.00</t>
+        </is>
+      </c>
       <c r="C717" t="inlineStr"/>
       <c r="D717" t="inlineStr"/>
       <c r="E717" s="4" t="inlineStr">
@@ -17493,8 +18430,18 @@
       <c r="K717" t="inlineStr"/>
     </row>
     <row r="718">
-      <c r="A718" t="inlineStr"/>
-      <c r="B718" t="inlineStr"/>
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>M047</t>
+        </is>
+      </c>
+      <c r="B718" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 299000.00
+Borrower Amount: 299000.00</t>
+        </is>
+      </c>
       <c r="C718" t="inlineStr"/>
       <c r="D718" t="inlineStr">
         <is>
@@ -17594,8 +18541,7 @@
       </c>
       <c r="B722" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
+          <t>LC Match: L/C-308524026037/24
 Lender Amount: 13743.52
 Borrower Amount: 13743.52</t>
         </is>
@@ -17633,8 +18579,18 @@
       <c r="K722" t="inlineStr"/>
     </row>
     <row r="723">
-      <c r="A723" t="inlineStr"/>
-      <c r="B723" t="inlineStr"/>
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>M048</t>
+        </is>
+      </c>
+      <c r="B723" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524026037/24
+Lender Amount: 13743.52
+Borrower Amount: 13743.52</t>
+        </is>
+      </c>
       <c r="C723" t="inlineStr"/>
       <c r="D723" t="inlineStr"/>
       <c r="E723" s="4" t="inlineStr">
@@ -17650,8 +18606,18 @@
       <c r="K723" t="inlineStr"/>
     </row>
     <row r="724">
-      <c r="A724" t="inlineStr"/>
-      <c r="B724" t="inlineStr"/>
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>M048</t>
+        </is>
+      </c>
+      <c r="B724" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524026037/24
+Lender Amount: 13743.52
+Borrower Amount: 13743.52</t>
+        </is>
+      </c>
       <c r="C724" t="inlineStr"/>
       <c r="D724" t="inlineStr">
         <is>
@@ -17919,8 +18885,7 @@
       </c>
       <c r="B736" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-155825020020/25
+          <t>LC Match: LC-155825020020/25
 Lender Amount: 60302.55
 Borrower Amount: 60302.55</t>
         </is>
@@ -17958,8 +18923,18 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" t="inlineStr"/>
-      <c r="B737" t="inlineStr"/>
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>M049</t>
+        </is>
+      </c>
+      <c r="B737" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155825020020/25
+Lender Amount: 60302.55
+Borrower Amount: 60302.55</t>
+        </is>
+      </c>
       <c r="C737" t="inlineStr"/>
       <c r="D737" t="inlineStr"/>
       <c r="E737" s="4" t="inlineStr">
@@ -17975,8 +18950,18 @@
       <c r="K737" t="inlineStr"/>
     </row>
     <row r="738">
-      <c r="A738" t="inlineStr"/>
-      <c r="B738" t="inlineStr"/>
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>M049</t>
+        </is>
+      </c>
+      <c r="B738" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155825020020/25
+Lender Amount: 60302.55
+Borrower Amount: 60302.55</t>
+        </is>
+      </c>
       <c r="C738" t="inlineStr"/>
       <c r="D738" t="inlineStr">
         <is>
@@ -18003,8 +18988,7 @@
       </c>
       <c r="B739" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
+          <t>LC Match: L/C-141325020104/25
 Lender Amount: 124008.78
 Borrower Amount: 124008.78</t>
         </is>
@@ -18042,8 +19026,18 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" t="inlineStr"/>
-      <c r="B740" t="inlineStr"/>
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>M050</t>
+        </is>
+      </c>
+      <c r="B740" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 124008.78
+Borrower Amount: 124008.78</t>
+        </is>
+      </c>
       <c r="C740" t="inlineStr"/>
       <c r="D740" t="inlineStr"/>
       <c r="E740" s="4" t="inlineStr">
@@ -18059,8 +19053,18 @@
       <c r="K740" t="inlineStr"/>
     </row>
     <row r="741">
-      <c r="A741" t="inlineStr"/>
-      <c r="B741" t="inlineStr"/>
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>M050</t>
+        </is>
+      </c>
+      <c r="B741" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 124008.78
+Borrower Amount: 124008.78</t>
+        </is>
+      </c>
       <c r="C741" t="inlineStr"/>
       <c r="D741" t="inlineStr">
         <is>
@@ -18087,8 +19091,7 @@
       </c>
       <c r="B742" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
+          <t>LC Match: LC-141325020063/25
 Lender Amount: 31609.80
 Borrower Amount: 31609.80</t>
         </is>
@@ -18126,8 +19129,18 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" t="inlineStr"/>
-      <c r="B743" t="inlineStr"/>
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>M051</t>
+        </is>
+      </c>
+      <c r="B743" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/25
+Lender Amount: 31609.80
+Borrower Amount: 31609.80</t>
+        </is>
+      </c>
       <c r="C743" t="inlineStr"/>
       <c r="D743" t="inlineStr"/>
       <c r="E743" s="4" t="inlineStr">
@@ -18143,8 +19156,18 @@
       <c r="K743" t="inlineStr"/>
     </row>
     <row r="744">
-      <c r="A744" t="inlineStr"/>
-      <c r="B744" t="inlineStr"/>
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>M051</t>
+        </is>
+      </c>
+      <c r="B744" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/25
+Lender Amount: 31609.80
+Borrower Amount: 31609.80</t>
+        </is>
+      </c>
       <c r="C744" t="inlineStr"/>
       <c r="D744" t="inlineStr">
         <is>
@@ -18574,8 +19597,7 @@
       </c>
       <c r="B762" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020104/25
+          <t>LC Match: L/C-141325020104/25
 Lender Amount: 10424886.36
 Borrower Amount: 10424886.36</t>
         </is>
@@ -18613,8 +19635,18 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" t="inlineStr"/>
-      <c r="B763" t="inlineStr"/>
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>M052</t>
+        </is>
+      </c>
+      <c r="B763" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 10424886.36
+Borrower Amount: 10424886.36</t>
+        </is>
+      </c>
       <c r="C763" t="inlineStr"/>
       <c r="D763" t="inlineStr"/>
       <c r="E763" s="4" t="inlineStr">
@@ -18630,8 +19662,18 @@
       <c r="K763" t="inlineStr"/>
     </row>
     <row r="764">
-      <c r="A764" t="inlineStr"/>
-      <c r="B764" t="inlineStr"/>
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>M052</t>
+        </is>
+      </c>
+      <c r="B764" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 10424886.36
+Borrower Amount: 10424886.36</t>
+        </is>
+      </c>
       <c r="C764" t="inlineStr"/>
       <c r="D764" t="inlineStr">
         <is>
@@ -18658,8 +19700,7 @@
       </c>
       <c r="B765" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-147125020063/25
+          <t>LC Match: L/C-147125020063/25
 Lender Amount: 2168751.40
 Borrower Amount: 2168751.40</t>
         </is>
@@ -18697,8 +19738,18 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" t="inlineStr"/>
-      <c r="B766" t="inlineStr"/>
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>M053</t>
+        </is>
+      </c>
+      <c r="B766" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020063/25
+Lender Amount: 2168751.40
+Borrower Amount: 2168751.40</t>
+        </is>
+      </c>
       <c r="C766" t="inlineStr"/>
       <c r="D766" t="inlineStr"/>
       <c r="E766" s="4" t="inlineStr">
@@ -18714,8 +19765,18 @@
       <c r="K766" t="inlineStr"/>
     </row>
     <row r="767">
-      <c r="A767" t="inlineStr"/>
-      <c r="B767" t="inlineStr"/>
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>M053</t>
+        </is>
+      </c>
+      <c r="B767" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020063/25
+Lender Amount: 2168751.40
+Borrower Amount: 2168751.40</t>
+        </is>
+      </c>
       <c r="C767" t="inlineStr"/>
       <c r="D767" t="inlineStr">
         <is>
@@ -18815,8 +19876,7 @@
       </c>
       <c r="B771" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-141325020068/25
+          <t>LC Match: L/C-141325020068/25
 Lender Amount: 63787.54
 Borrower Amount: 63787.54</t>
         </is>
@@ -18854,8 +19914,18 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" t="inlineStr"/>
-      <c r="B772" t="inlineStr"/>
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
+      <c r="B772" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020068/25
+Lender Amount: 63787.54
+Borrower Amount: 63787.54</t>
+        </is>
+      </c>
       <c r="C772" t="inlineStr"/>
       <c r="D772" t="inlineStr"/>
       <c r="E772" s="4" t="inlineStr">
@@ -18871,8 +19941,18 @@
       <c r="K772" t="inlineStr"/>
     </row>
     <row r="773">
-      <c r="A773" t="inlineStr"/>
-      <c r="B773" t="inlineStr"/>
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
+      <c r="B773" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020068/25
+Lender Amount: 63787.54
+Borrower Amount: 63787.54</t>
+        </is>
+      </c>
       <c r="C773" t="inlineStr"/>
       <c r="D773" t="inlineStr">
         <is>
@@ -22282,8 +23362,7 @@
       </c>
       <c r="B920" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020104/25
+          <t>LC Match: LC-141325020104/25
 Lender Amount: 111771.42
 Borrower Amount: 111771.42</t>
         </is>
@@ -22321,8 +23400,18 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" t="inlineStr"/>
-      <c r="B921" t="inlineStr"/>
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>M055</t>
+        </is>
+      </c>
+      <c r="B921" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020104/25
+Lender Amount: 111771.42
+Borrower Amount: 111771.42</t>
+        </is>
+      </c>
       <c r="C921" t="inlineStr"/>
       <c r="D921" t="inlineStr"/>
       <c r="E921" s="4" t="inlineStr">
@@ -22338,8 +23427,18 @@
       <c r="K921" t="inlineStr"/>
     </row>
     <row r="922">
-      <c r="A922" t="inlineStr"/>
-      <c r="B922" t="inlineStr"/>
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>M055</t>
+        </is>
+      </c>
+      <c r="B922" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020104/25
+Lender Amount: 111771.42
+Borrower Amount: 111771.42</t>
+        </is>
+      </c>
       <c r="C922" t="inlineStr"/>
       <c r="D922" t="inlineStr">
         <is>
@@ -22366,8 +23465,7 @@
       </c>
       <c r="B923" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020112/25
+          <t>LC Match: LC-141325020112/25
 Lender Amount: 80701.76
 Borrower Amount: 80701.76</t>
         </is>
@@ -22405,8 +23503,18 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" t="inlineStr"/>
-      <c r="B924" t="inlineStr"/>
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>M056</t>
+        </is>
+      </c>
+      <c r="B924" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020112/25
+Lender Amount: 80701.76
+Borrower Amount: 80701.76</t>
+        </is>
+      </c>
       <c r="C924" t="inlineStr"/>
       <c r="D924" t="inlineStr"/>
       <c r="E924" s="4" t="inlineStr">
@@ -22422,8 +23530,18 @@
       <c r="K924" t="inlineStr"/>
     </row>
     <row r="925">
-      <c r="A925" t="inlineStr"/>
-      <c r="B925" t="inlineStr"/>
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>M056</t>
+        </is>
+      </c>
+      <c r="B925" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020112/25
+Lender Amount: 80701.76
+Borrower Amount: 80701.76</t>
+        </is>
+      </c>
       <c r="C925" t="inlineStr"/>
       <c r="D925" t="inlineStr">
         <is>
@@ -22450,8 +23568,7 @@
       </c>
       <c r="B926" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020112/25
+          <t>LC Match: LC-141325020112/25
 Lender Amount: 657.81
 Borrower Amount: 657.81</t>
         </is>
@@ -22489,8 +23606,18 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" t="inlineStr"/>
-      <c r="B927" t="inlineStr"/>
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>M057</t>
+        </is>
+      </c>
+      <c r="B927" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020112/25
+Lender Amount: 657.81
+Borrower Amount: 657.81</t>
+        </is>
+      </c>
       <c r="C927" t="inlineStr"/>
       <c r="D927" t="inlineStr"/>
       <c r="E927" s="4" t="inlineStr">
@@ -22506,8 +23633,18 @@
       <c r="K927" t="inlineStr"/>
     </row>
     <row r="928">
-      <c r="A928" t="inlineStr"/>
-      <c r="B928" t="inlineStr"/>
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>M057</t>
+        </is>
+      </c>
+      <c r="B928" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020112/25
+Lender Amount: 657.81
+Borrower Amount: 657.81</t>
+        </is>
+      </c>
       <c r="C928" t="inlineStr"/>
       <c r="D928" t="inlineStr">
         <is>
@@ -22826,8 +23963,7 @@
       </c>
       <c r="B941" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020063/25
+          <t>LC Match: LC-141325020063/25
 Lender Amount: 81730.06
 Borrower Amount: 81730.06</t>
         </is>
@@ -22865,8 +24001,18 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" t="inlineStr"/>
-      <c r="B942" t="inlineStr"/>
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>M058</t>
+        </is>
+      </c>
+      <c r="B942" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/25
+Lender Amount: 81730.06
+Borrower Amount: 81730.06</t>
+        </is>
+      </c>
       <c r="C942" t="inlineStr"/>
       <c r="D942" t="inlineStr"/>
       <c r="E942" s="4" t="inlineStr">
@@ -22882,8 +24028,18 @@
       <c r="K942" t="inlineStr"/>
     </row>
     <row r="943">
-      <c r="A943" t="inlineStr"/>
-      <c r="B943" t="inlineStr"/>
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>M058</t>
+        </is>
+      </c>
+      <c r="B943" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/25
+Lender Amount: 81730.06
+Borrower Amount: 81730.06</t>
+        </is>
+      </c>
       <c r="C943" t="inlineStr"/>
       <c r="D943" t="inlineStr">
         <is>
@@ -23275,8 +24431,7 @@
       </c>
       <c r="B959" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020163/25
+          <t>LC Match: LC-141325020163/25
 Lender Amount: 341847.68
 Borrower Amount: 341847.68</t>
         </is>
@@ -23314,8 +24469,18 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" t="inlineStr"/>
-      <c r="B960" t="inlineStr"/>
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>M059</t>
+        </is>
+      </c>
+      <c r="B960" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020163/25
+Lender Amount: 341847.68
+Borrower Amount: 341847.68</t>
+        </is>
+      </c>
       <c r="C960" t="inlineStr"/>
       <c r="D960" t="inlineStr"/>
       <c r="E960" s="4" t="inlineStr">
@@ -23333,8 +24498,18 @@
       <c r="K960" t="inlineStr"/>
     </row>
     <row r="961">
-      <c r="A961" t="inlineStr"/>
-      <c r="B961" t="inlineStr"/>
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>M059</t>
+        </is>
+      </c>
+      <c r="B961" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020163/25
+Lender Amount: 341847.68
+Borrower Amount: 341847.68</t>
+        </is>
+      </c>
       <c r="C961" t="inlineStr"/>
       <c r="D961" t="inlineStr"/>
       <c r="E961" s="4" t="inlineStr">
@@ -23352,8 +24527,18 @@
       <c r="K961" t="inlineStr"/>
     </row>
     <row r="962">
-      <c r="A962" t="inlineStr"/>
-      <c r="B962" t="inlineStr"/>
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>M059</t>
+        </is>
+      </c>
+      <c r="B962" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020163/25
+Lender Amount: 341847.68
+Borrower Amount: 341847.68</t>
+        </is>
+      </c>
       <c r="C962" t="inlineStr"/>
       <c r="D962" t="inlineStr"/>
       <c r="E962" s="4" t="inlineStr">
@@ -23369,8 +24554,18 @@
       <c r="K962" t="inlineStr"/>
     </row>
     <row r="963">
-      <c r="A963" t="inlineStr"/>
-      <c r="B963" t="inlineStr"/>
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>M059</t>
+        </is>
+      </c>
+      <c r="B963" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020163/25
+Lender Amount: 341847.68
+Borrower Amount: 341847.68</t>
+        </is>
+      </c>
       <c r="C963" t="inlineStr"/>
       <c r="D963" t="inlineStr">
         <is>
@@ -23581,8 +24776,7 @@
       </c>
       <c r="B972" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-222825150235/25
+          <t>LC Match: LC-222825150235/25
 Lender Amount: 36757.00
 Borrower Amount: 36757.00</t>
         </is>
@@ -23620,8 +24814,18 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" t="inlineStr"/>
-      <c r="B973" t="inlineStr"/>
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>M060</t>
+        </is>
+      </c>
+      <c r="B973" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-222825150235/25
+Lender Amount: 36757.00
+Borrower Amount: 36757.00</t>
+        </is>
+      </c>
       <c r="C973" t="inlineStr"/>
       <c r="D973" t="inlineStr"/>
       <c r="E973" s="4" t="inlineStr">
@@ -23637,8 +24841,18 @@
       <c r="K973" t="inlineStr"/>
     </row>
     <row r="974">
-      <c r="A974" t="inlineStr"/>
-      <c r="B974" t="inlineStr"/>
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>M060</t>
+        </is>
+      </c>
+      <c r="B974" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-222825150235/25
+Lender Amount: 36757.00
+Borrower Amount: 36757.00</t>
+        </is>
+      </c>
       <c r="C974" t="inlineStr"/>
       <c r="D974" t="inlineStr">
         <is>
@@ -23738,8 +24952,7 @@
       </c>
       <c r="B978" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020068/25
+          <t>LC Match: LC-141325020068/25
 Lender Amount: 3587219.00
 Borrower Amount: 3587219.00</t>
         </is>
@@ -23777,8 +24990,18 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" t="inlineStr"/>
-      <c r="B979" t="inlineStr"/>
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>M061</t>
+        </is>
+      </c>
+      <c r="B979" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020068/25
+Lender Amount: 3587219.00
+Borrower Amount: 3587219.00</t>
+        </is>
+      </c>
       <c r="C979" t="inlineStr"/>
       <c r="D979" t="inlineStr"/>
       <c r="E979" s="4" t="inlineStr">
@@ -23796,8 +25019,18 @@
       <c r="K979" t="inlineStr"/>
     </row>
     <row r="980">
-      <c r="A980" t="inlineStr"/>
-      <c r="B980" t="inlineStr"/>
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>M061</t>
+        </is>
+      </c>
+      <c r="B980" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020068/25
+Lender Amount: 3587219.00
+Borrower Amount: 3587219.00</t>
+        </is>
+      </c>
       <c r="C980" t="inlineStr"/>
       <c r="D980" t="inlineStr"/>
       <c r="E980" s="4" t="inlineStr">
@@ -23815,8 +25048,18 @@
       <c r="K980" t="inlineStr"/>
     </row>
     <row r="981">
-      <c r="A981" t="inlineStr"/>
-      <c r="B981" t="inlineStr"/>
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>M061</t>
+        </is>
+      </c>
+      <c r="B981" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020068/25
+Lender Amount: 3587219.00
+Borrower Amount: 3587219.00</t>
+        </is>
+      </c>
       <c r="C981" t="inlineStr"/>
       <c r="D981" t="inlineStr"/>
       <c r="E981" s="4" t="inlineStr">
@@ -23834,8 +25077,18 @@
       <c r="K981" t="inlineStr"/>
     </row>
     <row r="982">
-      <c r="A982" t="inlineStr"/>
-      <c r="B982" t="inlineStr"/>
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>M061</t>
+        </is>
+      </c>
+      <c r="B982" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020068/25
+Lender Amount: 3587219.00
+Borrower Amount: 3587219.00</t>
+        </is>
+      </c>
       <c r="C982" t="inlineStr"/>
       <c r="D982" t="inlineStr"/>
       <c r="E982" s="4" t="inlineStr">
@@ -23851,8 +25104,18 @@
       <c r="K982" t="inlineStr"/>
     </row>
     <row r="983">
-      <c r="A983" t="inlineStr"/>
-      <c r="B983" t="inlineStr"/>
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>M061</t>
+        </is>
+      </c>
+      <c r="B983" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020068/25
+Lender Amount: 3587219.00
+Borrower Amount: 3587219.00</t>
+        </is>
+      </c>
       <c r="C983" t="inlineStr"/>
       <c r="D983" t="inlineStr">
         <is>
@@ -23879,8 +25142,7 @@
       </c>
       <c r="B984" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-308524990243/24
+          <t>LC Match: LC-308524990243/24
 Lender Amount: 68747.06
 Borrower Amount: 68747.06</t>
         </is>
@@ -23918,8 +25180,18 @@
       <c r="K984" t="inlineStr"/>
     </row>
     <row r="985">
-      <c r="A985" t="inlineStr"/>
-      <c r="B985" t="inlineStr"/>
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>M062</t>
+        </is>
+      </c>
+      <c r="B985" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524990243/24
+Lender Amount: 68747.06
+Borrower Amount: 68747.06</t>
+        </is>
+      </c>
       <c r="C985" t="inlineStr"/>
       <c r="D985" t="inlineStr"/>
       <c r="E985" s="4" t="inlineStr">
@@ -23935,8 +25207,18 @@
       <c r="K985" t="inlineStr"/>
     </row>
     <row r="986">
-      <c r="A986" t="inlineStr"/>
-      <c r="B986" t="inlineStr"/>
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>M062</t>
+        </is>
+      </c>
+      <c r="B986" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524990243/24
+Lender Amount: 68747.06
+Borrower Amount: 68747.06</t>
+        </is>
+      </c>
       <c r="C986" t="inlineStr"/>
       <c r="D986" t="inlineStr">
         <is>
@@ -24497,8 +25779,7 @@
       </c>
       <c r="B1010" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-308525021741/25
+          <t>LC Match: LC-308525021741/25
 Lender Amount: 31411.11
 Borrower Amount: 31411.11</t>
         </is>
@@ -24536,8 +25817,18 @@
       <c r="K1010" t="inlineStr"/>
     </row>
     <row r="1011">
-      <c r="A1011" t="inlineStr"/>
-      <c r="B1011" t="inlineStr"/>
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>M063</t>
+        </is>
+      </c>
+      <c r="B1011" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308525021741/25
+Lender Amount: 31411.11
+Borrower Amount: 31411.11</t>
+        </is>
+      </c>
       <c r="C1011" t="inlineStr"/>
       <c r="D1011" t="inlineStr"/>
       <c r="E1011" s="4" t="inlineStr">
@@ -24553,8 +25844,18 @@
       <c r="K1011" t="inlineStr"/>
     </row>
     <row r="1012">
-      <c r="A1012" t="inlineStr"/>
-      <c r="B1012" t="inlineStr"/>
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>M063</t>
+        </is>
+      </c>
+      <c r="B1012" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308525021741/25
+Lender Amount: 31411.11
+Borrower Amount: 31411.11</t>
+        </is>
+      </c>
       <c r="C1012" t="inlineStr"/>
       <c r="D1012" t="inlineStr">
         <is>
@@ -25020,8 +26321,7 @@
       </c>
       <c r="B1031" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-155825010037/25
+          <t>LC Match: LC-155825010037/25
 Lender Amount: 853297.01
 Borrower Amount: 853297.01</t>
         </is>
@@ -25059,8 +26359,18 @@
       <c r="K1031" t="inlineStr"/>
     </row>
     <row r="1032">
-      <c r="A1032" t="inlineStr"/>
-      <c r="B1032" t="inlineStr"/>
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>M064</t>
+        </is>
+      </c>
+      <c r="B1032" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155825010037/25
+Lender Amount: 853297.01
+Borrower Amount: 853297.01</t>
+        </is>
+      </c>
       <c r="C1032" t="inlineStr"/>
       <c r="D1032" t="inlineStr"/>
       <c r="E1032" s="4" t="inlineStr">
@@ -25076,8 +26386,18 @@
       <c r="K1032" t="inlineStr"/>
     </row>
     <row r="1033">
-      <c r="A1033" t="inlineStr"/>
-      <c r="B1033" t="inlineStr"/>
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>M064</t>
+        </is>
+      </c>
+      <c r="B1033" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155825010037/25
+Lender Amount: 853297.01
+Borrower Amount: 853297.01</t>
+        </is>
+      </c>
       <c r="C1033" t="inlineStr"/>
       <c r="D1033" t="inlineStr">
         <is>
@@ -26694,8 +28014,7 @@
       </c>
       <c r="B1100" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020163/25
+          <t>LC Match: LC-141325020163/25
 Lender Amount: 1725.00
 Borrower Amount: 1725.00</t>
         </is>
@@ -26733,8 +28052,18 @@
       </c>
     </row>
     <row r="1101">
-      <c r="A1101" t="inlineStr"/>
-      <c r="B1101" t="inlineStr"/>
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>M065</t>
+        </is>
+      </c>
+      <c r="B1101" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020163/25
+Lender Amount: 1725.00
+Borrower Amount: 1725.00</t>
+        </is>
+      </c>
       <c r="C1101" t="inlineStr"/>
       <c r="D1101" t="inlineStr"/>
       <c r="E1101" s="4" t="inlineStr">
@@ -26750,8 +28079,18 @@
       <c r="K1101" t="inlineStr"/>
     </row>
     <row r="1102">
-      <c r="A1102" t="inlineStr"/>
-      <c r="B1102" t="inlineStr"/>
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>M065</t>
+        </is>
+      </c>
+      <c r="B1102" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020163/25
+Lender Amount: 1725.00
+Borrower Amount: 1725.00</t>
+        </is>
+      </c>
       <c r="C1102" t="inlineStr"/>
       <c r="D1102" t="inlineStr">
         <is>
@@ -26778,8 +28117,7 @@
       </c>
       <c r="B1103" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-308525021746/25
+          <t>LC Match: LC-308525021746/25
 Lender Amount: 35373.50
 Borrower Amount: 35373.50</t>
         </is>
@@ -26817,8 +28155,18 @@
       <c r="K1103" t="inlineStr"/>
     </row>
     <row r="1104">
-      <c r="A1104" t="inlineStr"/>
-      <c r="B1104" t="inlineStr"/>
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>M066</t>
+        </is>
+      </c>
+      <c r="B1104" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308525021746/25
+Lender Amount: 35373.50
+Borrower Amount: 35373.50</t>
+        </is>
+      </c>
       <c r="C1104" t="inlineStr"/>
       <c r="D1104" t="inlineStr"/>
       <c r="E1104" s="4" t="inlineStr">
@@ -26834,8 +28182,18 @@
       <c r="K1104" t="inlineStr"/>
     </row>
     <row r="1105">
-      <c r="A1105" t="inlineStr"/>
-      <c r="B1105" t="inlineStr"/>
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>M066</t>
+        </is>
+      </c>
+      <c r="B1105" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308525021746/25
+Lender Amount: 35373.50
+Borrower Amount: 35373.50</t>
+        </is>
+      </c>
       <c r="C1105" t="inlineStr"/>
       <c r="D1105" t="inlineStr">
         <is>
@@ -27338,8 +28696,7 @@
       </c>
       <c r="B1126" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-141325020063/141325020112
+          <t>LC Match: LC-141325020063/141325020112
 Lender Amount: 576120.39
 Borrower Amount: 576120.39</t>
         </is>
@@ -27377,8 +28734,18 @@
       <c r="K1126" t="inlineStr"/>
     </row>
     <row r="1127">
-      <c r="A1127" t="inlineStr"/>
-      <c r="B1127" t="inlineStr"/>
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>M067</t>
+        </is>
+      </c>
+      <c r="B1127" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/141325020112
+Lender Amount: 576120.39
+Borrower Amount: 576120.39</t>
+        </is>
+      </c>
       <c r="C1127" t="inlineStr"/>
       <c r="D1127" t="inlineStr"/>
       <c r="E1127" s="4" t="inlineStr">
@@ -27396,8 +28763,18 @@
       </c>
     </row>
     <row r="1128">
-      <c r="A1128" t="inlineStr"/>
-      <c r="B1128" t="inlineStr"/>
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>M067</t>
+        </is>
+      </c>
+      <c r="B1128" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/141325020112
+Lender Amount: 576120.39
+Borrower Amount: 576120.39</t>
+        </is>
+      </c>
       <c r="C1128" t="inlineStr"/>
       <c r="D1128" t="inlineStr"/>
       <c r="E1128" s="4" t="inlineStr">
@@ -27415,8 +28792,18 @@
       </c>
     </row>
     <row r="1129">
-      <c r="A1129" t="inlineStr"/>
-      <c r="B1129" t="inlineStr"/>
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>M067</t>
+        </is>
+      </c>
+      <c r="B1129" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/141325020112
+Lender Amount: 576120.39
+Borrower Amount: 576120.39</t>
+        </is>
+      </c>
       <c r="C1129" t="inlineStr"/>
       <c r="D1129" t="inlineStr"/>
       <c r="E1129" s="4" t="inlineStr">
@@ -27434,8 +28821,18 @@
       </c>
     </row>
     <row r="1130">
-      <c r="A1130" t="inlineStr"/>
-      <c r="B1130" t="inlineStr"/>
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>M067</t>
+        </is>
+      </c>
+      <c r="B1130" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/141325020112
+Lender Amount: 576120.39
+Borrower Amount: 576120.39</t>
+        </is>
+      </c>
       <c r="C1130" t="inlineStr"/>
       <c r="D1130" t="inlineStr"/>
       <c r="E1130" s="4" t="inlineStr">
@@ -27453,8 +28850,18 @@
       </c>
     </row>
     <row r="1131">
-      <c r="A1131" t="inlineStr"/>
-      <c r="B1131" t="inlineStr"/>
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>M067</t>
+        </is>
+      </c>
+      <c r="B1131" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/141325020112
+Lender Amount: 576120.39
+Borrower Amount: 576120.39</t>
+        </is>
+      </c>
       <c r="C1131" t="inlineStr"/>
       <c r="D1131" t="inlineStr"/>
       <c r="E1131" s="4" t="inlineStr">
@@ -27470,8 +28877,18 @@
       <c r="K1131" t="inlineStr"/>
     </row>
     <row r="1132">
-      <c r="A1132" t="inlineStr"/>
-      <c r="B1132" t="inlineStr"/>
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>M067</t>
+        </is>
+      </c>
+      <c r="B1132" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/141325020112
+Lender Amount: 576120.39
+Borrower Amount: 576120.39</t>
+        </is>
+      </c>
       <c r="C1132" t="inlineStr"/>
       <c r="D1132" t="inlineStr">
         <is>
@@ -27498,8 +28915,7 @@
       </c>
       <c r="B1133" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-308524022166 
+          <t>LC Match: LC-308524022166 
 Lender Amount: 758000.00
 Borrower Amount: 758000.00</t>
         </is>
@@ -27537,8 +28953,18 @@
       </c>
     </row>
     <row r="1134">
-      <c r="A1134" t="inlineStr"/>
-      <c r="B1134" t="inlineStr"/>
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>M068</t>
+        </is>
+      </c>
+      <c r="B1134" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524022166 
+Lender Amount: 758000.00
+Borrower Amount: 758000.00</t>
+        </is>
+      </c>
       <c r="C1134" t="inlineStr"/>
       <c r="D1134" t="inlineStr"/>
       <c r="E1134" s="4" t="inlineStr">
@@ -27554,8 +28980,18 @@
       <c r="K1134" t="inlineStr"/>
     </row>
     <row r="1135">
-      <c r="A1135" t="inlineStr"/>
-      <c r="B1135" t="inlineStr"/>
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>M068</t>
+        </is>
+      </c>
+      <c r="B1135" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524022166 
+Lender Amount: 758000.00
+Borrower Amount: 758000.00</t>
+        </is>
+      </c>
       <c r="C1135" t="inlineStr"/>
       <c r="D1135" t="inlineStr">
         <is>
@@ -28166,8 +29602,7 @@
       </c>
       <c r="B1160" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-LC-308524022166 
+          <t>LC Match: LC-308524022166 
 Lender Amount: 4009000.00
 Borrower Amount: 4009000.00</t>
         </is>
@@ -28205,8 +29640,18 @@
       </c>
     </row>
     <row r="1161">
-      <c r="A1161" t="inlineStr"/>
-      <c r="B1161" t="inlineStr"/>
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>M069</t>
+        </is>
+      </c>
+      <c r="B1161" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524022166 
+Lender Amount: 4009000.00
+Borrower Amount: 4009000.00</t>
+        </is>
+      </c>
       <c r="C1161" t="inlineStr"/>
       <c r="D1161" t="inlineStr"/>
       <c r="E1161" s="4" t="inlineStr">
@@ -28222,8 +29667,18 @@
       <c r="K1161" t="inlineStr"/>
     </row>
     <row r="1162">
-      <c r="A1162" t="inlineStr"/>
-      <c r="B1162" t="inlineStr"/>
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>M069</t>
+        </is>
+      </c>
+      <c r="B1162" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524022166 
+Lender Amount: 4009000.00
+Borrower Amount: 4009000.00</t>
+        </is>
+      </c>
       <c r="C1162" t="inlineStr"/>
       <c r="D1162" t="inlineStr">
         <is>
@@ -28396,8 +29851,7 @@
       </c>
       <c r="B1169" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-308524026037/24
+          <t>LC Match: L/C-308524026037/24
 Lender Amount: 14417.98
 Borrower Amount: 14417.98</t>
         </is>
@@ -28435,8 +29889,18 @@
       <c r="K1169" t="inlineStr"/>
     </row>
     <row r="1170">
-      <c r="A1170" t="inlineStr"/>
-      <c r="B1170" t="inlineStr"/>
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>M070</t>
+        </is>
+      </c>
+      <c r="B1170" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524026037/24
+Lender Amount: 14417.98
+Borrower Amount: 14417.98</t>
+        </is>
+      </c>
       <c r="C1170" t="inlineStr"/>
       <c r="D1170" t="inlineStr"/>
       <c r="E1170" s="4" t="inlineStr">
@@ -28452,8 +29916,18 @@
       <c r="K1170" t="inlineStr"/>
     </row>
     <row r="1171">
-      <c r="A1171" t="inlineStr"/>
-      <c r="B1171" t="inlineStr"/>
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>M070</t>
+        </is>
+      </c>
+      <c r="B1171" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524026037/24
+Lender Amount: 14417.98
+Borrower Amount: 14417.98</t>
+        </is>
+      </c>
       <c r="C1171" t="inlineStr"/>
       <c r="D1171" t="inlineStr">
         <is>
@@ -29064,8 +30538,7 @@
       </c>
       <c r="B1196" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-147125020202/25
+          <t>LC Match: L/C-147125020202/25
 Lender Amount: 3499168.01
 Borrower Amount: 3499168.01</t>
         </is>
@@ -29103,8 +30576,18 @@
       <c r="K1196" t="inlineStr"/>
     </row>
     <row r="1197">
-      <c r="A1197" t="inlineStr"/>
-      <c r="B1197" t="inlineStr"/>
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>M071</t>
+        </is>
+      </c>
+      <c r="B1197" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020202/25
+Lender Amount: 3499168.01
+Borrower Amount: 3499168.01</t>
+        </is>
+      </c>
       <c r="C1197" t="inlineStr"/>
       <c r="D1197" t="inlineStr"/>
       <c r="E1197" s="4" t="inlineStr">
@@ -29120,8 +30603,18 @@
       <c r="K1197" t="inlineStr"/>
     </row>
     <row r="1198">
-      <c r="A1198" t="inlineStr"/>
-      <c r="B1198" t="inlineStr"/>
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>M071</t>
+        </is>
+      </c>
+      <c r="B1198" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020202/25
+Lender Amount: 3499168.01
+Borrower Amount: 3499168.01</t>
+        </is>
+      </c>
       <c r="C1198" t="inlineStr"/>
       <c r="D1198" t="inlineStr">
         <is>
@@ -29576,8 +31069,7 @@
       </c>
       <c r="B1219" s="4" t="inlineStr">
         <is>
-          <t>Match Type: LC Match
-L/C-147124020074/24
+          <t>LC Match: L/C-147124020074/24
 Lender Amount: 6242871.55
 Borrower Amount: 6242871.55</t>
         </is>
@@ -29615,8 +31107,18 @@
       <c r="K1219" t="inlineStr"/>
     </row>
     <row r="1220">
-      <c r="A1220" t="inlineStr"/>
-      <c r="B1220" t="inlineStr"/>
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>M072</t>
+        </is>
+      </c>
+      <c r="B1220" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020074/24
+Lender Amount: 6242871.55
+Borrower Amount: 6242871.55</t>
+        </is>
+      </c>
       <c r="C1220" t="inlineStr"/>
       <c r="D1220" t="inlineStr"/>
       <c r="E1220" s="4" t="inlineStr">
@@ -29632,8 +31134,18 @@
       <c r="K1220" t="inlineStr"/>
     </row>
     <row r="1221">
-      <c r="A1221" t="inlineStr"/>
-      <c r="B1221" t="inlineStr"/>
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>M072</t>
+        </is>
+      </c>
+      <c r="B1221" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020074/24
+Lender Amount: 6242871.55
+Borrower Amount: 6242871.55</t>
+        </is>
+      </c>
       <c r="C1221" t="inlineStr"/>
       <c r="D1221" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Refactor transaction matching logic to implement new criteria: Match ID assigned only when amounts, transaction types, and 'Entered By' names match. Removed alternative DataFrame creation and adjusted Audit Info population to only the second-to-last row of transaction blocks.
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -1542,13 +1542,7 @@
           <t>M001</t>
         </is>
       </c>
-      <c r="B53" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 5040781.68
-Borrower Amount: 5040781.68</t>
-        </is>
-      </c>
+      <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
         <is>
           <t>01/Jan/2025</t>
@@ -1614,13 +1608,7 @@
           <t>M001</t>
         </is>
       </c>
-      <c r="B55" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 5040781.68
-Borrower Amount: 5040781.68</t>
-        </is>
-      </c>
+      <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
@@ -1640,18 +1628,8 @@
       <c r="K55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
-      <c r="B56" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
           <t>01/Jan/2025</t>
@@ -1685,18 +1663,8 @@
       <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
-      <c r="B57" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
       <c r="E57" s="4" t="inlineStr">
@@ -1714,18 +1682,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
-      <c r="B58" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" s="4" t="inlineStr">
@@ -1743,18 +1701,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
-      <c r="B59" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" s="4" t="inlineStr">
@@ -1772,18 +1720,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
-      <c r="B60" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" s="4" t="inlineStr">
@@ -1799,18 +1737,8 @@
       <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
-      <c r="B61" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 15737222.22
-Borrower Amount: 15737222.22</t>
-        </is>
-      </c>
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
@@ -1976,18 +1904,8 @@
       <c r="K67" t="inlineStr"/>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
-      <c r="B68" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 8884.77
-Borrower Amount: 8884.77</t>
-        </is>
-      </c>
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
           <t>02/Jan/2025</t>
@@ -2021,18 +1939,8 @@
       <c r="K68" t="inlineStr"/>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
-      <c r="B69" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 8884.77
-Borrower Amount: 8884.77</t>
-        </is>
-      </c>
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" s="4" t="inlineStr">
@@ -2048,18 +1956,8 @@
       <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
-      <c r="B70" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 8884.77
-Borrower Amount: 8884.77</t>
-        </is>
-      </c>
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
@@ -2079,18 +1977,8 @@
       <c r="K70" t="inlineStr"/>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>M005</t>
-        </is>
-      </c>
-      <c r="B71" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
           <t>05/Jan/2025</t>
@@ -2124,18 +2012,8 @@
       <c r="K71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>M005</t>
-        </is>
-      </c>
-      <c r="B72" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
       <c r="E72" s="4" t="inlineStr">
@@ -2151,18 +2029,8 @@
       <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>M005</t>
-        </is>
-      </c>
-      <c r="B73" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
@@ -2474,18 +2342,8 @@
       <c r="K85" t="inlineStr"/>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>M007</t>
-        </is>
-      </c>
-      <c r="B86" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
           <t>15/Jan/2025</t>
@@ -2519,18 +2377,8 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>M007</t>
-        </is>
-      </c>
-      <c r="B87" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
       <c r="E87" s="4" t="inlineStr">
@@ -2546,18 +2394,8 @@
       <c r="K87" t="inlineStr"/>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>M007</t>
-        </is>
-      </c>
-      <c r="B88" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
@@ -2577,18 +2415,8 @@
       <c r="K88" t="inlineStr"/>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>M009</t>
-        </is>
-      </c>
-      <c r="B89" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr">
         <is>
           <t>15/Jan/2025</t>
@@ -2622,18 +2450,8 @@
       <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>M009</t>
-        </is>
-      </c>
-      <c r="B90" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
       <c r="E90" s="4" t="inlineStr">
@@ -2649,18 +2467,8 @@
       <c r="K90" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>M009</t>
-        </is>
-      </c>
-      <c r="B91" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1575.00
-Borrower Amount: 1575.00</t>
-        </is>
-      </c>
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
         <is>
@@ -3045,18 +2853,8 @@
       <c r="K106" t="inlineStr"/>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>M010</t>
-        </is>
-      </c>
-      <c r="B107" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 26246.93
-Borrower Amount: 26246.93</t>
-        </is>
-      </c>
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr"/>
       <c r="C107" t="inlineStr">
         <is>
           <t>28/Jan/2025</t>
@@ -3090,18 +2888,8 @@
       <c r="K107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>M010</t>
-        </is>
-      </c>
-      <c r="B108" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 26246.93
-Borrower Amount: 26246.93</t>
-        </is>
-      </c>
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr"/>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
       <c r="E108" s="4" t="inlineStr">
@@ -3117,18 +2905,8 @@
       <c r="K108" t="inlineStr"/>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>M010</t>
-        </is>
-      </c>
-      <c r="B109" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 26246.93
-Borrower Amount: 26246.93</t>
-        </is>
-      </c>
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr"/>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr">
         <is>
@@ -5889,18 +5667,8 @@
       <c r="K228" t="inlineStr"/>
     </row>
     <row r="229">
-      <c r="A229" t="inlineStr">
-        <is>
-          <t>M012</t>
-        </is>
-      </c>
-      <c r="B229" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="A229" t="inlineStr"/>
+      <c r="B229" t="inlineStr"/>
       <c r="C229" t="inlineStr">
         <is>
           <t>04/Feb/2025</t>
@@ -5934,18 +5702,8 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" t="inlineStr">
-        <is>
-          <t>M012</t>
-        </is>
-      </c>
-      <c r="B230" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="A230" t="inlineStr"/>
+      <c r="B230" t="inlineStr"/>
       <c r="C230" t="inlineStr"/>
       <c r="D230" t="inlineStr"/>
       <c r="E230" s="4" t="inlineStr">
@@ -5961,18 +5719,8 @@
       <c r="K230" t="inlineStr"/>
     </row>
     <row r="231">
-      <c r="A231" t="inlineStr">
-        <is>
-          <t>M012</t>
-        </is>
-      </c>
-      <c r="B231" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010124/24
-Lender Amount: 1150.00
-Borrower Amount: 1150.00</t>
-        </is>
-      </c>
+      <c r="A231" t="inlineStr"/>
+      <c r="B231" t="inlineStr"/>
       <c r="C231" t="inlineStr"/>
       <c r="D231" t="inlineStr">
         <is>
@@ -6065,18 +5813,8 @@
       <c r="K234" t="inlineStr"/>
     </row>
     <row r="235">
-      <c r="A235" t="inlineStr">
-        <is>
-          <t>M013</t>
-        </is>
-      </c>
-      <c r="B235" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010124/24
-Lender Amount: 8761.79
-Borrower Amount: 8761.79</t>
-        </is>
-      </c>
+      <c r="A235" t="inlineStr"/>
+      <c r="B235" t="inlineStr"/>
       <c r="C235" t="inlineStr">
         <is>
           <t>04/Feb/2025</t>
@@ -6110,18 +5848,8 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" t="inlineStr">
-        <is>
-          <t>M013</t>
-        </is>
-      </c>
-      <c r="B236" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010124/24
-Lender Amount: 8761.79
-Borrower Amount: 8761.79</t>
-        </is>
-      </c>
+      <c r="A236" t="inlineStr"/>
+      <c r="B236" t="inlineStr"/>
       <c r="C236" t="inlineStr"/>
       <c r="D236" t="inlineStr"/>
       <c r="E236" s="4" t="inlineStr">
@@ -6137,18 +5865,8 @@
       <c r="K236" t="inlineStr"/>
     </row>
     <row r="237">
-      <c r="A237" t="inlineStr">
-        <is>
-          <t>M013</t>
-        </is>
-      </c>
-      <c r="B237" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010124/24
-Lender Amount: 8761.79
-Borrower Amount: 8761.79</t>
-        </is>
-      </c>
+      <c r="A237" t="inlineStr"/>
+      <c r="B237" t="inlineStr"/>
       <c r="C237" t="inlineStr"/>
       <c r="D237" t="inlineStr">
         <is>
@@ -6571,18 +6289,8 @@
       <c r="K254" t="inlineStr"/>
     </row>
     <row r="255">
-      <c r="A255" t="inlineStr">
-        <is>
-          <t>M014</t>
-        </is>
-      </c>
-      <c r="B255" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1862.50
-Borrower Amount: 1862.50</t>
-        </is>
-      </c>
+      <c r="A255" t="inlineStr"/>
+      <c r="B255" t="inlineStr"/>
       <c r="C255" t="inlineStr">
         <is>
           <t>09/Feb/2025</t>
@@ -6616,18 +6324,8 @@
       <c r="K255" t="inlineStr"/>
     </row>
     <row r="256">
-      <c r="A256" t="inlineStr">
-        <is>
-          <t>M014</t>
-        </is>
-      </c>
-      <c r="B256" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1862.50
-Borrower Amount: 1862.50</t>
-        </is>
-      </c>
+      <c r="A256" t="inlineStr"/>
+      <c r="B256" t="inlineStr"/>
       <c r="C256" t="inlineStr"/>
       <c r="D256" t="inlineStr"/>
       <c r="E256" s="4" t="inlineStr">
@@ -6643,18 +6341,8 @@
       <c r="K256" t="inlineStr"/>
     </row>
     <row r="257">
-      <c r="A257" t="inlineStr">
-        <is>
-          <t>M014</t>
-        </is>
-      </c>
-      <c r="B257" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1862.50
-Borrower Amount: 1862.50</t>
-        </is>
-      </c>
+      <c r="A257" t="inlineStr"/>
+      <c r="B257" t="inlineStr"/>
       <c r="C257" t="inlineStr"/>
       <c r="D257" t="inlineStr">
         <is>
@@ -7096,18 +6784,8 @@
       <c r="K275" t="inlineStr"/>
     </row>
     <row r="276">
-      <c r="A276" t="inlineStr">
-        <is>
-          <t>M015</t>
-        </is>
-      </c>
-      <c r="B276" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020003/25
-Lender Amount: 27383.77
-Borrower Amount: 27383.77</t>
-        </is>
-      </c>
+      <c r="A276" t="inlineStr"/>
+      <c r="B276" t="inlineStr"/>
       <c r="C276" t="inlineStr">
         <is>
           <t>11/Feb/2025</t>
@@ -7141,18 +6819,8 @@
       <c r="K276" t="inlineStr"/>
     </row>
     <row r="277">
-      <c r="A277" t="inlineStr">
-        <is>
-          <t>M015</t>
-        </is>
-      </c>
-      <c r="B277" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020003/25
-Lender Amount: 27383.77
-Borrower Amount: 27383.77</t>
-        </is>
-      </c>
+      <c r="A277" t="inlineStr"/>
+      <c r="B277" t="inlineStr"/>
       <c r="C277" t="inlineStr"/>
       <c r="D277" t="inlineStr"/>
       <c r="E277" s="4" t="inlineStr">
@@ -7168,18 +6836,8 @@
       <c r="K277" t="inlineStr"/>
     </row>
     <row r="278">
-      <c r="A278" t="inlineStr">
-        <is>
-          <t>M015</t>
-        </is>
-      </c>
-      <c r="B278" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020003/25
-Lender Amount: 27383.77
-Borrower Amount: 27383.77</t>
-        </is>
-      </c>
+      <c r="A278" t="inlineStr"/>
+      <c r="B278" t="inlineStr"/>
       <c r="C278" t="inlineStr"/>
       <c r="D278" t="inlineStr">
         <is>
@@ -8573,18 +8231,8 @@
       <c r="K336" t="inlineStr"/>
     </row>
     <row r="337">
-      <c r="A337" t="inlineStr">
-        <is>
-          <t>M016</t>
-        </is>
-      </c>
-      <c r="B337" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524990243/24
-Lender Amount: 71971.54
-Borrower Amount: 71971.54</t>
-        </is>
-      </c>
+      <c r="A337" t="inlineStr"/>
+      <c r="B337" t="inlineStr"/>
       <c r="C337" t="inlineStr">
         <is>
           <t>18/Feb/2025</t>
@@ -8618,18 +8266,8 @@
       <c r="K337" t="inlineStr"/>
     </row>
     <row r="338">
-      <c r="A338" t="inlineStr">
-        <is>
-          <t>M016</t>
-        </is>
-      </c>
-      <c r="B338" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524990243/24
-Lender Amount: 71971.54
-Borrower Amount: 71971.54</t>
-        </is>
-      </c>
+      <c r="A338" t="inlineStr"/>
+      <c r="B338" t="inlineStr"/>
       <c r="C338" t="inlineStr"/>
       <c r="D338" t="inlineStr"/>
       <c r="E338" s="4" t="inlineStr">
@@ -8645,18 +8283,8 @@
       <c r="K338" t="inlineStr"/>
     </row>
     <row r="339">
-      <c r="A339" t="inlineStr">
-        <is>
-          <t>M016</t>
-        </is>
-      </c>
-      <c r="B339" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524990243/24
-Lender Amount: 71971.54
-Borrower Amount: 71971.54</t>
-        </is>
-      </c>
+      <c r="A339" t="inlineStr"/>
+      <c r="B339" t="inlineStr"/>
       <c r="C339" t="inlineStr"/>
       <c r="D339" t="inlineStr">
         <is>
@@ -8676,18 +8304,8 @@
       <c r="K339" t="inlineStr"/>
     </row>
     <row r="340">
-      <c r="A340" t="inlineStr">
-        <is>
-          <t>M017</t>
-        </is>
-      </c>
-      <c r="B340" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524990243/24
-Lender Amount: 20527984.90
-Borrower Amount: 20527984.90</t>
-        </is>
-      </c>
+      <c r="A340" t="inlineStr"/>
+      <c r="B340" t="inlineStr"/>
       <c r="C340" t="inlineStr">
         <is>
           <t>19/Feb/2025</t>
@@ -8721,18 +8339,8 @@
       <c r="K340" t="inlineStr"/>
     </row>
     <row r="341">
-      <c r="A341" t="inlineStr">
-        <is>
-          <t>M017</t>
-        </is>
-      </c>
-      <c r="B341" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524990243/24
-Lender Amount: 20527984.90
-Borrower Amount: 20527984.90</t>
-        </is>
-      </c>
+      <c r="A341" t="inlineStr"/>
+      <c r="B341" t="inlineStr"/>
       <c r="C341" t="inlineStr"/>
       <c r="D341" t="inlineStr"/>
       <c r="E341" s="4" t="inlineStr">
@@ -8748,18 +8356,8 @@
       <c r="K341" t="inlineStr"/>
     </row>
     <row r="342">
-      <c r="A342" t="inlineStr">
-        <is>
-          <t>M017</t>
-        </is>
-      </c>
-      <c r="B342" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524990243/24
-Lender Amount: 20527984.90
-Borrower Amount: 20527984.90</t>
-        </is>
-      </c>
+      <c r="A342" t="inlineStr"/>
+      <c r="B342" t="inlineStr"/>
       <c r="C342" t="inlineStr"/>
       <c r="D342" t="inlineStr">
         <is>
@@ -8779,18 +8377,8 @@
       <c r="K342" t="inlineStr"/>
     </row>
     <row r="343">
-      <c r="A343" t="inlineStr">
-        <is>
-          <t>M018</t>
-        </is>
-      </c>
-      <c r="B343" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020653/25
-Lender Amount: 665048.82
-Borrower Amount: 665048.82</t>
-        </is>
-      </c>
+      <c r="A343" t="inlineStr"/>
+      <c r="B343" t="inlineStr"/>
       <c r="C343" t="inlineStr">
         <is>
           <t>23/Feb/2025</t>
@@ -8824,18 +8412,8 @@
       <c r="K343" t="inlineStr"/>
     </row>
     <row r="344">
-      <c r="A344" t="inlineStr">
-        <is>
-          <t>M018</t>
-        </is>
-      </c>
-      <c r="B344" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020653/25
-Lender Amount: 665048.82
-Borrower Amount: 665048.82</t>
-        </is>
-      </c>
+      <c r="A344" t="inlineStr"/>
+      <c r="B344" t="inlineStr"/>
       <c r="C344" t="inlineStr"/>
       <c r="D344" t="inlineStr"/>
       <c r="E344" s="4" t="inlineStr">
@@ -8851,18 +8429,8 @@
       <c r="K344" t="inlineStr"/>
     </row>
     <row r="345">
-      <c r="A345" t="inlineStr">
-        <is>
-          <t>M018</t>
-        </is>
-      </c>
-      <c r="B345" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020653/25
-Lender Amount: 665048.82
-Borrower Amount: 665048.82</t>
-        </is>
-      </c>
+      <c r="A345" t="inlineStr"/>
+      <c r="B345" t="inlineStr"/>
       <c r="C345" t="inlineStr"/>
       <c r="D345" t="inlineStr">
         <is>
@@ -8882,18 +8450,8 @@
       <c r="K345" t="inlineStr"/>
     </row>
     <row r="346">
-      <c r="A346" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="B346" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020708/24
-Lender Amount: 25042.61
-Borrower Amount: 25042.61</t>
-        </is>
-      </c>
+      <c r="A346" t="inlineStr"/>
+      <c r="B346" t="inlineStr"/>
       <c r="C346" t="inlineStr">
         <is>
           <t>23/Feb/2025</t>
@@ -8927,18 +8485,8 @@
       <c r="K346" t="inlineStr"/>
     </row>
     <row r="347">
-      <c r="A347" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="B347" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020708/24
-Lender Amount: 25042.61
-Borrower Amount: 25042.61</t>
-        </is>
-      </c>
+      <c r="A347" t="inlineStr"/>
+      <c r="B347" t="inlineStr"/>
       <c r="C347" t="inlineStr"/>
       <c r="D347" t="inlineStr"/>
       <c r="E347" s="4" t="inlineStr">
@@ -8954,18 +8502,8 @@
       <c r="K347" t="inlineStr"/>
     </row>
     <row r="348">
-      <c r="A348" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="B348" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020708/24
-Lender Amount: 25042.61
-Borrower Amount: 25042.61</t>
-        </is>
-      </c>
+      <c r="A348" t="inlineStr"/>
+      <c r="B348" t="inlineStr"/>
       <c r="C348" t="inlineStr"/>
       <c r="D348" t="inlineStr">
         <is>
@@ -9278,18 +8816,8 @@
       <c r="K360" t="inlineStr"/>
     </row>
     <row r="361">
-      <c r="A361" t="inlineStr">
-        <is>
-          <t>M020</t>
-        </is>
-      </c>
-      <c r="B361" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 5995080.00
-Borrower Amount: 5995080.00</t>
-        </is>
-      </c>
+      <c r="A361" t="inlineStr"/>
+      <c r="B361" t="inlineStr"/>
       <c r="C361" t="inlineStr">
         <is>
           <t>25/Feb/2025</t>
@@ -9323,18 +8851,8 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" t="inlineStr">
-        <is>
-          <t>M020</t>
-        </is>
-      </c>
-      <c r="B362" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 5995080.00
-Borrower Amount: 5995080.00</t>
-        </is>
-      </c>
+      <c r="A362" t="inlineStr"/>
+      <c r="B362" t="inlineStr"/>
       <c r="C362" t="inlineStr"/>
       <c r="D362" t="inlineStr"/>
       <c r="E362" s="4" t="inlineStr">
@@ -9350,18 +8868,8 @@
       <c r="K362" t="inlineStr"/>
     </row>
     <row r="363">
-      <c r="A363" t="inlineStr">
-        <is>
-          <t>M020</t>
-        </is>
-      </c>
-      <c r="B363" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 5995080.00
-Borrower Amount: 5995080.00</t>
-        </is>
-      </c>
+      <c r="A363" t="inlineStr"/>
+      <c r="B363" t="inlineStr"/>
       <c r="C363" t="inlineStr"/>
       <c r="D363" t="inlineStr">
         <is>
@@ -9381,18 +8889,8 @@
       <c r="K363" t="inlineStr"/>
     </row>
     <row r="364">
-      <c r="A364" t="inlineStr">
-        <is>
-          <t>M021</t>
-        </is>
-      </c>
-      <c r="B364" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020068/25
-Lender Amount: 33573.89
-Borrower Amount: 33573.89</t>
-        </is>
-      </c>
+      <c r="A364" t="inlineStr"/>
+      <c r="B364" t="inlineStr"/>
       <c r="C364" t="inlineStr">
         <is>
           <t>26/Feb/2025</t>
@@ -9426,18 +8924,8 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" t="inlineStr">
-        <is>
-          <t>M021</t>
-        </is>
-      </c>
-      <c r="B365" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020068/25
-Lender Amount: 33573.89
-Borrower Amount: 33573.89</t>
-        </is>
-      </c>
+      <c r="A365" t="inlineStr"/>
+      <c r="B365" t="inlineStr"/>
       <c r="C365" t="inlineStr"/>
       <c r="D365" t="inlineStr"/>
       <c r="E365" s="4" t="inlineStr">
@@ -9453,18 +8941,8 @@
       <c r="K365" t="inlineStr"/>
     </row>
     <row r="366">
-      <c r="A366" t="inlineStr">
-        <is>
-          <t>M021</t>
-        </is>
-      </c>
-      <c r="B366" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020068/25
-Lender Amount: 33573.89
-Borrower Amount: 33573.89</t>
-        </is>
-      </c>
+      <c r="A366" t="inlineStr"/>
+      <c r="B366" t="inlineStr"/>
       <c r="C366" t="inlineStr"/>
       <c r="D366" t="inlineStr">
         <is>
@@ -9484,18 +8962,8 @@
       <c r="K366" t="inlineStr"/>
     </row>
     <row r="367">
-      <c r="A367" t="inlineStr">
-        <is>
-          <t>M022</t>
-        </is>
-      </c>
-      <c r="B367" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020068/25
-Lender Amount: 1650660.00
-Borrower Amount: 1650660.00</t>
-        </is>
-      </c>
+      <c r="A367" t="inlineStr"/>
+      <c r="B367" t="inlineStr"/>
       <c r="C367" t="inlineStr">
         <is>
           <t>26/Feb/2025</t>
@@ -9529,18 +8997,8 @@
       </c>
     </row>
     <row r="368">
-      <c r="A368" t="inlineStr">
-        <is>
-          <t>M022</t>
-        </is>
-      </c>
-      <c r="B368" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020068/25
-Lender Amount: 1650660.00
-Borrower Amount: 1650660.00</t>
-        </is>
-      </c>
+      <c r="A368" t="inlineStr"/>
+      <c r="B368" t="inlineStr"/>
       <c r="C368" t="inlineStr"/>
       <c r="D368" t="inlineStr"/>
       <c r="E368" s="4" t="inlineStr">
@@ -9556,18 +9014,8 @@
       <c r="K368" t="inlineStr"/>
     </row>
     <row r="369">
-      <c r="A369" t="inlineStr">
-        <is>
-          <t>M022</t>
-        </is>
-      </c>
-      <c r="B369" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020068/25
-Lender Amount: 1650660.00
-Borrower Amount: 1650660.00</t>
-        </is>
-      </c>
+      <c r="A369" t="inlineStr"/>
+      <c r="B369" t="inlineStr"/>
       <c r="C369" t="inlineStr"/>
       <c r="D369" t="inlineStr">
         <is>
@@ -9807,18 +9255,8 @@
       <c r="K378" t="inlineStr"/>
     </row>
     <row r="379">
-      <c r="A379" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
-      <c r="B379" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="A379" t="inlineStr"/>
+      <c r="B379" t="inlineStr"/>
       <c r="C379" t="inlineStr">
         <is>
           <t>27/Feb/2025</t>
@@ -9852,18 +9290,8 @@
       <c r="K379" t="inlineStr"/>
     </row>
     <row r="380">
-      <c r="A380" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
-      <c r="B380" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="A380" t="inlineStr"/>
+      <c r="B380" t="inlineStr"/>
       <c r="C380" t="inlineStr"/>
       <c r="D380" t="inlineStr"/>
       <c r="E380" s="4" t="inlineStr">
@@ -9881,18 +9309,8 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
-      <c r="B381" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="A381" t="inlineStr"/>
+      <c r="B381" t="inlineStr"/>
       <c r="C381" t="inlineStr"/>
       <c r="D381" t="inlineStr"/>
       <c r="E381" s="4" t="inlineStr">
@@ -9910,18 +9328,8 @@
       </c>
     </row>
     <row r="382">
-      <c r="A382" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
-      <c r="B382" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="A382" t="inlineStr"/>
+      <c r="B382" t="inlineStr"/>
       <c r="C382" t="inlineStr"/>
       <c r="D382" t="inlineStr"/>
       <c r="E382" s="4" t="inlineStr">
@@ -9937,18 +9345,8 @@
       <c r="K382" t="inlineStr"/>
     </row>
     <row r="383">
-      <c r="A383" t="inlineStr">
-        <is>
-          <t>M023</t>
-        </is>
-      </c>
-      <c r="B383" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155824020001/24
-Lender Amount: 7641878.37
-Borrower Amount: 7641878.37</t>
-        </is>
-      </c>
+      <c r="A383" t="inlineStr"/>
+      <c r="B383" t="inlineStr"/>
       <c r="C383" t="inlineStr"/>
       <c r="D383" t="inlineStr">
         <is>
@@ -10992,18 +10390,8 @@
       <c r="K431" t="inlineStr"/>
     </row>
     <row r="432">
-      <c r="A432" t="inlineStr">
-        <is>
-          <t>M024</t>
-        </is>
-      </c>
-      <c r="B432" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 246401.97
-Borrower Amount: 246401.97</t>
-        </is>
-      </c>
+      <c r="A432" t="inlineStr"/>
+      <c r="B432" t="inlineStr"/>
       <c r="C432" t="inlineStr">
         <is>
           <t>01/Mar/2025</t>
@@ -11037,18 +10425,8 @@
       </c>
     </row>
     <row r="433">
-      <c r="A433" t="inlineStr">
-        <is>
-          <t>M024</t>
-        </is>
-      </c>
-      <c r="B433" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 246401.97
-Borrower Amount: 246401.97</t>
-        </is>
-      </c>
+      <c r="A433" t="inlineStr"/>
+      <c r="B433" t="inlineStr"/>
       <c r="C433" t="inlineStr"/>
       <c r="D433" t="inlineStr"/>
       <c r="E433" s="4" t="inlineStr">
@@ -11064,18 +10442,8 @@
       <c r="K433" t="inlineStr"/>
     </row>
     <row r="434">
-      <c r="A434" t="inlineStr">
-        <is>
-          <t>M024</t>
-        </is>
-      </c>
-      <c r="B434" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 246401.97
-Borrower Amount: 246401.97</t>
-        </is>
-      </c>
+      <c r="A434" t="inlineStr"/>
+      <c r="B434" t="inlineStr"/>
       <c r="C434" t="inlineStr"/>
       <c r="D434" t="inlineStr">
         <is>
@@ -11241,18 +10609,8 @@
       <c r="K440" t="inlineStr"/>
     </row>
     <row r="441">
-      <c r="A441" t="inlineStr">
-        <is>
-          <t>M025</t>
-        </is>
-      </c>
-      <c r="B441" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 26369.63
-Borrower Amount: 26369.63</t>
-        </is>
-      </c>
+      <c r="A441" t="inlineStr"/>
+      <c r="B441" t="inlineStr"/>
       <c r="C441" t="inlineStr">
         <is>
           <t>01/Mar/2025</t>
@@ -11286,18 +10644,8 @@
       <c r="K441" t="inlineStr"/>
     </row>
     <row r="442">
-      <c r="A442" t="inlineStr">
-        <is>
-          <t>M025</t>
-        </is>
-      </c>
-      <c r="B442" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 26369.63
-Borrower Amount: 26369.63</t>
-        </is>
-      </c>
+      <c r="A442" t="inlineStr"/>
+      <c r="B442" t="inlineStr"/>
       <c r="C442" t="inlineStr"/>
       <c r="D442" t="inlineStr"/>
       <c r="E442" s="4" t="inlineStr">
@@ -11313,18 +10661,8 @@
       <c r="K442" t="inlineStr"/>
     </row>
     <row r="443">
-      <c r="A443" t="inlineStr">
-        <is>
-          <t>M025</t>
-        </is>
-      </c>
-      <c r="B443" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022796/24
-Lender Amount: 26369.63
-Borrower Amount: 26369.63</t>
-        </is>
-      </c>
+      <c r="A443" t="inlineStr"/>
+      <c r="B443" t="inlineStr"/>
       <c r="C443" t="inlineStr"/>
       <c r="D443" t="inlineStr">
         <is>
@@ -11747,18 +11085,8 @@
       <c r="K460" t="inlineStr"/>
     </row>
     <row r="461">
-      <c r="A461" t="inlineStr">
-        <is>
-          <t>M026</t>
-        </is>
-      </c>
-      <c r="B461" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-222825150235/25
-Lender Amount: 2357.50
-Borrower Amount: 2357.50</t>
-        </is>
-      </c>
+      <c r="A461" t="inlineStr"/>
+      <c r="B461" t="inlineStr"/>
       <c r="C461" t="inlineStr">
         <is>
           <t>06/Mar/2025</t>
@@ -11792,18 +11120,8 @@
       </c>
     </row>
     <row r="462">
-      <c r="A462" t="inlineStr">
-        <is>
-          <t>M026</t>
-        </is>
-      </c>
-      <c r="B462" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-222825150235/25
-Lender Amount: 2357.50
-Borrower Amount: 2357.50</t>
-        </is>
-      </c>
+      <c r="A462" t="inlineStr"/>
+      <c r="B462" t="inlineStr"/>
       <c r="C462" t="inlineStr"/>
       <c r="D462" t="inlineStr"/>
       <c r="E462" s="4" t="inlineStr">
@@ -11819,18 +11137,8 @@
       <c r="K462" t="inlineStr"/>
     </row>
     <row r="463">
-      <c r="A463" t="inlineStr">
-        <is>
-          <t>M026</t>
-        </is>
-      </c>
-      <c r="B463" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-222825150235/25
-Lender Amount: 2357.50
-Borrower Amount: 2357.50</t>
-        </is>
-      </c>
+      <c r="A463" t="inlineStr"/>
+      <c r="B463" t="inlineStr"/>
       <c r="C463" t="inlineStr"/>
       <c r="D463" t="inlineStr">
         <is>
@@ -11923,18 +11231,8 @@
       <c r="K466" t="inlineStr"/>
     </row>
     <row r="467">
-      <c r="A467" t="inlineStr">
-        <is>
-          <t>M027</t>
-        </is>
-      </c>
-      <c r="B467" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-222825150235/25
-Lender Amount: 213500.00
-Borrower Amount: 213500.00</t>
-        </is>
-      </c>
+      <c r="A467" t="inlineStr"/>
+      <c r="B467" t="inlineStr"/>
       <c r="C467" t="inlineStr">
         <is>
           <t>09/Mar/2025</t>
@@ -11968,18 +11266,8 @@
       </c>
     </row>
     <row r="468">
-      <c r="A468" t="inlineStr">
-        <is>
-          <t>M027</t>
-        </is>
-      </c>
-      <c r="B468" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-222825150235/25
-Lender Amount: 213500.00
-Borrower Amount: 213500.00</t>
-        </is>
-      </c>
+      <c r="A468" t="inlineStr"/>
+      <c r="B468" t="inlineStr"/>
       <c r="C468" t="inlineStr"/>
       <c r="D468" t="inlineStr"/>
       <c r="E468" s="4" t="inlineStr">
@@ -11995,18 +11283,8 @@
       <c r="K468" t="inlineStr"/>
     </row>
     <row r="469">
-      <c r="A469" t="inlineStr">
-        <is>
-          <t>M027</t>
-        </is>
-      </c>
-      <c r="B469" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-222825150235/25
-Lender Amount: 213500.00
-Borrower Amount: 213500.00</t>
-        </is>
-      </c>
+      <c r="A469" t="inlineStr"/>
+      <c r="B469" t="inlineStr"/>
       <c r="C469" t="inlineStr"/>
       <c r="D469" t="inlineStr">
         <is>
@@ -12028,16 +11306,10 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>M028</t>
-        </is>
-      </c>
-      <c r="B470" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr"/>
       <c r="C470" t="inlineStr">
         <is>
           <t>09/Mar/2025</t>
@@ -12073,7 +11345,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>M028</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="B471" s="4" t="inlineStr">
@@ -12100,16 +11372,10 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>M028</t>
-        </is>
-      </c>
-      <c r="B472" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr"/>
       <c r="C472" t="inlineStr"/>
       <c r="D472" t="inlineStr">
         <is>
@@ -12129,18 +11395,8 @@
       <c r="K472" t="inlineStr"/>
     </row>
     <row r="473">
-      <c r="A473" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
-      <c r="B473" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="A473" t="inlineStr"/>
+      <c r="B473" t="inlineStr"/>
       <c r="C473" t="inlineStr">
         <is>
           <t>10/Mar/2025</t>
@@ -12174,18 +11430,8 @@
       <c r="K473" t="inlineStr"/>
     </row>
     <row r="474">
-      <c r="A474" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
-      <c r="B474" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="A474" t="inlineStr"/>
+      <c r="B474" t="inlineStr"/>
       <c r="C474" t="inlineStr"/>
       <c r="D474" t="inlineStr"/>
       <c r="E474" s="4" t="inlineStr">
@@ -12203,18 +11449,8 @@
       </c>
     </row>
     <row r="475">
-      <c r="A475" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
-      <c r="B475" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="A475" t="inlineStr"/>
+      <c r="B475" t="inlineStr"/>
       <c r="C475" t="inlineStr"/>
       <c r="D475" t="inlineStr"/>
       <c r="E475" s="4" t="inlineStr">
@@ -12232,18 +11468,8 @@
       </c>
     </row>
     <row r="476">
-      <c r="A476" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
-      <c r="B476" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="A476" t="inlineStr"/>
+      <c r="B476" t="inlineStr"/>
       <c r="C476" t="inlineStr"/>
       <c r="D476" t="inlineStr"/>
       <c r="E476" s="4" t="inlineStr">
@@ -12259,18 +11485,8 @@
       <c r="K476" t="inlineStr"/>
     </row>
     <row r="477">
-      <c r="A477" t="inlineStr">
-        <is>
-          <t>M029</t>
-        </is>
-      </c>
-      <c r="B477" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-187724010122/24
-Lender Amount: 276518.90
-Borrower Amount: 276518.90</t>
-        </is>
-      </c>
+      <c r="A477" t="inlineStr"/>
+      <c r="B477" t="inlineStr"/>
       <c r="C477" t="inlineStr"/>
       <c r="D477" t="inlineStr">
         <is>
@@ -13020,18 +12236,8 @@
       <c r="K507" t="inlineStr"/>
     </row>
     <row r="508">
-      <c r="A508" t="inlineStr">
-        <is>
-          <t>M030</t>
-        </is>
-      </c>
-      <c r="B508" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020027/25
-Lender Amount: 54431.58
-Borrower Amount: 54431.58</t>
-        </is>
-      </c>
+      <c r="A508" t="inlineStr"/>
+      <c r="B508" t="inlineStr"/>
       <c r="C508" t="inlineStr">
         <is>
           <t>18/Mar/2025</t>
@@ -13065,18 +12271,8 @@
       <c r="K508" t="inlineStr"/>
     </row>
     <row r="509">
-      <c r="A509" t="inlineStr">
-        <is>
-          <t>M030</t>
-        </is>
-      </c>
-      <c r="B509" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020027/25
-Lender Amount: 54431.58
-Borrower Amount: 54431.58</t>
-        </is>
-      </c>
+      <c r="A509" t="inlineStr"/>
+      <c r="B509" t="inlineStr"/>
       <c r="C509" t="inlineStr"/>
       <c r="D509" t="inlineStr"/>
       <c r="E509" s="4" t="inlineStr">
@@ -13092,18 +12288,8 @@
       <c r="K509" t="inlineStr"/>
     </row>
     <row r="510">
-      <c r="A510" t="inlineStr">
-        <is>
-          <t>M030</t>
-        </is>
-      </c>
-      <c r="B510" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020027/25
-Lender Amount: 54431.58
-Borrower Amount: 54431.58</t>
-        </is>
-      </c>
+      <c r="A510" t="inlineStr"/>
+      <c r="B510" t="inlineStr"/>
       <c r="C510" t="inlineStr"/>
       <c r="D510" t="inlineStr">
         <is>
@@ -13342,18 +12528,8 @@
       <c r="K519" t="inlineStr"/>
     </row>
     <row r="520">
-      <c r="A520" t="inlineStr">
-        <is>
-          <t>M031</t>
-        </is>
-      </c>
-      <c r="B520" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 8231.99
-Borrower Amount: 8231.99</t>
-        </is>
-      </c>
+      <c r="A520" t="inlineStr"/>
+      <c r="B520" t="inlineStr"/>
       <c r="C520" t="inlineStr">
         <is>
           <t>19/Mar/2025</t>
@@ -13387,18 +12563,8 @@
       <c r="K520" t="inlineStr"/>
     </row>
     <row r="521">
-      <c r="A521" t="inlineStr">
-        <is>
-          <t>M031</t>
-        </is>
-      </c>
-      <c r="B521" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 8231.99
-Borrower Amount: 8231.99</t>
-        </is>
-      </c>
+      <c r="A521" t="inlineStr"/>
+      <c r="B521" t="inlineStr"/>
       <c r="C521" t="inlineStr"/>
       <c r="D521" t="inlineStr"/>
       <c r="E521" s="4" t="inlineStr">
@@ -13414,18 +12580,8 @@
       <c r="K521" t="inlineStr"/>
     </row>
     <row r="522">
-      <c r="A522" t="inlineStr">
-        <is>
-          <t>M031</t>
-        </is>
-      </c>
-      <c r="B522" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524027065/24
-Lender Amount: 8231.99
-Borrower Amount: 8231.99</t>
-        </is>
-      </c>
+      <c r="A522" t="inlineStr"/>
+      <c r="B522" t="inlineStr"/>
       <c r="C522" t="inlineStr"/>
       <c r="D522" t="inlineStr">
         <is>
@@ -14482,18 +13638,8 @@
       <c r="K569" t="inlineStr"/>
     </row>
     <row r="570">
-      <c r="A570" t="inlineStr">
-        <is>
-          <t>M032</t>
-        </is>
-      </c>
-      <c r="B570" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020708/24
-Lender Amount: 19399.10
-Borrower Amount: 19399.10</t>
-        </is>
-      </c>
+      <c r="A570" t="inlineStr"/>
+      <c r="B570" t="inlineStr"/>
       <c r="C570" t="inlineStr">
         <is>
           <t>25/Mar/2025</t>
@@ -14527,18 +13673,8 @@
       <c r="K570" t="inlineStr"/>
     </row>
     <row r="571">
-      <c r="A571" t="inlineStr">
-        <is>
-          <t>M032</t>
-        </is>
-      </c>
-      <c r="B571" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020708/24
-Lender Amount: 19399.10
-Borrower Amount: 19399.10</t>
-        </is>
-      </c>
+      <c r="A571" t="inlineStr"/>
+      <c r="B571" t="inlineStr"/>
       <c r="C571" t="inlineStr"/>
       <c r="D571" t="inlineStr"/>
       <c r="E571" s="4" t="inlineStr">
@@ -14554,18 +13690,8 @@
       <c r="K571" t="inlineStr"/>
     </row>
     <row r="572">
-      <c r="A572" t="inlineStr">
-        <is>
-          <t>M032</t>
-        </is>
-      </c>
-      <c r="B572" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020708/24
-Lender Amount: 19399.10
-Borrower Amount: 19399.10</t>
-        </is>
-      </c>
+      <c r="A572" t="inlineStr"/>
+      <c r="B572" t="inlineStr"/>
       <c r="C572" t="inlineStr"/>
       <c r="D572" t="inlineStr">
         <is>
@@ -14587,16 +13713,10 @@
     <row r="573">
       <c r="A573" t="inlineStr">
         <is>
-          <t>M033</t>
-        </is>
-      </c>
-      <c r="B573" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524990243/24
-Lender Amount: 15160.97
-Borrower Amount: 15160.97</t>
-        </is>
-      </c>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr"/>
       <c r="C573" t="inlineStr">
         <is>
           <t>25/Mar/2025</t>
@@ -14632,7 +13752,7 @@
     <row r="574">
       <c r="A574" t="inlineStr">
         <is>
-          <t>M033</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="B574" s="4" t="inlineStr">
@@ -14659,16 +13779,10 @@
     <row r="575">
       <c r="A575" t="inlineStr">
         <is>
-          <t>M033</t>
-        </is>
-      </c>
-      <c r="B575" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524990243/24
-Lender Amount: 15160.97
-Borrower Amount: 15160.97</t>
-        </is>
-      </c>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr"/>
       <c r="C575" t="inlineStr"/>
       <c r="D575" t="inlineStr">
         <is>
@@ -14837,18 +13951,8 @@
       <c r="K582" t="inlineStr"/>
     </row>
     <row r="583">
-      <c r="A583" t="inlineStr">
-        <is>
-          <t>M034</t>
-        </is>
-      </c>
-      <c r="B583" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 6125933.94
-Borrower Amount: 6125933.94</t>
-        </is>
-      </c>
+      <c r="A583" t="inlineStr"/>
+      <c r="B583" t="inlineStr"/>
       <c r="C583" t="inlineStr">
         <is>
           <t>27/Mar/2025</t>
@@ -14882,18 +13986,8 @@
       </c>
     </row>
     <row r="584">
-      <c r="A584" t="inlineStr">
-        <is>
-          <t>M034</t>
-        </is>
-      </c>
-      <c r="B584" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 6125933.94
-Borrower Amount: 6125933.94</t>
-        </is>
-      </c>
+      <c r="A584" t="inlineStr"/>
+      <c r="B584" t="inlineStr"/>
       <c r="C584" t="inlineStr"/>
       <c r="D584" t="inlineStr"/>
       <c r="E584" s="4" t="inlineStr">
@@ -14911,18 +14005,8 @@
       <c r="K584" t="inlineStr"/>
     </row>
     <row r="585">
-      <c r="A585" t="inlineStr">
-        <is>
-          <t>M034</t>
-        </is>
-      </c>
-      <c r="B585" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 6125933.94
-Borrower Amount: 6125933.94</t>
-        </is>
-      </c>
+      <c r="A585" t="inlineStr"/>
+      <c r="B585" t="inlineStr"/>
       <c r="C585" t="inlineStr"/>
       <c r="D585" t="inlineStr"/>
       <c r="E585" s="4" t="inlineStr">
@@ -14940,18 +14024,8 @@
       <c r="K585" t="inlineStr"/>
     </row>
     <row r="586">
-      <c r="A586" t="inlineStr">
-        <is>
-          <t>M034</t>
-        </is>
-      </c>
-      <c r="B586" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 6125933.94
-Borrower Amount: 6125933.94</t>
-        </is>
-      </c>
+      <c r="A586" t="inlineStr"/>
+      <c r="B586" t="inlineStr"/>
       <c r="C586" t="inlineStr"/>
       <c r="D586" t="inlineStr"/>
       <c r="E586" s="4" t="inlineStr">
@@ -14967,18 +14041,8 @@
       <c r="K586" t="inlineStr"/>
     </row>
     <row r="587">
-      <c r="A587" t="inlineStr">
-        <is>
-          <t>M034</t>
-        </is>
-      </c>
-      <c r="B587" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 6125933.94
-Borrower Amount: 6125933.94</t>
-        </is>
-      </c>
+      <c r="A587" t="inlineStr"/>
+      <c r="B587" t="inlineStr"/>
       <c r="C587" t="inlineStr"/>
       <c r="D587" t="inlineStr">
         <is>
@@ -14998,18 +14062,8 @@
       <c r="K587" t="inlineStr"/>
     </row>
     <row r="588">
-      <c r="A588" t="inlineStr">
-        <is>
-          <t>M035</t>
-        </is>
-      </c>
-      <c r="B588" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022495/24
-Lender Amount: 12425.77
-Borrower Amount: 12425.77</t>
-        </is>
-      </c>
+      <c r="A588" t="inlineStr"/>
+      <c r="B588" t="inlineStr"/>
       <c r="C588" t="inlineStr">
         <is>
           <t>27/Mar/2025</t>
@@ -15043,18 +14097,8 @@
       <c r="K588" t="inlineStr"/>
     </row>
     <row r="589">
-      <c r="A589" t="inlineStr">
-        <is>
-          <t>M035</t>
-        </is>
-      </c>
-      <c r="B589" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022495/24
-Lender Amount: 12425.77
-Borrower Amount: 12425.77</t>
-        </is>
-      </c>
+      <c r="A589" t="inlineStr"/>
+      <c r="B589" t="inlineStr"/>
       <c r="C589" t="inlineStr"/>
       <c r="D589" t="inlineStr"/>
       <c r="E589" s="4" t="inlineStr">
@@ -15070,18 +14114,8 @@
       <c r="K589" t="inlineStr"/>
     </row>
     <row r="590">
-      <c r="A590" t="inlineStr">
-        <is>
-          <t>M035</t>
-        </is>
-      </c>
-      <c r="B590" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022495/24
-Lender Amount: 12425.77
-Borrower Amount: 12425.77</t>
-        </is>
-      </c>
+      <c r="A590" t="inlineStr"/>
+      <c r="B590" t="inlineStr"/>
       <c r="C590" t="inlineStr"/>
       <c r="D590" t="inlineStr">
         <is>
@@ -15101,18 +14135,8 @@
       <c r="K590" t="inlineStr"/>
     </row>
     <row r="591">
-      <c r="A591" t="inlineStr">
-        <is>
-          <t>M036</t>
-        </is>
-      </c>
-      <c r="B591" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022495/24
-Lender Amount: 23580.68
-Borrower Amount: 23580.68</t>
-        </is>
-      </c>
+      <c r="A591" t="inlineStr"/>
+      <c r="B591" t="inlineStr"/>
       <c r="C591" t="inlineStr">
         <is>
           <t>27/Mar/2025</t>
@@ -15146,18 +14170,8 @@
       <c r="K591" t="inlineStr"/>
     </row>
     <row r="592">
-      <c r="A592" t="inlineStr">
-        <is>
-          <t>M036</t>
-        </is>
-      </c>
-      <c r="B592" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022495/24
-Lender Amount: 23580.68
-Borrower Amount: 23580.68</t>
-        </is>
-      </c>
+      <c r="A592" t="inlineStr"/>
+      <c r="B592" t="inlineStr"/>
       <c r="C592" t="inlineStr"/>
       <c r="D592" t="inlineStr"/>
       <c r="E592" s="4" t="inlineStr">
@@ -15173,18 +14187,8 @@
       <c r="K592" t="inlineStr"/>
     </row>
     <row r="593">
-      <c r="A593" t="inlineStr">
-        <is>
-          <t>M036</t>
-        </is>
-      </c>
-      <c r="B593" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524022495/24
-Lender Amount: 23580.68
-Borrower Amount: 23580.68</t>
-        </is>
-      </c>
+      <c r="A593" t="inlineStr"/>
+      <c r="B593" t="inlineStr"/>
       <c r="C593" t="inlineStr"/>
       <c r="D593" t="inlineStr">
         <is>
@@ -16190,18 +15194,8 @@
       <c r="K639" t="inlineStr"/>
     </row>
     <row r="640">
-      <c r="A640" t="inlineStr">
-        <is>
-          <t>M037</t>
-        </is>
-      </c>
-      <c r="B640" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308525021741/25
-Lender Amount: 22671.95
-Borrower Amount: 22671.95</t>
-        </is>
-      </c>
+      <c r="A640" t="inlineStr"/>
+      <c r="B640" t="inlineStr"/>
       <c r="C640" t="inlineStr">
         <is>
           <t>07/Apr/2025</t>
@@ -16235,18 +15229,8 @@
       <c r="K640" t="inlineStr"/>
     </row>
     <row r="641">
-      <c r="A641" t="inlineStr">
-        <is>
-          <t>M037</t>
-        </is>
-      </c>
-      <c r="B641" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308525021741/25
-Lender Amount: 22671.95
-Borrower Amount: 22671.95</t>
-        </is>
-      </c>
+      <c r="A641" t="inlineStr"/>
+      <c r="B641" t="inlineStr"/>
       <c r="C641" t="inlineStr"/>
       <c r="D641" t="inlineStr"/>
       <c r="E641" s="4" t="inlineStr">
@@ -16262,18 +15246,8 @@
       <c r="K641" t="inlineStr"/>
     </row>
     <row r="642">
-      <c r="A642" t="inlineStr">
-        <is>
-          <t>M037</t>
-        </is>
-      </c>
-      <c r="B642" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308525021741/25
-Lender Amount: 22671.95
-Borrower Amount: 22671.95</t>
-        </is>
-      </c>
+      <c r="A642" t="inlineStr"/>
+      <c r="B642" t="inlineStr"/>
       <c r="C642" t="inlineStr"/>
       <c r="D642" t="inlineStr">
         <is>
@@ -16293,18 +15267,8 @@
       <c r="K642" t="inlineStr"/>
     </row>
     <row r="643">
-      <c r="A643" t="inlineStr">
-        <is>
-          <t>M038</t>
-        </is>
-      </c>
-      <c r="B643" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308525021745/25
-Lender Amount: 28854.86
-Borrower Amount: 28854.86</t>
-        </is>
-      </c>
+      <c r="A643" t="inlineStr"/>
+      <c r="B643" t="inlineStr"/>
       <c r="C643" t="inlineStr">
         <is>
           <t>07/Apr/2025</t>
@@ -16338,18 +15302,8 @@
       <c r="K643" t="inlineStr"/>
     </row>
     <row r="644">
-      <c r="A644" t="inlineStr">
-        <is>
-          <t>M038</t>
-        </is>
-      </c>
-      <c r="B644" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308525021745/25
-Lender Amount: 28854.86
-Borrower Amount: 28854.86</t>
-        </is>
-      </c>
+      <c r="A644" t="inlineStr"/>
+      <c r="B644" t="inlineStr"/>
       <c r="C644" t="inlineStr"/>
       <c r="D644" t="inlineStr"/>
       <c r="E644" s="4" t="inlineStr">
@@ -16365,18 +15319,8 @@
       <c r="K644" t="inlineStr"/>
     </row>
     <row r="645">
-      <c r="A645" t="inlineStr">
-        <is>
-          <t>M038</t>
-        </is>
-      </c>
-      <c r="B645" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308525021745/25
-Lender Amount: 28854.86
-Borrower Amount: 28854.86</t>
-        </is>
-      </c>
+      <c r="A645" t="inlineStr"/>
+      <c r="B645" t="inlineStr"/>
       <c r="C645" t="inlineStr"/>
       <c r="D645" t="inlineStr">
         <is>
@@ -16396,18 +15340,8 @@
       <c r="K645" t="inlineStr"/>
     </row>
     <row r="646">
-      <c r="A646" t="inlineStr">
-        <is>
-          <t>M039</t>
-        </is>
-      </c>
-      <c r="B646" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524026037/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="A646" t="inlineStr"/>
+      <c r="B646" t="inlineStr"/>
       <c r="C646" t="inlineStr">
         <is>
           <t>07/Apr/2025</t>
@@ -16441,18 +15375,8 @@
       <c r="K646" t="inlineStr"/>
     </row>
     <row r="647">
-      <c r="A647" t="inlineStr">
-        <is>
-          <t>M039</t>
-        </is>
-      </c>
-      <c r="B647" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524026037/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="A647" t="inlineStr"/>
+      <c r="B647" t="inlineStr"/>
       <c r="C647" t="inlineStr"/>
       <c r="D647" t="inlineStr"/>
       <c r="E647" s="4" t="inlineStr">
@@ -16468,18 +15392,8 @@
       <c r="K647" t="inlineStr"/>
     </row>
     <row r="648">
-      <c r="A648" t="inlineStr">
-        <is>
-          <t>M039</t>
-        </is>
-      </c>
-      <c r="B648" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524026037/24
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="A648" t="inlineStr"/>
+      <c r="B648" t="inlineStr"/>
       <c r="C648" t="inlineStr"/>
       <c r="D648" t="inlineStr">
         <is>
@@ -17012,16 +15926,10 @@
     <row r="670">
       <c r="A670" t="inlineStr">
         <is>
-          <t>M040</t>
-        </is>
-      </c>
-      <c r="B670" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/25
-Lender Amount: 80051.03
-Borrower Amount: 80051.03</t>
-        </is>
-      </c>
+          <t>M004</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr"/>
       <c r="C670" t="inlineStr">
         <is>
           <t>15/Apr/2025</t>
@@ -17057,7 +15965,7 @@
     <row r="671">
       <c r="A671" t="inlineStr">
         <is>
-          <t>M040</t>
+          <t>M004</t>
         </is>
       </c>
       <c r="B671" s="4" t="inlineStr">
@@ -17084,16 +15992,10 @@
     <row r="672">
       <c r="A672" t="inlineStr">
         <is>
-          <t>M040</t>
-        </is>
-      </c>
-      <c r="B672" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/25
-Lender Amount: 80051.03
-Borrower Amount: 80051.03</t>
-        </is>
-      </c>
+          <t>M004</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr"/>
       <c r="C672" t="inlineStr"/>
       <c r="D672" t="inlineStr">
         <is>
@@ -17113,18 +16015,8 @@
       <c r="K672" t="inlineStr"/>
     </row>
     <row r="673">
-      <c r="A673" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
-      <c r="B673" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="A673" t="inlineStr"/>
+      <c r="B673" t="inlineStr"/>
       <c r="C673" t="inlineStr">
         <is>
           <t>16/Apr/2025</t>
@@ -17158,18 +16050,8 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
-      <c r="B674" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="A674" t="inlineStr"/>
+      <c r="B674" t="inlineStr"/>
       <c r="C674" t="inlineStr"/>
       <c r="D674" t="inlineStr"/>
       <c r="E674" s="4" t="inlineStr">
@@ -17187,18 +16069,8 @@
       <c r="K674" t="inlineStr"/>
     </row>
     <row r="675">
-      <c r="A675" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
-      <c r="B675" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="A675" t="inlineStr"/>
+      <c r="B675" t="inlineStr"/>
       <c r="C675" t="inlineStr"/>
       <c r="D675" t="inlineStr"/>
       <c r="E675" s="4" t="inlineStr">
@@ -17216,18 +16088,8 @@
       <c r="K675" t="inlineStr"/>
     </row>
     <row r="676">
-      <c r="A676" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
-      <c r="B676" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="A676" t="inlineStr"/>
+      <c r="B676" t="inlineStr"/>
       <c r="C676" t="inlineStr"/>
       <c r="D676" t="inlineStr"/>
       <c r="E676" s="4" t="inlineStr">
@@ -17243,18 +16105,8 @@
       <c r="K676" t="inlineStr"/>
     </row>
     <row r="677">
-      <c r="A677" t="inlineStr">
-        <is>
-          <t>M041</t>
-        </is>
-      </c>
-      <c r="B677" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 6777058.20
-Borrower Amount: 6777058.20</t>
-        </is>
-      </c>
+      <c r="A677" t="inlineStr"/>
+      <c r="B677" t="inlineStr"/>
       <c r="C677" t="inlineStr"/>
       <c r="D677" t="inlineStr">
         <is>
@@ -17347,18 +16199,8 @@
       <c r="K680" t="inlineStr"/>
     </row>
     <row r="681">
-      <c r="A681" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
-      <c r="B681" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="A681" t="inlineStr"/>
+      <c r="B681" t="inlineStr"/>
       <c r="C681" t="inlineStr">
         <is>
           <t>17/Apr/2025</t>
@@ -17392,18 +16234,8 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
-      <c r="B682" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="A682" t="inlineStr"/>
+      <c r="B682" t="inlineStr"/>
       <c r="C682" t="inlineStr"/>
       <c r="D682" t="inlineStr"/>
       <c r="E682" s="4" t="inlineStr">
@@ -17421,18 +16253,8 @@
       <c r="K682" t="inlineStr"/>
     </row>
     <row r="683">
-      <c r="A683" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
-      <c r="B683" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="A683" t="inlineStr"/>
+      <c r="B683" t="inlineStr"/>
       <c r="C683" t="inlineStr"/>
       <c r="D683" t="inlineStr"/>
       <c r="E683" s="4" t="inlineStr">
@@ -17450,18 +16272,8 @@
       <c r="K683" t="inlineStr"/>
     </row>
     <row r="684">
-      <c r="A684" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
-      <c r="B684" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="A684" t="inlineStr"/>
+      <c r="B684" t="inlineStr"/>
       <c r="C684" t="inlineStr"/>
       <c r="D684" t="inlineStr"/>
       <c r="E684" s="4" t="inlineStr">
@@ -17477,18 +16289,8 @@
       <c r="K684" t="inlineStr"/>
     </row>
     <row r="685">
-      <c r="A685" t="inlineStr">
-        <is>
-          <t>M042</t>
-        </is>
-      </c>
-      <c r="B685" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-155823010186/23
-Lender Amount: 76000.00
-Borrower Amount: 76000.00</t>
-        </is>
-      </c>
+      <c r="A685" t="inlineStr"/>
+      <c r="B685" t="inlineStr"/>
       <c r="C685" t="inlineStr"/>
       <c r="D685" t="inlineStr">
         <is>
@@ -17727,18 +16529,8 @@
       <c r="K694" t="inlineStr"/>
     </row>
     <row r="695">
-      <c r="A695" t="inlineStr">
-        <is>
-          <t>M043</t>
-        </is>
-      </c>
-      <c r="B695" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524026037/222824023549
-Lender Amount: 1226351.09
-Borrower Amount: 1226351.09</t>
-        </is>
-      </c>
+      <c r="A695" t="inlineStr"/>
+      <c r="B695" t="inlineStr"/>
       <c r="C695" t="inlineStr">
         <is>
           <t>21/Apr/2025</t>
@@ -17772,18 +16564,8 @@
       <c r="K695" t="inlineStr"/>
     </row>
     <row r="696">
-      <c r="A696" t="inlineStr">
-        <is>
-          <t>M043</t>
-        </is>
-      </c>
-      <c r="B696" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524026037/222824023549
-Lender Amount: 1226351.09
-Borrower Amount: 1226351.09</t>
-        </is>
-      </c>
+      <c r="A696" t="inlineStr"/>
+      <c r="B696" t="inlineStr"/>
       <c r="C696" t="inlineStr"/>
       <c r="D696" t="inlineStr"/>
       <c r="E696" s="4" t="inlineStr">
@@ -17799,18 +16581,8 @@
       <c r="K696" t="inlineStr"/>
     </row>
     <row r="697">
-      <c r="A697" t="inlineStr">
-        <is>
-          <t>M043</t>
-        </is>
-      </c>
-      <c r="B697" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524026037/222824023549
-Lender Amount: 1226351.09
-Borrower Amount: 1226351.09</t>
-        </is>
-      </c>
+      <c r="A697" t="inlineStr"/>
+      <c r="B697" t="inlineStr"/>
       <c r="C697" t="inlineStr"/>
       <c r="D697" t="inlineStr">
         <is>
@@ -17903,18 +16675,8 @@
       <c r="K700" t="inlineStr"/>
     </row>
     <row r="701">
-      <c r="A701" t="inlineStr">
-        <is>
-          <t>M044</t>
-        </is>
-      </c>
-      <c r="B701" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524022495/24
-Lender Amount: 1675000.00
-Borrower Amount: 1675000.00</t>
-        </is>
-      </c>
+      <c r="A701" t="inlineStr"/>
+      <c r="B701" t="inlineStr"/>
       <c r="C701" t="inlineStr">
         <is>
           <t>21/Apr/2025</t>
@@ -17948,18 +16710,8 @@
       </c>
     </row>
     <row r="702">
-      <c r="A702" t="inlineStr">
-        <is>
-          <t>M044</t>
-        </is>
-      </c>
-      <c r="B702" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524022495/24
-Lender Amount: 1675000.00
-Borrower Amount: 1675000.00</t>
-        </is>
-      </c>
+      <c r="A702" t="inlineStr"/>
+      <c r="B702" t="inlineStr"/>
       <c r="C702" t="inlineStr"/>
       <c r="D702" t="inlineStr"/>
       <c r="E702" s="4" t="inlineStr">
@@ -17975,18 +16727,8 @@
       <c r="K702" t="inlineStr"/>
     </row>
     <row r="703">
-      <c r="A703" t="inlineStr">
-        <is>
-          <t>M044</t>
-        </is>
-      </c>
-      <c r="B703" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524022495/24
-Lender Amount: 1675000.00
-Borrower Amount: 1675000.00</t>
-        </is>
-      </c>
+      <c r="A703" t="inlineStr"/>
+      <c r="B703" t="inlineStr"/>
       <c r="C703" t="inlineStr"/>
       <c r="D703" t="inlineStr">
         <is>
@@ -18152,18 +16894,8 @@
       <c r="K709" t="inlineStr"/>
     </row>
     <row r="710">
-      <c r="A710" t="inlineStr">
-        <is>
-          <t>M045</t>
-        </is>
-      </c>
-      <c r="B710" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020027/25
-Lender Amount: 10691988.92
-Borrower Amount: 10691988.92</t>
-        </is>
-      </c>
+      <c r="A710" t="inlineStr"/>
+      <c r="B710" t="inlineStr"/>
       <c r="C710" t="inlineStr">
         <is>
           <t>22/Apr/2025</t>
@@ -18197,18 +16929,8 @@
       <c r="K710" t="inlineStr"/>
     </row>
     <row r="711">
-      <c r="A711" t="inlineStr">
-        <is>
-          <t>M045</t>
-        </is>
-      </c>
-      <c r="B711" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020027/25
-Lender Amount: 10691988.92
-Borrower Amount: 10691988.92</t>
-        </is>
-      </c>
+      <c r="A711" t="inlineStr"/>
+      <c r="B711" t="inlineStr"/>
       <c r="C711" t="inlineStr"/>
       <c r="D711" t="inlineStr"/>
       <c r="E711" s="4" t="inlineStr">
@@ -18224,18 +16946,8 @@
       <c r="K711" t="inlineStr"/>
     </row>
     <row r="712">
-      <c r="A712" t="inlineStr">
-        <is>
-          <t>M045</t>
-        </is>
-      </c>
-      <c r="B712" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020027/25
-Lender Amount: 10691988.92
-Borrower Amount: 10691988.92</t>
-        </is>
-      </c>
+      <c r="A712" t="inlineStr"/>
+      <c r="B712" t="inlineStr"/>
       <c r="C712" t="inlineStr"/>
       <c r="D712" t="inlineStr">
         <is>
@@ -18255,18 +16967,8 @@
       <c r="K712" t="inlineStr"/>
     </row>
     <row r="713">
-      <c r="A713" t="inlineStr">
-        <is>
-          <t>M046</t>
-        </is>
-      </c>
-      <c r="B713" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-222825150151/25
-Lender Amount: 333706.76
-Borrower Amount: 333706.76</t>
-        </is>
-      </c>
+      <c r="A713" t="inlineStr"/>
+      <c r="B713" t="inlineStr"/>
       <c r="C713" t="inlineStr">
         <is>
           <t>22/Apr/2025</t>
@@ -18300,18 +17002,8 @@
       <c r="K713" t="inlineStr"/>
     </row>
     <row r="714">
-      <c r="A714" t="inlineStr">
-        <is>
-          <t>M046</t>
-        </is>
-      </c>
-      <c r="B714" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-222825150151/25
-Lender Amount: 333706.76
-Borrower Amount: 333706.76</t>
-        </is>
-      </c>
+      <c r="A714" t="inlineStr"/>
+      <c r="B714" t="inlineStr"/>
       <c r="C714" t="inlineStr"/>
       <c r="D714" t="inlineStr"/>
       <c r="E714" s="4" t="inlineStr">
@@ -18327,18 +17019,8 @@
       <c r="K714" t="inlineStr"/>
     </row>
     <row r="715">
-      <c r="A715" t="inlineStr">
-        <is>
-          <t>M046</t>
-        </is>
-      </c>
-      <c r="B715" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-222825150151/25
-Lender Amount: 333706.76
-Borrower Amount: 333706.76</t>
-        </is>
-      </c>
+      <c r="A715" t="inlineStr"/>
+      <c r="B715" t="inlineStr"/>
       <c r="C715" t="inlineStr"/>
       <c r="D715" t="inlineStr">
         <is>
@@ -18358,18 +17040,8 @@
       <c r="K715" t="inlineStr"/>
     </row>
     <row r="716">
-      <c r="A716" t="inlineStr">
-        <is>
-          <t>M047</t>
-        </is>
-      </c>
-      <c r="B716" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 299000.00
-Borrower Amount: 299000.00</t>
-        </is>
-      </c>
+      <c r="A716" t="inlineStr"/>
+      <c r="B716" t="inlineStr"/>
       <c r="C716" t="inlineStr">
         <is>
           <t>23/Apr/2025</t>
@@ -18403,18 +17075,8 @@
       </c>
     </row>
     <row r="717">
-      <c r="A717" t="inlineStr">
-        <is>
-          <t>M047</t>
-        </is>
-      </c>
-      <c r="B717" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 299000.00
-Borrower Amount: 299000.00</t>
-        </is>
-      </c>
+      <c r="A717" t="inlineStr"/>
+      <c r="B717" t="inlineStr"/>
       <c r="C717" t="inlineStr"/>
       <c r="D717" t="inlineStr"/>
       <c r="E717" s="4" t="inlineStr">
@@ -18430,18 +17092,8 @@
       <c r="K717" t="inlineStr"/>
     </row>
     <row r="718">
-      <c r="A718" t="inlineStr">
-        <is>
-          <t>M047</t>
-        </is>
-      </c>
-      <c r="B718" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020063/25
-Lender Amount: 299000.00
-Borrower Amount: 299000.00</t>
-        </is>
-      </c>
+      <c r="A718" t="inlineStr"/>
+      <c r="B718" t="inlineStr"/>
       <c r="C718" t="inlineStr"/>
       <c r="D718" t="inlineStr">
         <is>
@@ -18534,18 +17186,8 @@
       <c r="K721" t="inlineStr"/>
     </row>
     <row r="722">
-      <c r="A722" t="inlineStr">
-        <is>
-          <t>M048</t>
-        </is>
-      </c>
-      <c r="B722" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524026037/24
-Lender Amount: 13743.52
-Borrower Amount: 13743.52</t>
-        </is>
-      </c>
+      <c r="A722" t="inlineStr"/>
+      <c r="B722" t="inlineStr"/>
       <c r="C722" t="inlineStr">
         <is>
           <t>23/Apr/2025</t>
@@ -18579,18 +17221,8 @@
       <c r="K722" t="inlineStr"/>
     </row>
     <row r="723">
-      <c r="A723" t="inlineStr">
-        <is>
-          <t>M048</t>
-        </is>
-      </c>
-      <c r="B723" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524026037/24
-Lender Amount: 13743.52
-Borrower Amount: 13743.52</t>
-        </is>
-      </c>
+      <c r="A723" t="inlineStr"/>
+      <c r="B723" t="inlineStr"/>
       <c r="C723" t="inlineStr"/>
       <c r="D723" t="inlineStr"/>
       <c r="E723" s="4" t="inlineStr">
@@ -18606,18 +17238,8 @@
       <c r="K723" t="inlineStr"/>
     </row>
     <row r="724">
-      <c r="A724" t="inlineStr">
-        <is>
-          <t>M048</t>
-        </is>
-      </c>
-      <c r="B724" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524026037/24
-Lender Amount: 13743.52
-Borrower Amount: 13743.52</t>
-        </is>
-      </c>
+      <c r="A724" t="inlineStr"/>
+      <c r="B724" t="inlineStr"/>
       <c r="C724" t="inlineStr"/>
       <c r="D724" t="inlineStr">
         <is>
@@ -18878,18 +17500,8 @@
       <c r="K735" t="inlineStr"/>
     </row>
     <row r="736">
-      <c r="A736" t="inlineStr">
-        <is>
-          <t>M049</t>
-        </is>
-      </c>
-      <c r="B736" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155825020020/25
-Lender Amount: 60302.55
-Borrower Amount: 60302.55</t>
-        </is>
-      </c>
+      <c r="A736" t="inlineStr"/>
+      <c r="B736" t="inlineStr"/>
       <c r="C736" t="inlineStr">
         <is>
           <t>27/Apr/2025</t>
@@ -18923,18 +17535,8 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" t="inlineStr">
-        <is>
-          <t>M049</t>
-        </is>
-      </c>
-      <c r="B737" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155825020020/25
-Lender Amount: 60302.55
-Borrower Amount: 60302.55</t>
-        </is>
-      </c>
+      <c r="A737" t="inlineStr"/>
+      <c r="B737" t="inlineStr"/>
       <c r="C737" t="inlineStr"/>
       <c r="D737" t="inlineStr"/>
       <c r="E737" s="4" t="inlineStr">
@@ -18950,18 +17552,8 @@
       <c r="K737" t="inlineStr"/>
     </row>
     <row r="738">
-      <c r="A738" t="inlineStr">
-        <is>
-          <t>M049</t>
-        </is>
-      </c>
-      <c r="B738" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155825020020/25
-Lender Amount: 60302.55
-Borrower Amount: 60302.55</t>
-        </is>
-      </c>
+      <c r="A738" t="inlineStr"/>
+      <c r="B738" t="inlineStr"/>
       <c r="C738" t="inlineStr"/>
       <c r="D738" t="inlineStr">
         <is>
@@ -18981,18 +17573,8 @@
       <c r="K738" t="inlineStr"/>
     </row>
     <row r="739">
-      <c r="A739" t="inlineStr">
-        <is>
-          <t>M050</t>
-        </is>
-      </c>
-      <c r="B739" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 124008.78
-Borrower Amount: 124008.78</t>
-        </is>
-      </c>
+      <c r="A739" t="inlineStr"/>
+      <c r="B739" t="inlineStr"/>
       <c r="C739" t="inlineStr">
         <is>
           <t>27/Apr/2025</t>
@@ -19026,18 +17608,8 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" t="inlineStr">
-        <is>
-          <t>M050</t>
-        </is>
-      </c>
-      <c r="B740" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 124008.78
-Borrower Amount: 124008.78</t>
-        </is>
-      </c>
+      <c r="A740" t="inlineStr"/>
+      <c r="B740" t="inlineStr"/>
       <c r="C740" t="inlineStr"/>
       <c r="D740" t="inlineStr"/>
       <c r="E740" s="4" t="inlineStr">
@@ -19053,18 +17625,8 @@
       <c r="K740" t="inlineStr"/>
     </row>
     <row r="741">
-      <c r="A741" t="inlineStr">
-        <is>
-          <t>M050</t>
-        </is>
-      </c>
-      <c r="B741" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 124008.78
-Borrower Amount: 124008.78</t>
-        </is>
-      </c>
+      <c r="A741" t="inlineStr"/>
+      <c r="B741" t="inlineStr"/>
       <c r="C741" t="inlineStr"/>
       <c r="D741" t="inlineStr">
         <is>
@@ -19084,18 +17646,8 @@
       <c r="K741" t="inlineStr"/>
     </row>
     <row r="742">
-      <c r="A742" t="inlineStr">
-        <is>
-          <t>M051</t>
-        </is>
-      </c>
-      <c r="B742" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/25
-Lender Amount: 31609.80
-Borrower Amount: 31609.80</t>
-        </is>
-      </c>
+      <c r="A742" t="inlineStr"/>
+      <c r="B742" t="inlineStr"/>
       <c r="C742" t="inlineStr">
         <is>
           <t>28/Apr/2025</t>
@@ -19129,18 +17681,8 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" t="inlineStr">
-        <is>
-          <t>M051</t>
-        </is>
-      </c>
-      <c r="B743" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/25
-Lender Amount: 31609.80
-Borrower Amount: 31609.80</t>
-        </is>
-      </c>
+      <c r="A743" t="inlineStr"/>
+      <c r="B743" t="inlineStr"/>
       <c r="C743" t="inlineStr"/>
       <c r="D743" t="inlineStr"/>
       <c r="E743" s="4" t="inlineStr">
@@ -19156,18 +17698,8 @@
       <c r="K743" t="inlineStr"/>
     </row>
     <row r="744">
-      <c r="A744" t="inlineStr">
-        <is>
-          <t>M051</t>
-        </is>
-      </c>
-      <c r="B744" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/25
-Lender Amount: 31609.80
-Borrower Amount: 31609.80</t>
-        </is>
-      </c>
+      <c r="A744" t="inlineStr"/>
+      <c r="B744" t="inlineStr"/>
       <c r="C744" t="inlineStr"/>
       <c r="D744" t="inlineStr">
         <is>
@@ -19590,18 +18122,8 @@
       <c r="K761" t="inlineStr"/>
     </row>
     <row r="762">
-      <c r="A762" t="inlineStr">
-        <is>
-          <t>M052</t>
-        </is>
-      </c>
-      <c r="B762" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 10424886.36
-Borrower Amount: 10424886.36</t>
-        </is>
-      </c>
+      <c r="A762" t="inlineStr"/>
+      <c r="B762" t="inlineStr"/>
       <c r="C762" t="inlineStr">
         <is>
           <t>30/Apr/2025</t>
@@ -19635,18 +18157,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" t="inlineStr">
-        <is>
-          <t>M052</t>
-        </is>
-      </c>
-      <c r="B763" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 10424886.36
-Borrower Amount: 10424886.36</t>
-        </is>
-      </c>
+      <c r="A763" t="inlineStr"/>
+      <c r="B763" t="inlineStr"/>
       <c r="C763" t="inlineStr"/>
       <c r="D763" t="inlineStr"/>
       <c r="E763" s="4" t="inlineStr">
@@ -19662,18 +18174,8 @@
       <c r="K763" t="inlineStr"/>
     </row>
     <row r="764">
-      <c r="A764" t="inlineStr">
-        <is>
-          <t>M052</t>
-        </is>
-      </c>
-      <c r="B764" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020104/25
-Lender Amount: 10424886.36
-Borrower Amount: 10424886.36</t>
-        </is>
-      </c>
+      <c r="A764" t="inlineStr"/>
+      <c r="B764" t="inlineStr"/>
       <c r="C764" t="inlineStr"/>
       <c r="D764" t="inlineStr">
         <is>
@@ -19693,18 +18195,8 @@
       <c r="K764" t="inlineStr"/>
     </row>
     <row r="765">
-      <c r="A765" t="inlineStr">
-        <is>
-          <t>M053</t>
-        </is>
-      </c>
-      <c r="B765" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020063/25
-Lender Amount: 2168751.40
-Borrower Amount: 2168751.40</t>
-        </is>
-      </c>
+      <c r="A765" t="inlineStr"/>
+      <c r="B765" t="inlineStr"/>
       <c r="C765" t="inlineStr">
         <is>
           <t>30/Apr/2025</t>
@@ -19738,18 +18230,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" t="inlineStr">
-        <is>
-          <t>M053</t>
-        </is>
-      </c>
-      <c r="B766" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020063/25
-Lender Amount: 2168751.40
-Borrower Amount: 2168751.40</t>
-        </is>
-      </c>
+      <c r="A766" t="inlineStr"/>
+      <c r="B766" t="inlineStr"/>
       <c r="C766" t="inlineStr"/>
       <c r="D766" t="inlineStr"/>
       <c r="E766" s="4" t="inlineStr">
@@ -19765,18 +18247,8 @@
       <c r="K766" t="inlineStr"/>
     </row>
     <row r="767">
-      <c r="A767" t="inlineStr">
-        <is>
-          <t>M053</t>
-        </is>
-      </c>
-      <c r="B767" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020063/25
-Lender Amount: 2168751.40
-Borrower Amount: 2168751.40</t>
-        </is>
-      </c>
+      <c r="A767" t="inlineStr"/>
+      <c r="B767" t="inlineStr"/>
       <c r="C767" t="inlineStr"/>
       <c r="D767" t="inlineStr">
         <is>
@@ -19869,18 +18341,8 @@
       <c r="K770" t="inlineStr"/>
     </row>
     <row r="771">
-      <c r="A771" t="inlineStr">
-        <is>
-          <t>M054</t>
-        </is>
-      </c>
-      <c r="B771" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020068/25
-Lender Amount: 63787.54
-Borrower Amount: 63787.54</t>
-        </is>
-      </c>
+      <c r="A771" t="inlineStr"/>
+      <c r="B771" t="inlineStr"/>
       <c r="C771" t="inlineStr">
         <is>
           <t>30/Apr/2025</t>
@@ -19914,18 +18376,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" t="inlineStr">
-        <is>
-          <t>M054</t>
-        </is>
-      </c>
-      <c r="B772" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020068/25
-Lender Amount: 63787.54
-Borrower Amount: 63787.54</t>
-        </is>
-      </c>
+      <c r="A772" t="inlineStr"/>
+      <c r="B772" t="inlineStr"/>
       <c r="C772" t="inlineStr"/>
       <c r="D772" t="inlineStr"/>
       <c r="E772" s="4" t="inlineStr">
@@ -19941,18 +18393,8 @@
       <c r="K772" t="inlineStr"/>
     </row>
     <row r="773">
-      <c r="A773" t="inlineStr">
-        <is>
-          <t>M054</t>
-        </is>
-      </c>
-      <c r="B773" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-141325020068/25
-Lender Amount: 63787.54
-Borrower Amount: 63787.54</t>
-        </is>
-      </c>
+      <c r="A773" t="inlineStr"/>
+      <c r="B773" t="inlineStr"/>
       <c r="C773" t="inlineStr"/>
       <c r="D773" t="inlineStr">
         <is>
@@ -23355,18 +21797,8 @@
       <c r="K919" t="inlineStr"/>
     </row>
     <row r="920">
-      <c r="A920" t="inlineStr">
-        <is>
-          <t>M055</t>
-        </is>
-      </c>
-      <c r="B920" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020104/25
-Lender Amount: 111771.42
-Borrower Amount: 111771.42</t>
-        </is>
-      </c>
+      <c r="A920" t="inlineStr"/>
+      <c r="B920" t="inlineStr"/>
       <c r="C920" t="inlineStr">
         <is>
           <t>17/May/2025</t>
@@ -23400,18 +21832,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" t="inlineStr">
-        <is>
-          <t>M055</t>
-        </is>
-      </c>
-      <c r="B921" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020104/25
-Lender Amount: 111771.42
-Borrower Amount: 111771.42</t>
-        </is>
-      </c>
+      <c r="A921" t="inlineStr"/>
+      <c r="B921" t="inlineStr"/>
       <c r="C921" t="inlineStr"/>
       <c r="D921" t="inlineStr"/>
       <c r="E921" s="4" t="inlineStr">
@@ -23427,18 +21849,8 @@
       <c r="K921" t="inlineStr"/>
     </row>
     <row r="922">
-      <c r="A922" t="inlineStr">
-        <is>
-          <t>M055</t>
-        </is>
-      </c>
-      <c r="B922" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020104/25
-Lender Amount: 111771.42
-Borrower Amount: 111771.42</t>
-        </is>
-      </c>
+      <c r="A922" t="inlineStr"/>
+      <c r="B922" t="inlineStr"/>
       <c r="C922" t="inlineStr"/>
       <c r="D922" t="inlineStr">
         <is>
@@ -23458,18 +21870,8 @@
       <c r="K922" t="inlineStr"/>
     </row>
     <row r="923">
-      <c r="A923" t="inlineStr">
-        <is>
-          <t>M056</t>
-        </is>
-      </c>
-      <c r="B923" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020112/25
-Lender Amount: 80701.76
-Borrower Amount: 80701.76</t>
-        </is>
-      </c>
+      <c r="A923" t="inlineStr"/>
+      <c r="B923" t="inlineStr"/>
       <c r="C923" t="inlineStr">
         <is>
           <t>17/May/2025</t>
@@ -23503,18 +21905,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" t="inlineStr">
-        <is>
-          <t>M056</t>
-        </is>
-      </c>
-      <c r="B924" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020112/25
-Lender Amount: 80701.76
-Borrower Amount: 80701.76</t>
-        </is>
-      </c>
+      <c r="A924" t="inlineStr"/>
+      <c r="B924" t="inlineStr"/>
       <c r="C924" t="inlineStr"/>
       <c r="D924" t="inlineStr"/>
       <c r="E924" s="4" t="inlineStr">
@@ -23530,18 +21922,8 @@
       <c r="K924" t="inlineStr"/>
     </row>
     <row r="925">
-      <c r="A925" t="inlineStr">
-        <is>
-          <t>M056</t>
-        </is>
-      </c>
-      <c r="B925" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020112/25
-Lender Amount: 80701.76
-Borrower Amount: 80701.76</t>
-        </is>
-      </c>
+      <c r="A925" t="inlineStr"/>
+      <c r="B925" t="inlineStr"/>
       <c r="C925" t="inlineStr"/>
       <c r="D925" t="inlineStr">
         <is>
@@ -23561,18 +21943,8 @@
       <c r="K925" t="inlineStr"/>
     </row>
     <row r="926">
-      <c r="A926" t="inlineStr">
-        <is>
-          <t>M057</t>
-        </is>
-      </c>
-      <c r="B926" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020112/25
-Lender Amount: 657.81
-Borrower Amount: 657.81</t>
-        </is>
-      </c>
+      <c r="A926" t="inlineStr"/>
+      <c r="B926" t="inlineStr"/>
       <c r="C926" t="inlineStr">
         <is>
           <t>17/May/2025</t>
@@ -23606,18 +21978,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" t="inlineStr">
-        <is>
-          <t>M057</t>
-        </is>
-      </c>
-      <c r="B927" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020112/25
-Lender Amount: 657.81
-Borrower Amount: 657.81</t>
-        </is>
-      </c>
+      <c r="A927" t="inlineStr"/>
+      <c r="B927" t="inlineStr"/>
       <c r="C927" t="inlineStr"/>
       <c r="D927" t="inlineStr"/>
       <c r="E927" s="4" t="inlineStr">
@@ -23633,18 +21995,8 @@
       <c r="K927" t="inlineStr"/>
     </row>
     <row r="928">
-      <c r="A928" t="inlineStr">
-        <is>
-          <t>M057</t>
-        </is>
-      </c>
-      <c r="B928" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020112/25
-Lender Amount: 657.81
-Borrower Amount: 657.81</t>
-        </is>
-      </c>
+      <c r="A928" t="inlineStr"/>
+      <c r="B928" t="inlineStr"/>
       <c r="C928" t="inlineStr"/>
       <c r="D928" t="inlineStr">
         <is>
@@ -23956,18 +22308,8 @@
       <c r="K940" t="inlineStr"/>
     </row>
     <row r="941">
-      <c r="A941" t="inlineStr">
-        <is>
-          <t>M058</t>
-        </is>
-      </c>
-      <c r="B941" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/25
-Lender Amount: 81730.06
-Borrower Amount: 81730.06</t>
-        </is>
-      </c>
+      <c r="A941" t="inlineStr"/>
+      <c r="B941" t="inlineStr"/>
       <c r="C941" t="inlineStr">
         <is>
           <t>18/May/2025</t>
@@ -24001,18 +22343,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" t="inlineStr">
-        <is>
-          <t>M058</t>
-        </is>
-      </c>
-      <c r="B942" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/25
-Lender Amount: 81730.06
-Borrower Amount: 81730.06</t>
-        </is>
-      </c>
+      <c r="A942" t="inlineStr"/>
+      <c r="B942" t="inlineStr"/>
       <c r="C942" t="inlineStr"/>
       <c r="D942" t="inlineStr"/>
       <c r="E942" s="4" t="inlineStr">
@@ -24028,18 +22360,8 @@
       <c r="K942" t="inlineStr"/>
     </row>
     <row r="943">
-      <c r="A943" t="inlineStr">
-        <is>
-          <t>M058</t>
-        </is>
-      </c>
-      <c r="B943" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/25
-Lender Amount: 81730.06
-Borrower Amount: 81730.06</t>
-        </is>
-      </c>
+      <c r="A943" t="inlineStr"/>
+      <c r="B943" t="inlineStr"/>
       <c r="C943" t="inlineStr"/>
       <c r="D943" t="inlineStr">
         <is>
@@ -24426,16 +22748,10 @@
     <row r="959">
       <c r="A959" t="inlineStr">
         <is>
-          <t>M059</t>
-        </is>
-      </c>
-      <c r="B959" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020163/25
-Lender Amount: 341847.68
-Borrower Amount: 341847.68</t>
-        </is>
-      </c>
+          <t>M005</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr"/>
       <c r="C959" t="inlineStr">
         <is>
           <t>25/May/2025</t>
@@ -24471,16 +22787,10 @@
     <row r="960">
       <c r="A960" t="inlineStr">
         <is>
-          <t>M059</t>
-        </is>
-      </c>
-      <c r="B960" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020163/25
-Lender Amount: 341847.68
-Borrower Amount: 341847.68</t>
-        </is>
-      </c>
+          <t>M005</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr"/>
       <c r="C960" t="inlineStr"/>
       <c r="D960" t="inlineStr"/>
       <c r="E960" s="4" t="inlineStr">
@@ -24500,16 +22810,10 @@
     <row r="961">
       <c r="A961" t="inlineStr">
         <is>
-          <t>M059</t>
-        </is>
-      </c>
-      <c r="B961" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020163/25
-Lender Amount: 341847.68
-Borrower Amount: 341847.68</t>
-        </is>
-      </c>
+          <t>M005</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr"/>
       <c r="C961" t="inlineStr"/>
       <c r="D961" t="inlineStr"/>
       <c r="E961" s="4" t="inlineStr">
@@ -24529,7 +22833,7 @@
     <row r="962">
       <c r="A962" t="inlineStr">
         <is>
-          <t>M059</t>
+          <t>M005</t>
         </is>
       </c>
       <c r="B962" s="4" t="inlineStr">
@@ -24556,16 +22860,10 @@
     <row r="963">
       <c r="A963" t="inlineStr">
         <is>
-          <t>M059</t>
-        </is>
-      </c>
-      <c r="B963" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020163/25
-Lender Amount: 341847.68
-Borrower Amount: 341847.68</t>
-        </is>
-      </c>
+          <t>M005</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr"/>
       <c r="C963" t="inlineStr"/>
       <c r="D963" t="inlineStr">
         <is>
@@ -24769,18 +23067,8 @@
       <c r="K971" t="inlineStr"/>
     </row>
     <row r="972">
-      <c r="A972" t="inlineStr">
-        <is>
-          <t>M060</t>
-        </is>
-      </c>
-      <c r="B972" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-222825150235/25
-Lender Amount: 36757.00
-Borrower Amount: 36757.00</t>
-        </is>
-      </c>
+      <c r="A972" t="inlineStr"/>
+      <c r="B972" t="inlineStr"/>
       <c r="C972" t="inlineStr">
         <is>
           <t>29/May/2025</t>
@@ -24814,18 +23102,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" t="inlineStr">
-        <is>
-          <t>M060</t>
-        </is>
-      </c>
-      <c r="B973" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-222825150235/25
-Lender Amount: 36757.00
-Borrower Amount: 36757.00</t>
-        </is>
-      </c>
+      <c r="A973" t="inlineStr"/>
+      <c r="B973" t="inlineStr"/>
       <c r="C973" t="inlineStr"/>
       <c r="D973" t="inlineStr"/>
       <c r="E973" s="4" t="inlineStr">
@@ -24841,18 +23119,8 @@
       <c r="K973" t="inlineStr"/>
     </row>
     <row r="974">
-      <c r="A974" t="inlineStr">
-        <is>
-          <t>M060</t>
-        </is>
-      </c>
-      <c r="B974" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-222825150235/25
-Lender Amount: 36757.00
-Borrower Amount: 36757.00</t>
-        </is>
-      </c>
+      <c r="A974" t="inlineStr"/>
+      <c r="B974" t="inlineStr"/>
       <c r="C974" t="inlineStr"/>
       <c r="D974" t="inlineStr">
         <is>
@@ -24945,18 +23213,8 @@
       <c r="K977" t="inlineStr"/>
     </row>
     <row r="978">
-      <c r="A978" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
-      <c r="B978" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="A978" t="inlineStr"/>
+      <c r="B978" t="inlineStr"/>
       <c r="C978" t="inlineStr">
         <is>
           <t>29/May/2025</t>
@@ -24990,18 +23248,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
-      <c r="B979" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="A979" t="inlineStr"/>
+      <c r="B979" t="inlineStr"/>
       <c r="C979" t="inlineStr"/>
       <c r="D979" t="inlineStr"/>
       <c r="E979" s="4" t="inlineStr">
@@ -25019,18 +23267,8 @@
       <c r="K979" t="inlineStr"/>
     </row>
     <row r="980">
-      <c r="A980" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
-      <c r="B980" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="A980" t="inlineStr"/>
+      <c r="B980" t="inlineStr"/>
       <c r="C980" t="inlineStr"/>
       <c r="D980" t="inlineStr"/>
       <c r="E980" s="4" t="inlineStr">
@@ -25048,18 +23286,8 @@
       <c r="K980" t="inlineStr"/>
     </row>
     <row r="981">
-      <c r="A981" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
-      <c r="B981" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="A981" t="inlineStr"/>
+      <c r="B981" t="inlineStr"/>
       <c r="C981" t="inlineStr"/>
       <c r="D981" t="inlineStr"/>
       <c r="E981" s="4" t="inlineStr">
@@ -25077,18 +23305,8 @@
       <c r="K981" t="inlineStr"/>
     </row>
     <row r="982">
-      <c r="A982" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
-      <c r="B982" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="A982" t="inlineStr"/>
+      <c r="B982" t="inlineStr"/>
       <c r="C982" t="inlineStr"/>
       <c r="D982" t="inlineStr"/>
       <c r="E982" s="4" t="inlineStr">
@@ -25104,18 +23322,8 @@
       <c r="K982" t="inlineStr"/>
     </row>
     <row r="983">
-      <c r="A983" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
-      <c r="B983" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020068/25
-Lender Amount: 3587219.00
-Borrower Amount: 3587219.00</t>
-        </is>
-      </c>
+      <c r="A983" t="inlineStr"/>
+      <c r="B983" t="inlineStr"/>
       <c r="C983" t="inlineStr"/>
       <c r="D983" t="inlineStr">
         <is>
@@ -25135,18 +23343,8 @@
       <c r="K983" t="inlineStr"/>
     </row>
     <row r="984">
-      <c r="A984" t="inlineStr">
-        <is>
-          <t>M062</t>
-        </is>
-      </c>
-      <c r="B984" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524990243/24
-Lender Amount: 68747.06
-Borrower Amount: 68747.06</t>
-        </is>
-      </c>
+      <c r="A984" t="inlineStr"/>
+      <c r="B984" t="inlineStr"/>
       <c r="C984" t="inlineStr">
         <is>
           <t>29/May/2025</t>
@@ -25180,18 +23378,8 @@
       <c r="K984" t="inlineStr"/>
     </row>
     <row r="985">
-      <c r="A985" t="inlineStr">
-        <is>
-          <t>M062</t>
-        </is>
-      </c>
-      <c r="B985" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524990243/24
-Lender Amount: 68747.06
-Borrower Amount: 68747.06</t>
-        </is>
-      </c>
+      <c r="A985" t="inlineStr"/>
+      <c r="B985" t="inlineStr"/>
       <c r="C985" t="inlineStr"/>
       <c r="D985" t="inlineStr"/>
       <c r="E985" s="4" t="inlineStr">
@@ -25207,18 +23395,8 @@
       <c r="K985" t="inlineStr"/>
     </row>
     <row r="986">
-      <c r="A986" t="inlineStr">
-        <is>
-          <t>M062</t>
-        </is>
-      </c>
-      <c r="B986" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524990243/24
-Lender Amount: 68747.06
-Borrower Amount: 68747.06</t>
-        </is>
-      </c>
+      <c r="A986" t="inlineStr"/>
+      <c r="B986" t="inlineStr"/>
       <c r="C986" t="inlineStr"/>
       <c r="D986" t="inlineStr">
         <is>
@@ -25772,18 +23950,8 @@
       <c r="K1009" t="inlineStr"/>
     </row>
     <row r="1010">
-      <c r="A1010" t="inlineStr">
-        <is>
-          <t>M063</t>
-        </is>
-      </c>
-      <c r="B1010" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308525021741/25
-Lender Amount: 31411.11
-Borrower Amount: 31411.11</t>
-        </is>
-      </c>
+      <c r="A1010" t="inlineStr"/>
+      <c r="B1010" t="inlineStr"/>
       <c r="C1010" t="inlineStr">
         <is>
           <t>01/Jun/2025</t>
@@ -25817,18 +23985,8 @@
       <c r="K1010" t="inlineStr"/>
     </row>
     <row r="1011">
-      <c r="A1011" t="inlineStr">
-        <is>
-          <t>M063</t>
-        </is>
-      </c>
-      <c r="B1011" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308525021741/25
-Lender Amount: 31411.11
-Borrower Amount: 31411.11</t>
-        </is>
-      </c>
+      <c r="A1011" t="inlineStr"/>
+      <c r="B1011" t="inlineStr"/>
       <c r="C1011" t="inlineStr"/>
       <c r="D1011" t="inlineStr"/>
       <c r="E1011" s="4" t="inlineStr">
@@ -25844,18 +24002,8 @@
       <c r="K1011" t="inlineStr"/>
     </row>
     <row r="1012">
-      <c r="A1012" t="inlineStr">
-        <is>
-          <t>M063</t>
-        </is>
-      </c>
-      <c r="B1012" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308525021741/25
-Lender Amount: 31411.11
-Borrower Amount: 31411.11</t>
-        </is>
-      </c>
+      <c r="A1012" t="inlineStr"/>
+      <c r="B1012" t="inlineStr"/>
       <c r="C1012" t="inlineStr"/>
       <c r="D1012" t="inlineStr">
         <is>
@@ -26314,18 +24462,8 @@
       <c r="K1030" t="inlineStr"/>
     </row>
     <row r="1031">
-      <c r="A1031" t="inlineStr">
-        <is>
-          <t>M064</t>
-        </is>
-      </c>
-      <c r="B1031" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155825010037/25
-Lender Amount: 853297.01
-Borrower Amount: 853297.01</t>
-        </is>
-      </c>
+      <c r="A1031" t="inlineStr"/>
+      <c r="B1031" t="inlineStr"/>
       <c r="C1031" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
@@ -26359,18 +24497,8 @@
       <c r="K1031" t="inlineStr"/>
     </row>
     <row r="1032">
-      <c r="A1032" t="inlineStr">
-        <is>
-          <t>M064</t>
-        </is>
-      </c>
-      <c r="B1032" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155825010037/25
-Lender Amount: 853297.01
-Borrower Amount: 853297.01</t>
-        </is>
-      </c>
+      <c r="A1032" t="inlineStr"/>
+      <c r="B1032" t="inlineStr"/>
       <c r="C1032" t="inlineStr"/>
       <c r="D1032" t="inlineStr"/>
       <c r="E1032" s="4" t="inlineStr">
@@ -26386,18 +24514,8 @@
       <c r="K1032" t="inlineStr"/>
     </row>
     <row r="1033">
-      <c r="A1033" t="inlineStr">
-        <is>
-          <t>M064</t>
-        </is>
-      </c>
-      <c r="B1033" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-155825010037/25
-Lender Amount: 853297.01
-Borrower Amount: 853297.01</t>
-        </is>
-      </c>
+      <c r="A1033" t="inlineStr"/>
+      <c r="B1033" t="inlineStr"/>
       <c r="C1033" t="inlineStr"/>
       <c r="D1033" t="inlineStr">
         <is>
@@ -28007,18 +26125,8 @@
       <c r="K1099" t="inlineStr"/>
     </row>
     <row r="1100">
-      <c r="A1100" t="inlineStr">
-        <is>
-          <t>M065</t>
-        </is>
-      </c>
-      <c r="B1100" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020163/25
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="A1100" t="inlineStr"/>
+      <c r="B1100" t="inlineStr"/>
       <c r="C1100" t="inlineStr">
         <is>
           <t>16/Jun/2025</t>
@@ -28052,18 +26160,8 @@
       </c>
     </row>
     <row r="1101">
-      <c r="A1101" t="inlineStr">
-        <is>
-          <t>M065</t>
-        </is>
-      </c>
-      <c r="B1101" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020163/25
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="A1101" t="inlineStr"/>
+      <c r="B1101" t="inlineStr"/>
       <c r="C1101" t="inlineStr"/>
       <c r="D1101" t="inlineStr"/>
       <c r="E1101" s="4" t="inlineStr">
@@ -28079,18 +26177,8 @@
       <c r="K1101" t="inlineStr"/>
     </row>
     <row r="1102">
-      <c r="A1102" t="inlineStr">
-        <is>
-          <t>M065</t>
-        </is>
-      </c>
-      <c r="B1102" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020163/25
-Lender Amount: 1725.00
-Borrower Amount: 1725.00</t>
-        </is>
-      </c>
+      <c r="A1102" t="inlineStr"/>
+      <c r="B1102" t="inlineStr"/>
       <c r="C1102" t="inlineStr"/>
       <c r="D1102" t="inlineStr">
         <is>
@@ -28110,18 +26198,8 @@
       <c r="K1102" t="inlineStr"/>
     </row>
     <row r="1103">
-      <c r="A1103" t="inlineStr">
-        <is>
-          <t>M066</t>
-        </is>
-      </c>
-      <c r="B1103" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308525021746/25
-Lender Amount: 35373.50
-Borrower Amount: 35373.50</t>
-        </is>
-      </c>
+      <c r="A1103" t="inlineStr"/>
+      <c r="B1103" t="inlineStr"/>
       <c r="C1103" t="inlineStr">
         <is>
           <t>17/Jun/2025</t>
@@ -28155,18 +26233,8 @@
       <c r="K1103" t="inlineStr"/>
     </row>
     <row r="1104">
-      <c r="A1104" t="inlineStr">
-        <is>
-          <t>M066</t>
-        </is>
-      </c>
-      <c r="B1104" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308525021746/25
-Lender Amount: 35373.50
-Borrower Amount: 35373.50</t>
-        </is>
-      </c>
+      <c r="A1104" t="inlineStr"/>
+      <c r="B1104" t="inlineStr"/>
       <c r="C1104" t="inlineStr"/>
       <c r="D1104" t="inlineStr"/>
       <c r="E1104" s="4" t="inlineStr">
@@ -28182,18 +26250,8 @@
       <c r="K1104" t="inlineStr"/>
     </row>
     <row r="1105">
-      <c r="A1105" t="inlineStr">
-        <is>
-          <t>M066</t>
-        </is>
-      </c>
-      <c r="B1105" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308525021746/25
-Lender Amount: 35373.50
-Borrower Amount: 35373.50</t>
-        </is>
-      </c>
+      <c r="A1105" t="inlineStr"/>
+      <c r="B1105" t="inlineStr"/>
       <c r="C1105" t="inlineStr"/>
       <c r="D1105" t="inlineStr">
         <is>
@@ -28689,18 +26747,8 @@
       <c r="K1125" t="inlineStr"/>
     </row>
     <row r="1126">
-      <c r="A1126" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B1126" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="A1126" t="inlineStr"/>
+      <c r="B1126" t="inlineStr"/>
       <c r="C1126" t="inlineStr">
         <is>
           <t>22/Jun/2025</t>
@@ -28734,18 +26782,8 @@
       <c r="K1126" t="inlineStr"/>
     </row>
     <row r="1127">
-      <c r="A1127" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B1127" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="A1127" t="inlineStr"/>
+      <c r="B1127" t="inlineStr"/>
       <c r="C1127" t="inlineStr"/>
       <c r="D1127" t="inlineStr"/>
       <c r="E1127" s="4" t="inlineStr">
@@ -28763,18 +26801,8 @@
       </c>
     </row>
     <row r="1128">
-      <c r="A1128" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B1128" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="A1128" t="inlineStr"/>
+      <c r="B1128" t="inlineStr"/>
       <c r="C1128" t="inlineStr"/>
       <c r="D1128" t="inlineStr"/>
       <c r="E1128" s="4" t="inlineStr">
@@ -28792,18 +26820,8 @@
       </c>
     </row>
     <row r="1129">
-      <c r="A1129" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B1129" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="A1129" t="inlineStr"/>
+      <c r="B1129" t="inlineStr"/>
       <c r="C1129" t="inlineStr"/>
       <c r="D1129" t="inlineStr"/>
       <c r="E1129" s="4" t="inlineStr">
@@ -28821,18 +26839,8 @@
       </c>
     </row>
     <row r="1130">
-      <c r="A1130" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B1130" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="A1130" t="inlineStr"/>
+      <c r="B1130" t="inlineStr"/>
       <c r="C1130" t="inlineStr"/>
       <c r="D1130" t="inlineStr"/>
       <c r="E1130" s="4" t="inlineStr">
@@ -28850,18 +26858,8 @@
       </c>
     </row>
     <row r="1131">
-      <c r="A1131" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B1131" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="A1131" t="inlineStr"/>
+      <c r="B1131" t="inlineStr"/>
       <c r="C1131" t="inlineStr"/>
       <c r="D1131" t="inlineStr"/>
       <c r="E1131" s="4" t="inlineStr">
@@ -28877,18 +26875,8 @@
       <c r="K1131" t="inlineStr"/>
     </row>
     <row r="1132">
-      <c r="A1132" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B1132" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-141325020063/141325020112
-Lender Amount: 576120.39
-Borrower Amount: 576120.39</t>
-        </is>
-      </c>
+      <c r="A1132" t="inlineStr"/>
+      <c r="B1132" t="inlineStr"/>
       <c r="C1132" t="inlineStr"/>
       <c r="D1132" t="inlineStr">
         <is>
@@ -28908,18 +26896,8 @@
       <c r="K1132" t="inlineStr"/>
     </row>
     <row r="1133">
-      <c r="A1133" t="inlineStr">
-        <is>
-          <t>M068</t>
-        </is>
-      </c>
-      <c r="B1133" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524022166 
-Lender Amount: 758000.00
-Borrower Amount: 758000.00</t>
-        </is>
-      </c>
+      <c r="A1133" t="inlineStr"/>
+      <c r="B1133" t="inlineStr"/>
       <c r="C1133" t="inlineStr">
         <is>
           <t>23/Jun/2025</t>
@@ -28953,18 +26931,8 @@
       </c>
     </row>
     <row r="1134">
-      <c r="A1134" t="inlineStr">
-        <is>
-          <t>M068</t>
-        </is>
-      </c>
-      <c r="B1134" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524022166 
-Lender Amount: 758000.00
-Borrower Amount: 758000.00</t>
-        </is>
-      </c>
+      <c r="A1134" t="inlineStr"/>
+      <c r="B1134" t="inlineStr"/>
       <c r="C1134" t="inlineStr"/>
       <c r="D1134" t="inlineStr"/>
       <c r="E1134" s="4" t="inlineStr">
@@ -28980,18 +26948,8 @@
       <c r="K1134" t="inlineStr"/>
     </row>
     <row r="1135">
-      <c r="A1135" t="inlineStr">
-        <is>
-          <t>M068</t>
-        </is>
-      </c>
-      <c r="B1135" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524022166 
-Lender Amount: 758000.00
-Borrower Amount: 758000.00</t>
-        </is>
-      </c>
+      <c r="A1135" t="inlineStr"/>
+      <c r="B1135" t="inlineStr"/>
       <c r="C1135" t="inlineStr"/>
       <c r="D1135" t="inlineStr">
         <is>
@@ -29595,18 +27553,8 @@
       <c r="K1159" t="inlineStr"/>
     </row>
     <row r="1160">
-      <c r="A1160" t="inlineStr">
-        <is>
-          <t>M069</t>
-        </is>
-      </c>
-      <c r="B1160" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524022166 
-Lender Amount: 4009000.00
-Borrower Amount: 4009000.00</t>
-        </is>
-      </c>
+      <c r="A1160" t="inlineStr"/>
+      <c r="B1160" t="inlineStr"/>
       <c r="C1160" t="inlineStr">
         <is>
           <t>24/Jun/2025</t>
@@ -29640,18 +27588,8 @@
       </c>
     </row>
     <row r="1161">
-      <c r="A1161" t="inlineStr">
-        <is>
-          <t>M069</t>
-        </is>
-      </c>
-      <c r="B1161" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524022166 
-Lender Amount: 4009000.00
-Borrower Amount: 4009000.00</t>
-        </is>
-      </c>
+      <c r="A1161" t="inlineStr"/>
+      <c r="B1161" t="inlineStr"/>
       <c r="C1161" t="inlineStr"/>
       <c r="D1161" t="inlineStr"/>
       <c r="E1161" s="4" t="inlineStr">
@@ -29667,18 +27605,8 @@
       <c r="K1161" t="inlineStr"/>
     </row>
     <row r="1162">
-      <c r="A1162" t="inlineStr">
-        <is>
-          <t>M069</t>
-        </is>
-      </c>
-      <c r="B1162" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: LC-308524022166 
-Lender Amount: 4009000.00
-Borrower Amount: 4009000.00</t>
-        </is>
-      </c>
+      <c r="A1162" t="inlineStr"/>
+      <c r="B1162" t="inlineStr"/>
       <c r="C1162" t="inlineStr"/>
       <c r="D1162" t="inlineStr">
         <is>
@@ -29844,18 +27772,8 @@
       <c r="K1168" t="inlineStr"/>
     </row>
     <row r="1169">
-      <c r="A1169" t="inlineStr">
-        <is>
-          <t>M070</t>
-        </is>
-      </c>
-      <c r="B1169" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524026037/24
-Lender Amount: 14417.98
-Borrower Amount: 14417.98</t>
-        </is>
-      </c>
+      <c r="A1169" t="inlineStr"/>
+      <c r="B1169" t="inlineStr"/>
       <c r="C1169" t="inlineStr">
         <is>
           <t>24/Jun/2025</t>
@@ -29889,18 +27807,8 @@
       <c r="K1169" t="inlineStr"/>
     </row>
     <row r="1170">
-      <c r="A1170" t="inlineStr">
-        <is>
-          <t>M070</t>
-        </is>
-      </c>
-      <c r="B1170" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524026037/24
-Lender Amount: 14417.98
-Borrower Amount: 14417.98</t>
-        </is>
-      </c>
+      <c r="A1170" t="inlineStr"/>
+      <c r="B1170" t="inlineStr"/>
       <c r="C1170" t="inlineStr"/>
       <c r="D1170" t="inlineStr"/>
       <c r="E1170" s="4" t="inlineStr">
@@ -29916,18 +27824,8 @@
       <c r="K1170" t="inlineStr"/>
     </row>
     <row r="1171">
-      <c r="A1171" t="inlineStr">
-        <is>
-          <t>M070</t>
-        </is>
-      </c>
-      <c r="B1171" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-308524026037/24
-Lender Amount: 14417.98
-Borrower Amount: 14417.98</t>
-        </is>
-      </c>
+      <c r="A1171" t="inlineStr"/>
+      <c r="B1171" t="inlineStr"/>
       <c r="C1171" t="inlineStr"/>
       <c r="D1171" t="inlineStr">
         <is>
@@ -30531,18 +28429,8 @@
       <c r="K1195" t="inlineStr"/>
     </row>
     <row r="1196">
-      <c r="A1196" t="inlineStr">
-        <is>
-          <t>M071</t>
-        </is>
-      </c>
-      <c r="B1196" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020202/25
-Lender Amount: 3499168.01
-Borrower Amount: 3499168.01</t>
-        </is>
-      </c>
+      <c r="A1196" t="inlineStr"/>
+      <c r="B1196" t="inlineStr"/>
       <c r="C1196" t="inlineStr">
         <is>
           <t>25/Jun/2025</t>
@@ -30576,18 +28464,8 @@
       <c r="K1196" t="inlineStr"/>
     </row>
     <row r="1197">
-      <c r="A1197" t="inlineStr">
-        <is>
-          <t>M071</t>
-        </is>
-      </c>
-      <c r="B1197" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020202/25
-Lender Amount: 3499168.01
-Borrower Amount: 3499168.01</t>
-        </is>
-      </c>
+      <c r="A1197" t="inlineStr"/>
+      <c r="B1197" t="inlineStr"/>
       <c r="C1197" t="inlineStr"/>
       <c r="D1197" t="inlineStr"/>
       <c r="E1197" s="4" t="inlineStr">
@@ -30603,18 +28481,8 @@
       <c r="K1197" t="inlineStr"/>
     </row>
     <row r="1198">
-      <c r="A1198" t="inlineStr">
-        <is>
-          <t>M071</t>
-        </is>
-      </c>
-      <c r="B1198" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147125020202/25
-Lender Amount: 3499168.01
-Borrower Amount: 3499168.01</t>
-        </is>
-      </c>
+      <c r="A1198" t="inlineStr"/>
+      <c r="B1198" t="inlineStr"/>
       <c r="C1198" t="inlineStr"/>
       <c r="D1198" t="inlineStr">
         <is>
@@ -31062,18 +28930,8 @@
       <c r="K1218" t="inlineStr"/>
     </row>
     <row r="1219">
-      <c r="A1219" t="inlineStr">
-        <is>
-          <t>M072</t>
-        </is>
-      </c>
-      <c r="B1219" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020074/24
-Lender Amount: 6242871.55
-Borrower Amount: 6242871.55</t>
-        </is>
-      </c>
+      <c r="A1219" t="inlineStr"/>
+      <c r="B1219" t="inlineStr"/>
       <c r="C1219" t="inlineStr">
         <is>
           <t>29/Jun/2025</t>
@@ -31107,18 +28965,8 @@
       <c r="K1219" t="inlineStr"/>
     </row>
     <row r="1220">
-      <c r="A1220" t="inlineStr">
-        <is>
-          <t>M072</t>
-        </is>
-      </c>
-      <c r="B1220" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020074/24
-Lender Amount: 6242871.55
-Borrower Amount: 6242871.55</t>
-        </is>
-      </c>
+      <c r="A1220" t="inlineStr"/>
+      <c r="B1220" t="inlineStr"/>
       <c r="C1220" t="inlineStr"/>
       <c r="D1220" t="inlineStr"/>
       <c r="E1220" s="4" t="inlineStr">
@@ -31134,18 +28982,8 @@
       <c r="K1220" t="inlineStr"/>
     </row>
     <row r="1221">
-      <c r="A1221" t="inlineStr">
-        <is>
-          <t>M072</t>
-        </is>
-      </c>
-      <c r="B1221" s="4" t="inlineStr">
-        <is>
-          <t>LC Match: L/C-147124020074/24
-Lender Amount: 6242871.55
-Borrower Amount: 6242871.55</t>
-        </is>
-      </c>
+      <c r="A1221" t="inlineStr"/>
+      <c r="B1221" t="inlineStr"/>
       <c r="C1221" t="inlineStr"/>
       <c r="D1221" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Integrate TransactionBlockIdentifier into ExcelTransactionMatcher for improved transaction block identification. Update narration extraction logic to differentiate between italic and regular text. Refactor transaction block retrieval methods to utilize the new identifier class, enhancing code clarity and maintainability.
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -1628,7 +1628,11 @@
       <c r="K55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr"/>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
@@ -1663,7 +1667,11 @@
       <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr"/>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
@@ -1682,7 +1690,11 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr"/>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
@@ -1701,7 +1713,11 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr"/>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
@@ -1720,8 +1736,18 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr"/>
-      <c r="B60" t="inlineStr"/>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 15737222.22
+Borrower Amount: 15737222.22</t>
+        </is>
+      </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" s="4" t="inlineStr">
@@ -1737,7 +1763,11 @@
       <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr"/>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
@@ -1904,7 +1934,11 @@
       <c r="K67" t="inlineStr"/>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr"/>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
@@ -1939,8 +1973,18 @@
       <c r="K68" t="inlineStr"/>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr"/>
-      <c r="B69" t="inlineStr"/>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="B69" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 8884.77
+Borrower Amount: 8884.77</t>
+        </is>
+      </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" s="4" t="inlineStr">
@@ -1956,7 +2000,11 @@
       <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr"/>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
@@ -1977,7 +2025,11 @@
       <c r="K70" t="inlineStr"/>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr"/>
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>M004</t>
+        </is>
+      </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
@@ -2012,8 +2064,18 @@
       <c r="K71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr"/>
-      <c r="B72" t="inlineStr"/>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>M004</t>
+        </is>
+      </c>
+      <c r="B72" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1575.00
+Borrower Amount: 1575.00</t>
+        </is>
+      </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
       <c r="E72" s="4" t="inlineStr">
@@ -2029,7 +2091,11 @@
       <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr"/>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>M004</t>
+        </is>
+      </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
@@ -2342,7 +2408,11 @@
       <c r="K85" t="inlineStr"/>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr"/>
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>M005</t>
+        </is>
+      </c>
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
@@ -2377,8 +2447,18 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr"/>
-      <c r="B87" t="inlineStr"/>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>M005</t>
+        </is>
+      </c>
+      <c r="B87" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010124/24
+Lender Amount: 1150.00
+Borrower Amount: 1150.00</t>
+        </is>
+      </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
       <c r="E87" s="4" t="inlineStr">
@@ -2394,7 +2474,11 @@
       <c r="K87" t="inlineStr"/>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr"/>
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>M005</t>
+        </is>
+      </c>
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
@@ -2415,7 +2499,11 @@
       <c r="K88" t="inlineStr"/>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr"/>
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>M004</t>
+        </is>
+      </c>
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr">
         <is>
@@ -2450,8 +2538,18 @@
       <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr"/>
-      <c r="B90" t="inlineStr"/>
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>M004</t>
+        </is>
+      </c>
+      <c r="B90" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1575.00
+Borrower Amount: 1575.00</t>
+        </is>
+      </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
       <c r="E90" s="4" t="inlineStr">
@@ -2467,7 +2565,11 @@
       <c r="K90" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr"/>
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>M004</t>
+        </is>
+      </c>
       <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
@@ -2853,7 +2955,11 @@
       <c r="K106" t="inlineStr"/>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr"/>
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>M006</t>
+        </is>
+      </c>
       <c r="B107" t="inlineStr"/>
       <c r="C107" t="inlineStr">
         <is>
@@ -2888,8 +2994,18 @@
       <c r="K107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr"/>
-      <c r="B108" t="inlineStr"/>
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>M006</t>
+        </is>
+      </c>
+      <c r="B108" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022796/24
+Lender Amount: 26246.93
+Borrower Amount: 26246.93</t>
+        </is>
+      </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
       <c r="E108" s="4" t="inlineStr">
@@ -2905,7 +3021,11 @@
       <c r="K108" t="inlineStr"/>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr"/>
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>M006</t>
+        </is>
+      </c>
       <c r="B109" t="inlineStr"/>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr">
@@ -5667,7 +5787,11 @@
       <c r="K228" t="inlineStr"/>
     </row>
     <row r="229">
-      <c r="A229" t="inlineStr"/>
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>M005</t>
+        </is>
+      </c>
       <c r="B229" t="inlineStr"/>
       <c r="C229" t="inlineStr">
         <is>
@@ -5702,8 +5826,18 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" t="inlineStr"/>
-      <c r="B230" t="inlineStr"/>
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>M005</t>
+        </is>
+      </c>
+      <c r="B230" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010124/24
+Lender Amount: 1150.00
+Borrower Amount: 1150.00</t>
+        </is>
+      </c>
       <c r="C230" t="inlineStr"/>
       <c r="D230" t="inlineStr"/>
       <c r="E230" s="4" t="inlineStr">
@@ -5719,7 +5853,11 @@
       <c r="K230" t="inlineStr"/>
     </row>
     <row r="231">
-      <c r="A231" t="inlineStr"/>
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>M005</t>
+        </is>
+      </c>
       <c r="B231" t="inlineStr"/>
       <c r="C231" t="inlineStr"/>
       <c r="D231" t="inlineStr">
@@ -5813,7 +5951,11 @@
       <c r="K234" t="inlineStr"/>
     </row>
     <row r="235">
-      <c r="A235" t="inlineStr"/>
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>M007</t>
+        </is>
+      </c>
       <c r="B235" t="inlineStr"/>
       <c r="C235" t="inlineStr">
         <is>
@@ -5848,8 +5990,18 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" t="inlineStr"/>
-      <c r="B236" t="inlineStr"/>
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>M007</t>
+        </is>
+      </c>
+      <c r="B236" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010124/24
+Lender Amount: 8761.79
+Borrower Amount: 8761.79</t>
+        </is>
+      </c>
       <c r="C236" t="inlineStr"/>
       <c r="D236" t="inlineStr"/>
       <c r="E236" s="4" t="inlineStr">
@@ -5865,7 +6017,11 @@
       <c r="K236" t="inlineStr"/>
     </row>
     <row r="237">
-      <c r="A237" t="inlineStr"/>
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>M007</t>
+        </is>
+      </c>
       <c r="B237" t="inlineStr"/>
       <c r="C237" t="inlineStr"/>
       <c r="D237" t="inlineStr">
@@ -6289,7 +6445,11 @@
       <c r="K254" t="inlineStr"/>
     </row>
     <row r="255">
-      <c r="A255" t="inlineStr"/>
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>M008</t>
+        </is>
+      </c>
       <c r="B255" t="inlineStr"/>
       <c r="C255" t="inlineStr">
         <is>
@@ -6324,8 +6484,18 @@
       <c r="K255" t="inlineStr"/>
     </row>
     <row r="256">
-      <c r="A256" t="inlineStr"/>
-      <c r="B256" t="inlineStr"/>
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>M008</t>
+        </is>
+      </c>
+      <c r="B256" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 1862.50
+Borrower Amount: 1862.50</t>
+        </is>
+      </c>
       <c r="C256" t="inlineStr"/>
       <c r="D256" t="inlineStr"/>
       <c r="E256" s="4" t="inlineStr">
@@ -6341,7 +6511,11 @@
       <c r="K256" t="inlineStr"/>
     </row>
     <row r="257">
-      <c r="A257" t="inlineStr"/>
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>M008</t>
+        </is>
+      </c>
       <c r="B257" t="inlineStr"/>
       <c r="C257" t="inlineStr"/>
       <c r="D257" t="inlineStr">
@@ -6784,7 +6958,11 @@
       <c r="K275" t="inlineStr"/>
     </row>
     <row r="276">
-      <c r="A276" t="inlineStr"/>
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>M009</t>
+        </is>
+      </c>
       <c r="B276" t="inlineStr"/>
       <c r="C276" t="inlineStr">
         <is>
@@ -6819,8 +6997,18 @@
       <c r="K276" t="inlineStr"/>
     </row>
     <row r="277">
-      <c r="A277" t="inlineStr"/>
-      <c r="B277" t="inlineStr"/>
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>M009</t>
+        </is>
+      </c>
+      <c r="B277" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020003/25
+Lender Amount: 27383.77
+Borrower Amount: 27383.77</t>
+        </is>
+      </c>
       <c r="C277" t="inlineStr"/>
       <c r="D277" t="inlineStr"/>
       <c r="E277" s="4" t="inlineStr">
@@ -6836,7 +7024,11 @@
       <c r="K277" t="inlineStr"/>
     </row>
     <row r="278">
-      <c r="A278" t="inlineStr"/>
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>M009</t>
+        </is>
+      </c>
       <c r="B278" t="inlineStr"/>
       <c r="C278" t="inlineStr"/>
       <c r="D278" t="inlineStr">
@@ -8231,7 +8423,11 @@
       <c r="K336" t="inlineStr"/>
     </row>
     <row r="337">
-      <c r="A337" t="inlineStr"/>
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>M010</t>
+        </is>
+      </c>
       <c r="B337" t="inlineStr"/>
       <c r="C337" t="inlineStr">
         <is>
@@ -8266,8 +8462,18 @@
       <c r="K337" t="inlineStr"/>
     </row>
     <row r="338">
-      <c r="A338" t="inlineStr"/>
-      <c r="B338" t="inlineStr"/>
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>M010</t>
+        </is>
+      </c>
+      <c r="B338" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524990243/24
+Lender Amount: 71971.54
+Borrower Amount: 71971.54</t>
+        </is>
+      </c>
       <c r="C338" t="inlineStr"/>
       <c r="D338" t="inlineStr"/>
       <c r="E338" s="4" t="inlineStr">
@@ -8283,7 +8489,11 @@
       <c r="K338" t="inlineStr"/>
     </row>
     <row r="339">
-      <c r="A339" t="inlineStr"/>
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>M010</t>
+        </is>
+      </c>
       <c r="B339" t="inlineStr"/>
       <c r="C339" t="inlineStr"/>
       <c r="D339" t="inlineStr">
@@ -8304,7 +8514,11 @@
       <c r="K339" t="inlineStr"/>
     </row>
     <row r="340">
-      <c r="A340" t="inlineStr"/>
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>M011</t>
+        </is>
+      </c>
       <c r="B340" t="inlineStr"/>
       <c r="C340" t="inlineStr">
         <is>
@@ -8339,8 +8553,18 @@
       <c r="K340" t="inlineStr"/>
     </row>
     <row r="341">
-      <c r="A341" t="inlineStr"/>
-      <c r="B341" t="inlineStr"/>
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>M011</t>
+        </is>
+      </c>
+      <c r="B341" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524990243/24
+Lender Amount: 20527984.90
+Borrower Amount: 20527984.90</t>
+        </is>
+      </c>
       <c r="C341" t="inlineStr"/>
       <c r="D341" t="inlineStr"/>
       <c r="E341" s="4" t="inlineStr">
@@ -8356,7 +8580,11 @@
       <c r="K341" t="inlineStr"/>
     </row>
     <row r="342">
-      <c r="A342" t="inlineStr"/>
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>M011</t>
+        </is>
+      </c>
       <c r="B342" t="inlineStr"/>
       <c r="C342" t="inlineStr"/>
       <c r="D342" t="inlineStr">
@@ -8377,7 +8605,11 @@
       <c r="K342" t="inlineStr"/>
     </row>
     <row r="343">
-      <c r="A343" t="inlineStr"/>
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>M012</t>
+        </is>
+      </c>
       <c r="B343" t="inlineStr"/>
       <c r="C343" t="inlineStr">
         <is>
@@ -8412,8 +8644,18 @@
       <c r="K343" t="inlineStr"/>
     </row>
     <row r="344">
-      <c r="A344" t="inlineStr"/>
-      <c r="B344" t="inlineStr"/>
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>M012</t>
+        </is>
+      </c>
+      <c r="B344" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020653/25
+Lender Amount: 665048.82
+Borrower Amount: 665048.82</t>
+        </is>
+      </c>
       <c r="C344" t="inlineStr"/>
       <c r="D344" t="inlineStr"/>
       <c r="E344" s="4" t="inlineStr">
@@ -8429,7 +8671,11 @@
       <c r="K344" t="inlineStr"/>
     </row>
     <row r="345">
-      <c r="A345" t="inlineStr"/>
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>M012</t>
+        </is>
+      </c>
       <c r="B345" t="inlineStr"/>
       <c r="C345" t="inlineStr"/>
       <c r="D345" t="inlineStr">
@@ -8450,7 +8696,11 @@
       <c r="K345" t="inlineStr"/>
     </row>
     <row r="346">
-      <c r="A346" t="inlineStr"/>
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>M013</t>
+        </is>
+      </c>
       <c r="B346" t="inlineStr"/>
       <c r="C346" t="inlineStr">
         <is>
@@ -8485,8 +8735,18 @@
       <c r="K346" t="inlineStr"/>
     </row>
     <row r="347">
-      <c r="A347" t="inlineStr"/>
-      <c r="B347" t="inlineStr"/>
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>M013</t>
+        </is>
+      </c>
+      <c r="B347" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020708/24
+Lender Amount: 25042.61
+Borrower Amount: 25042.61</t>
+        </is>
+      </c>
       <c r="C347" t="inlineStr"/>
       <c r="D347" t="inlineStr"/>
       <c r="E347" s="4" t="inlineStr">
@@ -8502,7 +8762,11 @@
       <c r="K347" t="inlineStr"/>
     </row>
     <row r="348">
-      <c r="A348" t="inlineStr"/>
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>M013</t>
+        </is>
+      </c>
       <c r="B348" t="inlineStr"/>
       <c r="C348" t="inlineStr"/>
       <c r="D348" t="inlineStr">
@@ -8816,7 +9080,11 @@
       <c r="K360" t="inlineStr"/>
     </row>
     <row r="361">
-      <c r="A361" t="inlineStr"/>
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>M014</t>
+        </is>
+      </c>
       <c r="B361" t="inlineStr"/>
       <c r="C361" t="inlineStr">
         <is>
@@ -8851,8 +9119,18 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" t="inlineStr"/>
-      <c r="B362" t="inlineStr"/>
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>M014</t>
+        </is>
+      </c>
+      <c r="B362" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 5995080.00
+Borrower Amount: 5995080.00</t>
+        </is>
+      </c>
       <c r="C362" t="inlineStr"/>
       <c r="D362" t="inlineStr"/>
       <c r="E362" s="4" t="inlineStr">
@@ -8868,7 +9146,11 @@
       <c r="K362" t="inlineStr"/>
     </row>
     <row r="363">
-      <c r="A363" t="inlineStr"/>
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>M014</t>
+        </is>
+      </c>
       <c r="B363" t="inlineStr"/>
       <c r="C363" t="inlineStr"/>
       <c r="D363" t="inlineStr">
@@ -8889,7 +9171,11 @@
       <c r="K363" t="inlineStr"/>
     </row>
     <row r="364">
-      <c r="A364" t="inlineStr"/>
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>M015</t>
+        </is>
+      </c>
       <c r="B364" t="inlineStr"/>
       <c r="C364" t="inlineStr">
         <is>
@@ -8924,8 +9210,18 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" t="inlineStr"/>
-      <c r="B365" t="inlineStr"/>
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>M015</t>
+        </is>
+      </c>
+      <c r="B365" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020068/25
+Lender Amount: 33573.89
+Borrower Amount: 33573.89</t>
+        </is>
+      </c>
       <c r="C365" t="inlineStr"/>
       <c r="D365" t="inlineStr"/>
       <c r="E365" s="4" t="inlineStr">
@@ -8941,7 +9237,11 @@
       <c r="K365" t="inlineStr"/>
     </row>
     <row r="366">
-      <c r="A366" t="inlineStr"/>
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>M015</t>
+        </is>
+      </c>
       <c r="B366" t="inlineStr"/>
       <c r="C366" t="inlineStr"/>
       <c r="D366" t="inlineStr">
@@ -8962,7 +9262,11 @@
       <c r="K366" t="inlineStr"/>
     </row>
     <row r="367">
-      <c r="A367" t="inlineStr"/>
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>M016</t>
+        </is>
+      </c>
       <c r="B367" t="inlineStr"/>
       <c r="C367" t="inlineStr">
         <is>
@@ -8997,8 +9301,18 @@
       </c>
     </row>
     <row r="368">
-      <c r="A368" t="inlineStr"/>
-      <c r="B368" t="inlineStr"/>
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>M016</t>
+        </is>
+      </c>
+      <c r="B368" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020068/25
+Lender Amount: 1650660.00
+Borrower Amount: 1650660.00</t>
+        </is>
+      </c>
       <c r="C368" t="inlineStr"/>
       <c r="D368" t="inlineStr"/>
       <c r="E368" s="4" t="inlineStr">
@@ -9014,7 +9328,11 @@
       <c r="K368" t="inlineStr"/>
     </row>
     <row r="369">
-      <c r="A369" t="inlineStr"/>
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>M016</t>
+        </is>
+      </c>
       <c r="B369" t="inlineStr"/>
       <c r="C369" t="inlineStr"/>
       <c r="D369" t="inlineStr">
@@ -9255,7 +9573,11 @@
       <c r="K378" t="inlineStr"/>
     </row>
     <row r="379">
-      <c r="A379" t="inlineStr"/>
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>M017</t>
+        </is>
+      </c>
       <c r="B379" t="inlineStr"/>
       <c r="C379" t="inlineStr">
         <is>
@@ -9290,7 +9612,11 @@
       <c r="K379" t="inlineStr"/>
     </row>
     <row r="380">
-      <c r="A380" t="inlineStr"/>
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>M017</t>
+        </is>
+      </c>
       <c r="B380" t="inlineStr"/>
       <c r="C380" t="inlineStr"/>
       <c r="D380" t="inlineStr"/>
@@ -9309,7 +9635,11 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" t="inlineStr"/>
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>M017</t>
+        </is>
+      </c>
       <c r="B381" t="inlineStr"/>
       <c r="C381" t="inlineStr"/>
       <c r="D381" t="inlineStr"/>
@@ -9328,8 +9658,18 @@
       </c>
     </row>
     <row r="382">
-      <c r="A382" t="inlineStr"/>
-      <c r="B382" t="inlineStr"/>
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>M017</t>
+        </is>
+      </c>
+      <c r="B382" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155824020001/24
+Lender Amount: 7641878.37
+Borrower Amount: 7641878.37</t>
+        </is>
+      </c>
       <c r="C382" t="inlineStr"/>
       <c r="D382" t="inlineStr"/>
       <c r="E382" s="4" t="inlineStr">
@@ -9345,7 +9685,11 @@
       <c r="K382" t="inlineStr"/>
     </row>
     <row r="383">
-      <c r="A383" t="inlineStr"/>
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>M017</t>
+        </is>
+      </c>
       <c r="B383" t="inlineStr"/>
       <c r="C383" t="inlineStr"/>
       <c r="D383" t="inlineStr">
@@ -10390,7 +10734,11 @@
       <c r="K431" t="inlineStr"/>
     </row>
     <row r="432">
-      <c r="A432" t="inlineStr"/>
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>M018</t>
+        </is>
+      </c>
       <c r="B432" t="inlineStr"/>
       <c r="C432" t="inlineStr">
         <is>
@@ -10425,8 +10773,18 @@
       </c>
     </row>
     <row r="433">
-      <c r="A433" t="inlineStr"/>
-      <c r="B433" t="inlineStr"/>
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>M018</t>
+        </is>
+      </c>
+      <c r="B433" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 246401.97
+Borrower Amount: 246401.97</t>
+        </is>
+      </c>
       <c r="C433" t="inlineStr"/>
       <c r="D433" t="inlineStr"/>
       <c r="E433" s="4" t="inlineStr">
@@ -10442,7 +10800,11 @@
       <c r="K433" t="inlineStr"/>
     </row>
     <row r="434">
-      <c r="A434" t="inlineStr"/>
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>M018</t>
+        </is>
+      </c>
       <c r="B434" t="inlineStr"/>
       <c r="C434" t="inlineStr"/>
       <c r="D434" t="inlineStr">
@@ -11085,7 +11447,11 @@
       <c r="K460" t="inlineStr"/>
     </row>
     <row r="461">
-      <c r="A461" t="inlineStr"/>
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
       <c r="B461" t="inlineStr"/>
       <c r="C461" t="inlineStr">
         <is>
@@ -11120,8 +11486,18 @@
       </c>
     </row>
     <row r="462">
-      <c r="A462" t="inlineStr"/>
-      <c r="B462" t="inlineStr"/>
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
+      <c r="B462" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-222825150235/25
+Lender Amount: 2357.50
+Borrower Amount: 2357.50</t>
+        </is>
+      </c>
       <c r="C462" t="inlineStr"/>
       <c r="D462" t="inlineStr"/>
       <c r="E462" s="4" t="inlineStr">
@@ -11137,7 +11513,11 @@
       <c r="K462" t="inlineStr"/>
     </row>
     <row r="463">
-      <c r="A463" t="inlineStr"/>
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
       <c r="B463" t="inlineStr"/>
       <c r="C463" t="inlineStr"/>
       <c r="D463" t="inlineStr">
@@ -11231,7 +11611,11 @@
       <c r="K466" t="inlineStr"/>
     </row>
     <row r="467">
-      <c r="A467" t="inlineStr"/>
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>M020</t>
+        </is>
+      </c>
       <c r="B467" t="inlineStr"/>
       <c r="C467" t="inlineStr">
         <is>
@@ -11266,8 +11650,18 @@
       </c>
     </row>
     <row r="468">
-      <c r="A468" t="inlineStr"/>
-      <c r="B468" t="inlineStr"/>
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>M020</t>
+        </is>
+      </c>
+      <c r="B468" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-222825150235/25
+Lender Amount: 213500.00
+Borrower Amount: 213500.00</t>
+        </is>
+      </c>
       <c r="C468" t="inlineStr"/>
       <c r="D468" t="inlineStr"/>
       <c r="E468" s="4" t="inlineStr">
@@ -11283,7 +11677,11 @@
       <c r="K468" t="inlineStr"/>
     </row>
     <row r="469">
-      <c r="A469" t="inlineStr"/>
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>M020</t>
+        </is>
+      </c>
       <c r="B469" t="inlineStr"/>
       <c r="C469" t="inlineStr"/>
       <c r="D469" t="inlineStr">
@@ -11306,7 +11704,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M021</t>
         </is>
       </c>
       <c r="B470" t="inlineStr"/>
@@ -11345,7 +11743,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M021</t>
         </is>
       </c>
       <c r="B471" s="4" t="inlineStr">
@@ -11372,7 +11770,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M021</t>
         </is>
       </c>
       <c r="B472" t="inlineStr"/>
@@ -11395,7 +11793,11 @@
       <c r="K472" t="inlineStr"/>
     </row>
     <row r="473">
-      <c r="A473" t="inlineStr"/>
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>M022</t>
+        </is>
+      </c>
       <c r="B473" t="inlineStr"/>
       <c r="C473" t="inlineStr">
         <is>
@@ -11430,7 +11832,11 @@
       <c r="K473" t="inlineStr"/>
     </row>
     <row r="474">
-      <c r="A474" t="inlineStr"/>
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>M022</t>
+        </is>
+      </c>
       <c r="B474" t="inlineStr"/>
       <c r="C474" t="inlineStr"/>
       <c r="D474" t="inlineStr"/>
@@ -11449,7 +11855,11 @@
       </c>
     </row>
     <row r="475">
-      <c r="A475" t="inlineStr"/>
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>M022</t>
+        </is>
+      </c>
       <c r="B475" t="inlineStr"/>
       <c r="C475" t="inlineStr"/>
       <c r="D475" t="inlineStr"/>
@@ -11468,8 +11878,18 @@
       </c>
     </row>
     <row r="476">
-      <c r="A476" t="inlineStr"/>
-      <c r="B476" t="inlineStr"/>
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>M022</t>
+        </is>
+      </c>
+      <c r="B476" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-187724010122/24
+Lender Amount: 276518.90
+Borrower Amount: 276518.90</t>
+        </is>
+      </c>
       <c r="C476" t="inlineStr"/>
       <c r="D476" t="inlineStr"/>
       <c r="E476" s="4" t="inlineStr">
@@ -11485,7 +11905,11 @@
       <c r="K476" t="inlineStr"/>
     </row>
     <row r="477">
-      <c r="A477" t="inlineStr"/>
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>M022</t>
+        </is>
+      </c>
       <c r="B477" t="inlineStr"/>
       <c r="C477" t="inlineStr"/>
       <c r="D477" t="inlineStr">
@@ -12236,7 +12660,11 @@
       <c r="K507" t="inlineStr"/>
     </row>
     <row r="508">
-      <c r="A508" t="inlineStr"/>
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>M023</t>
+        </is>
+      </c>
       <c r="B508" t="inlineStr"/>
       <c r="C508" t="inlineStr">
         <is>
@@ -12271,8 +12699,18 @@
       <c r="K508" t="inlineStr"/>
     </row>
     <row r="509">
-      <c r="A509" t="inlineStr"/>
-      <c r="B509" t="inlineStr"/>
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>M023</t>
+        </is>
+      </c>
+      <c r="B509" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020027/25
+Lender Amount: 54431.58
+Borrower Amount: 54431.58</t>
+        </is>
+      </c>
       <c r="C509" t="inlineStr"/>
       <c r="D509" t="inlineStr"/>
       <c r="E509" s="4" t="inlineStr">
@@ -12288,7 +12726,11 @@
       <c r="K509" t="inlineStr"/>
     </row>
     <row r="510">
-      <c r="A510" t="inlineStr"/>
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>M023</t>
+        </is>
+      </c>
       <c r="B510" t="inlineStr"/>
       <c r="C510" t="inlineStr"/>
       <c r="D510" t="inlineStr">
@@ -12528,7 +12970,11 @@
       <c r="K519" t="inlineStr"/>
     </row>
     <row r="520">
-      <c r="A520" t="inlineStr"/>
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>M024</t>
+        </is>
+      </c>
       <c r="B520" t="inlineStr"/>
       <c r="C520" t="inlineStr">
         <is>
@@ -12563,8 +13009,18 @@
       <c r="K520" t="inlineStr"/>
     </row>
     <row r="521">
-      <c r="A521" t="inlineStr"/>
-      <c r="B521" t="inlineStr"/>
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>M024</t>
+        </is>
+      </c>
+      <c r="B521" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524027065/24
+Lender Amount: 8231.99
+Borrower Amount: 8231.99</t>
+        </is>
+      </c>
       <c r="C521" t="inlineStr"/>
       <c r="D521" t="inlineStr"/>
       <c r="E521" s="4" t="inlineStr">
@@ -12580,7 +13036,11 @@
       <c r="K521" t="inlineStr"/>
     </row>
     <row r="522">
-      <c r="A522" t="inlineStr"/>
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>M024</t>
+        </is>
+      </c>
       <c r="B522" t="inlineStr"/>
       <c r="C522" t="inlineStr"/>
       <c r="D522" t="inlineStr">
@@ -13638,7 +14098,11 @@
       <c r="K569" t="inlineStr"/>
     </row>
     <row r="570">
-      <c r="A570" t="inlineStr"/>
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>M025</t>
+        </is>
+      </c>
       <c r="B570" t="inlineStr"/>
       <c r="C570" t="inlineStr">
         <is>
@@ -13673,8 +14137,18 @@
       <c r="K570" t="inlineStr"/>
     </row>
     <row r="571">
-      <c r="A571" t="inlineStr"/>
-      <c r="B571" t="inlineStr"/>
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>M025</t>
+        </is>
+      </c>
+      <c r="B571" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020708/24
+Lender Amount: 19399.10
+Borrower Amount: 19399.10</t>
+        </is>
+      </c>
       <c r="C571" t="inlineStr"/>
       <c r="D571" t="inlineStr"/>
       <c r="E571" s="4" t="inlineStr">
@@ -13690,7 +14164,11 @@
       <c r="K571" t="inlineStr"/>
     </row>
     <row r="572">
-      <c r="A572" t="inlineStr"/>
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>M025</t>
+        </is>
+      </c>
       <c r="B572" t="inlineStr"/>
       <c r="C572" t="inlineStr"/>
       <c r="D572" t="inlineStr">
@@ -13713,7 +14191,7 @@
     <row r="573">
       <c r="A573" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M026</t>
         </is>
       </c>
       <c r="B573" t="inlineStr"/>
@@ -13752,7 +14230,7 @@
     <row r="574">
       <c r="A574" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M026</t>
         </is>
       </c>
       <c r="B574" s="4" t="inlineStr">
@@ -13779,7 +14257,7 @@
     <row r="575">
       <c r="A575" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M026</t>
         </is>
       </c>
       <c r="B575" t="inlineStr"/>
@@ -13951,7 +14429,11 @@
       <c r="K582" t="inlineStr"/>
     </row>
     <row r="583">
-      <c r="A583" t="inlineStr"/>
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>M027</t>
+        </is>
+      </c>
       <c r="B583" t="inlineStr"/>
       <c r="C583" t="inlineStr">
         <is>
@@ -13986,7 +14468,11 @@
       </c>
     </row>
     <row r="584">
-      <c r="A584" t="inlineStr"/>
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>M027</t>
+        </is>
+      </c>
       <c r="B584" t="inlineStr"/>
       <c r="C584" t="inlineStr"/>
       <c r="D584" t="inlineStr"/>
@@ -14005,7 +14491,11 @@
       <c r="K584" t="inlineStr"/>
     </row>
     <row r="585">
-      <c r="A585" t="inlineStr"/>
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>M027</t>
+        </is>
+      </c>
       <c r="B585" t="inlineStr"/>
       <c r="C585" t="inlineStr"/>
       <c r="D585" t="inlineStr"/>
@@ -14024,8 +14514,18 @@
       <c r="K585" t="inlineStr"/>
     </row>
     <row r="586">
-      <c r="A586" t="inlineStr"/>
-      <c r="B586" t="inlineStr"/>
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>M027</t>
+        </is>
+      </c>
+      <c r="B586" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 6125933.94
+Borrower Amount: 6125933.94</t>
+        </is>
+      </c>
       <c r="C586" t="inlineStr"/>
       <c r="D586" t="inlineStr"/>
       <c r="E586" s="4" t="inlineStr">
@@ -14041,7 +14541,11 @@
       <c r="K586" t="inlineStr"/>
     </row>
     <row r="587">
-      <c r="A587" t="inlineStr"/>
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>M027</t>
+        </is>
+      </c>
       <c r="B587" t="inlineStr"/>
       <c r="C587" t="inlineStr"/>
       <c r="D587" t="inlineStr">
@@ -14062,7 +14566,11 @@
       <c r="K587" t="inlineStr"/>
     </row>
     <row r="588">
-      <c r="A588" t="inlineStr"/>
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>M028</t>
+        </is>
+      </c>
       <c r="B588" t="inlineStr"/>
       <c r="C588" t="inlineStr">
         <is>
@@ -14097,8 +14605,18 @@
       <c r="K588" t="inlineStr"/>
     </row>
     <row r="589">
-      <c r="A589" t="inlineStr"/>
-      <c r="B589" t="inlineStr"/>
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>M028</t>
+        </is>
+      </c>
+      <c r="B589" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022495/24
+Lender Amount: 12425.77
+Borrower Amount: 12425.77</t>
+        </is>
+      </c>
       <c r="C589" t="inlineStr"/>
       <c r="D589" t="inlineStr"/>
       <c r="E589" s="4" t="inlineStr">
@@ -14114,7 +14632,11 @@
       <c r="K589" t="inlineStr"/>
     </row>
     <row r="590">
-      <c r="A590" t="inlineStr"/>
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>M028</t>
+        </is>
+      </c>
       <c r="B590" t="inlineStr"/>
       <c r="C590" t="inlineStr"/>
       <c r="D590" t="inlineStr">
@@ -14135,7 +14657,11 @@
       <c r="K590" t="inlineStr"/>
     </row>
     <row r="591">
-      <c r="A591" t="inlineStr"/>
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
       <c r="B591" t="inlineStr"/>
       <c r="C591" t="inlineStr">
         <is>
@@ -14170,8 +14696,18 @@
       <c r="K591" t="inlineStr"/>
     </row>
     <row r="592">
-      <c r="A592" t="inlineStr"/>
-      <c r="B592" t="inlineStr"/>
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
+      <c r="B592" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524022495/24
+Lender Amount: 23580.68
+Borrower Amount: 23580.68</t>
+        </is>
+      </c>
       <c r="C592" t="inlineStr"/>
       <c r="D592" t="inlineStr"/>
       <c r="E592" s="4" t="inlineStr">
@@ -14187,7 +14723,11 @@
       <c r="K592" t="inlineStr"/>
     </row>
     <row r="593">
-      <c r="A593" t="inlineStr"/>
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>M029</t>
+        </is>
+      </c>
       <c r="B593" t="inlineStr"/>
       <c r="C593" t="inlineStr"/>
       <c r="D593" t="inlineStr">
@@ -15194,7 +15734,11 @@
       <c r="K639" t="inlineStr"/>
     </row>
     <row r="640">
-      <c r="A640" t="inlineStr"/>
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>M030</t>
+        </is>
+      </c>
       <c r="B640" t="inlineStr"/>
       <c r="C640" t="inlineStr">
         <is>
@@ -15229,8 +15773,18 @@
       <c r="K640" t="inlineStr"/>
     </row>
     <row r="641">
-      <c r="A641" t="inlineStr"/>
-      <c r="B641" t="inlineStr"/>
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>M030</t>
+        </is>
+      </c>
+      <c r="B641" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308525021741/25
+Lender Amount: 22671.95
+Borrower Amount: 22671.95</t>
+        </is>
+      </c>
       <c r="C641" t="inlineStr"/>
       <c r="D641" t="inlineStr"/>
       <c r="E641" s="4" t="inlineStr">
@@ -15246,7 +15800,11 @@
       <c r="K641" t="inlineStr"/>
     </row>
     <row r="642">
-      <c r="A642" t="inlineStr"/>
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>M030</t>
+        </is>
+      </c>
       <c r="B642" t="inlineStr"/>
       <c r="C642" t="inlineStr"/>
       <c r="D642" t="inlineStr">
@@ -15267,7 +15825,11 @@
       <c r="K642" t="inlineStr"/>
     </row>
     <row r="643">
-      <c r="A643" t="inlineStr"/>
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>M031</t>
+        </is>
+      </c>
       <c r="B643" t="inlineStr"/>
       <c r="C643" t="inlineStr">
         <is>
@@ -15302,8 +15864,18 @@
       <c r="K643" t="inlineStr"/>
     </row>
     <row r="644">
-      <c r="A644" t="inlineStr"/>
-      <c r="B644" t="inlineStr"/>
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>M031</t>
+        </is>
+      </c>
+      <c r="B644" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308525021745/25
+Lender Amount: 28854.86
+Borrower Amount: 28854.86</t>
+        </is>
+      </c>
       <c r="C644" t="inlineStr"/>
       <c r="D644" t="inlineStr"/>
       <c r="E644" s="4" t="inlineStr">
@@ -15319,7 +15891,11 @@
       <c r="K644" t="inlineStr"/>
     </row>
     <row r="645">
-      <c r="A645" t="inlineStr"/>
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>M031</t>
+        </is>
+      </c>
       <c r="B645" t="inlineStr"/>
       <c r="C645" t="inlineStr"/>
       <c r="D645" t="inlineStr">
@@ -15340,7 +15916,11 @@
       <c r="K645" t="inlineStr"/>
     </row>
     <row r="646">
-      <c r="A646" t="inlineStr"/>
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>M032</t>
+        </is>
+      </c>
       <c r="B646" t="inlineStr"/>
       <c r="C646" t="inlineStr">
         <is>
@@ -15375,8 +15955,18 @@
       <c r="K646" t="inlineStr"/>
     </row>
     <row r="647">
-      <c r="A647" t="inlineStr"/>
-      <c r="B647" t="inlineStr"/>
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>M032</t>
+        </is>
+      </c>
+      <c r="B647" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524026037/24
+Lender Amount: 1725.00
+Borrower Amount: 1725.00</t>
+        </is>
+      </c>
       <c r="C647" t="inlineStr"/>
       <c r="D647" t="inlineStr"/>
       <c r="E647" s="4" t="inlineStr">
@@ -15392,7 +15982,11 @@
       <c r="K647" t="inlineStr"/>
     </row>
     <row r="648">
-      <c r="A648" t="inlineStr"/>
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>M032</t>
+        </is>
+      </c>
       <c r="B648" t="inlineStr"/>
       <c r="C648" t="inlineStr"/>
       <c r="D648" t="inlineStr">
@@ -15926,7 +16520,7 @@
     <row r="670">
       <c r="A670" t="inlineStr">
         <is>
-          <t>M004</t>
+          <t>M033</t>
         </is>
       </c>
       <c r="B670" t="inlineStr"/>
@@ -15965,7 +16559,7 @@
     <row r="671">
       <c r="A671" t="inlineStr">
         <is>
-          <t>M004</t>
+          <t>M033</t>
         </is>
       </c>
       <c r="B671" s="4" t="inlineStr">
@@ -15992,7 +16586,7 @@
     <row r="672">
       <c r="A672" t="inlineStr">
         <is>
-          <t>M004</t>
+          <t>M033</t>
         </is>
       </c>
       <c r="B672" t="inlineStr"/>
@@ -16015,7 +16609,11 @@
       <c r="K672" t="inlineStr"/>
     </row>
     <row r="673">
-      <c r="A673" t="inlineStr"/>
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>M034</t>
+        </is>
+      </c>
       <c r="B673" t="inlineStr"/>
       <c r="C673" t="inlineStr">
         <is>
@@ -16050,7 +16648,11 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" t="inlineStr"/>
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>M034</t>
+        </is>
+      </c>
       <c r="B674" t="inlineStr"/>
       <c r="C674" t="inlineStr"/>
       <c r="D674" t="inlineStr"/>
@@ -16069,7 +16671,11 @@
       <c r="K674" t="inlineStr"/>
     </row>
     <row r="675">
-      <c r="A675" t="inlineStr"/>
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>M034</t>
+        </is>
+      </c>
       <c r="B675" t="inlineStr"/>
       <c r="C675" t="inlineStr"/>
       <c r="D675" t="inlineStr"/>
@@ -16088,8 +16694,18 @@
       <c r="K675" t="inlineStr"/>
     </row>
     <row r="676">
-      <c r="A676" t="inlineStr"/>
-      <c r="B676" t="inlineStr"/>
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>M034</t>
+        </is>
+      </c>
+      <c r="B676" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 6777058.20
+Borrower Amount: 6777058.20</t>
+        </is>
+      </c>
       <c r="C676" t="inlineStr"/>
       <c r="D676" t="inlineStr"/>
       <c r="E676" s="4" t="inlineStr">
@@ -16105,7 +16721,11 @@
       <c r="K676" t="inlineStr"/>
     </row>
     <row r="677">
-      <c r="A677" t="inlineStr"/>
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>M034</t>
+        </is>
+      </c>
       <c r="B677" t="inlineStr"/>
       <c r="C677" t="inlineStr"/>
       <c r="D677" t="inlineStr">
@@ -16199,7 +16819,11 @@
       <c r="K680" t="inlineStr"/>
     </row>
     <row r="681">
-      <c r="A681" t="inlineStr"/>
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>M035</t>
+        </is>
+      </c>
       <c r="B681" t="inlineStr"/>
       <c r="C681" t="inlineStr">
         <is>
@@ -16234,7 +16858,11 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" t="inlineStr"/>
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>M035</t>
+        </is>
+      </c>
       <c r="B682" t="inlineStr"/>
       <c r="C682" t="inlineStr"/>
       <c r="D682" t="inlineStr"/>
@@ -16253,7 +16881,11 @@
       <c r="K682" t="inlineStr"/>
     </row>
     <row r="683">
-      <c r="A683" t="inlineStr"/>
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>M035</t>
+        </is>
+      </c>
       <c r="B683" t="inlineStr"/>
       <c r="C683" t="inlineStr"/>
       <c r="D683" t="inlineStr"/>
@@ -16272,8 +16904,18 @@
       <c r="K683" t="inlineStr"/>
     </row>
     <row r="684">
-      <c r="A684" t="inlineStr"/>
-      <c r="B684" t="inlineStr"/>
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>M035</t>
+        </is>
+      </c>
+      <c r="B684" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-155823010186/23
+Lender Amount: 76000.00
+Borrower Amount: 76000.00</t>
+        </is>
+      </c>
       <c r="C684" t="inlineStr"/>
       <c r="D684" t="inlineStr"/>
       <c r="E684" s="4" t="inlineStr">
@@ -16289,7 +16931,11 @@
       <c r="K684" t="inlineStr"/>
     </row>
     <row r="685">
-      <c r="A685" t="inlineStr"/>
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>M035</t>
+        </is>
+      </c>
       <c r="B685" t="inlineStr"/>
       <c r="C685" t="inlineStr"/>
       <c r="D685" t="inlineStr">
@@ -16529,7 +17175,11 @@
       <c r="K694" t="inlineStr"/>
     </row>
     <row r="695">
-      <c r="A695" t="inlineStr"/>
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>M036</t>
+        </is>
+      </c>
       <c r="B695" t="inlineStr"/>
       <c r="C695" t="inlineStr">
         <is>
@@ -16564,8 +17214,18 @@
       <c r="K695" t="inlineStr"/>
     </row>
     <row r="696">
-      <c r="A696" t="inlineStr"/>
-      <c r="B696" t="inlineStr"/>
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>M036</t>
+        </is>
+      </c>
+      <c r="B696" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524026037/222824023549
+Lender Amount: 1226351.09
+Borrower Amount: 1226351.09</t>
+        </is>
+      </c>
       <c r="C696" t="inlineStr"/>
       <c r="D696" t="inlineStr"/>
       <c r="E696" s="4" t="inlineStr">
@@ -16581,7 +17241,11 @@
       <c r="K696" t="inlineStr"/>
     </row>
     <row r="697">
-      <c r="A697" t="inlineStr"/>
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>M036</t>
+        </is>
+      </c>
       <c r="B697" t="inlineStr"/>
       <c r="C697" t="inlineStr"/>
       <c r="D697" t="inlineStr">
@@ -16675,7 +17339,11 @@
       <c r="K700" t="inlineStr"/>
     </row>
     <row r="701">
-      <c r="A701" t="inlineStr"/>
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>M037</t>
+        </is>
+      </c>
       <c r="B701" t="inlineStr"/>
       <c r="C701" t="inlineStr">
         <is>
@@ -16710,8 +17378,18 @@
       </c>
     </row>
     <row r="702">
-      <c r="A702" t="inlineStr"/>
-      <c r="B702" t="inlineStr"/>
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>M037</t>
+        </is>
+      </c>
+      <c r="B702" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524022495/24
+Lender Amount: 1675000.00
+Borrower Amount: 1675000.00</t>
+        </is>
+      </c>
       <c r="C702" t="inlineStr"/>
       <c r="D702" t="inlineStr"/>
       <c r="E702" s="4" t="inlineStr">
@@ -16727,7 +17405,11 @@
       <c r="K702" t="inlineStr"/>
     </row>
     <row r="703">
-      <c r="A703" t="inlineStr"/>
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>M037</t>
+        </is>
+      </c>
       <c r="B703" t="inlineStr"/>
       <c r="C703" t="inlineStr"/>
       <c r="D703" t="inlineStr">
@@ -16894,7 +17576,11 @@
       <c r="K709" t="inlineStr"/>
     </row>
     <row r="710">
-      <c r="A710" t="inlineStr"/>
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>M038</t>
+        </is>
+      </c>
       <c r="B710" t="inlineStr"/>
       <c r="C710" t="inlineStr">
         <is>
@@ -16929,8 +17615,18 @@
       <c r="K710" t="inlineStr"/>
     </row>
     <row r="711">
-      <c r="A711" t="inlineStr"/>
-      <c r="B711" t="inlineStr"/>
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>M038</t>
+        </is>
+      </c>
+      <c r="B711" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020027/25
+Lender Amount: 10691988.92
+Borrower Amount: 10691988.92</t>
+        </is>
+      </c>
       <c r="C711" t="inlineStr"/>
       <c r="D711" t="inlineStr"/>
       <c r="E711" s="4" t="inlineStr">
@@ -16946,7 +17642,11 @@
       <c r="K711" t="inlineStr"/>
     </row>
     <row r="712">
-      <c r="A712" t="inlineStr"/>
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>M038</t>
+        </is>
+      </c>
       <c r="B712" t="inlineStr"/>
       <c r="C712" t="inlineStr"/>
       <c r="D712" t="inlineStr">
@@ -16967,7 +17667,11 @@
       <c r="K712" t="inlineStr"/>
     </row>
     <row r="713">
-      <c r="A713" t="inlineStr"/>
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>M039</t>
+        </is>
+      </c>
       <c r="B713" t="inlineStr"/>
       <c r="C713" t="inlineStr">
         <is>
@@ -17002,8 +17706,18 @@
       <c r="K713" t="inlineStr"/>
     </row>
     <row r="714">
-      <c r="A714" t="inlineStr"/>
-      <c r="B714" t="inlineStr"/>
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>M039</t>
+        </is>
+      </c>
+      <c r="B714" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-222825150151/25
+Lender Amount: 333706.76
+Borrower Amount: 333706.76</t>
+        </is>
+      </c>
       <c r="C714" t="inlineStr"/>
       <c r="D714" t="inlineStr"/>
       <c r="E714" s="4" t="inlineStr">
@@ -17019,7 +17733,11 @@
       <c r="K714" t="inlineStr"/>
     </row>
     <row r="715">
-      <c r="A715" t="inlineStr"/>
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>M039</t>
+        </is>
+      </c>
       <c r="B715" t="inlineStr"/>
       <c r="C715" t="inlineStr"/>
       <c r="D715" t="inlineStr">
@@ -17040,7 +17758,11 @@
       <c r="K715" t="inlineStr"/>
     </row>
     <row r="716">
-      <c r="A716" t="inlineStr"/>
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>M040</t>
+        </is>
+      </c>
       <c r="B716" t="inlineStr"/>
       <c r="C716" t="inlineStr">
         <is>
@@ -17075,8 +17797,18 @@
       </c>
     </row>
     <row r="717">
-      <c r="A717" t="inlineStr"/>
-      <c r="B717" t="inlineStr"/>
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>M040</t>
+        </is>
+      </c>
+      <c r="B717" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020063/25
+Lender Amount: 299000.00
+Borrower Amount: 299000.00</t>
+        </is>
+      </c>
       <c r="C717" t="inlineStr"/>
       <c r="D717" t="inlineStr"/>
       <c r="E717" s="4" t="inlineStr">
@@ -17092,7 +17824,11 @@
       <c r="K717" t="inlineStr"/>
     </row>
     <row r="718">
-      <c r="A718" t="inlineStr"/>
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>M040</t>
+        </is>
+      </c>
       <c r="B718" t="inlineStr"/>
       <c r="C718" t="inlineStr"/>
       <c r="D718" t="inlineStr">
@@ -17186,7 +17922,11 @@
       <c r="K721" t="inlineStr"/>
     </row>
     <row r="722">
-      <c r="A722" t="inlineStr"/>
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>M041</t>
+        </is>
+      </c>
       <c r="B722" t="inlineStr"/>
       <c r="C722" t="inlineStr">
         <is>
@@ -17221,8 +17961,18 @@
       <c r="K722" t="inlineStr"/>
     </row>
     <row r="723">
-      <c r="A723" t="inlineStr"/>
-      <c r="B723" t="inlineStr"/>
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>M041</t>
+        </is>
+      </c>
+      <c r="B723" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524026037/24
+Lender Amount: 13743.52
+Borrower Amount: 13743.52</t>
+        </is>
+      </c>
       <c r="C723" t="inlineStr"/>
       <c r="D723" t="inlineStr"/>
       <c r="E723" s="4" t="inlineStr">
@@ -17238,7 +17988,11 @@
       <c r="K723" t="inlineStr"/>
     </row>
     <row r="724">
-      <c r="A724" t="inlineStr"/>
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>M041</t>
+        </is>
+      </c>
       <c r="B724" t="inlineStr"/>
       <c r="C724" t="inlineStr"/>
       <c r="D724" t="inlineStr">
@@ -17500,7 +18254,11 @@
       <c r="K735" t="inlineStr"/>
     </row>
     <row r="736">
-      <c r="A736" t="inlineStr"/>
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>M042</t>
+        </is>
+      </c>
       <c r="B736" t="inlineStr"/>
       <c r="C736" t="inlineStr">
         <is>
@@ -17535,8 +18293,18 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" t="inlineStr"/>
-      <c r="B737" t="inlineStr"/>
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>M042</t>
+        </is>
+      </c>
+      <c r="B737" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155825020020/25
+Lender Amount: 60302.55
+Borrower Amount: 60302.55</t>
+        </is>
+      </c>
       <c r="C737" t="inlineStr"/>
       <c r="D737" t="inlineStr"/>
       <c r="E737" s="4" t="inlineStr">
@@ -17552,7 +18320,11 @@
       <c r="K737" t="inlineStr"/>
     </row>
     <row r="738">
-      <c r="A738" t="inlineStr"/>
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>M042</t>
+        </is>
+      </c>
       <c r="B738" t="inlineStr"/>
       <c r="C738" t="inlineStr"/>
       <c r="D738" t="inlineStr">
@@ -17573,7 +18345,11 @@
       <c r="K738" t="inlineStr"/>
     </row>
     <row r="739">
-      <c r="A739" t="inlineStr"/>
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>M043</t>
+        </is>
+      </c>
       <c r="B739" t="inlineStr"/>
       <c r="C739" t="inlineStr">
         <is>
@@ -17608,8 +18384,18 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" t="inlineStr"/>
-      <c r="B740" t="inlineStr"/>
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>M043</t>
+        </is>
+      </c>
+      <c r="B740" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 124008.78
+Borrower Amount: 124008.78</t>
+        </is>
+      </c>
       <c r="C740" t="inlineStr"/>
       <c r="D740" t="inlineStr"/>
       <c r="E740" s="4" t="inlineStr">
@@ -17625,7 +18411,11 @@
       <c r="K740" t="inlineStr"/>
     </row>
     <row r="741">
-      <c r="A741" t="inlineStr"/>
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>M043</t>
+        </is>
+      </c>
       <c r="B741" t="inlineStr"/>
       <c r="C741" t="inlineStr"/>
       <c r="D741" t="inlineStr">
@@ -17646,7 +18436,11 @@
       <c r="K741" t="inlineStr"/>
     </row>
     <row r="742">
-      <c r="A742" t="inlineStr"/>
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>M044</t>
+        </is>
+      </c>
       <c r="B742" t="inlineStr"/>
       <c r="C742" t="inlineStr">
         <is>
@@ -17681,8 +18475,18 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" t="inlineStr"/>
-      <c r="B743" t="inlineStr"/>
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>M044</t>
+        </is>
+      </c>
+      <c r="B743" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/25
+Lender Amount: 31609.80
+Borrower Amount: 31609.80</t>
+        </is>
+      </c>
       <c r="C743" t="inlineStr"/>
       <c r="D743" t="inlineStr"/>
       <c r="E743" s="4" t="inlineStr">
@@ -17698,7 +18502,11 @@
       <c r="K743" t="inlineStr"/>
     </row>
     <row r="744">
-      <c r="A744" t="inlineStr"/>
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>M044</t>
+        </is>
+      </c>
       <c r="B744" t="inlineStr"/>
       <c r="C744" t="inlineStr"/>
       <c r="D744" t="inlineStr">
@@ -18122,7 +18930,11 @@
       <c r="K761" t="inlineStr"/>
     </row>
     <row r="762">
-      <c r="A762" t="inlineStr"/>
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>M045</t>
+        </is>
+      </c>
       <c r="B762" t="inlineStr"/>
       <c r="C762" t="inlineStr">
         <is>
@@ -18157,8 +18969,18 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" t="inlineStr"/>
-      <c r="B763" t="inlineStr"/>
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>M045</t>
+        </is>
+      </c>
+      <c r="B763" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020104/25
+Lender Amount: 10424886.36
+Borrower Amount: 10424886.36</t>
+        </is>
+      </c>
       <c r="C763" t="inlineStr"/>
       <c r="D763" t="inlineStr"/>
       <c r="E763" s="4" t="inlineStr">
@@ -18174,7 +18996,11 @@
       <c r="K763" t="inlineStr"/>
     </row>
     <row r="764">
-      <c r="A764" t="inlineStr"/>
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>M045</t>
+        </is>
+      </c>
       <c r="B764" t="inlineStr"/>
       <c r="C764" t="inlineStr"/>
       <c r="D764" t="inlineStr">
@@ -18195,7 +19021,11 @@
       <c r="K764" t="inlineStr"/>
     </row>
     <row r="765">
-      <c r="A765" t="inlineStr"/>
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>M046</t>
+        </is>
+      </c>
       <c r="B765" t="inlineStr"/>
       <c r="C765" t="inlineStr">
         <is>
@@ -18230,8 +19060,18 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" t="inlineStr"/>
-      <c r="B766" t="inlineStr"/>
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>M046</t>
+        </is>
+      </c>
+      <c r="B766" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020063/25
+Lender Amount: 2168751.40
+Borrower Amount: 2168751.40</t>
+        </is>
+      </c>
       <c r="C766" t="inlineStr"/>
       <c r="D766" t="inlineStr"/>
       <c r="E766" s="4" t="inlineStr">
@@ -18247,7 +19087,11 @@
       <c r="K766" t="inlineStr"/>
     </row>
     <row r="767">
-      <c r="A767" t="inlineStr"/>
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>M046</t>
+        </is>
+      </c>
       <c r="B767" t="inlineStr"/>
       <c r="C767" t="inlineStr"/>
       <c r="D767" t="inlineStr">
@@ -18341,7 +19185,11 @@
       <c r="K770" t="inlineStr"/>
     </row>
     <row r="771">
-      <c r="A771" t="inlineStr"/>
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>M047</t>
+        </is>
+      </c>
       <c r="B771" t="inlineStr"/>
       <c r="C771" t="inlineStr">
         <is>
@@ -18376,8 +19224,18 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" t="inlineStr"/>
-      <c r="B772" t="inlineStr"/>
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>M047</t>
+        </is>
+      </c>
+      <c r="B772" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-141325020068/25
+Lender Amount: 63787.54
+Borrower Amount: 63787.54</t>
+        </is>
+      </c>
       <c r="C772" t="inlineStr"/>
       <c r="D772" t="inlineStr"/>
       <c r="E772" s="4" t="inlineStr">
@@ -18393,7 +19251,11 @@
       <c r="K772" t="inlineStr"/>
     </row>
     <row r="773">
-      <c r="A773" t="inlineStr"/>
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>M047</t>
+        </is>
+      </c>
       <c r="B773" t="inlineStr"/>
       <c r="C773" t="inlineStr"/>
       <c r="D773" t="inlineStr">
@@ -21797,7 +22659,11 @@
       <c r="K919" t="inlineStr"/>
     </row>
     <row r="920">
-      <c r="A920" t="inlineStr"/>
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>M048</t>
+        </is>
+      </c>
       <c r="B920" t="inlineStr"/>
       <c r="C920" t="inlineStr">
         <is>
@@ -21832,8 +22698,18 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" t="inlineStr"/>
-      <c r="B921" t="inlineStr"/>
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>M048</t>
+        </is>
+      </c>
+      <c r="B921" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020104/25
+Lender Amount: 111771.42
+Borrower Amount: 111771.42</t>
+        </is>
+      </c>
       <c r="C921" t="inlineStr"/>
       <c r="D921" t="inlineStr"/>
       <c r="E921" s="4" t="inlineStr">
@@ -21849,7 +22725,11 @@
       <c r="K921" t="inlineStr"/>
     </row>
     <row r="922">
-      <c r="A922" t="inlineStr"/>
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>M048</t>
+        </is>
+      </c>
       <c r="B922" t="inlineStr"/>
       <c r="C922" t="inlineStr"/>
       <c r="D922" t="inlineStr">
@@ -21870,7 +22750,11 @@
       <c r="K922" t="inlineStr"/>
     </row>
     <row r="923">
-      <c r="A923" t="inlineStr"/>
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>M049</t>
+        </is>
+      </c>
       <c r="B923" t="inlineStr"/>
       <c r="C923" t="inlineStr">
         <is>
@@ -21905,8 +22789,18 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" t="inlineStr"/>
-      <c r="B924" t="inlineStr"/>
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>M049</t>
+        </is>
+      </c>
+      <c r="B924" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020112/25
+Lender Amount: 80701.76
+Borrower Amount: 80701.76</t>
+        </is>
+      </c>
       <c r="C924" t="inlineStr"/>
       <c r="D924" t="inlineStr"/>
       <c r="E924" s="4" t="inlineStr">
@@ -21922,7 +22816,11 @@
       <c r="K924" t="inlineStr"/>
     </row>
     <row r="925">
-      <c r="A925" t="inlineStr"/>
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>M049</t>
+        </is>
+      </c>
       <c r="B925" t="inlineStr"/>
       <c r="C925" t="inlineStr"/>
       <c r="D925" t="inlineStr">
@@ -21943,7 +22841,11 @@
       <c r="K925" t="inlineStr"/>
     </row>
     <row r="926">
-      <c r="A926" t="inlineStr"/>
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>M050</t>
+        </is>
+      </c>
       <c r="B926" t="inlineStr"/>
       <c r="C926" t="inlineStr">
         <is>
@@ -21978,8 +22880,18 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" t="inlineStr"/>
-      <c r="B927" t="inlineStr"/>
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>M050</t>
+        </is>
+      </c>
+      <c r="B927" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020112/25
+Lender Amount: 657.81
+Borrower Amount: 657.81</t>
+        </is>
+      </c>
       <c r="C927" t="inlineStr"/>
       <c r="D927" t="inlineStr"/>
       <c r="E927" s="4" t="inlineStr">
@@ -21995,7 +22907,11 @@
       <c r="K927" t="inlineStr"/>
     </row>
     <row r="928">
-      <c r="A928" t="inlineStr"/>
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>M050</t>
+        </is>
+      </c>
       <c r="B928" t="inlineStr"/>
       <c r="C928" t="inlineStr"/>
       <c r="D928" t="inlineStr">
@@ -22308,7 +23224,11 @@
       <c r="K940" t="inlineStr"/>
     </row>
     <row r="941">
-      <c r="A941" t="inlineStr"/>
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>M051</t>
+        </is>
+      </c>
       <c r="B941" t="inlineStr"/>
       <c r="C941" t="inlineStr">
         <is>
@@ -22343,8 +23263,18 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" t="inlineStr"/>
-      <c r="B942" t="inlineStr"/>
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>M051</t>
+        </is>
+      </c>
+      <c r="B942" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/25
+Lender Amount: 81730.06
+Borrower Amount: 81730.06</t>
+        </is>
+      </c>
       <c r="C942" t="inlineStr"/>
       <c r="D942" t="inlineStr"/>
       <c r="E942" s="4" t="inlineStr">
@@ -22360,7 +23290,11 @@
       <c r="K942" t="inlineStr"/>
     </row>
     <row r="943">
-      <c r="A943" t="inlineStr"/>
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>M051</t>
+        </is>
+      </c>
       <c r="B943" t="inlineStr"/>
       <c r="C943" t="inlineStr"/>
       <c r="D943" t="inlineStr">
@@ -22748,7 +23682,7 @@
     <row r="959">
       <c r="A959" t="inlineStr">
         <is>
-          <t>M005</t>
+          <t>M052</t>
         </is>
       </c>
       <c r="B959" t="inlineStr"/>
@@ -22787,7 +23721,7 @@
     <row r="960">
       <c r="A960" t="inlineStr">
         <is>
-          <t>M005</t>
+          <t>M052</t>
         </is>
       </c>
       <c r="B960" t="inlineStr"/>
@@ -22810,7 +23744,7 @@
     <row r="961">
       <c r="A961" t="inlineStr">
         <is>
-          <t>M005</t>
+          <t>M052</t>
         </is>
       </c>
       <c r="B961" t="inlineStr"/>
@@ -22833,7 +23767,7 @@
     <row r="962">
       <c r="A962" t="inlineStr">
         <is>
-          <t>M005</t>
+          <t>M052</t>
         </is>
       </c>
       <c r="B962" s="4" t="inlineStr">
@@ -22860,7 +23794,7 @@
     <row r="963">
       <c r="A963" t="inlineStr">
         <is>
-          <t>M005</t>
+          <t>M052</t>
         </is>
       </c>
       <c r="B963" t="inlineStr"/>
@@ -23067,7 +24001,11 @@
       <c r="K971" t="inlineStr"/>
     </row>
     <row r="972">
-      <c r="A972" t="inlineStr"/>
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>M053</t>
+        </is>
+      </c>
       <c r="B972" t="inlineStr"/>
       <c r="C972" t="inlineStr">
         <is>
@@ -23102,8 +24040,18 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" t="inlineStr"/>
-      <c r="B973" t="inlineStr"/>
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>M053</t>
+        </is>
+      </c>
+      <c r="B973" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-222825150235/25
+Lender Amount: 36757.00
+Borrower Amount: 36757.00</t>
+        </is>
+      </c>
       <c r="C973" t="inlineStr"/>
       <c r="D973" t="inlineStr"/>
       <c r="E973" s="4" t="inlineStr">
@@ -23119,7 +24067,11 @@
       <c r="K973" t="inlineStr"/>
     </row>
     <row r="974">
-      <c r="A974" t="inlineStr"/>
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>M053</t>
+        </is>
+      </c>
       <c r="B974" t="inlineStr"/>
       <c r="C974" t="inlineStr"/>
       <c r="D974" t="inlineStr">
@@ -23213,7 +24165,11 @@
       <c r="K977" t="inlineStr"/>
     </row>
     <row r="978">
-      <c r="A978" t="inlineStr"/>
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
       <c r="B978" t="inlineStr"/>
       <c r="C978" t="inlineStr">
         <is>
@@ -23248,7 +24204,11 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" t="inlineStr"/>
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
       <c r="B979" t="inlineStr"/>
       <c r="C979" t="inlineStr"/>
       <c r="D979" t="inlineStr"/>
@@ -23267,7 +24227,11 @@
       <c r="K979" t="inlineStr"/>
     </row>
     <row r="980">
-      <c r="A980" t="inlineStr"/>
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
       <c r="B980" t="inlineStr"/>
       <c r="C980" t="inlineStr"/>
       <c r="D980" t="inlineStr"/>
@@ -23286,7 +24250,11 @@
       <c r="K980" t="inlineStr"/>
     </row>
     <row r="981">
-      <c r="A981" t="inlineStr"/>
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
       <c r="B981" t="inlineStr"/>
       <c r="C981" t="inlineStr"/>
       <c r="D981" t="inlineStr"/>
@@ -23305,8 +24273,18 @@
       <c r="K981" t="inlineStr"/>
     </row>
     <row r="982">
-      <c r="A982" t="inlineStr"/>
-      <c r="B982" t="inlineStr"/>
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
+      <c r="B982" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020068/25
+Lender Amount: 3587219.00
+Borrower Amount: 3587219.00</t>
+        </is>
+      </c>
       <c r="C982" t="inlineStr"/>
       <c r="D982" t="inlineStr"/>
       <c r="E982" s="4" t="inlineStr">
@@ -23322,7 +24300,11 @@
       <c r="K982" t="inlineStr"/>
     </row>
     <row r="983">
-      <c r="A983" t="inlineStr"/>
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
       <c r="B983" t="inlineStr"/>
       <c r="C983" t="inlineStr"/>
       <c r="D983" t="inlineStr">
@@ -23343,7 +24325,11 @@
       <c r="K983" t="inlineStr"/>
     </row>
     <row r="984">
-      <c r="A984" t="inlineStr"/>
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>M055</t>
+        </is>
+      </c>
       <c r="B984" t="inlineStr"/>
       <c r="C984" t="inlineStr">
         <is>
@@ -23378,8 +24364,18 @@
       <c r="K984" t="inlineStr"/>
     </row>
     <row r="985">
-      <c r="A985" t="inlineStr"/>
-      <c r="B985" t="inlineStr"/>
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>M055</t>
+        </is>
+      </c>
+      <c r="B985" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524990243/24
+Lender Amount: 68747.06
+Borrower Amount: 68747.06</t>
+        </is>
+      </c>
       <c r="C985" t="inlineStr"/>
       <c r="D985" t="inlineStr"/>
       <c r="E985" s="4" t="inlineStr">
@@ -23395,7 +24391,11 @@
       <c r="K985" t="inlineStr"/>
     </row>
     <row r="986">
-      <c r="A986" t="inlineStr"/>
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>M055</t>
+        </is>
+      </c>
       <c r="B986" t="inlineStr"/>
       <c r="C986" t="inlineStr"/>
       <c r="D986" t="inlineStr">
@@ -23950,7 +24950,11 @@
       <c r="K1009" t="inlineStr"/>
     </row>
     <row r="1010">
-      <c r="A1010" t="inlineStr"/>
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>M056</t>
+        </is>
+      </c>
       <c r="B1010" t="inlineStr"/>
       <c r="C1010" t="inlineStr">
         <is>
@@ -23985,8 +24989,18 @@
       <c r="K1010" t="inlineStr"/>
     </row>
     <row r="1011">
-      <c r="A1011" t="inlineStr"/>
-      <c r="B1011" t="inlineStr"/>
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>M056</t>
+        </is>
+      </c>
+      <c r="B1011" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308525021741/25
+Lender Amount: 31411.11
+Borrower Amount: 31411.11</t>
+        </is>
+      </c>
       <c r="C1011" t="inlineStr"/>
       <c r="D1011" t="inlineStr"/>
       <c r="E1011" s="4" t="inlineStr">
@@ -24002,7 +25016,11 @@
       <c r="K1011" t="inlineStr"/>
     </row>
     <row r="1012">
-      <c r="A1012" t="inlineStr"/>
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>M056</t>
+        </is>
+      </c>
       <c r="B1012" t="inlineStr"/>
       <c r="C1012" t="inlineStr"/>
       <c r="D1012" t="inlineStr">
@@ -24462,7 +25480,11 @@
       <c r="K1030" t="inlineStr"/>
     </row>
     <row r="1031">
-      <c r="A1031" t="inlineStr"/>
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>M057</t>
+        </is>
+      </c>
       <c r="B1031" t="inlineStr"/>
       <c r="C1031" t="inlineStr">
         <is>
@@ -24497,8 +25519,18 @@
       <c r="K1031" t="inlineStr"/>
     </row>
     <row r="1032">
-      <c r="A1032" t="inlineStr"/>
-      <c r="B1032" t="inlineStr"/>
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>M057</t>
+        </is>
+      </c>
+      <c r="B1032" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-155825010037/25
+Lender Amount: 853297.01
+Borrower Amount: 853297.01</t>
+        </is>
+      </c>
       <c r="C1032" t="inlineStr"/>
       <c r="D1032" t="inlineStr"/>
       <c r="E1032" s="4" t="inlineStr">
@@ -24514,7 +25546,11 @@
       <c r="K1032" t="inlineStr"/>
     </row>
     <row r="1033">
-      <c r="A1033" t="inlineStr"/>
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>M057</t>
+        </is>
+      </c>
       <c r="B1033" t="inlineStr"/>
       <c r="C1033" t="inlineStr"/>
       <c r="D1033" t="inlineStr">
@@ -26125,7 +27161,11 @@
       <c r="K1099" t="inlineStr"/>
     </row>
     <row r="1100">
-      <c r="A1100" t="inlineStr"/>
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>M058</t>
+        </is>
+      </c>
       <c r="B1100" t="inlineStr"/>
       <c r="C1100" t="inlineStr">
         <is>
@@ -26160,8 +27200,18 @@
       </c>
     </row>
     <row r="1101">
-      <c r="A1101" t="inlineStr"/>
-      <c r="B1101" t="inlineStr"/>
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>M058</t>
+        </is>
+      </c>
+      <c r="B1101" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020163/25
+Lender Amount: 1725.00
+Borrower Amount: 1725.00</t>
+        </is>
+      </c>
       <c r="C1101" t="inlineStr"/>
       <c r="D1101" t="inlineStr"/>
       <c r="E1101" s="4" t="inlineStr">
@@ -26177,7 +27227,11 @@
       <c r="K1101" t="inlineStr"/>
     </row>
     <row r="1102">
-      <c r="A1102" t="inlineStr"/>
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>M058</t>
+        </is>
+      </c>
       <c r="B1102" t="inlineStr"/>
       <c r="C1102" t="inlineStr"/>
       <c r="D1102" t="inlineStr">
@@ -26198,7 +27252,11 @@
       <c r="K1102" t="inlineStr"/>
     </row>
     <row r="1103">
-      <c r="A1103" t="inlineStr"/>
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>M059</t>
+        </is>
+      </c>
       <c r="B1103" t="inlineStr"/>
       <c r="C1103" t="inlineStr">
         <is>
@@ -26233,8 +27291,18 @@
       <c r="K1103" t="inlineStr"/>
     </row>
     <row r="1104">
-      <c r="A1104" t="inlineStr"/>
-      <c r="B1104" t="inlineStr"/>
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>M059</t>
+        </is>
+      </c>
+      <c r="B1104" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308525021746/25
+Lender Amount: 35373.50
+Borrower Amount: 35373.50</t>
+        </is>
+      </c>
       <c r="C1104" t="inlineStr"/>
       <c r="D1104" t="inlineStr"/>
       <c r="E1104" s="4" t="inlineStr">
@@ -26250,7 +27318,11 @@
       <c r="K1104" t="inlineStr"/>
     </row>
     <row r="1105">
-      <c r="A1105" t="inlineStr"/>
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>M059</t>
+        </is>
+      </c>
       <c r="B1105" t="inlineStr"/>
       <c r="C1105" t="inlineStr"/>
       <c r="D1105" t="inlineStr">
@@ -26747,7 +27819,11 @@
       <c r="K1125" t="inlineStr"/>
     </row>
     <row r="1126">
-      <c r="A1126" t="inlineStr"/>
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>M060</t>
+        </is>
+      </c>
       <c r="B1126" t="inlineStr"/>
       <c r="C1126" t="inlineStr">
         <is>
@@ -26782,7 +27858,11 @@
       <c r="K1126" t="inlineStr"/>
     </row>
     <row r="1127">
-      <c r="A1127" t="inlineStr"/>
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>M060</t>
+        </is>
+      </c>
       <c r="B1127" t="inlineStr"/>
       <c r="C1127" t="inlineStr"/>
       <c r="D1127" t="inlineStr"/>
@@ -26801,7 +27881,11 @@
       </c>
     </row>
     <row r="1128">
-      <c r="A1128" t="inlineStr"/>
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>M060</t>
+        </is>
+      </c>
       <c r="B1128" t="inlineStr"/>
       <c r="C1128" t="inlineStr"/>
       <c r="D1128" t="inlineStr"/>
@@ -26820,7 +27904,11 @@
       </c>
     </row>
     <row r="1129">
-      <c r="A1129" t="inlineStr"/>
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>M060</t>
+        </is>
+      </c>
       <c r="B1129" t="inlineStr"/>
       <c r="C1129" t="inlineStr"/>
       <c r="D1129" t="inlineStr"/>
@@ -26839,7 +27927,11 @@
       </c>
     </row>
     <row r="1130">
-      <c r="A1130" t="inlineStr"/>
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>M060</t>
+        </is>
+      </c>
       <c r="B1130" t="inlineStr"/>
       <c r="C1130" t="inlineStr"/>
       <c r="D1130" t="inlineStr"/>
@@ -26858,8 +27950,18 @@
       </c>
     </row>
     <row r="1131">
-      <c r="A1131" t="inlineStr"/>
-      <c r="B1131" t="inlineStr"/>
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>M060</t>
+        </is>
+      </c>
+      <c r="B1131" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-141325020063/141325020112
+Lender Amount: 576120.39
+Borrower Amount: 576120.39</t>
+        </is>
+      </c>
       <c r="C1131" t="inlineStr"/>
       <c r="D1131" t="inlineStr"/>
       <c r="E1131" s="4" t="inlineStr">
@@ -26875,7 +27977,11 @@
       <c r="K1131" t="inlineStr"/>
     </row>
     <row r="1132">
-      <c r="A1132" t="inlineStr"/>
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>M060</t>
+        </is>
+      </c>
       <c r="B1132" t="inlineStr"/>
       <c r="C1132" t="inlineStr"/>
       <c r="D1132" t="inlineStr">
@@ -26896,7 +28002,11 @@
       <c r="K1132" t="inlineStr"/>
     </row>
     <row r="1133">
-      <c r="A1133" t="inlineStr"/>
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>M061</t>
+        </is>
+      </c>
       <c r="B1133" t="inlineStr"/>
       <c r="C1133" t="inlineStr">
         <is>
@@ -26931,8 +28041,18 @@
       </c>
     </row>
     <row r="1134">
-      <c r="A1134" t="inlineStr"/>
-      <c r="B1134" t="inlineStr"/>
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>M061</t>
+        </is>
+      </c>
+      <c r="B1134" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524022166 
+Lender Amount: 758000.00
+Borrower Amount: 758000.00</t>
+        </is>
+      </c>
       <c r="C1134" t="inlineStr"/>
       <c r="D1134" t="inlineStr"/>
       <c r="E1134" s="4" t="inlineStr">
@@ -26948,7 +28068,11 @@
       <c r="K1134" t="inlineStr"/>
     </row>
     <row r="1135">
-      <c r="A1135" t="inlineStr"/>
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>M061</t>
+        </is>
+      </c>
       <c r="B1135" t="inlineStr"/>
       <c r="C1135" t="inlineStr"/>
       <c r="D1135" t="inlineStr">
@@ -27553,7 +28677,11 @@
       <c r="K1159" t="inlineStr"/>
     </row>
     <row r="1160">
-      <c r="A1160" t="inlineStr"/>
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>M062</t>
+        </is>
+      </c>
       <c r="B1160" t="inlineStr"/>
       <c r="C1160" t="inlineStr">
         <is>
@@ -27588,8 +28716,18 @@
       </c>
     </row>
     <row r="1161">
-      <c r="A1161" t="inlineStr"/>
-      <c r="B1161" t="inlineStr"/>
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>M062</t>
+        </is>
+      </c>
+      <c r="B1161" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: LC-308524022166 
+Lender Amount: 4009000.00
+Borrower Amount: 4009000.00</t>
+        </is>
+      </c>
       <c r="C1161" t="inlineStr"/>
       <c r="D1161" t="inlineStr"/>
       <c r="E1161" s="4" t="inlineStr">
@@ -27605,7 +28743,11 @@
       <c r="K1161" t="inlineStr"/>
     </row>
     <row r="1162">
-      <c r="A1162" t="inlineStr"/>
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>M062</t>
+        </is>
+      </c>
       <c r="B1162" t="inlineStr"/>
       <c r="C1162" t="inlineStr"/>
       <c r="D1162" t="inlineStr">
@@ -27772,7 +28914,11 @@
       <c r="K1168" t="inlineStr"/>
     </row>
     <row r="1169">
-      <c r="A1169" t="inlineStr"/>
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>M063</t>
+        </is>
+      </c>
       <c r="B1169" t="inlineStr"/>
       <c r="C1169" t="inlineStr">
         <is>
@@ -27807,8 +28953,18 @@
       <c r="K1169" t="inlineStr"/>
     </row>
     <row r="1170">
-      <c r="A1170" t="inlineStr"/>
-      <c r="B1170" t="inlineStr"/>
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>M063</t>
+        </is>
+      </c>
+      <c r="B1170" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-308524026037/24
+Lender Amount: 14417.98
+Borrower Amount: 14417.98</t>
+        </is>
+      </c>
       <c r="C1170" t="inlineStr"/>
       <c r="D1170" t="inlineStr"/>
       <c r="E1170" s="4" t="inlineStr">
@@ -27824,7 +28980,11 @@
       <c r="K1170" t="inlineStr"/>
     </row>
     <row r="1171">
-      <c r="A1171" t="inlineStr"/>
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>M063</t>
+        </is>
+      </c>
       <c r="B1171" t="inlineStr"/>
       <c r="C1171" t="inlineStr"/>
       <c r="D1171" t="inlineStr">
@@ -28429,7 +29589,11 @@
       <c r="K1195" t="inlineStr"/>
     </row>
     <row r="1196">
-      <c r="A1196" t="inlineStr"/>
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>M064</t>
+        </is>
+      </c>
       <c r="B1196" t="inlineStr"/>
       <c r="C1196" t="inlineStr">
         <is>
@@ -28464,8 +29628,18 @@
       <c r="K1196" t="inlineStr"/>
     </row>
     <row r="1197">
-      <c r="A1197" t="inlineStr"/>
-      <c r="B1197" t="inlineStr"/>
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>M064</t>
+        </is>
+      </c>
+      <c r="B1197" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147125020202/25
+Lender Amount: 3499168.01
+Borrower Amount: 3499168.01</t>
+        </is>
+      </c>
       <c r="C1197" t="inlineStr"/>
       <c r="D1197" t="inlineStr"/>
       <c r="E1197" s="4" t="inlineStr">
@@ -28481,7 +29655,11 @@
       <c r="K1197" t="inlineStr"/>
     </row>
     <row r="1198">
-      <c r="A1198" t="inlineStr"/>
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>M064</t>
+        </is>
+      </c>
       <c r="B1198" t="inlineStr"/>
       <c r="C1198" t="inlineStr"/>
       <c r="D1198" t="inlineStr">
@@ -28930,7 +30108,11 @@
       <c r="K1218" t="inlineStr"/>
     </row>
     <row r="1219">
-      <c r="A1219" t="inlineStr"/>
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>M065</t>
+        </is>
+      </c>
       <c r="B1219" t="inlineStr"/>
       <c r="C1219" t="inlineStr">
         <is>
@@ -28965,8 +30147,18 @@
       <c r="K1219" t="inlineStr"/>
     </row>
     <row r="1220">
-      <c r="A1220" t="inlineStr"/>
-      <c r="B1220" t="inlineStr"/>
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>M065</t>
+        </is>
+      </c>
+      <c r="B1220" s="4" t="inlineStr">
+        <is>
+          <t>LC Match: L/C-147124020074/24
+Lender Amount: 6242871.55
+Borrower Amount: 6242871.55</t>
+        </is>
+      </c>
       <c r="C1220" t="inlineStr"/>
       <c r="D1220" t="inlineStr"/>
       <c r="E1220" s="4" t="inlineStr">
@@ -28982,7 +30174,11 @@
       <c r="K1220" t="inlineStr"/>
     </row>
     <row r="1221">
-      <c r="A1221" t="inlineStr"/>
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>M065</t>
+        </is>
+      </c>
       <c r="B1221" t="inlineStr"/>
       <c r="C1221" t="inlineStr"/>
       <c r="D1221" t="inlineStr">

</xml_diff>

<commit_message>
Header row filter added
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$9:$L$9</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -32186,6 +32188,7 @@
       <c r="L1233" s="1" t="inlineStr"/>
     </row>
   </sheetData>
+  <autoFilter ref="A9:L9"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Interunit loan match added
</commit_message>
<xml_diff>
--- a/Output/Interunit GeoTex_MATCHED.xlsx
+++ b/Output/Interunit GeoTex_MATCHED.xlsx
@@ -1983,7 +1983,11 @@
       <c r="L64" s="1" t="inlineStr"/>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr"/>
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>M074</t>
+        </is>
+      </c>
       <c r="B65" s="2" t="inlineStr"/>
       <c r="C65" s="1" t="inlineStr">
         <is>
@@ -2019,8 +2023,18 @@
       <c r="L65" s="1" t="inlineStr"/>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr"/>
-      <c r="B66" s="2" t="inlineStr"/>
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>M074</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>Interunit Loan Match: PBL#11502 ↔ PBL#10855
+Lender Amount: 104470400.00
+Borrower Amount: 104470400.00</t>
+        </is>
+      </c>
       <c r="C66" s="1" t="inlineStr"/>
       <c r="D66" s="1" t="inlineStr"/>
       <c r="E66" s="2" t="inlineStr">
@@ -2034,10 +2048,18 @@
       <c r="I66" s="1" t="inlineStr"/>
       <c r="J66" s="1" t="inlineStr"/>
       <c r="K66" s="1" t="inlineStr"/>
-      <c r="L66" s="1" t="inlineStr"/>
+      <c r="L66" s="1" t="inlineStr">
+        <is>
+          <t>Interunit</t>
+        </is>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr"/>
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>M074</t>
+        </is>
+      </c>
       <c r="B67" s="2" t="inlineStr"/>
       <c r="C67" s="1" t="inlineStr"/>
       <c r="D67" s="1" t="inlineStr">
@@ -8035,7 +8057,11 @@
       <c r="L302" s="1" t="inlineStr"/>
     </row>
     <row r="303">
-      <c r="A303" s="1" t="inlineStr"/>
+      <c r="A303" s="1" t="inlineStr">
+        <is>
+          <t>M075</t>
+        </is>
+      </c>
       <c r="B303" s="2" t="inlineStr"/>
       <c r="C303" s="1" t="inlineStr">
         <is>
@@ -8071,7 +8097,11 @@
       <c r="L303" s="1" t="inlineStr"/>
     </row>
     <row r="304">
-      <c r="A304" s="1" t="inlineStr"/>
+      <c r="A304" s="1" t="inlineStr">
+        <is>
+          <t>M075</t>
+        </is>
+      </c>
       <c r="B304" s="2" t="inlineStr"/>
       <c r="C304" s="1" t="inlineStr"/>
       <c r="D304" s="1" t="inlineStr"/>
@@ -8091,7 +8121,11 @@
       <c r="L304" s="1" t="inlineStr"/>
     </row>
     <row r="305">
-      <c r="A305" s="1" t="inlineStr"/>
+      <c r="A305" s="1" t="inlineStr">
+        <is>
+          <t>M075</t>
+        </is>
+      </c>
       <c r="B305" s="2" t="inlineStr"/>
       <c r="C305" s="1" t="inlineStr"/>
       <c r="D305" s="1" t="inlineStr"/>
@@ -8111,8 +8145,18 @@
       <c r="L305" s="1" t="inlineStr"/>
     </row>
     <row r="306">
-      <c r="A306" s="1" t="inlineStr"/>
-      <c r="B306" s="2" t="inlineStr"/>
+      <c r="A306" s="1" t="inlineStr">
+        <is>
+          <t>M075</t>
+        </is>
+      </c>
+      <c r="B306" s="2" t="inlineStr">
+        <is>
+          <t>Interunit Loan Match: EBL#5503 ↔ EBL#3129
+Lender Amount: 52816886.08
+Borrower Amount: 52816886.08</t>
+        </is>
+      </c>
       <c r="C306" s="1" t="inlineStr"/>
       <c r="D306" s="1" t="inlineStr"/>
       <c r="E306" s="2" t="inlineStr">
@@ -8126,10 +8170,18 @@
       <c r="I306" s="1" t="inlineStr"/>
       <c r="J306" s="1" t="inlineStr"/>
       <c r="K306" s="1" t="inlineStr"/>
-      <c r="L306" s="1" t="inlineStr"/>
+      <c r="L306" s="1" t="inlineStr">
+        <is>
+          <t>Interunit</t>
+        </is>
+      </c>
     </row>
     <row r="307">
-      <c r="A307" s="1" t="inlineStr"/>
+      <c r="A307" s="1" t="inlineStr">
+        <is>
+          <t>M075</t>
+        </is>
+      </c>
       <c r="B307" s="2" t="inlineStr"/>
       <c r="C307" s="1" t="inlineStr"/>
       <c r="D307" s="1" t="inlineStr">
@@ -17705,7 +17757,11 @@
       <c r="L677" s="1" t="inlineStr"/>
     </row>
     <row r="678">
-      <c r="A678" s="1" t="inlineStr"/>
+      <c r="A678" s="1" t="inlineStr">
+        <is>
+          <t>M076</t>
+        </is>
+      </c>
       <c r="B678" s="2" t="inlineStr"/>
       <c r="C678" s="1" t="inlineStr">
         <is>
@@ -17741,8 +17797,18 @@
       <c r="L678" s="1" t="inlineStr"/>
     </row>
     <row r="679">
-      <c r="A679" s="1" t="inlineStr"/>
-      <c r="B679" s="2" t="inlineStr"/>
+      <c r="A679" s="1" t="inlineStr">
+        <is>
+          <t>M076</t>
+        </is>
+      </c>
+      <c r="B679" s="2" t="inlineStr">
+        <is>
+          <t>Interunit Loan Match: EBL#5503 ↔ EBL#3265
+Lender Amount: 236808.62
+Borrower Amount: 236808.62</t>
+        </is>
+      </c>
       <c r="C679" s="1" t="inlineStr"/>
       <c r="D679" s="1" t="inlineStr"/>
       <c r="E679" s="2" t="inlineStr">
@@ -17756,10 +17822,18 @@
       <c r="I679" s="1" t="inlineStr"/>
       <c r="J679" s="1" t="inlineStr"/>
       <c r="K679" s="1" t="inlineStr"/>
-      <c r="L679" s="1" t="inlineStr"/>
+      <c r="L679" s="1" t="inlineStr">
+        <is>
+          <t>Interunit</t>
+        </is>
+      </c>
     </row>
     <row r="680">
-      <c r="A680" s="1" t="inlineStr"/>
+      <c r="A680" s="1" t="inlineStr">
+        <is>
+          <t>M076</t>
+        </is>
+      </c>
       <c r="B680" s="2" t="inlineStr"/>
       <c r="C680" s="1" t="inlineStr"/>
       <c r="D680" s="1" t="inlineStr">
@@ -23052,7 +23126,11 @@
       <c r="L883" s="1" t="inlineStr"/>
     </row>
     <row r="884">
-      <c r="A884" s="1" t="inlineStr"/>
+      <c r="A884" s="1" t="inlineStr">
+        <is>
+          <t>M077</t>
+        </is>
+      </c>
       <c r="B884" s="2" t="inlineStr"/>
       <c r="C884" s="1" t="inlineStr">
         <is>
@@ -23088,8 +23166,18 @@
       <c r="L884" s="1" t="inlineStr"/>
     </row>
     <row r="885">
-      <c r="A885" s="1" t="inlineStr"/>
-      <c r="B885" s="2" t="inlineStr"/>
+      <c r="A885" s="1" t="inlineStr">
+        <is>
+          <t>M077</t>
+        </is>
+      </c>
+      <c r="B885" s="2" t="inlineStr">
+        <is>
+          <t>Interunit Loan Match: EBL#5503 ↔ EBL#3129
+Lender Amount: 618489.91
+Borrower Amount: 618489.91</t>
+        </is>
+      </c>
       <c r="C885" s="1" t="inlineStr"/>
       <c r="D885" s="1" t="inlineStr"/>
       <c r="E885" s="2" t="inlineStr">
@@ -23103,10 +23191,18 @@
       <c r="I885" s="1" t="inlineStr"/>
       <c r="J885" s="1" t="inlineStr"/>
       <c r="K885" s="1" t="inlineStr"/>
-      <c r="L885" s="1" t="inlineStr"/>
+      <c r="L885" s="1" t="inlineStr">
+        <is>
+          <t>Interunit</t>
+        </is>
+      </c>
     </row>
     <row r="886">
-      <c r="A886" s="1" t="inlineStr"/>
+      <c r="A886" s="1" t="inlineStr">
+        <is>
+          <t>M077</t>
+        </is>
+      </c>
       <c r="B886" s="2" t="inlineStr"/>
       <c r="C886" s="1" t="inlineStr"/>
       <c r="D886" s="1" t="inlineStr">
@@ -23432,7 +23528,11 @@
       <c r="L898" s="1" t="inlineStr"/>
     </row>
     <row r="899">
-      <c r="A899" s="1" t="inlineStr"/>
+      <c r="A899" s="1" t="inlineStr">
+        <is>
+          <t>M078</t>
+        </is>
+      </c>
       <c r="B899" s="2" t="inlineStr"/>
       <c r="C899" s="1" t="inlineStr">
         <is>
@@ -23468,8 +23568,18 @@
       <c r="L899" s="1" t="inlineStr"/>
     </row>
     <row r="900">
-      <c r="A900" s="1" t="inlineStr"/>
-      <c r="B900" s="2" t="inlineStr"/>
+      <c r="A900" s="1" t="inlineStr">
+        <is>
+          <t>M078</t>
+        </is>
+      </c>
+      <c r="B900" s="2" t="inlineStr">
+        <is>
+          <t>Interunit Loan Match: EBL#5503 ↔ EBL#3129
+Lender Amount: 90000.00
+Borrower Amount: 90000.00</t>
+        </is>
+      </c>
       <c r="C900" s="1" t="inlineStr"/>
       <c r="D900" s="1" t="inlineStr"/>
       <c r="E900" s="2" t="inlineStr">
@@ -23483,10 +23593,18 @@
       <c r="I900" s="1" t="inlineStr"/>
       <c r="J900" s="1" t="inlineStr"/>
       <c r="K900" s="1" t="inlineStr"/>
-      <c r="L900" s="1" t="inlineStr"/>
+      <c r="L900" s="1" t="inlineStr">
+        <is>
+          <t>Interunit</t>
+        </is>
+      </c>
     </row>
     <row r="901">
-      <c r="A901" s="1" t="inlineStr"/>
+      <c r="A901" s="1" t="inlineStr">
+        <is>
+          <t>M078</t>
+        </is>
+      </c>
       <c r="B901" s="2" t="inlineStr"/>
       <c r="C901" s="1" t="inlineStr"/>
       <c r="D901" s="1" t="inlineStr">
@@ -24258,7 +24376,11 @@
       <c r="L928" s="1" t="inlineStr"/>
     </row>
     <row r="929">
-      <c r="A929" s="1" t="inlineStr"/>
+      <c r="A929" s="1" t="inlineStr">
+        <is>
+          <t>M079</t>
+        </is>
+      </c>
       <c r="B929" s="2" t="inlineStr"/>
       <c r="C929" s="1" t="inlineStr">
         <is>
@@ -24294,8 +24416,18 @@
       <c r="L929" s="1" t="inlineStr"/>
     </row>
     <row r="930">
-      <c r="A930" s="1" t="inlineStr"/>
-      <c r="B930" s="2" t="inlineStr"/>
+      <c r="A930" s="1" t="inlineStr">
+        <is>
+          <t>M079</t>
+        </is>
+      </c>
+      <c r="B930" s="2" t="inlineStr">
+        <is>
+          <t>Interunit Loan Match: OBL#2451 ↔ MDB#0331
+Lender Amount: 500000.00
+Borrower Amount: 500000.00</t>
+        </is>
+      </c>
       <c r="C930" s="1" t="inlineStr"/>
       <c r="D930" s="1" t="inlineStr"/>
       <c r="E930" s="2" t="inlineStr">
@@ -24309,10 +24441,18 @@
       <c r="I930" s="1" t="inlineStr"/>
       <c r="J930" s="1" t="inlineStr"/>
       <c r="K930" s="1" t="inlineStr"/>
-      <c r="L930" s="1" t="inlineStr"/>
+      <c r="L930" s="1" t="inlineStr">
+        <is>
+          <t>Interunit</t>
+        </is>
+      </c>
     </row>
     <row r="931">
-      <c r="A931" s="1" t="inlineStr"/>
+      <c r="A931" s="1" t="inlineStr">
+        <is>
+          <t>M079</t>
+        </is>
+      </c>
       <c r="B931" s="2" t="inlineStr"/>
       <c r="C931" s="1" t="inlineStr"/>
       <c r="D931" s="1" t="inlineStr">
@@ -26726,7 +26866,11 @@
       <c r="L1021" s="1" t="inlineStr"/>
     </row>
     <row r="1022">
-      <c r="A1022" s="1" t="inlineStr"/>
+      <c r="A1022" s="1" t="inlineStr">
+        <is>
+          <t>M080</t>
+        </is>
+      </c>
       <c r="B1022" s="2" t="inlineStr"/>
       <c r="C1022" s="1" t="inlineStr">
         <is>
@@ -26762,8 +26906,18 @@
       <c r="L1022" s="1" t="inlineStr"/>
     </row>
     <row r="1023">
-      <c r="A1023" s="1" t="inlineStr"/>
-      <c r="B1023" s="2" t="inlineStr"/>
+      <c r="A1023" s="1" t="inlineStr">
+        <is>
+          <t>M080</t>
+        </is>
+      </c>
+      <c r="B1023" s="2" t="inlineStr">
+        <is>
+          <t>Interunit Loan Match: EBL#5503 ↔ EBL#3265
+Lender Amount: 2100000.00
+Borrower Amount: 2100000.00</t>
+        </is>
+      </c>
       <c r="C1023" s="1" t="inlineStr"/>
       <c r="D1023" s="1" t="inlineStr"/>
       <c r="E1023" s="2" t="inlineStr">
@@ -26777,10 +26931,18 @@
       <c r="I1023" s="1" t="inlineStr"/>
       <c r="J1023" s="1" t="inlineStr"/>
       <c r="K1023" s="1" t="inlineStr"/>
-      <c r="L1023" s="1" t="inlineStr"/>
+      <c r="L1023" s="1" t="inlineStr">
+        <is>
+          <t>Interunit</t>
+        </is>
+      </c>
     </row>
     <row r="1024">
-      <c r="A1024" s="1" t="inlineStr"/>
+      <c r="A1024" s="1" t="inlineStr">
+        <is>
+          <t>M080</t>
+        </is>
+      </c>
       <c r="B1024" s="2" t="inlineStr"/>
       <c r="C1024" s="1" t="inlineStr"/>
       <c r="D1024" s="1" t="inlineStr">
@@ -27888,7 +28050,11 @@
       <c r="L1066" s="1" t="inlineStr"/>
     </row>
     <row r="1067">
-      <c r="A1067" s="1" t="inlineStr"/>
+      <c r="A1067" s="1" t="inlineStr">
+        <is>
+          <t>M081</t>
+        </is>
+      </c>
       <c r="B1067" s="2" t="inlineStr"/>
       <c r="C1067" s="1" t="inlineStr">
         <is>
@@ -27924,8 +28090,18 @@
       <c r="L1067" s="1" t="inlineStr"/>
     </row>
     <row r="1068">
-      <c r="A1068" s="1" t="inlineStr"/>
-      <c r="B1068" s="2" t="inlineStr"/>
+      <c r="A1068" s="1" t="inlineStr">
+        <is>
+          <t>M081</t>
+        </is>
+      </c>
+      <c r="B1068" s="2" t="inlineStr">
+        <is>
+          <t>Interunit Loan Match: MDB#11026 ↔ MDB#0331
+Lender Amount: 12000000.00
+Borrower Amount: 12000000.00</t>
+        </is>
+      </c>
       <c r="C1068" s="1" t="inlineStr"/>
       <c r="D1068" s="1" t="inlineStr"/>
       <c r="E1068" s="2" t="inlineStr">
@@ -27939,10 +28115,18 @@
       <c r="I1068" s="1" t="inlineStr"/>
       <c r="J1068" s="1" t="inlineStr"/>
       <c r="K1068" s="1" t="inlineStr"/>
-      <c r="L1068" s="1" t="inlineStr"/>
+      <c r="L1068" s="1" t="inlineStr">
+        <is>
+          <t>Interunit</t>
+        </is>
+      </c>
     </row>
     <row r="1069">
-      <c r="A1069" s="1" t="inlineStr"/>
+      <c r="A1069" s="1" t="inlineStr">
+        <is>
+          <t>M081</t>
+        </is>
+      </c>
       <c r="B1069" s="2" t="inlineStr"/>
       <c r="C1069" s="1" t="inlineStr"/>
       <c r="D1069" s="1" t="inlineStr">

</xml_diff>